<commit_message>
added SDA title and abs
</commit_message>
<xml_diff>
--- a/data/MACSI seminar series.xlsx
+++ b/data/MACSI seminar series.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ulcampus-my.sharepoint.com/personal/david_osullivan_ul_ie/Documents/Academic_work/_Misc/MACSI_Seminars/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ulcampus-my.sharepoint.com/personal/david_osullivan_ul_ie/Documents/Academic_work/_Misc/MACSI_Seminars/macsi-seminars.github.io/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2354" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E0793FFE-932A-41FA-80FD-5AF6B08A1E5A}"/>
+  <xr:revisionPtr revIDLastSave="2380" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F23E4818-1409-4DB5-B371-3E08D86DF036}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AY2023-2024 Sem 2" sheetId="3" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="324">
   <si>
     <t>Fill in as much of the green boxes as possible. Ideally, this would be before you have finished your visitors travel dates (just to avoid double booking).</t>
   </si>
@@ -141,7 +141,7 @@
     <t>Spatial confounding is defined as the confounding between the fixed and spatial random effects in generalized linear mixed models (GLMMs). It gained attention in the past years, as it may generate unexpected results in modeling. We introduce solutions to alleviate the spatial confounding beyond GLMMs for two families of statistical models. In the shared component models, multiple count responses are recorded at each spatial location, which may exhibit similar spatial patterns. Therefore, the spatial effect terms may be shared between the outcomes in addition to specific spatial patterns. Our proposal relies on the use of modified spatial structures for each shared component and specific effects. Spatial frailty models can incorporate spatially structured effects and it is common to observe more than one sample unit per area which means that the support of fixed and spatial effects differs. Thus, we introduce a projection-based approach for reducing the dimension of the data. An R package named "RASCO: An R package to Alleviate Spatial Confounding" is provided. Cases of lung and bronchus cancer in the state of California are investigated under both methodologies and the results prove the efficiency of the proposed methodology.</t>
   </si>
   <si>
-    <t>here</t>
+    <t>https://scholar.google.com.br/citations?user=Ujun714AAAAJ&amp;hl=en</t>
   </si>
   <si>
     <t>N</t>
@@ -166,6 +166,9 @@
 In the talk I will present recent results on how to design and analyse hypocoercivity-preserving Galerkin discretisations, in an effort to port the concept of hypocoercivity in the design and analysis of cutting-edge numerical methods. To that end I plan to start by presenting the first provably hypocoercivity-preserving Galerkin (non-conforming) finite element method for the model problem of Kolmogorov equation and discuss some very recent results on a different approach for the same equation. I plan to conclude with some first results of Galerkin methods for the inhomogeneous  Fokker-Plack equation on exponentially weighted function spaces. Some of the results are joint work with Zhaonan Dong (INRIA, Paris) and Philip Herbert (Sussex). </t>
   </si>
   <si>
+    <t>https://scholar.google.com/citations?user=SgSV1gIAAAAJ&amp;hl=en</t>
+  </si>
+  <si>
     <t>Y</t>
   </si>
   <si>
@@ -179,6 +182,9 @@
   </si>
   <si>
     <t>Coffee is a drink made by dissolving the soluble parts of ground, roast coffee beans in water. In espresso coffee this is done at high temperatures and pressures. It seems obvious that grinding coffee more finely will lead to more coffee being extracted. However, a recent experiment showed that, beyond a cutoff point grinding coffee more finely results in lower extraction. One possible explanation for this is that fine grinding promotes uneven extraction in the coffee bed. To explore this a low dimensional model in which there are two possible pathways for flow and coffee extraction is derived and analysed. This model shows that, below a critical grind size, there is decreasing extraction with decreasing grind size as is seen experimentally. In the model this is due to a complicated interplay between an initial imbalance in the porosities and permeabilities of the two pathways which is increased by flow and extraction, leading to the complete extraction of all soluble coffee from one pathway.</t>
+  </si>
+  <si>
+    <t>https://scholar.google.com/citations?user=fZNoYSMAAAAJ&amp;hl=en</t>
   </si>
   <si>
     <t>Cameron Hall</t>
@@ -191,6 +197,9 @@
 One key tool for ensuring grid stability is mathematical modelling. Models of power grids can be used to estimate the inherent stability of the system, and models can be used to optimise the controllable features of generators to help ensure grid stability. Recent sophisticated optimisation methods have been proposed for finding optimal generator parameters for power grids. In this talk, I will describe some of these optimisation methods and explore some of their strengths and weaknesses. In particular, I will look at how robust the optimisation methods are when certain model parameters are not known exactly, or when multiple generators are combined in a model and treated as a single generator.</t>
   </si>
   <si>
+    <t>https://scholar.google.com/citations?user=MJVJ8pUAAAAJ&amp;hl=en&amp;oi=ao</t>
+  </si>
+  <si>
     <t>8th feb</t>
   </si>
   <si>
@@ -207,6 +216,9 @@
   </si>
   <si>
     <t xml:space="preserve"> In this talk, I will show how tools from statistical physics can be used to study the Earth’s climate. The specific problem addressed is the geophysical-scale evolution of Arctic sea ice. Using an analogy with Brownian motion, the original evolution equation for the sea ice thickness distribution function, g(h), by Thorndike et al. (J. Geophys. Res. 80(33), 4501(1975)) is transformed to a Fokker-Planck-like equation. The steady solution for wintertime is g(h) = N(q, H) * h^q * exp(-h/H), where q and H are expressible in terms of moments over the transition probabilities between thickness categories. This solution exhibits the functional form used in observational fits and shows that for h &lt;&lt; 1, g(h) is controlled by both thermodynamics and mechanics, whereas for h &gt;&gt; 1 only mechanics controls g(h). Furthermore, seasonality is introduced by using the Eisenman-Wettlaufer (Proc. Natl. Acad. Sci. USA 106, 28 (2009)) and Semtner (J. Phys. Oceanogr. 6, 379 (1976)) models for the thermal growth of sea ice. The time-dependent problem is studied by numerically integrating the Fokker-Planck equation. The results obtained from these numerical integrations and their comparison with submarine and satellite observations of ice thickness will also be discussed. </t>
+  </si>
+  <si>
+    <t>https://eps.leeds.ac.uk/maths/staff/10606/dr-srikanth-toppaladoddi</t>
   </si>
   <si>
     <t>2</t>
@@ -252,6 +264,9 @@
     <t>Networks represent complex systems that capture interactions among entities, often resulting in the formation of communities. Additionally, networks frequently depict flows of quantities between nodes. For instance, in the Erasmus programme exchange network, interactions between European countries correspond to volumes of students being transferred among them. When modeling such networks, the exchanged volumes are influenced by the nodes' capacities to send and receive quantities, which can vary significantly across the network and may be associated with uninteresting aspects of the data. In the Erasmus programme network, for example, the volume of outgoing students from a country is limited by the size of its student population. Similarly, the volume of incoming students to a country is associated with the number of universities, which is also related to its student population. Clustering nodes in such networks by directly modeling these volumes often results in clustering solutions that merely reflect the capacities of sending and receiving nodes, masking interesting patterns associated with the relative strength of the connecting flows. We propose a model-based clustering approach that utilizes the relative strength of connections, leveraging concepts from compositional data analysis. We introduce a novel Dirichlet stochastic block model for clustering nodes in networks with compositional edge weights. The model relies on a mixture of Dirichlet distributions, whose parameters are determined by the cluster allocations of sender and receiver nodes, allowing for different propensities for retaining or transferring quantities over the network between the clusters. Consequently, nodes are clustered based on flows as parts of a whole, rather than raw volumes. Inference is implemented using a variation of the classification expectation-maximization algorithm, enabling efficient computations. The model is tested in a number of synthetic data experiments, showing good performance. Furthermore, we showcase the model on two datasets: the Erasmus programme exchange network among European countries and a bike-sharing network for the city of London.</t>
   </si>
   <si>
+    <t>https://scholar.google.com/citations?user=yVUdTdUAAAAJ&amp;hl=en</t>
+  </si>
+  <si>
     <t xml:space="preserve">Y </t>
   </si>
   <si>
@@ -277,6 +292,9 @@
 In this seminar I will present a new theory for wave-driven propulsion based on coupling the equations of motion of a floating raft to a quasi-potential flow model of the fluid. Using this model, expressions are derived for the drift speed and propulsive thrust of the raft which in turn are shown to be consistent with global momentum conservation. The validity of the model is explored by describing the motion of SurferBot, demonstrating close agreement with the experimentally determined drift speed and oscillatory dynamics. The efficiency of wave-driven propulsion is then computed as a function of driving oscillation frequency and the forcing location, revealing optimal values for both of these parameters which await confirmation in experiments. </t>
   </si>
   <si>
+    <t>https://scholar.google.co.uk/citations?user=xupsCdUAAAAJ&amp;hl=en</t>
+  </si>
+  <si>
     <t>27th</t>
   </si>
   <si>
@@ -312,6 +330,12 @@
   </si>
   <si>
     <t>The Arctic is the fastest warming region on Earth. Understanding how a rapidly changing climate change impacts Arctic systems is therefore an important challenge. This is the basis of the `Compost-Bomb' instability, a theorized runaway heating of northern latitude peat soils when atmospheric temperature rises faster than some critical rate, first proposed in [Luke &amp; Cox, European Journal of Soil Science (2011), 62.1] and analysed in [Wieczorek et al, Proceedings of the Royal Society A (2011), 467.2129]. The Compost Bomb instability was one of the first examples of what is known as Rate-induced tipping or R-tipping.The key trigger for the compost bomb instability is heat produced by microbial respiration. Here, the original soil carbon and temperature model of Luke &amp; Cox is augmented with a non-monotone microbial respiration function, for a more realistic representation of the process. This gives rise to a meta-stable state, reproducing the results of [Khvorostyanov et al, Tellus (2008), 60B] where a complex PDE model is used. Two non-autonomous climate forcings are examined: (i) a rise in mean air temperature over decades (ii) a short-lived extreme weather event, with the rate-induced compost bomb observed in each. Using techniques of compactification, singular perturbation theory and desingularisation, we reduce the R-tipping problem to one of heteroclinic orbits, uncovering the tipping mechanism for each climate change scenario.</t>
+  </si>
+  <si>
+    <t>https://scholar.google.com/citations?user=5QMkI0gAAAAJ&amp;hl=en</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/pdf/2210.02376.pdf</t>
   </si>
   <si>
     <t>Ann Smith</t>
@@ -327,6 +351,9 @@
 If system dynamics can be reliably recovered from data along with insights into the complexities of predictive maintenance this will pave the way for a more reliable future.</t>
   </si>
   <si>
+    <t>https://scholar.google.com/citations?user=j_8nzt8AAAAJ&amp;hl=en</t>
+  </si>
+  <si>
     <t>Allan Greenleaf</t>
   </si>
   <si>
@@ -339,6 +366,9 @@
     <t>Multilinear operators arise in a wide range of settings, from pure to applied maths. Estimates for multilinear operators are generally more difficult to obtain than for linear ones. I will discuss a very general `cheap’ method of leveraging known estimates for linear operators to (possibly) get estimates for multilinear ones, and give some examples, focusing on generalized Radon transforms.</t>
   </si>
   <si>
+    <t>https://scholar.google.com/citations?user=obekKC8AAAAJ&amp;hl=en</t>
+  </si>
+  <si>
     <t>Y --- already booked through Niamh</t>
   </si>
   <si>
@@ -370,6 +400,9 @@
   </si>
   <si>
     <t xml:space="preserve">Regression models that incorporate smooth functions of predictor variables to explain the relationships with a response variable have gained widespread usage and proved successful in various applications. By incorporating smooth functions of predictor variables, these models can capture complex relationships between the response and predictors while still allowing for interpretation of the results. In situations where the relationships between a response variable and predictors are explored, it is not uncommon to assume that these relationships adhere to certain shape constraints. Examples of such constraints include monotonicity and convexity.  Shape-constrained additive models (SCAM) offer a general framework for fitting exponential family generalized additive models with shape restrictions on smooths. The main objective of this talk is to provide extensions of the existing framework for SCAM with a mixture of unconstrained terms and various shape-restricted terms to accommodate smooth interaction of covariates, varying coefficient terms, linear functionals with or without shape constraints as model components, and data with short-term temporal or spatial autocorrelation. The practical usage of the suggested extensions will be illustrated in several examples. </t>
+  </si>
+  <si>
+    <t>https://scholar.google.com/citations?user=eoA_1iUAAAAJ&amp;hl=en</t>
   </si>
   <si>
     <t>Natalya's husband (also a statistician) Per Arnqvist will also be visiting and may say a few words too. They are interested in building a collaborative link to UL following their daughter doing Erasmus here.</t>
@@ -781,7 +814,7 @@
     <t>Hlib Husarov &amp; Eberhard Mayerhofer</t>
   </si>
   <si>
-    <t>University of Limerick &amp; Mary Immaculate Secondary School, Lisdoonvarna</t>
+    <t>Mary Immaculate Secondary School, Lisdoonvarna &amp; University of Limerick</t>
   </si>
   <si>
     <t>Eberhard Mayerhofer</t>
@@ -791,6 +824,12 @@
   </si>
   <si>
     <t>We propose a recursive algorithm for identifying all finite sequences of positive integers whose product equals their sum. Our method uses solutions of strictly shorter length that are iteratively extended in pursuit of a valid solution. The algorithm is efficient, with a time complexity similar to the quick sort algorithm. Arxiv: https://arxiv.org/abs/2508.09647</t>
+  </si>
+  <si>
+    <t>https://scholar.google.com/citations?user=N-A7h6EAAAAJ&amp;hl=en</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> https://arxiv.org/abs/2508.09647</t>
   </si>
   <si>
     <t>4pm</t>
@@ -839,6 +878,9 @@
     <t>Queen's University Belfast</t>
   </si>
   <si>
+    <t>Advances in Robust Mixed Effects Modelling</t>
+  </si>
+  <si>
     <t>Oct</t>
   </si>
   <si>
@@ -1026,6 +1068,13 @@
   </si>
   <si>
     <t>Leornard Henckel</t>
+  </si>
+  <si>
+    <t>Clustering high-dimensional discrete data: a compressed approach</t>
+  </si>
+  <si>
+    <t>Custering high-dimensional data is a challenging task, typically addressed in the context of continuous numerical data. Recent literature is exploring strategies to cluster high-dimensional categorical and discrete data, which finds numerous applications, such as RNA sequencing and text data analysis. We propose a fast and easy-to-implement approach to cluster high-dimensional discrete data, scalable to datasets with thousands of dimensions where other strategies may be computationally unfeasible. Our approach relies on reducing the dimension of the data by performing a deterministic compression to a drastically lower dimension. The method employs a lossy compression that reduces the data to a collection of continuous features.
+We demonstrate that such compressed features can be treated as approximately normally distributed, allowing the application of standard finite Gaussian mixture models for model-based clustering. We discuss the approach and study its performance on a series of simulated scenarios with different dimensions and levels of complexity, involving both categorical and count data. Additionally, we illustrate the method on real-world data.</t>
   </si>
 </sst>
 </file>
@@ -1035,7 +1084,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1835,10 +1884,14 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1876,7 +1929,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1982,7 +2035,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2124,7 +2177,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2134,11 +2187,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7958562-D4BB-4776-9668-682A6F2E2AD0}">
   <dimension ref="A1:X20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="11.140625" customWidth="1"/>
@@ -2163,7 +2216,7 @@
     <col min="24" max="24" width="37.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15.75" thickBot="1">
+    <row r="1" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2174,7 +2227,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="15.75" thickBot="1">
+    <row r="2" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -2248,7 +2301,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="13.5" customHeight="1">
+    <row r="3" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>45317</v>
       </c>
@@ -2260,7 +2313,7 @@
         <v>Jan</v>
       </c>
       <c r="D3" s="26" t="str">
-        <f>TEXT(A3, "dddd")</f>
+        <f t="shared" ref="D3:D19" si="1">TEXT(A3, "dddd")</f>
         <v>Friday</v>
       </c>
       <c r="E3" s="27">
@@ -2312,7 +2365,7 @@
       <c r="W3" s="13"/>
       <c r="X3" s="13"/>
     </row>
-    <row r="4" spans="1:24" ht="13.5" customHeight="1">
+    <row r="4" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>45323</v>
       </c>
@@ -2324,7 +2377,7 @@
         <v>Feb</v>
       </c>
       <c r="D4" s="26" t="str">
-        <f>TEXT(A4, "dddd")</f>
+        <f t="shared" si="1"/>
         <v>Thursday</v>
       </c>
       <c r="E4" s="27">
@@ -2344,23 +2397,23 @@
         <v>39</v>
       </c>
       <c r="K4" s="12" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="L4" s="5"/>
       <c r="M4" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="N4" s="13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="O4" s="14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="P4" s="16"/>
       <c r="Q4" s="14"/>
       <c r="R4" s="5"/>
       <c r="S4" s="15" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="T4" s="5" t="s">
         <v>35</v>
@@ -2372,7 +2425,7 @@
       <c r="W4" s="13"/>
       <c r="X4" s="13"/>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>45324</v>
       </c>
@@ -2384,43 +2437,43 @@
         <v>Feb</v>
       </c>
       <c r="D5" s="26" t="str">
-        <f>TEXT(A5, "dddd")</f>
+        <f t="shared" si="1"/>
         <v>Friday</v>
       </c>
       <c r="E5" s="27">
         <v>1</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G5" s="14"/>
       <c r="H5" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="L5" s="5"/>
       <c r="M5" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="N5" s="13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="O5" s="14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="P5" s="16"/>
       <c r="Q5" s="14"/>
       <c r="R5" s="5"/>
       <c r="S5" s="15" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="T5" s="5" t="s">
         <v>35</v>
@@ -2430,7 +2483,7 @@
       <c r="W5" s="13"/>
       <c r="X5" s="13"/>
     </row>
-    <row r="6" spans="1:24" ht="12.75" customHeight="1">
+    <row r="6" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>45331</v>
       </c>
@@ -2442,47 +2495,47 @@
         <v>Feb</v>
       </c>
       <c r="D6" s="26" t="str">
-        <f>TEXT(A6, "dddd")</f>
+        <f t="shared" si="1"/>
         <v>Friday</v>
       </c>
       <c r="E6" s="27">
         <v>2</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G6" s="14"/>
       <c r="H6" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="J6" s="25" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="L6" s="5"/>
       <c r="M6" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="N6" s="13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="O6" s="14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="P6" s="16"/>
       <c r="Q6" s="14" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="R6" s="5" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="S6" s="15" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="T6" s="5" t="s">
         <v>35</v>
@@ -2494,7 +2547,7 @@
       <c r="W6" s="13"/>
       <c r="X6" s="13"/>
     </row>
-    <row r="7" spans="1:24">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>45338</v>
       </c>
@@ -2506,47 +2559,47 @@
         <v>Feb</v>
       </c>
       <c r="D7" s="26" t="str">
-        <f>TEXT(A7, "dddd")</f>
+        <f t="shared" si="1"/>
         <v>Friday</v>
       </c>
       <c r="E7" s="27">
         <v>3</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="G7" s="14"/>
       <c r="H7" s="5" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="L7" s="5"/>
       <c r="M7" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="N7" s="13"/>
       <c r="O7" s="14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="P7" s="16" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="Q7" s="14" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="R7" s="5" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="S7" s="15" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="T7" s="5" t="s">
         <v>35</v>
@@ -2554,13 +2607,13 @@
       <c r="U7" s="16"/>
       <c r="V7" s="14"/>
       <c r="W7" s="13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="X7" s="13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24" ht="15" customHeight="1">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>45345</v>
       </c>
@@ -2572,24 +2625,24 @@
         <v>Feb</v>
       </c>
       <c r="D8" s="26" t="str">
-        <f>TEXT(A8, "dddd")</f>
+        <f t="shared" si="1"/>
         <v>Friday</v>
       </c>
       <c r="E8" s="27">
         <v>4</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="G8" s="14"/>
       <c r="H8" s="5" t="s">
         <v>29</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="J8" s="25" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -2615,16 +2668,16 @@
         <v>34</v>
       </c>
       <c r="T8" s="5" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="U8" s="16"/>
       <c r="V8" s="14"/>
       <c r="W8" s="13"/>
       <c r="X8" s="13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>45359</v>
       </c>
@@ -2636,29 +2689,29 @@
         <v>Mar</v>
       </c>
       <c r="D9" s="26" t="str">
-        <f>TEXT(A9, "dddd")</f>
+        <f t="shared" si="1"/>
         <v>Friday</v>
       </c>
       <c r="E9" s="27">
         <v>6</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="G9" s="14"/>
       <c r="H9" s="5" t="s">
         <v>29</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
       <c r="M9" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="N9" s="13"/>
       <c r="O9" s="14"/>
@@ -2674,7 +2727,7 @@
       <c r="W9" s="13"/>
       <c r="X9" s="13"/>
     </row>
-    <row r="10" spans="1:24">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>45366</v>
       </c>
@@ -2686,53 +2739,53 @@
         <v>Mar</v>
       </c>
       <c r="D10" s="26" t="str">
-        <f>TEXT(A10, "dddd")</f>
+        <f t="shared" si="1"/>
         <v>Friday</v>
       </c>
       <c r="E10" s="27">
         <v>7</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="G10" s="14"/>
       <c r="H10" s="5" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="K10" s="24" t="s">
-        <v>32</v>
+        <v>72</v>
       </c>
       <c r="L10" s="5"/>
       <c r="M10" s="5" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="N10" s="13"/>
       <c r="O10" s="14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="P10" s="16" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="Q10" s="14" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="R10" s="5" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="S10" s="15" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="T10" s="5" t="s">
         <v>35</v>
       </c>
       <c r="U10" s="16" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="V10" s="14" t="s">
         <v>34</v>
@@ -2740,7 +2793,7 @@
       <c r="W10" s="13"/>
       <c r="X10" s="13"/>
     </row>
-    <row r="11" spans="1:24" ht="15" customHeight="1">
+    <row r="11" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>45379</v>
       </c>
@@ -2748,46 +2801,46 @@
         <v>27</v>
       </c>
       <c r="C11" s="26" t="str">
-        <f t="shared" ref="C11:C19" si="1">TEXT(A11, "mmm")</f>
+        <f t="shared" ref="C11:C19" si="2">TEXT(A11, "mmm")</f>
         <v>Mar</v>
       </c>
       <c r="D11" s="26" t="str">
-        <f>TEXT(A11, "dddd")</f>
+        <f t="shared" si="1"/>
         <v>Thursday</v>
       </c>
       <c r="E11" s="28">
         <v>9</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="G11" s="14"/>
       <c r="H11" s="5" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="J11" s="25" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="K11" s="24" t="s">
-        <v>32</v>
+        <v>81</v>
       </c>
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
       <c r="N11" s="13"/>
       <c r="O11" s="14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="P11" s="16" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="Q11" s="14" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="R11" s="5" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="S11" s="15"/>
       <c r="T11" s="5" t="s">
@@ -2798,7 +2851,7 @@
       <c r="W11" s="13"/>
       <c r="X11" s="13"/>
     </row>
-    <row r="12" spans="1:24" ht="13.5" customHeight="1">
+    <row r="12" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>45386</v>
       </c>
@@ -2806,48 +2859,48 @@
         <v>27</v>
       </c>
       <c r="C12" s="26" t="str">
+        <f t="shared" si="2"/>
+        <v>Apr</v>
+      </c>
+      <c r="D12" s="26" t="str">
         <f t="shared" si="1"/>
-        <v>Apr</v>
-      </c>
-      <c r="D12" s="26" t="str">
-        <f>TEXT(A12, "dddd")</f>
         <v>Thursday</v>
       </c>
       <c r="E12" s="27">
         <v>10</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="G12" s="14"/>
       <c r="H12" s="5" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="J12" s="30" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="K12" s="12"/>
       <c r="L12" s="12"/>
       <c r="M12" s="5" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="N12" s="13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="O12" s="14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="P12" s="16" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="Q12" s="14" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="R12" s="5" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="S12" s="15"/>
       <c r="T12" s="5" t="s">
@@ -2858,7 +2911,7 @@
       <c r="W12" s="13"/>
       <c r="X12" s="13"/>
     </row>
-    <row r="13" spans="1:24" ht="16.5" customHeight="1">
+    <row r="13" spans="1:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>45387</v>
       </c>
@@ -2866,37 +2919,37 @@
         <v>27</v>
       </c>
       <c r="C13" s="26" t="str">
+        <f t="shared" si="2"/>
+        <v>Apr</v>
+      </c>
+      <c r="D13" s="26" t="str">
         <f t="shared" si="1"/>
-        <v>Apr</v>
-      </c>
-      <c r="D13" s="26" t="str">
-        <f>TEXT(A13, "dddd")</f>
         <v>Friday</v>
       </c>
       <c r="E13" s="27">
         <v>10</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="G13" s="14"/>
       <c r="H13" s="5" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="K13" s="12" t="s">
-        <v>32</v>
+        <v>94</v>
       </c>
       <c r="L13" s="12" t="s">
-        <v>32</v>
+        <v>95</v>
       </c>
       <c r="M13" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="N13" s="13"/>
       <c r="O13" s="14" t="s">
@@ -2924,7 +2977,7 @@
       <c r="W13" s="13"/>
       <c r="X13" s="13"/>
     </row>
-    <row r="14" spans="1:24" ht="15.75" customHeight="1">
+    <row r="14" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>45394</v>
       </c>
@@ -2932,48 +2985,48 @@
         <v>27</v>
       </c>
       <c r="C14" s="26" t="str">
+        <f t="shared" si="2"/>
+        <v>Apr</v>
+      </c>
+      <c r="D14" s="26" t="str">
         <f t="shared" si="1"/>
-        <v>Apr</v>
-      </c>
-      <c r="D14" s="26" t="str">
-        <f>TEXT(A14, "dddd")</f>
         <v>Friday</v>
       </c>
       <c r="E14" s="27">
         <v>11</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="G14" s="14"/>
       <c r="H14" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I14" s="32" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="J14" s="32" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="K14" s="24" t="s">
-        <v>32</v>
+        <v>99</v>
       </c>
       <c r="L14" s="5"/>
       <c r="M14" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="N14" s="13"/>
       <c r="O14" s="14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="P14" s="16" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="Q14" s="14"/>
       <c r="R14" s="5"/>
       <c r="S14" s="15"/>
       <c r="T14" s="5" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="U14" s="16" t="s">
         <v>34</v>
@@ -2982,7 +3035,7 @@
       <c r="W14" s="13"/>
       <c r="X14" s="13"/>
     </row>
-    <row r="15" spans="1:24" ht="17.25" customHeight="1">
+    <row r="15" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>45398</v>
       </c>
@@ -2990,48 +3043,48 @@
         <v>27</v>
       </c>
       <c r="C15" s="26" t="str">
+        <f t="shared" si="2"/>
+        <v>Apr</v>
+      </c>
+      <c r="D15" s="26" t="str">
         <f t="shared" si="1"/>
-        <v>Apr</v>
-      </c>
-      <c r="D15" s="26" t="str">
-        <f>TEXT(A15, "dddd")</f>
         <v>Tuesday</v>
       </c>
       <c r="E15" s="27">
         <v>12</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="G15" s="14"/>
       <c r="H15" s="5" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="I15" s="33" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="J15" s="33" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="K15" s="31" t="s">
-        <v>32</v>
+        <v>104</v>
       </c>
       <c r="L15" s="5"/>
       <c r="M15" s="5" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="N15" s="13"/>
       <c r="O15" s="14" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="P15" s="16" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="Q15" s="14" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="R15" s="5" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="S15" s="15" t="s">
         <v>34</v>
@@ -3048,7 +3101,7 @@
       <c r="W15" s="13"/>
       <c r="X15" s="13"/>
     </row>
-    <row r="16" spans="1:24" ht="15.75" thickBot="1">
+    <row r="16" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>45401</v>
       </c>
@@ -3056,33 +3109,33 @@
         <v>27</v>
       </c>
       <c r="C16" s="26" t="str">
+        <f t="shared" si="2"/>
+        <v>Apr</v>
+      </c>
+      <c r="D16" s="26" t="str">
         <f t="shared" si="1"/>
-        <v>Apr</v>
-      </c>
-      <c r="D16" s="26" t="str">
-        <f>TEXT(A16, "dddd")</f>
         <v>Friday</v>
       </c>
       <c r="E16" s="27">
         <v>12</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="G16" s="19"/>
       <c r="H16" s="17" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="I16" s="34" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="J16" s="34" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="K16" s="23"/>
       <c r="L16" s="17"/>
       <c r="M16" s="17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="N16" s="18"/>
       <c r="O16" s="19" t="s">
@@ -3103,12 +3156,12 @@
         <v>34</v>
       </c>
       <c r="V16" s="19" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="W16" s="18"/>
       <c r="X16" s="18"/>
     </row>
-    <row r="17" spans="1:24" ht="15.75" thickBot="1">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>45421</v>
       </c>
@@ -3116,31 +3169,31 @@
         <v>27</v>
       </c>
       <c r="C17" s="26" t="str">
+        <f t="shared" si="2"/>
+        <v>May</v>
+      </c>
+      <c r="D17" s="26" t="str">
         <f t="shared" si="1"/>
-        <v>May</v>
-      </c>
-      <c r="D17" s="26" t="str">
-        <f>TEXT(A17, "dddd")</f>
         <v>Thursday</v>
       </c>
       <c r="E17" s="27">
         <v>15</v>
       </c>
       <c r="F17" s="19" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="G17" s="19"/>
       <c r="H17" s="17" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="I17" s="34" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="J17" s="34" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="K17" s="23" t="s">
-        <v>32</v>
+        <v>116</v>
       </c>
       <c r="L17" s="17"/>
       <c r="M17" s="17" t="s">
@@ -3165,18 +3218,18 @@
         <v>34</v>
       </c>
       <c r="T17" s="17" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="U17" s="21" t="s">
         <v>34</v>
       </c>
       <c r="V17" s="19" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="W17" s="18"/>
       <c r="X17" s="18"/>
     </row>
-    <row r="18" spans="1:24" ht="15.75" thickBot="1">
+    <row r="18" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="26">
         <v>45474</v>
       </c>
@@ -3184,28 +3237,28 @@
         <v>27</v>
       </c>
       <c r="C18" s="26" t="str">
+        <f t="shared" si="2"/>
+        <v>Jul</v>
+      </c>
+      <c r="D18" s="26" t="str">
         <f t="shared" si="1"/>
-        <v>Jul</v>
-      </c>
-      <c r="D18" s="26" t="str">
-        <f>TEXT(A18, "dddd")</f>
         <v>Monday</v>
       </c>
       <c r="E18" s="27">
         <v>16</v>
       </c>
       <c r="F18" s="19" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="G18" s="19"/>
       <c r="H18" s="17" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="I18" s="34" t="s">
-        <v>108</v>
+        <v>119</v>
       </c>
       <c r="J18" s="34" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="K18" s="23"/>
       <c r="L18" s="17"/>
@@ -3224,7 +3277,7 @@
       <c r="W18" s="18"/>
       <c r="X18" s="18"/>
     </row>
-    <row r="19" spans="1:24" ht="17.25" customHeight="1" thickBot="1">
+    <row r="19" spans="1:24" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="26">
         <v>45505</v>
       </c>
@@ -3232,28 +3285,28 @@
         <v>27</v>
       </c>
       <c r="C19" s="26" t="str">
+        <f t="shared" si="2"/>
+        <v>Aug</v>
+      </c>
+      <c r="D19" s="26" t="str">
         <f t="shared" si="1"/>
-        <v>Aug</v>
-      </c>
-      <c r="D19" s="26" t="str">
-        <f>TEXT(A19, "dddd")</f>
         <v>Thursday</v>
       </c>
       <c r="E19" s="27">
         <v>19</v>
       </c>
       <c r="F19" s="19" t="s">
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="G19" s="19"/>
       <c r="H19" s="17" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="I19" s="34" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="J19" s="60" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="K19" s="23"/>
       <c r="L19" s="17"/>
@@ -3265,14 +3318,14 @@
       <c r="R19" s="17"/>
       <c r="S19" s="20"/>
       <c r="T19" s="17" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="U19" s="21"/>
       <c r="V19" s="19"/>
       <c r="W19" s="18"/>
       <c r="X19" s="18"/>
     </row>
-    <row r="20" spans="1:24">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="26"/>
       <c r="B20" s="26"/>
       <c r="C20" s="26"/>
@@ -3296,14 +3349,14 @@
     <hyperlink ref="K6" r:id="rId2" xr:uid="{D50B6574-EA67-421C-A06C-511763C2CECC}"/>
     <hyperlink ref="K13" r:id="rId3" xr:uid="{81D25FB2-5DF9-414F-B2AA-D04B200F1303}"/>
     <hyperlink ref="L13" r:id="rId4" xr:uid="{5BC626BC-6B93-4451-B351-1C290775A798}"/>
-    <hyperlink ref="K4" r:id="rId5" xr:uid="{7DA8F1F7-6C53-42A5-8DF1-F69372FA29E1}"/>
-    <hyperlink ref="K3" r:id="rId6" xr:uid="{AA5A6F67-6D40-4017-A0BF-C0555655149E}"/>
-    <hyperlink ref="K7" r:id="rId7" xr:uid="{D594D734-8A49-46FA-9C99-BF312BB87C4C}"/>
-    <hyperlink ref="K10" r:id="rId8" xr:uid="{A42BA110-594C-4702-8BBB-6FEBB117FEB1}"/>
-    <hyperlink ref="K11" r:id="rId9" xr:uid="{CA02B488-FA07-461F-AA14-616AE99D302F}"/>
-    <hyperlink ref="K14" r:id="rId10" xr:uid="{3AEAB718-97D2-4D83-B216-29567CA622BC}"/>
-    <hyperlink ref="K17" r:id="rId11" xr:uid="{1536CC25-4ADA-4A6B-BA94-9CD661751DC8}"/>
-    <hyperlink ref="K15" r:id="rId12" display="https://scholar.google.com/citations?user=obekKC8AAAAJ&amp;hl=en" xr:uid="{76AD086E-ACC7-425D-8974-7A203532CC1B}"/>
+    <hyperlink ref="K3" r:id="rId5" xr:uid="{AA5A6F67-6D40-4017-A0BF-C0555655149E}"/>
+    <hyperlink ref="K7" r:id="rId6" xr:uid="{D594D734-8A49-46FA-9C99-BF312BB87C4C}"/>
+    <hyperlink ref="K10" r:id="rId7" xr:uid="{A42BA110-594C-4702-8BBB-6FEBB117FEB1}"/>
+    <hyperlink ref="K14" r:id="rId8" xr:uid="{3AEAB718-97D2-4D83-B216-29567CA622BC}"/>
+    <hyperlink ref="K17" r:id="rId9" xr:uid="{1536CC25-4ADA-4A6B-BA94-9CD661751DC8}"/>
+    <hyperlink ref="K15" r:id="rId10" xr:uid="{76AD086E-ACC7-425D-8974-7A203532CC1B}"/>
+    <hyperlink ref="K4" r:id="rId11" xr:uid="{7DA8F1F7-6C53-42A5-8DF1-F69372FA29E1}"/>
+    <hyperlink ref="K11" r:id="rId12" xr:uid="{CA02B488-FA07-461F-AA14-616AE99D302F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -3314,11 +3367,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="11.140625" customWidth="1"/>
@@ -3344,7 +3397,7 @@
     <col min="25" max="25" width="37.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="15.75" thickBot="1">
+    <row r="1" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3355,7 +3408,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="30.75" thickBot="1">
+    <row r="2" spans="1:25" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="151" t="s">
         <v>3</v>
       </c>
@@ -3366,7 +3419,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="154" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="E2" s="155" t="s">
         <v>7</v>
@@ -3423,7 +3476,7 @@
         <v>23</v>
       </c>
       <c r="W2" s="39" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="X2" s="46" t="s">
         <v>25</v>
@@ -3432,12 +3485,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="13.5" customHeight="1">
+    <row r="3" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>45548</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="C3" s="26" t="str">
         <f t="shared" ref="C3:C10" si="0">TEXT(A3, "mmm")</f>
@@ -3451,58 +3504,58 @@
         <v>1</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="G3" s="40" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="H3" s="40" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="I3" s="38" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
       <c r="J3" s="14"/>
       <c r="K3" s="63" t="s">
-        <v>119</v>
+        <v>130</v>
       </c>
       <c r="L3" s="43" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="M3" s="40"/>
       <c r="N3" s="38" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
       <c r="O3" s="35"/>
       <c r="P3" s="40" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="Q3" s="40" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
       <c r="R3" s="40" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="S3" s="38" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="T3" s="35"/>
       <c r="U3" s="40" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="V3" s="40"/>
       <c r="W3" s="40" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="X3" s="47"/>
       <c r="Y3" s="45"/>
     </row>
-    <row r="4" spans="1:25" ht="13.5" customHeight="1">
+    <row r="4" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>45555</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="C4" s="26" t="str">
         <f t="shared" si="0"/>
@@ -3516,20 +3569,20 @@
         <v>2</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="I4" s="16" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="J4" s="14"/>
       <c r="K4" s="25" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="L4" s="12"/>
       <c r="M4" s="5"/>
@@ -3546,12 +3599,12 @@
       <c r="X4" s="15"/>
       <c r="Y4" s="13"/>
     </row>
-    <row r="5" spans="1:25" ht="14.25" customHeight="1">
+    <row r="5" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>45562</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="C5" s="26" t="str">
         <f t="shared" si="0"/>
@@ -3565,20 +3618,20 @@
         <v>3</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="I5" s="16" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="J5" s="14"/>
       <c r="K5" s="25" t="s">
-        <v>133</v>
+        <v>144</v>
       </c>
       <c r="L5" s="12"/>
       <c r="M5" s="5"/>
@@ -3595,12 +3648,12 @@
       <c r="X5" s="15"/>
       <c r="Y5" s="13"/>
     </row>
-    <row r="6" spans="1:25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>45576</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="C6" s="26" t="str">
         <f t="shared" si="0"/>
@@ -3614,20 +3667,20 @@
         <v>5</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>134</v>
+        <v>145</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="H6" t="s">
-        <v>136</v>
+        <v>147</v>
       </c>
       <c r="I6" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="J6" s="14"/>
       <c r="K6" s="5" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="L6" s="12"/>
       <c r="M6" s="5"/>
@@ -3644,12 +3697,12 @@
       <c r="X6" s="15"/>
       <c r="Y6" s="13"/>
     </row>
-    <row r="7" spans="1:25" ht="15" customHeight="1">
+    <row r="7" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>45583</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="C7" s="26" t="str">
         <f t="shared" si="0"/>
@@ -3663,20 +3716,20 @@
         <v>6</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>139</v>
+        <v>150</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>141</v>
+        <v>152</v>
       </c>
       <c r="I7" s="16" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
       <c r="J7" s="14"/>
       <c r="K7" s="25" t="s">
-        <v>143</v>
+        <v>154</v>
       </c>
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
@@ -3693,12 +3746,12 @@
       <c r="X7" s="15"/>
       <c r="Y7" s="13"/>
     </row>
-    <row r="8" spans="1:25" ht="14.25" customHeight="1">
+    <row r="8" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>45596</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="C8" s="26" t="str">
         <f t="shared" si="0"/>
@@ -3712,20 +3765,20 @@
         <v>8</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>144</v>
+        <v>155</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>145</v>
+        <v>156</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="I8" s="16" t="s">
-        <v>146</v>
+        <v>157</v>
       </c>
       <c r="J8" s="14"/>
       <c r="K8" s="25" t="s">
-        <v>147</v>
+        <v>158</v>
       </c>
       <c r="L8" s="5"/>
       <c r="M8" s="5"/>
@@ -3742,12 +3795,12 @@
       <c r="X8" s="15"/>
       <c r="Y8" s="13"/>
     </row>
-    <row r="9" spans="1:25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>45604</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="C9" s="26" t="str">
         <f t="shared" si="0"/>
@@ -3761,20 +3814,20 @@
         <v>9</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>149</v>
+        <v>160</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="I9" s="64" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="J9" s="14"/>
       <c r="K9" s="64" t="s">
-        <v>151</v>
+        <v>162</v>
       </c>
       <c r="L9" s="24"/>
       <c r="M9" s="5"/>
@@ -3791,12 +3844,12 @@
       <c r="X9" s="15"/>
       <c r="Y9" s="13"/>
     </row>
-    <row r="10" spans="1:25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>45611</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="C10" s="26" t="str">
         <f t="shared" si="0"/>
@@ -3810,20 +3863,20 @@
         <v>10</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>152</v>
+        <v>163</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>153</v>
+        <v>164</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="I10" s="67" t="s">
-        <v>154</v>
+        <v>165</v>
       </c>
       <c r="J10" s="14"/>
       <c r="K10" s="67" t="s">
-        <v>155</v>
+        <v>166</v>
       </c>
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
@@ -3840,12 +3893,12 @@
       <c r="X10" s="15"/>
       <c r="Y10" s="13"/>
     </row>
-    <row r="11" spans="1:25" ht="13.5" customHeight="1">
+    <row r="11" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>45625</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="C11" s="26" t="str">
         <f t="shared" ref="C11" si="2">TEXT(A11, "mmm")</f>
@@ -3859,20 +3912,20 @@
         <v>12</v>
       </c>
       <c r="F11" s="61" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="G11" s="62" t="s">
-        <v>157</v>
+        <v>168</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="I11" s="62" t="s">
-        <v>158</v>
+        <v>169</v>
       </c>
       <c r="J11" s="42"/>
       <c r="K11" s="62" t="s">
-        <v>159</v>
+        <v>170</v>
       </c>
       <c r="L11" s="12"/>
       <c r="M11" s="12"/>
@@ -3889,12 +3942,12 @@
       <c r="X11" s="15"/>
       <c r="Y11" s="13"/>
     </row>
-    <row r="12" spans="1:25" ht="16.5" customHeight="1" thickBot="1">
+    <row r="12" spans="1:25" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>45632</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="C12" s="48" t="str">
         <f>TEXT(A12, "mmm")</f>
@@ -3908,36 +3961,36 @@
         <v>13</v>
       </c>
       <c r="F12" s="17" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>161</v>
+        <v>172</v>
       </c>
       <c r="H12" s="17" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="I12" s="49" t="s">
-        <v>162</v>
+        <v>173</v>
       </c>
       <c r="J12" s="50"/>
       <c r="K12" s="51" t="s">
-        <v>162</v>
+        <v>173</v>
       </c>
       <c r="L12" s="52"/>
       <c r="M12" s="52"/>
       <c r="N12" s="21"/>
       <c r="O12" s="53"/>
       <c r="P12" s="17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="Q12" s="17" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
       <c r="R12" s="17" t="s">
-        <v>163</v>
+        <v>174</v>
       </c>
       <c r="S12" s="21" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="T12" s="53"/>
       <c r="U12" s="17"/>
@@ -3946,20 +3999,20 @@
       <c r="X12" s="20"/>
       <c r="Y12" s="18"/>
     </row>
-    <row r="13" spans="1:25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="26"/>
       <c r="B13" s="26"/>
       <c r="C13" s="26"/>
       <c r="D13" s="26"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="26"/>
       <c r="B14" s="26"/>
       <c r="C14" s="26"/>
       <c r="D14" s="26"/>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="66"/>
       <c r="B29" s="66"/>
       <c r="C29" s="66"/>
@@ -3972,59 +4025,59 @@
       <c r="J29" s="66"/>
       <c r="K29" s="66"/>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="65"/>
       <c r="B31" s="65"/>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="65"/>
       <c r="B32" s="65"/>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="65"/>
       <c r="B33" s="65"/>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="65"/>
       <c r="B34" s="65"/>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="65"/>
       <c r="B35" s="65"/>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="65"/>
       <c r="B36" s="65"/>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="65"/>
       <c r="B37" s="65"/>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="65"/>
       <c r="B38" s="65"/>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="65"/>
       <c r="B39" s="65"/>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="65"/>
       <c r="B40" s="65"/>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="65"/>
       <c r="B41" s="65"/>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="65"/>
       <c r="B42" s="65"/>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="65"/>
       <c r="B43" s="65"/>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="65"/>
       <c r="B44" s="65"/>
     </row>
@@ -4054,10 +4107,10 @@
   <dimension ref="A1:X45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" customWidth="1"/>
     <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1"/>
@@ -4085,7 +4138,7 @@
     <col min="24" max="24" width="37.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15.75" thickBot="1">
+    <row r="1" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4096,7 +4149,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="27.75" customHeight="1" thickBot="1">
+    <row r="2" spans="1:24" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="70" t="s">
         <v>3</v>
       </c>
@@ -4107,10 +4160,10 @@
         <v>5</v>
       </c>
       <c r="D2" s="84" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="E2" s="70" t="s">
-        <v>165</v>
+        <v>176</v>
       </c>
       <c r="F2" s="146" t="s">
         <v>8</v>
@@ -4161,7 +4214,7 @@
         <v>23</v>
       </c>
       <c r="V2" s="72" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="W2" s="76" t="s">
         <v>25</v>
@@ -4170,15 +4223,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="15" customHeight="1">
+    <row r="3" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>45694</v>
       </c>
       <c r="B3" s="132" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="C3" s="126" t="s">
-        <v>167</v>
+        <v>178</v>
       </c>
       <c r="D3" s="110" t="str">
         <f>TEXT(A3, "dddd")</f>
@@ -4191,14 +4244,14 @@
         <v>37</v>
       </c>
       <c r="G3" s="38" t="s">
-        <v>168</v>
+        <v>179</v>
       </c>
       <c r="H3" s="114"/>
       <c r="I3" s="119" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
       <c r="J3" s="105" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="K3" s="77"/>
       <c r="L3" s="40"/>
@@ -4212,22 +4265,22 @@
       <c r="R3" s="38"/>
       <c r="S3" s="35"/>
       <c r="T3" s="40" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="U3" s="40"/>
       <c r="V3" s="40"/>
       <c r="W3" s="47"/>
       <c r="X3" s="45"/>
     </row>
-    <row r="4" spans="1:24" ht="14.25" customHeight="1">
+    <row r="4" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>45708</v>
       </c>
       <c r="B4" s="133" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="C4" s="127" t="s">
-        <v>167</v>
+        <v>178</v>
       </c>
       <c r="D4" s="109" t="str">
         <f t="shared" ref="D4:D7" si="0">TEXT(A4, "dddd")</f>
@@ -4237,36 +4290,36 @@
         <v>4</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="H4" s="115" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="I4" s="120" t="s">
-        <v>173</v>
+        <v>184</v>
       </c>
       <c r="J4" s="104" t="s">
-        <v>174</v>
+        <v>185</v>
       </c>
       <c r="K4" s="78"/>
       <c r="L4" s="5"/>
       <c r="M4" s="16" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="N4" s="35"/>
       <c r="O4" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="P4" s="5" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
       <c r="Q4" s="5"/>
       <c r="R4" s="16"/>
       <c r="S4" s="35" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="T4" s="5" t="s">
         <v>35</v>
@@ -4276,15 +4329,15 @@
       <c r="W4" s="15"/>
       <c r="X4" s="13"/>
     </row>
-    <row r="5" spans="1:24" ht="14.25" customHeight="1">
+    <row r="5" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>45722</v>
       </c>
       <c r="B5" s="133" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="C5" s="127" t="s">
-        <v>175</v>
+        <v>186</v>
       </c>
       <c r="D5" s="109" t="str">
         <f t="shared" si="0"/>
@@ -4294,22 +4347,22 @@
         <v>6</v>
       </c>
       <c r="F5" s="113" t="s">
-        <v>176</v>
+        <v>187</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>168</v>
+        <v>179</v>
       </c>
       <c r="H5" s="115" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="I5" s="121" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
       <c r="J5" s="106" t="s">
-        <v>179</v>
+        <v>190</v>
       </c>
       <c r="K5" s="78" t="s">
-        <v>180</v>
+        <v>191</v>
       </c>
       <c r="L5" s="5"/>
       <c r="M5" s="16" t="s">
@@ -4331,15 +4384,15 @@
       <c r="W5" s="15"/>
       <c r="X5" s="13"/>
     </row>
-    <row r="6" spans="1:24" ht="16.5" customHeight="1">
+    <row r="6" spans="1:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>45735</v>
       </c>
       <c r="B6" s="133" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="C6" s="127" t="s">
-        <v>175</v>
+        <v>186</v>
       </c>
       <c r="D6" s="109" t="str">
         <f t="shared" si="0"/>
@@ -4349,27 +4402,27 @@
         <v>8</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>181</v>
+        <v>192</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>182</v>
+        <v>193</v>
       </c>
       <c r="H6" s="115" t="s">
-        <v>183</v>
+        <v>194</v>
       </c>
       <c r="I6" s="121" t="s">
-        <v>184</v>
+        <v>195</v>
       </c>
       <c r="J6" s="104" t="s">
-        <v>185</v>
+        <v>196</v>
       </c>
       <c r="K6" s="78"/>
       <c r="L6" s="5"/>
       <c r="M6" s="16" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="N6" s="35" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="O6" s="5" t="s">
         <v>33</v>
@@ -4386,15 +4439,15 @@
       <c r="W6" s="15"/>
       <c r="X6" s="13"/>
     </row>
-    <row r="7" spans="1:24" ht="18" customHeight="1">
+    <row r="7" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>45750</v>
       </c>
       <c r="B7" s="133" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="C7" s="127" t="s">
-        <v>186</v>
+        <v>197</v>
       </c>
       <c r="D7" s="109" t="str">
         <f t="shared" si="0"/>
@@ -4404,19 +4457,19 @@
         <v>10</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>187</v>
+        <v>198</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>168</v>
+        <v>179</v>
       </c>
       <c r="H7" s="115" t="s">
-        <v>188</v>
+        <v>199</v>
       </c>
       <c r="I7" s="121" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
       <c r="J7" s="104" t="s">
-        <v>190</v>
+        <v>201</v>
       </c>
       <c r="K7" s="79"/>
       <c r="L7" s="5"/>
@@ -4439,73 +4492,73 @@
       <c r="W7" s="15"/>
       <c r="X7" s="13"/>
     </row>
-    <row r="8" spans="1:24" ht="16.5" customHeight="1">
+    <row r="8" spans="1:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>45751</v>
       </c>
       <c r="B8" s="133" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="C8" s="128" t="s">
-        <v>186</v>
+        <v>197</v>
       </c>
       <c r="D8" s="109" t="s">
-        <v>191</v>
+        <v>202</v>
       </c>
       <c r="E8" s="109">
         <v>10</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>192</v>
+        <v>203</v>
       </c>
       <c r="G8" s="16" t="s">
-        <v>193</v>
+        <v>204</v>
       </c>
       <c r="H8" s="115" t="s">
-        <v>194</v>
+        <v>205</v>
       </c>
       <c r="I8" s="122" t="s">
-        <v>195</v>
+        <v>206</v>
       </c>
       <c r="J8" s="16" t="s">
-        <v>196</v>
+        <v>207</v>
       </c>
       <c r="K8" s="14"/>
       <c r="L8" s="5"/>
       <c r="M8" s="16" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="N8" s="35"/>
       <c r="O8" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="P8" s="5" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
       <c r="Q8" s="5" t="s">
-        <v>197</v>
+        <v>208</v>
       </c>
       <c r="R8" s="16" t="s">
-        <v>198</v>
+        <v>209</v>
       </c>
       <c r="S8" s="35"/>
       <c r="T8" s="5" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="U8" s="5"/>
       <c r="V8" s="5"/>
       <c r="W8" s="15"/>
       <c r="X8" s="13"/>
     </row>
-    <row r="9" spans="1:24" ht="15.75" customHeight="1">
+    <row r="9" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>45757</v>
       </c>
       <c r="B9" s="133" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="C9" s="127" t="s">
-        <v>186</v>
+        <v>197</v>
       </c>
       <c r="D9" s="109" t="str">
         <f>TEXT(A10, "dddd")</f>
@@ -4515,50 +4568,50 @@
         <v>11</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>199</v>
+        <v>210</v>
       </c>
       <c r="G9" s="16" t="s">
-        <v>200</v>
+        <v>211</v>
       </c>
       <c r="H9" s="115" t="s">
-        <v>201</v>
+        <v>212</v>
       </c>
       <c r="I9" s="121" t="s">
-        <v>202</v>
+        <v>213</v>
       </c>
       <c r="J9" s="104" t="s">
-        <v>203</v>
+        <v>214</v>
       </c>
       <c r="K9" s="79"/>
       <c r="L9" s="5"/>
       <c r="M9" s="16" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="N9" s="35"/>
       <c r="O9" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="P9" s="5" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
       <c r="Q9" s="5" t="s">
-        <v>204</v>
+        <v>215</v>
       </c>
       <c r="R9" s="16" t="s">
-        <v>205</v>
+        <v>216</v>
       </c>
       <c r="S9" s="35" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="T9" s="5" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="U9" s="5"/>
       <c r="V9" s="5"/>
       <c r="W9" s="15"/>
       <c r="X9" s="13"/>
     </row>
-    <row r="10" spans="1:24" ht="15.75" customHeight="1">
+    <row r="10" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>45758</v>
       </c>
@@ -4566,7 +4619,7 @@
         <v>27</v>
       </c>
       <c r="C10" s="127" t="s">
-        <v>186</v>
+        <v>197</v>
       </c>
       <c r="D10" s="109" t="str">
         <f t="shared" ref="D10:D15" si="1">TEXT(A10, "dddd")</f>
@@ -4576,28 +4629,28 @@
         <v>11</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>206</v>
+        <v>217</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>207</v>
+        <v>218</v>
       </c>
       <c r="H10" s="115" t="s">
         <v>29</v>
       </c>
       <c r="I10" s="121" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
       <c r="J10" s="104" t="s">
-        <v>209</v>
+        <v>220</v>
       </c>
       <c r="K10" s="80"/>
       <c r="L10" s="52"/>
       <c r="M10" s="21" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="N10" s="53"/>
       <c r="O10" s="17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="P10" s="17"/>
       <c r="Q10" s="17"/>
@@ -4611,15 +4664,15 @@
       <c r="W10" s="20"/>
       <c r="X10" s="18"/>
     </row>
-    <row r="11" spans="1:24" ht="15.75" customHeight="1">
+    <row r="11" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>45764</v>
       </c>
       <c r="B11" s="134" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="C11" s="129" t="s">
-        <v>186</v>
+        <v>197</v>
       </c>
       <c r="D11" s="111" t="str">
         <f t="shared" si="1"/>
@@ -4629,38 +4682,38 @@
         <v>12</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>210</v>
+        <v>221</v>
       </c>
       <c r="G11" s="21" t="s">
-        <v>211</v>
+        <v>222</v>
       </c>
       <c r="H11" s="116" t="s">
-        <v>212</v>
+        <v>223</v>
       </c>
       <c r="I11" s="123" t="s">
-        <v>213</v>
+        <v>224</v>
       </c>
       <c r="J11" s="118" t="s">
-        <v>214</v>
+        <v>225</v>
       </c>
       <c r="K11" s="78"/>
       <c r="L11" s="78"/>
       <c r="M11" s="14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="N11" s="35" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="O11" s="14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="P11" s="14" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="Q11" s="14"/>
       <c r="R11" s="14"/>
       <c r="S11" s="35" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="T11" s="14" t="s">
         <v>35</v>
@@ -4670,12 +4723,12 @@
       <c r="W11" s="35"/>
       <c r="X11" s="35"/>
     </row>
-    <row r="12" spans="1:24" ht="15.75" customHeight="1">
+    <row r="12" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>45771</v>
       </c>
       <c r="B12" s="134" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="C12" s="130" t="str">
         <f>TEXT(A12,"mmm")</f>
@@ -4689,53 +4742,53 @@
         <v>13</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>215</v>
+        <v>226</v>
       </c>
       <c r="G12" s="16" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="H12" s="115" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="I12" s="120" t="s">
-        <v>216</v>
+        <v>227</v>
       </c>
       <c r="J12" s="104" t="s">
-        <v>217</v>
+        <v>228</v>
       </c>
       <c r="K12" s="78"/>
       <c r="L12" s="78"/>
       <c r="M12" s="14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="N12" s="35" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="O12" s="14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="P12" s="14" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="Q12" s="14"/>
       <c r="R12" s="14"/>
       <c r="S12" s="35" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="T12" s="14" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="U12" s="14"/>
       <c r="V12" s="14"/>
       <c r="W12" s="35"/>
       <c r="X12" s="35"/>
     </row>
-    <row r="13" spans="1:24" ht="15.75" customHeight="1">
+    <row r="13" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>45785</v>
       </c>
       <c r="B13" s="134" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="C13" s="130" t="str">
         <f>TEXT(A13,"mmm")</f>
@@ -4749,26 +4802,26 @@
         <v>15</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>218</v>
+        <v>229</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="H13" s="115" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="I13" s="120" t="s">
-        <v>219</v>
+        <v>230</v>
       </c>
       <c r="J13" s="104" t="s">
-        <v>220</v>
+        <v>231</v>
       </c>
       <c r="K13" s="78"/>
       <c r="L13" s="78"/>
       <c r="M13" s="14"/>
       <c r="N13" s="35"/>
       <c r="O13" s="14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="P13" s="14"/>
       <c r="Q13" s="14"/>
@@ -4782,12 +4835,12 @@
       <c r="W13" s="35"/>
       <c r="X13" s="35"/>
     </row>
-    <row r="14" spans="1:24" ht="15.75" customHeight="1">
+    <row r="14" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>45799</v>
       </c>
       <c r="B14" s="125" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="C14" s="131" t="str">
         <f>TEXT(A14,"mmm")</f>
@@ -4801,25 +4854,25 @@
         <v>17</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>221</v>
+        <v>232</v>
       </c>
       <c r="G14" s="21" t="s">
-        <v>222</v>
+        <v>233</v>
       </c>
       <c r="H14" s="117" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="I14" s="124" t="s">
-        <v>223</v>
+        <v>234</v>
       </c>
       <c r="J14" s="118" t="s">
-        <v>224</v>
+        <v>235</v>
       </c>
       <c r="M14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="O14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="P14">
         <v>2</v>
@@ -4828,7 +4881,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:24" ht="15.75" customHeight="1">
+    <row r="15" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>45805</v>
       </c>
@@ -4847,116 +4900,116 @@
         <v>18</v>
       </c>
       <c r="F15" t="s">
-        <v>225</v>
+        <v>236</v>
       </c>
       <c r="G15" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="H15" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="I15" t="s">
-        <v>226</v>
+        <v>237</v>
       </c>
       <c r="J15" s="135" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="16" spans="1:24" ht="15.75" customHeight="1">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="81"/>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="26"/>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="26"/>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="26"/>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="81"/>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="26"/>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="81"/>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="26"/>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="26"/>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="26"/>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="26"/>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="26"/>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="26"/>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B31" s="65"/>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="65"/>
       <c r="B32" s="65"/>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="65"/>
       <c r="B33" s="65"/>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="65"/>
       <c r="B34" s="65"/>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="65"/>
       <c r="B35" s="65"/>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="65"/>
       <c r="B36" s="65"/>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="65"/>
       <c r="B37" s="65"/>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="65"/>
       <c r="B38" s="65"/>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="65"/>
       <c r="B39" s="65"/>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="65"/>
       <c r="B40" s="65"/>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="65"/>
       <c r="B41" s="65"/>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="65"/>
       <c r="B42" s="65"/>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="65"/>
       <c r="B43" s="65"/>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="65"/>
       <c r="B44" s="65"/>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="65"/>
     </row>
   </sheetData>
@@ -4984,11 +5037,11 @@
   </sheetPr>
   <dimension ref="A1:X16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" customWidth="1"/>
@@ -5015,7 +5068,7 @@
     <col min="24" max="24" width="37.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5026,7 +5079,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="30">
+    <row r="2" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="70" t="s">
         <v>3</v>
       </c>
@@ -5037,10 +5090,10 @@
         <v>5</v>
       </c>
       <c r="D2" s="84" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="E2" s="70" t="s">
-        <v>165</v>
+        <v>176</v>
       </c>
       <c r="F2" s="146" t="s">
         <v>8</v>
@@ -5091,7 +5144,7 @@
         <v>23</v>
       </c>
       <c r="V2" s="72" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="W2" s="76" t="s">
         <v>25</v>
@@ -5100,12 +5153,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="15" customHeight="1" thickBot="1">
+    <row r="3" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="81">
         <v>45911</v>
       </c>
       <c r="B3" s="83" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="C3" s="29" t="str">
         <f>TEXT(A3, "mmm")</f>
@@ -5119,22 +5172,26 @@
         <v>1</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>228</v>
+        <v>239</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>229</v>
+        <v>240</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>230</v>
+        <v>241</v>
       </c>
       <c r="I3" s="104" t="s">
-        <v>231</v>
+        <v>242</v>
       </c>
       <c r="J3" s="104" t="s">
-        <v>232</v>
-      </c>
-      <c r="K3" s="79"/>
-      <c r="L3" s="40"/>
+        <v>243</v>
+      </c>
+      <c r="K3" s="79" t="s">
+        <v>244</v>
+      </c>
+      <c r="L3" s="40" t="s">
+        <v>245</v>
+      </c>
       <c r="M3" s="38"/>
       <c r="N3" s="35" t="s">
         <v>33</v>
@@ -5152,12 +5209,12 @@
       <c r="W3" s="47"/>
       <c r="X3" s="45"/>
     </row>
-    <row r="4" spans="1:24" ht="15" customHeight="1">
+    <row r="4" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="81">
         <v>45917</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>233</v>
+        <v>246</v>
       </c>
       <c r="C4" s="29" t="str">
         <f>TEXT(A4, "mmm")</f>
@@ -5171,19 +5228,19 @@
         <v>2</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>234</v>
+        <v>247</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>235</v>
+        <v>248</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>236</v>
+        <v>249</v>
       </c>
       <c r="I4" s="104" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="J4" s="104" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="K4" s="79"/>
       <c r="L4" s="5"/>
@@ -5200,12 +5257,12 @@
       <c r="W4" s="15"/>
       <c r="X4" s="13"/>
     </row>
-    <row r="5" spans="1:24" ht="15.75" customHeight="1">
+    <row r="5" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="81">
         <v>45926</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>238</v>
+        <v>251</v>
       </c>
       <c r="C5" s="26" t="str">
         <f>TEXT(A5, "mmm")</f>
@@ -5220,19 +5277,19 @@
         <v>3</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>239</v>
+        <v>252</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>240</v>
+        <v>253</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>183</v>
+        <v>194</v>
       </c>
       <c r="I5" s="104" t="s">
-        <v>241</v>
+        <v>254</v>
       </c>
       <c r="J5" s="104" t="s">
-        <v>242</v>
+        <v>255</v>
       </c>
       <c r="K5" s="108"/>
       <c r="L5" s="5"/>
@@ -5251,12 +5308,12 @@
       <c r="W5" s="15"/>
       <c r="X5" s="13"/>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6" spans="1:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="81">
         <v>45939</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="C6" s="26" t="str">
         <f t="shared" ref="C6" si="0">TEXT(A6, "mmm")</f>
@@ -5271,26 +5328,26 @@
         <v>5</v>
       </c>
       <c r="F6" s="107" t="s">
-        <v>243</v>
+        <v>256</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>244</v>
+        <v>257</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="I6" s="102" t="s">
-        <v>237</v>
+        <v>258</v>
       </c>
       <c r="J6" s="106" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="K6" s="108"/>
       <c r="L6" s="5"/>
       <c r="M6" s="16"/>
       <c r="N6" s="35"/>
       <c r="O6" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="P6" s="5"/>
       <c r="Q6" s="5"/>
@@ -5302,36 +5359,36 @@
       <c r="W6" s="15"/>
       <c r="X6" s="13"/>
     </row>
-    <row r="7" spans="1:24" ht="15.75" customHeight="1">
+    <row r="7" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="81">
         <v>45946</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>245</v>
+        <v>259</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>246</v>
+        <v>260</v>
       </c>
       <c r="E7">
         <v>6</v>
       </c>
       <c r="F7" s="107" t="s">
-        <v>247</v>
+        <v>261</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>168</v>
+        <v>179</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>29</v>
       </c>
       <c r="I7" s="103" t="s">
-        <v>248</v>
+        <v>262</v>
       </c>
       <c r="J7" s="106" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="K7" s="108"/>
       <c r="L7" s="5"/>
@@ -5350,12 +5407,12 @@
       <c r="W7" s="15"/>
       <c r="X7" s="13"/>
     </row>
-    <row r="8" spans="1:24">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="81">
         <v>45953</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="C8" s="26" t="str">
         <f>TEXT(A8, "mmm")</f>
@@ -5370,26 +5427,26 @@
         <v>7</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>249</v>
+        <v>263</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>250</v>
+        <v>264</v>
       </c>
       <c r="H8" s="5" t="s">
         <v>29</v>
       </c>
       <c r="I8" s="103" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="J8" s="104" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="K8" s="108"/>
       <c r="L8" s="5"/>
       <c r="M8" s="16"/>
       <c r="N8" s="35"/>
       <c r="O8" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="P8" s="5"/>
       <c r="Q8" s="5"/>
@@ -5401,12 +5458,12 @@
       <c r="W8" s="15"/>
       <c r="X8" s="13"/>
     </row>
-    <row r="9" spans="1:24">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="81">
         <v>45967</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="C9" s="26" t="str">
         <f>TEXT(A9, "mmm")</f>
@@ -5421,19 +5478,19 @@
         <v>9</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>251</v>
+        <v>265</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>240</v>
+        <v>253</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="I9" s="103" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="J9" s="103" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="K9" s="108"/>
       <c r="L9" s="5"/>
@@ -5450,12 +5507,12 @@
       <c r="W9" s="15"/>
       <c r="X9" s="13"/>
     </row>
-    <row r="10" spans="1:24" ht="18.75" customHeight="1">
+    <row r="10" spans="1:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="81">
         <v>45974</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="C10" s="26" t="str">
         <f>TEXT(A10, "mmm")</f>
@@ -5469,26 +5526,26 @@
         <v>10</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>252</v>
+        <v>266</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>253</v>
+        <v>267</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="I10" s="103" t="s">
-        <v>254</v>
+        <v>268</v>
       </c>
       <c r="J10" s="103" t="s">
-        <v>255</v>
+        <v>269</v>
       </c>
       <c r="K10" s="108"/>
       <c r="L10" s="5"/>
       <c r="M10" s="16"/>
       <c r="N10" s="35"/>
       <c r="O10" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="P10" s="5"/>
       <c r="Q10" s="5"/>
@@ -5500,12 +5557,12 @@
       <c r="W10" s="15"/>
       <c r="X10" s="13"/>
     </row>
-    <row r="11" spans="1:24" ht="19.5" customHeight="1">
+    <row r="11" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="81">
         <v>45981</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="C11" s="26" t="str">
         <f>TEXT(A11, "mmm")</f>
@@ -5520,19 +5577,19 @@
         <v>11</v>
       </c>
       <c r="F11" s="16" t="s">
-        <v>256</v>
+        <v>270</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>168</v>
+        <v>179</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="I11" s="103" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="J11" s="106" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="K11" s="14"/>
       <c r="L11" s="5"/>
@@ -5551,12 +5608,12 @@
       <c r="W11" s="15"/>
       <c r="X11" s="13"/>
     </row>
-    <row r="12" spans="1:24" ht="19.5" customHeight="1">
+    <row r="12" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="81">
         <v>45995</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="C12" s="26" t="str">
         <f>TEXT(A12, "mmm")</f>
@@ -5571,26 +5628,26 @@
         <v>13</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>257</v>
+        <v>271</v>
       </c>
       <c r="G12" s="14" t="s">
-        <v>258</v>
+        <v>272</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="I12" s="103" t="s">
-        <v>237</v>
+        <v>322</v>
       </c>
       <c r="J12" s="138" t="s">
-        <v>237</v>
+        <v>323</v>
       </c>
       <c r="K12" s="108"/>
       <c r="L12" s="5"/>
       <c r="M12" s="16"/>
       <c r="N12" s="35"/>
       <c r="O12" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="P12" s="5"/>
       <c r="Q12" s="5"/>
@@ -5602,24 +5659,24 @@
       <c r="W12" s="15"/>
       <c r="X12" s="13"/>
     </row>
-    <row r="13" spans="1:24">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="26"/>
       <c r="B13" s="26"/>
       <c r="C13" s="26"/>
       <c r="W13" s="20"/>
       <c r="X13" s="18"/>
     </row>
-    <row r="14" spans="1:24" ht="12.75" customHeight="1">
+    <row r="14" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="26"/>
       <c r="B14" s="26"/>
       <c r="C14" s="26"/>
     </row>
-    <row r="15" spans="1:24">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="26"/>
       <c r="B15" s="26"/>
       <c r="C15" s="26"/>
     </row>
-    <row r="16" spans="1:24">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="26"/>
       <c r="B16" s="26"/>
       <c r="C16" s="26"/>
@@ -5632,6 +5689,9 @@
     <protectedRange algorithmName="SHA-512" hashValue="BKDH3ki5lE3XQdc5qZnIH6o8wW8E0PkHgMZFCkv/XYDEa+b/qenui0oReDIqPDXHceUVJ+rEgU3I9CDBHraDYg==" saltValue="ruXqG4NOhhm7cSLor8wHfw==" spinCount="100000" sqref="N2:N12" name="Range7_1"/>
     <protectedRange sqref="W13:X13 F3:X12" name="Range8_1"/>
   </protectedRanges>
+  <hyperlinks>
+    <hyperlink ref="K3" r:id="rId1" xr:uid="{CC4847BF-5CC0-41D9-9E80-86D0D78BEFCD}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5644,7 +5704,7 @@
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" customWidth="1"/>
     <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1"/>
@@ -5671,7 +5731,7 @@
     <col min="24" max="24" width="37.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15.75" thickBot="1">
+    <row r="1" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5682,7 +5742,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="30.75" thickBot="1">
+    <row r="2" spans="1:24" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="70" t="s">
         <v>3</v>
       </c>
@@ -5693,10 +5753,10 @@
         <v>5</v>
       </c>
       <c r="D2" s="84" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="E2" s="70" t="s">
-        <v>165</v>
+        <v>176</v>
       </c>
       <c r="F2" s="146" t="s">
         <v>8</v>
@@ -5747,7 +5807,7 @@
         <v>23</v>
       </c>
       <c r="V2" s="72" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="W2" s="76" t="s">
         <v>25</v>
@@ -5756,12 +5816,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="15" customHeight="1">
+    <row r="3" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="81">
         <v>46051</v>
       </c>
       <c r="B3" s="83" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="C3" s="29" t="str">
         <f>TEXT(A3, "mmm")</f>
@@ -5775,19 +5835,19 @@
         <v>1</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>259</v>
+        <v>273</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="I3" s="104" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="J3" s="104" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="K3" s="79"/>
       <c r="L3" s="40"/>
@@ -5808,13 +5868,13 @@
       <c r="W3" s="47"/>
       <c r="X3" s="45"/>
     </row>
-    <row r="4" spans="1:24" ht="15.75" customHeight="1">
+    <row r="4" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="81">
         <f>A3+14</f>
         <v>46065</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="C4" s="26" t="str">
         <f t="shared" ref="C4:C9" si="0">TEXT(A4, "mmm")</f>
@@ -5829,19 +5889,19 @@
         <v>3</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>259</v>
+        <v>273</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="I4" s="104" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="J4" s="104" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="K4" s="108"/>
       <c r="L4" s="5"/>
@@ -5860,13 +5920,13 @@
       <c r="W4" s="15"/>
       <c r="X4" s="13"/>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="81">
         <f t="shared" ref="A5:A9" si="2">A4+14</f>
         <v>46079</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="C5" s="26" t="str">
         <f t="shared" si="0"/>
@@ -5881,26 +5941,26 @@
         <v>5</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>259</v>
+        <v>273</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="I5" s="104" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="J5" s="104" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="K5" s="108"/>
       <c r="L5" s="5"/>
       <c r="M5" s="16"/>
       <c r="N5" s="35"/>
       <c r="O5" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
@@ -5912,13 +5972,13 @@
       <c r="W5" s="15"/>
       <c r="X5" s="13"/>
     </row>
-    <row r="6" spans="1:24" ht="15.75" customHeight="1">
+    <row r="6" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="81">
         <f t="shared" si="2"/>
         <v>46093</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="C6" s="26" t="str">
         <f t="shared" si="0"/>
@@ -5933,19 +5993,19 @@
         <v>7</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>259</v>
+        <v>273</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="I6" s="104" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="J6" s="104" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="K6" s="108"/>
       <c r="L6" s="5"/>
@@ -5964,13 +6024,13 @@
       <c r="W6" s="15"/>
       <c r="X6" s="13"/>
     </row>
-    <row r="7" spans="1:24">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="81">
         <f t="shared" si="2"/>
         <v>46107</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="C7" s="26" t="str">
         <f t="shared" si="0"/>
@@ -5985,26 +6045,26 @@
         <v>9</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>259</v>
+        <v>273</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="I7" s="104" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="J7" s="104" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="K7" s="108"/>
       <c r="L7" s="5"/>
       <c r="M7" s="16"/>
       <c r="N7" s="35"/>
       <c r="O7" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="P7" s="5"/>
       <c r="Q7" s="5"/>
@@ -6016,13 +6076,13 @@
       <c r="W7" s="15"/>
       <c r="X7" s="13"/>
     </row>
-    <row r="8" spans="1:24">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="81">
         <f t="shared" si="2"/>
         <v>46121</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="C8" s="26" t="str">
         <f t="shared" si="0"/>
@@ -6037,19 +6097,19 @@
         <v>11</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>259</v>
+        <v>273</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="I8" s="104" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="J8" s="104" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="K8" s="108"/>
       <c r="L8" s="5"/>
@@ -6066,13 +6126,13 @@
       <c r="W8" s="15"/>
       <c r="X8" s="13"/>
     </row>
-    <row r="9" spans="1:24" ht="18.75" customHeight="1">
+    <row r="9" spans="1:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="81">
         <f t="shared" si="2"/>
         <v>46135</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="C9" s="26" t="str">
         <f t="shared" si="0"/>
@@ -6087,26 +6147,26 @@
         <v>13</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>259</v>
+        <v>273</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="I9" s="104" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="J9" s="104" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="K9" s="108"/>
       <c r="L9" s="5"/>
       <c r="M9" s="16"/>
       <c r="N9" s="35"/>
       <c r="O9" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="P9" s="5"/>
       <c r="Q9" s="5"/>
@@ -6118,24 +6178,24 @@
       <c r="W9" s="15"/>
       <c r="X9" s="13"/>
     </row>
-    <row r="10" spans="1:24" ht="15.75" thickBot="1">
+    <row r="10" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="26"/>
       <c r="B10" s="26"/>
       <c r="C10" s="26"/>
       <c r="W10" s="20"/>
       <c r="X10" s="18"/>
     </row>
-    <row r="11" spans="1:24" ht="12.75" customHeight="1">
+    <row r="11" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="26"/>
       <c r="B11" s="26"/>
       <c r="C11" s="26"/>
     </row>
-    <row r="12" spans="1:24">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="26"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
     </row>
-    <row r="13" spans="1:24">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="26"/>
       <c r="B13" s="26"/>
       <c r="C13" s="26"/>
@@ -6160,231 +6220,231 @@
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.28515625" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
     <col min="3" max="3" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="59" t="s">
-        <v>261</v>
+        <v>275</v>
       </c>
       <c r="B2" s="58" t="s">
-        <v>262</v>
+        <v>276</v>
       </c>
       <c r="C2" s="58" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="142" t="s">
-        <v>264</v>
+        <v>278</v>
       </c>
       <c r="B3" s="143"/>
       <c r="C3" s="144" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>265</v>
+        <v>279</v>
       </c>
       <c r="B4" s="56"/>
       <c r="C4" s="54" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="56" t="s">
-        <v>266</v>
+        <v>280</v>
       </c>
       <c r="B5" s="56"/>
       <c r="C5" s="54" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="56" t="s">
-        <v>268</v>
+        <v>282</v>
       </c>
       <c r="B6" s="56" t="s">
-        <v>269</v>
+        <v>283</v>
       </c>
       <c r="C6" s="54" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="56" t="s">
-        <v>270</v>
+        <v>284</v>
       </c>
       <c r="B7" s="56" t="s">
-        <v>271</v>
+        <v>285</v>
       </c>
       <c r="C7" s="54" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="56" t="s">
-        <v>272</v>
+        <v>286</v>
       </c>
       <c r="B8" s="56" t="s">
-        <v>273</v>
+        <v>287</v>
       </c>
       <c r="C8" s="54" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="56" t="s">
-        <v>274</v>
+        <v>288</v>
       </c>
       <c r="B9" s="56"/>
       <c r="C9" s="54"/>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="56" t="s">
-        <v>275</v>
+        <v>289</v>
       </c>
       <c r="B10" s="56" t="s">
-        <v>276</v>
+        <v>290</v>
       </c>
       <c r="C10" s="54" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="56" t="s">
-        <v>278</v>
+        <v>292</v>
       </c>
       <c r="B11" s="56" t="s">
-        <v>279</v>
+        <v>293</v>
       </c>
       <c r="C11" s="54" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="56" t="s">
-        <v>281</v>
+        <v>295</v>
       </c>
       <c r="B12" s="56" t="s">
-        <v>282</v>
+        <v>296</v>
       </c>
       <c r="C12" s="54" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="56" t="s">
+        <v>297</v>
+      </c>
+      <c r="B13" s="56" t="s">
+        <v>298</v>
+      </c>
+      <c r="C13" s="54" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="56" t="s">
+        <v>299</v>
+      </c>
+      <c r="B14" s="56" t="s">
+        <v>300</v>
+      </c>
+      <c r="C14" s="54" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="56" t="s">
+        <v>301</v>
+      </c>
+      <c r="B15" s="56" t="s">
+        <v>302</v>
+      </c>
+      <c r="C15" s="54" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="143" t="s">
+        <v>271</v>
+      </c>
+      <c r="B16" s="143" t="s">
+        <v>303</v>
+      </c>
+      <c r="C16" s="145" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="56" t="s">
+        <v>305</v>
+      </c>
+      <c r="B17" s="56" t="s">
+        <v>306</v>
+      </c>
+      <c r="C17" s="54" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="56" t="s">
+        <v>307</v>
+      </c>
+      <c r="B18" s="56" t="s">
         <v>283</v>
       </c>
-      <c r="B13" s="56" t="s">
-        <v>284</v>
-      </c>
-      <c r="C13" s="54" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="56" t="s">
-        <v>285</v>
-      </c>
-      <c r="B14" s="56" t="s">
-        <v>286</v>
-      </c>
-      <c r="C14" s="54" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="56" t="s">
-        <v>287</v>
-      </c>
-      <c r="B15" s="56" t="s">
-        <v>288</v>
-      </c>
-      <c r="C15" s="54" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="143" t="s">
-        <v>257</v>
-      </c>
-      <c r="B16" s="143" t="s">
-        <v>289</v>
-      </c>
-      <c r="C16" s="145" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="56" t="s">
-        <v>291</v>
-      </c>
-      <c r="B17" s="56" t="s">
-        <v>292</v>
-      </c>
-      <c r="C17" s="54" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="56" t="s">
-        <v>293</v>
-      </c>
-      <c r="B18" s="56" t="s">
-        <v>269</v>
-      </c>
       <c r="C18" s="54" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="57" t="s">
-        <v>294</v>
+        <v>308</v>
       </c>
       <c r="B19" s="57" t="s">
-        <v>207</v>
+        <v>218</v>
       </c>
       <c r="C19" s="55" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>293</v>
+        <v>307</v>
       </c>
       <c r="B24" t="s">
-        <v>269</v>
+        <v>283</v>
       </c>
       <c r="C24" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>294</v>
+        <v>308</v>
       </c>
       <c r="B25" t="s">
-        <v>207</v>
+        <v>218</v>
       </c>
       <c r="C25" t="s">
-        <v>295</v>
+        <v>309</v>
       </c>
     </row>
   </sheetData>
@@ -6405,24 +6465,24 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
     <col min="6" max="6" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="141" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="137" t="s">
-        <v>297</v>
+        <v>311</v>
       </c>
       <c r="C1" s="136" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="15.75" thickTop="1">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="139">
         <v>45911</v>
       </c>
@@ -6430,13 +6490,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="140" t="s">
-        <v>299</v>
+        <v>313</v>
       </c>
       <c r="F2" s="81">
         <v>45911</v>
       </c>
       <c r="G2" s="83" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="H2" s="29" t="str">
         <f>TEXT(F2, "mmm")</f>
@@ -6450,7 +6510,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="139">
         <f>A2+7</f>
         <v>45918</v>
@@ -6460,13 +6520,13 @@
         <v>2</v>
       </c>
       <c r="C3" s="140" t="s">
-        <v>299</v>
+        <v>313</v>
       </c>
       <c r="F3" s="81">
         <v>45926</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>238</v>
+        <v>251</v>
       </c>
       <c r="H3" s="26" t="str">
         <f>TEXT(F3, "mmm")</f>
@@ -6481,7 +6541,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="139">
         <f t="shared" ref="A4:A12" si="0">A3+7</f>
         <v>45925</v>
@@ -6491,13 +6551,13 @@
         <v>3</v>
       </c>
       <c r="C4" s="140" t="s">
-        <v>299</v>
+        <v>313</v>
       </c>
       <c r="F4" s="81">
         <v>45939</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="H4" s="26" t="str">
         <f t="shared" ref="H4" si="2">TEXT(F4, "mmm")</f>
@@ -6512,7 +6572,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="139">
         <f t="shared" si="0"/>
         <v>45932</v>
@@ -6522,25 +6582,25 @@
         <v>4</v>
       </c>
       <c r="C5" s="140" t="s">
-        <v>299</v>
+        <v>313</v>
       </c>
       <c r="F5" s="81">
         <v>45946</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="H5" s="26" t="s">
-        <v>245</v>
+        <v>259</v>
       </c>
       <c r="I5" s="27" t="s">
-        <v>246</v>
+        <v>260</v>
       </c>
       <c r="J5">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="139">
         <f t="shared" si="0"/>
         <v>45939</v>
@@ -6550,13 +6610,13 @@
         <v>5</v>
       </c>
       <c r="C6" s="140" t="s">
-        <v>299</v>
+        <v>313</v>
       </c>
       <c r="F6" s="81">
         <v>45953</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="H6" s="26" t="str">
         <f>TEXT(F6, "mmm")</f>
@@ -6571,7 +6631,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="139">
         <f t="shared" si="0"/>
         <v>45946</v>
@@ -6581,13 +6641,13 @@
         <v>6</v>
       </c>
       <c r="C7" s="140" t="s">
-        <v>259</v>
+        <v>273</v>
       </c>
       <c r="F7" s="81">
         <v>45967</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="H7" s="26" t="str">
         <f>TEXT(F7, "mmm")</f>
@@ -6602,7 +6662,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="139">
         <f t="shared" si="0"/>
         <v>45953</v>
@@ -6612,13 +6672,13 @@
         <v>7</v>
       </c>
       <c r="C8" s="140" t="s">
-        <v>300</v>
+        <v>314</v>
       </c>
       <c r="F8" s="81">
         <v>45974</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="H8" s="26" t="str">
         <f>TEXT(F8, "mmm")</f>
@@ -6632,7 +6692,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="139">
         <f t="shared" si="0"/>
         <v>45960</v>
@@ -6642,13 +6702,13 @@
         <v>8</v>
       </c>
       <c r="C9" s="140" t="s">
-        <v>299</v>
+        <v>313</v>
       </c>
       <c r="F9" s="81">
         <v>45981</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="H9" s="26" t="str">
         <f>TEXT(F9, "mmm")</f>
@@ -6663,7 +6723,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="139">
         <f t="shared" si="0"/>
         <v>45967</v>
@@ -6673,13 +6733,13 @@
         <v>9</v>
       </c>
       <c r="C10" s="140" t="s">
-        <v>300</v>
+        <v>314</v>
       </c>
       <c r="F10" s="81">
         <v>45995</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="H10" s="26" t="str">
         <f>TEXT(F10, "mmm")</f>
@@ -6694,7 +6754,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="139">
         <f t="shared" si="0"/>
         <v>45974</v>
@@ -6704,10 +6764,10 @@
         <v>10</v>
       </c>
       <c r="C11" s="140" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="139">
         <f t="shared" si="0"/>
         <v>45981</v>
@@ -6717,10 +6777,10 @@
         <v>11</v>
       </c>
       <c r="C12" s="140" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="139">
         <f t="shared" ref="A13:A14" si="6">A12+7</f>
         <v>45988</v>
@@ -6730,10 +6790,10 @@
         <v>12</v>
       </c>
       <c r="C13" s="140" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="139">
         <f t="shared" si="6"/>
         <v>45995</v>
@@ -6743,15 +6803,15 @@
         <v>13</v>
       </c>
       <c r="C14" s="140" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="139"/>
       <c r="B15" s="140"/>
       <c r="C15" s="140"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G16" s="26"/>
     </row>
   </sheetData>
@@ -6782,7 +6842,7 @@
       <selection activeCell="F8" sqref="F8:H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.42578125" customWidth="1"/>
     <col min="2" max="2" width="9.140625" customWidth="1"/>
@@ -6794,17 +6854,17 @@
     <col min="9" max="9" width="64.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" ht="23.25">
+    <row r="2" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="97" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="18.75">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="85" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="37.5">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A5" s="86" t="s">
         <v>3</v>
       </c>
@@ -6815,10 +6875,10 @@
         <v>5</v>
       </c>
       <c r="D5" s="86" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="E5" s="86" t="s">
-        <v>165</v>
+        <v>176</v>
       </c>
       <c r="F5" s="86" t="s">
         <v>8</v>
@@ -6827,24 +6887,24 @@
         <v>9</v>
       </c>
       <c r="H5" s="88" t="s">
-        <v>303</v>
+        <v>317</v>
       </c>
       <c r="I5" s="87" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="18.75">
+    <row r="6" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="98">
         <v>45694</v>
       </c>
       <c r="B6" s="98" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="C6" s="98" t="s">
-        <v>167</v>
+        <v>178</v>
       </c>
       <c r="D6" s="99" t="s">
-        <v>246</v>
+        <v>260</v>
       </c>
       <c r="E6" s="99">
         <v>2</v>
@@ -6853,153 +6913,153 @@
         <v>37</v>
       </c>
       <c r="G6" s="91" t="s">
-        <v>168</v>
+        <v>179</v>
       </c>
       <c r="H6" s="91"/>
       <c r="I6" s="90" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="18.75">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="89">
         <v>45708</v>
       </c>
       <c r="B7" s="89" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="C7" s="89" t="s">
-        <v>167</v>
+        <v>178</v>
       </c>
       <c r="D7" s="100" t="s">
-        <v>246</v>
+        <v>260</v>
       </c>
       <c r="E7" s="100">
         <v>4</v>
       </c>
       <c r="F7" s="93" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="G7" s="93" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="H7" s="93" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="I7" s="92" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="18.75">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="89">
         <v>45722</v>
       </c>
       <c r="B8" s="89" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="C8" s="89" t="s">
-        <v>175</v>
+        <v>186</v>
       </c>
       <c r="D8" s="100" t="s">
-        <v>246</v>
+        <v>260</v>
       </c>
       <c r="E8" s="100">
         <v>6</v>
       </c>
       <c r="F8" s="93" t="s">
-        <v>176</v>
+        <v>187</v>
       </c>
       <c r="G8" s="93" t="s">
-        <v>168</v>
+        <v>179</v>
       </c>
       <c r="H8" s="93" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="I8" s="92"/>
     </row>
-    <row r="9" spans="1:9" ht="18.75">
+    <row r="9" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="89">
         <v>45735</v>
       </c>
       <c r="B9" s="89" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="C9" s="89" t="s">
-        <v>175</v>
+        <v>186</v>
       </c>
       <c r="D9" s="100" t="s">
-        <v>304</v>
+        <v>318</v>
       </c>
       <c r="E9" s="100">
         <v>8</v>
       </c>
       <c r="F9" s="93" t="s">
-        <v>181</v>
+        <v>192</v>
       </c>
       <c r="G9" s="93" t="s">
-        <v>182</v>
+        <v>193</v>
       </c>
       <c r="H9" s="93" t="s">
-        <v>183</v>
+        <v>194</v>
       </c>
       <c r="I9" s="92" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="18.75">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="89">
         <v>45744</v>
       </c>
       <c r="B10" s="89" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="C10" s="89" t="s">
-        <v>175</v>
+        <v>186</v>
       </c>
       <c r="D10" s="100" t="s">
-        <v>191</v>
+        <v>202</v>
       </c>
       <c r="E10" s="100">
         <v>9</v>
       </c>
       <c r="F10" s="93" t="s">
-        <v>199</v>
+        <v>210</v>
       </c>
       <c r="G10" s="93" t="s">
-        <v>200</v>
+        <v>211</v>
       </c>
       <c r="H10" s="93" t="s">
-        <v>201</v>
+        <v>212</v>
       </c>
       <c r="I10" s="92"/>
     </row>
-    <row r="11" spans="1:9" ht="18.75">
+    <row r="11" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="89">
         <v>45750</v>
       </c>
       <c r="B11" s="89" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="C11" s="89" t="s">
-        <v>186</v>
+        <v>197</v>
       </c>
       <c r="D11" s="100" t="s">
-        <v>246</v>
+        <v>260</v>
       </c>
       <c r="E11" s="100">
         <v>10</v>
       </c>
       <c r="F11" s="93" t="s">
-        <v>305</v>
+        <v>319</v>
       </c>
       <c r="G11" s="93" t="s">
-        <v>168</v>
+        <v>179</v>
       </c>
       <c r="H11" s="93"/>
       <c r="I11" s="92" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="18.75">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="89">
         <v>45758</v>
       </c>
@@ -7007,80 +7067,80 @@
         <v>27</v>
       </c>
       <c r="C12" s="89" t="s">
-        <v>186</v>
+        <v>197</v>
       </c>
       <c r="D12" s="100" t="s">
-        <v>191</v>
+        <v>202</v>
       </c>
       <c r="E12" s="100">
         <v>11</v>
       </c>
       <c r="F12" s="93" t="s">
-        <v>206</v>
+        <v>217</v>
       </c>
       <c r="G12" s="93" t="s">
-        <v>149</v>
+        <v>160</v>
       </c>
       <c r="H12" s="93" t="s">
         <v>29</v>
       </c>
       <c r="I12" s="92" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="18.75">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="89">
         <v>45764</v>
       </c>
       <c r="B13" s="89" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="C13" s="89" t="s">
-        <v>186</v>
+        <v>197</v>
       </c>
       <c r="D13" s="100" t="s">
-        <v>246</v>
+        <v>260</v>
       </c>
       <c r="E13" s="100">
         <v>12</v>
       </c>
       <c r="F13" s="93" t="s">
-        <v>306</v>
+        <v>320</v>
       </c>
       <c r="G13" s="93"/>
       <c r="H13" s="93"/>
       <c r="I13" s="92"/>
     </row>
-    <row r="14" spans="1:9" ht="18.75">
+    <row r="14" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="94">
         <v>45771</v>
       </c>
       <c r="B14" s="94" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="C14" s="94" t="s">
-        <v>186</v>
+        <v>197</v>
       </c>
       <c r="D14" s="101" t="s">
-        <v>246</v>
+        <v>260</v>
       </c>
       <c r="E14" s="101">
         <v>13</v>
       </c>
       <c r="F14" s="96" t="s">
-        <v>307</v>
+        <v>321</v>
       </c>
       <c r="G14" s="96" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="H14" s="96" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="I14" s="95" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="20" spans="8:8" ht="18.75">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="20" spans="8:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="H20" s="85"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added logo to tab
</commit_message>
<xml_diff>
--- a/data/MACSI seminar series.xlsx
+++ b/data/MACSI seminar series.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ulcampus-my.sharepoint.com/personal/david_osullivan_ul_ie/Documents/Academic_work/_Misc/MACSI_Seminars/macsi-seminars.github.io/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2383" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{439708A3-D07E-4B8C-81DF-7084FC42DA39}"/>
+  <xr:revisionPtr revIDLastSave="2386" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8A9DB52D-8063-43F8-A830-61E7396B1785}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AY2023-2024 Sem 2" sheetId="3" r:id="rId1"/>
@@ -923,158 +923,158 @@
     <t>Trinity College Dublin</t>
   </si>
   <si>
-    <t>Open</t>
-  </si>
-  <si>
-    <t>This is a just a place for those who are interested but that dont have a specific date in mind. (Ideally, a couple of these are people that we could invite with relatively short notice to fill missing slots.)</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Where are they from?</t>
-  </si>
-  <si>
-    <t>Adacemic Host</t>
-  </si>
-  <si>
-    <t>Colm</t>
-  </si>
-  <si>
-    <t>Niamh Cahill</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Niall Madden </t>
-  </si>
-  <si>
-    <t>Mehakpreet</t>
-  </si>
-  <si>
-    <t>Paul Weaver (invitation sent)</t>
-  </si>
-  <si>
-    <t>UL (Bernal)</t>
-  </si>
-  <si>
-    <t>Eleanor Doman</t>
-  </si>
-  <si>
-    <t>Manchester</t>
-  </si>
-  <si>
-    <t>Connor Hacket</t>
-  </si>
-  <si>
-    <t>MU</t>
-  </si>
-  <si>
-    <t>David Henry (?)</t>
-  </si>
-  <si>
-    <t>Jess Enright</t>
-  </si>
-  <si>
-    <t>Glasgow</t>
-  </si>
-  <si>
-    <t>JS/Networks</t>
-  </si>
-  <si>
-    <t>Ben Swallows</t>
-  </si>
-  <si>
-    <t>St Andrews</t>
-  </si>
-  <si>
-    <t>JS</t>
-  </si>
-  <si>
-    <t>Andrew Finlay</t>
-  </si>
-  <si>
-    <t>Uni Michigan</t>
-  </si>
-  <si>
-    <t>Denis Allard</t>
-  </si>
-  <si>
-    <t>INRAE</t>
-  </si>
-  <si>
-    <t>Nicholas J Clark</t>
-  </si>
-  <si>
-    <t>University of Queensland</t>
-  </si>
-  <si>
-    <t>Andrew Zammit Mangion</t>
-  </si>
-  <si>
-    <t>University of Wollongong</t>
-  </si>
-  <si>
-    <t>Trinity</t>
-  </si>
-  <si>
-    <t>DOS</t>
-  </si>
-  <si>
-    <t>Catherine Higgins</t>
-  </si>
-  <si>
-    <t>UCD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paul Weaver </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Suzanne Fielding </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Doireann O'Kiely and Anthony </t>
-  </si>
-  <si>
-    <t>Possible speaker for next semester</t>
-  </si>
-  <si>
-    <t>Week</t>
-  </si>
-  <si>
-    <t>Speaker</t>
-  </si>
-  <si>
-    <t>Taken</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Taken </t>
-  </si>
-  <si>
-    <t>Seminar Series AY2024-25 Sem 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contact david.osullivan@ul.ie &amp; mehakpreet.singh@ul.ie to book a speaker in. </t>
-  </si>
-  <si>
-    <t>Deptartmental contact</t>
-  </si>
-  <si>
-    <t>Wednesday</t>
-  </si>
-  <si>
-    <t>Robery Garvey</t>
-  </si>
-  <si>
-    <t>Tentative speaker</t>
-  </si>
-  <si>
-    <t>Leornard Henckel</t>
-  </si>
-  <si>
     <t>Clustering high-dimensional discrete data: a compressed approach</t>
   </si>
   <si>
     <t>Custering high-dimensional data is a challenging task, typically addressed in the context of continuous numerical data. Recent literature is exploring strategies to cluster high-dimensional categorical and discrete data, which finds numerous applications, such as RNA sequencing and text data analysis. We propose a fast and easy-to-implement approach to cluster high-dimensional discrete data, scalable to datasets with thousands of dimensions where other strategies may be computationally unfeasible. Our approach relies on reducing the dimension of the data by performing a deterministic compression to a drastically lower dimension. The method employs a lossy compression that reduces the data to a collection of continuous features.
 We demonstrate that such compressed features can be treated as approximately normally distributed, allowing the application of standard finite Gaussian mixture models for model-based clustering. We discuss the approach and study its performance on a series of simulated scenarios with different dimensions and levels of complexity, involving both categorical and count data. Additionally, we illustrate the method on real-world data.</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>This is a just a place for those who are interested but that dont have a specific date in mind. (Ideally, a couple of these are people that we could invite with relatively short notice to fill missing slots.)</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Where are they from?</t>
+  </si>
+  <si>
+    <t>Adacemic Host</t>
+  </si>
+  <si>
+    <t>Colm</t>
+  </si>
+  <si>
+    <t>Niamh Cahill</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Niall Madden </t>
+  </si>
+  <si>
+    <t>Mehakpreet</t>
+  </si>
+  <si>
+    <t>Paul Weaver (invitation sent)</t>
+  </si>
+  <si>
+    <t>UL (Bernal)</t>
+  </si>
+  <si>
+    <t>Eleanor Doman</t>
+  </si>
+  <si>
+    <t>Manchester</t>
+  </si>
+  <si>
+    <t>Connor Hacket</t>
+  </si>
+  <si>
+    <t>MU</t>
+  </si>
+  <si>
+    <t>David Henry (?)</t>
+  </si>
+  <si>
+    <t>Jess Enright</t>
+  </si>
+  <si>
+    <t>Glasgow</t>
+  </si>
+  <si>
+    <t>JS/Networks</t>
+  </si>
+  <si>
+    <t>Ben Swallows</t>
+  </si>
+  <si>
+    <t>St Andrews</t>
+  </si>
+  <si>
+    <t>JS</t>
+  </si>
+  <si>
+    <t>Andrew Finlay</t>
+  </si>
+  <si>
+    <t>Uni Michigan</t>
+  </si>
+  <si>
+    <t>Denis Allard</t>
+  </si>
+  <si>
+    <t>INRAE</t>
+  </si>
+  <si>
+    <t>Nicholas J Clark</t>
+  </si>
+  <si>
+    <t>University of Queensland</t>
+  </si>
+  <si>
+    <t>Andrew Zammit Mangion</t>
+  </si>
+  <si>
+    <t>University of Wollongong</t>
+  </si>
+  <si>
+    <t>Trinity</t>
+  </si>
+  <si>
+    <t>DOS</t>
+  </si>
+  <si>
+    <t>Catherine Higgins</t>
+  </si>
+  <si>
+    <t>UCD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paul Weaver </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suzanne Fielding </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Doireann O'Kiely and Anthony </t>
+  </si>
+  <si>
+    <t>Possible speaker for next semester</t>
+  </si>
+  <si>
+    <t>Week</t>
+  </si>
+  <si>
+    <t>Speaker</t>
+  </si>
+  <si>
+    <t>Taken</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Taken </t>
+  </si>
+  <si>
+    <t>Seminar Series AY2024-25 Sem 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact david.osullivan@ul.ie &amp; mehakpreet.singh@ul.ie to book a speaker in. </t>
+  </si>
+  <si>
+    <t>Deptartmental contact</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>Robery Garvey</t>
+  </si>
+  <si>
+    <t>Tentative speaker</t>
+  </si>
+  <si>
+    <t>Leornard Henckel</t>
   </si>
 </sst>
 </file>
@@ -1084,7 +1084,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1879,9 +1879,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1919,7 +1919,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2025,7 +2025,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2167,7 +2167,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2177,11 +2177,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7958562-D4BB-4776-9668-682A6F2E2AD0}">
   <dimension ref="A1:X20"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="11.140625" customWidth="1"/>
@@ -2206,7 +2206,7 @@
     <col min="24" max="24" width="37.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" ht="15.75" thickBot="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2217,7 +2217,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" ht="15.75" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -2291,7 +2291,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" ht="13.5" customHeight="1">
       <c r="A3" s="2">
         <v>45317</v>
       </c>
@@ -2355,7 +2355,7 @@
       <c r="W3" s="13"/>
       <c r="X3" s="13"/>
     </row>
-    <row r="4" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" ht="13.5" customHeight="1">
       <c r="A4" s="2">
         <v>45323</v>
       </c>
@@ -2415,7 +2415,7 @@
       <c r="W4" s="13"/>
       <c r="X4" s="13"/>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24">
       <c r="A5" s="2">
         <v>45324</v>
       </c>
@@ -2473,7 +2473,7 @@
       <c r="W5" s="13"/>
       <c r="X5" s="13"/>
     </row>
-    <row r="6" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" ht="12.75" customHeight="1">
       <c r="A6" s="2">
         <v>45331</v>
       </c>
@@ -2537,7 +2537,7 @@
       <c r="W6" s="13"/>
       <c r="X6" s="13"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24">
       <c r="A7" s="2">
         <v>45338</v>
       </c>
@@ -2603,7 +2603,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" ht="15" customHeight="1">
       <c r="A8" s="2">
         <v>45345</v>
       </c>
@@ -2667,7 +2667,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24">
       <c r="A9" s="2">
         <v>45359</v>
       </c>
@@ -2717,7 +2717,7 @@
       <c r="W9" s="13"/>
       <c r="X9" s="13"/>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24">
       <c r="A10" s="2">
         <v>45366</v>
       </c>
@@ -2783,7 +2783,7 @@
       <c r="W10" s="13"/>
       <c r="X10" s="13"/>
     </row>
-    <row r="11" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" ht="15" customHeight="1">
       <c r="A11" s="2">
         <v>45379</v>
       </c>
@@ -2841,7 +2841,7 @@
       <c r="W11" s="13"/>
       <c r="X11" s="13"/>
     </row>
-    <row r="12" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" ht="13.5" customHeight="1">
       <c r="A12" s="2">
         <v>45386</v>
       </c>
@@ -2901,7 +2901,7 @@
       <c r="W12" s="13"/>
       <c r="X12" s="13"/>
     </row>
-    <row r="13" spans="1:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" ht="16.5" customHeight="1">
       <c r="A13" s="2">
         <v>45387</v>
       </c>
@@ -2967,7 +2967,7 @@
       <c r="W13" s="13"/>
       <c r="X13" s="13"/>
     </row>
-    <row r="14" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" ht="15.75" customHeight="1">
       <c r="A14" s="2">
         <v>45394</v>
       </c>
@@ -3025,7 +3025,7 @@
       <c r="W14" s="13"/>
       <c r="X14" s="13"/>
     </row>
-    <row r="15" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" ht="17.25" customHeight="1">
       <c r="A15" s="2">
         <v>45398</v>
       </c>
@@ -3091,7 +3091,7 @@
       <c r="W15" s="13"/>
       <c r="X15" s="13"/>
     </row>
-    <row r="16" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" ht="15.75" thickBot="1">
       <c r="A16" s="2">
         <v>45401</v>
       </c>
@@ -3151,7 +3151,7 @@
       <c r="W16" s="18"/>
       <c r="X16" s="18"/>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24">
       <c r="A17" s="4">
         <v>45421</v>
       </c>
@@ -3219,7 +3219,7 @@
       <c r="W17" s="18"/>
       <c r="X17" s="18"/>
     </row>
-    <row r="18" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:24" ht="15.75" thickBot="1">
       <c r="A18" s="26">
         <v>45474</v>
       </c>
@@ -3267,7 +3267,7 @@
       <c r="W18" s="18"/>
       <c r="X18" s="18"/>
     </row>
-    <row r="19" spans="1:24" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:24" ht="17.25" customHeight="1" thickBot="1">
       <c r="A19" s="26">
         <v>45505</v>
       </c>
@@ -3315,7 +3315,7 @@
       <c r="W19" s="18"/>
       <c r="X19" s="18"/>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24">
       <c r="A20" s="26"/>
       <c r="B20" s="26"/>
       <c r="C20" s="26"/>
@@ -3358,10 +3358,10 @@
   <dimension ref="A1:X44"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J1048576"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="11.140625" customWidth="1"/>
@@ -3386,7 +3386,7 @@
     <col min="24" max="24" width="37.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" ht="15.75" thickBot="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3397,7 +3397,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" ht="30.75" thickBot="1">
       <c r="A2" s="149" t="s">
         <v>3</v>
       </c>
@@ -3471,7 +3471,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" ht="13.5" customHeight="1">
       <c r="A3" s="2">
         <v>45548</v>
       </c>
@@ -3535,7 +3535,7 @@
       <c r="W3" s="46"/>
       <c r="X3" s="44"/>
     </row>
-    <row r="4" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" ht="13.5" customHeight="1">
       <c r="A4" s="2">
         <v>45555</v>
       </c>
@@ -3583,7 +3583,7 @@
       <c r="W4" s="15"/>
       <c r="X4" s="13"/>
     </row>
-    <row r="5" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" ht="14.25" customHeight="1">
       <c r="A5" s="2">
         <v>45562</v>
       </c>
@@ -3631,7 +3631,7 @@
       <c r="W5" s="15"/>
       <c r="X5" s="13"/>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24">
       <c r="A6" s="2">
         <v>45576</v>
       </c>
@@ -3679,7 +3679,7 @@
       <c r="W6" s="15"/>
       <c r="X6" s="13"/>
     </row>
-    <row r="7" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" ht="15" customHeight="1">
       <c r="A7" s="2">
         <v>45583</v>
       </c>
@@ -3727,7 +3727,7 @@
       <c r="W7" s="15"/>
       <c r="X7" s="13"/>
     </row>
-    <row r="8" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" ht="14.25" customHeight="1">
       <c r="A8" s="2">
         <v>45596</v>
       </c>
@@ -3775,7 +3775,7 @@
       <c r="W8" s="15"/>
       <c r="X8" s="13"/>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24">
       <c r="A9" s="2">
         <v>45604</v>
       </c>
@@ -3823,7 +3823,7 @@
       <c r="W9" s="15"/>
       <c r="X9" s="13"/>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24">
       <c r="A10" s="2">
         <v>45611</v>
       </c>
@@ -3871,7 +3871,7 @@
       <c r="W10" s="15"/>
       <c r="X10" s="13"/>
     </row>
-    <row r="11" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" ht="13.5" customHeight="1">
       <c r="A11" s="2">
         <v>45625</v>
       </c>
@@ -3919,7 +3919,7 @@
       <c r="W11" s="15"/>
       <c r="X11" s="13"/>
     </row>
-    <row r="12" spans="1:24" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" ht="16.5" customHeight="1" thickBot="1">
       <c r="A12" s="4">
         <v>45632</v>
       </c>
@@ -3975,20 +3975,20 @@
       <c r="W12" s="20"/>
       <c r="X12" s="18"/>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24">
       <c r="A13" s="26"/>
       <c r="B13" s="26"/>
       <c r="C13" s="26"/>
       <c r="D13" s="26"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24">
       <c r="A14" s="26"/>
       <c r="B14" s="26"/>
       <c r="C14" s="26"/>
       <c r="D14" s="26"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10">
       <c r="A29" s="64"/>
       <c r="B29" s="64"/>
       <c r="C29" s="64"/>
@@ -4000,59 +4000,59 @@
       <c r="I29" s="64"/>
       <c r="J29" s="64"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10">
       <c r="A31" s="63"/>
       <c r="B31" s="63"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10">
       <c r="A32" s="63"/>
       <c r="B32" s="63"/>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2">
       <c r="A33" s="63"/>
       <c r="B33" s="63"/>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2">
       <c r="A34" s="63"/>
       <c r="B34" s="63"/>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2">
       <c r="A35" s="63"/>
       <c r="B35" s="63"/>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2">
       <c r="A36" s="63"/>
       <c r="B36" s="63"/>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2">
       <c r="A37" s="63"/>
       <c r="B37" s="63"/>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2">
       <c r="A38" s="63"/>
       <c r="B38" s="63"/>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2">
       <c r="A39" s="63"/>
       <c r="B39" s="63"/>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2">
       <c r="A40" s="63"/>
       <c r="B40" s="63"/>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2">
       <c r="A41" s="63"/>
       <c r="B41" s="63"/>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2">
       <c r="A42" s="63"/>
       <c r="B42" s="63"/>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2">
       <c r="A43" s="63"/>
       <c r="B43" s="63"/>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2">
       <c r="A44" s="63"/>
       <c r="B44" s="63"/>
     </row>
@@ -4085,7 +4085,7 @@
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.5703125" customWidth="1"/>
     <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1"/>
@@ -4113,7 +4113,7 @@
     <col min="24" max="24" width="37.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" ht="15.75" thickBot="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4124,7 +4124,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" ht="27.75" customHeight="1" thickBot="1">
       <c r="A2" s="68" t="s">
         <v>3</v>
       </c>
@@ -4198,7 +4198,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" ht="15" customHeight="1">
       <c r="A3" s="2">
         <v>45694</v>
       </c>
@@ -4247,7 +4247,7 @@
       <c r="W3" s="46"/>
       <c r="X3" s="44"/>
     </row>
-    <row r="4" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" ht="14.25" customHeight="1">
       <c r="A4" s="2">
         <v>45708</v>
       </c>
@@ -4304,7 +4304,7 @@
       <c r="W4" s="15"/>
       <c r="X4" s="13"/>
     </row>
-    <row r="5" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" ht="14.25" customHeight="1">
       <c r="A5" s="2">
         <v>45722</v>
       </c>
@@ -4359,7 +4359,7 @@
       <c r="W5" s="15"/>
       <c r="X5" s="13"/>
     </row>
-    <row r="6" spans="1:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" ht="16.5" customHeight="1">
       <c r="A6" s="2">
         <v>45735</v>
       </c>
@@ -4414,7 +4414,7 @@
       <c r="W6" s="15"/>
       <c r="X6" s="13"/>
     </row>
-    <row r="7" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" ht="18" customHeight="1">
       <c r="A7" s="2">
         <v>45750</v>
       </c>
@@ -4467,7 +4467,7 @@
       <c r="W7" s="15"/>
       <c r="X7" s="13"/>
     </row>
-    <row r="8" spans="1:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" ht="16.5" customHeight="1">
       <c r="A8" s="2">
         <v>45751</v>
       </c>
@@ -4525,7 +4525,7 @@
       <c r="W8" s="15"/>
       <c r="X8" s="13"/>
     </row>
-    <row r="9" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" ht="15.75" customHeight="1">
       <c r="A9" s="2">
         <v>45757</v>
       </c>
@@ -4586,7 +4586,7 @@
       <c r="W9" s="15"/>
       <c r="X9" s="13"/>
     </row>
-    <row r="10" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" ht="15.75" customHeight="1">
       <c r="A10" s="2">
         <v>45758</v>
       </c>
@@ -4639,7 +4639,7 @@
       <c r="W10" s="20"/>
       <c r="X10" s="18"/>
     </row>
-    <row r="11" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" ht="15.75" customHeight="1">
       <c r="A11" s="4">
         <v>45764</v>
       </c>
@@ -4698,7 +4698,7 @@
       <c r="W11" s="35"/>
       <c r="X11" s="35"/>
     </row>
-    <row r="12" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" ht="15.75" customHeight="1">
       <c r="A12" s="4">
         <v>45771</v>
       </c>
@@ -4758,7 +4758,7 @@
       <c r="W12" s="35"/>
       <c r="X12" s="35"/>
     </row>
-    <row r="13" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" ht="15.75" customHeight="1">
       <c r="A13" s="2">
         <v>45785</v>
       </c>
@@ -4810,7 +4810,7 @@
       <c r="W13" s="35"/>
       <c r="X13" s="35"/>
     </row>
-    <row r="14" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" ht="15.75" customHeight="1">
       <c r="A14" s="4">
         <v>45799</v>
       </c>
@@ -4856,7 +4856,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" ht="15.75" customHeight="1">
       <c r="A15" s="4">
         <v>45805</v>
       </c>
@@ -4890,101 +4890,101 @@
         <v>238</v>
       </c>
     </row>
-    <row r="16" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" ht="15.75" customHeight="1">
       <c r="A16" s="79"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="A17" s="26"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2">
       <c r="A18" s="26"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2">
       <c r="A19" s="26"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2">
       <c r="A20" s="79"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2">
       <c r="A21" s="26"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2">
       <c r="A22" s="79"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2">
       <c r="A23" s="26"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2">
       <c r="A24" s="26"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2">
       <c r="A25" s="26"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2">
       <c r="A26" s="26"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2">
       <c r="A27" s="26"/>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2">
       <c r="A28" s="26"/>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2">
       <c r="B31" s="63"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2">
       <c r="A32" s="63"/>
       <c r="B32" s="63"/>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2">
       <c r="A33" s="63"/>
       <c r="B33" s="63"/>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2">
       <c r="A34" s="63"/>
       <c r="B34" s="63"/>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2">
       <c r="A35" s="63"/>
       <c r="B35" s="63"/>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2">
       <c r="A36" s="63"/>
       <c r="B36" s="63"/>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2">
       <c r="A37" s="63"/>
       <c r="B37" s="63"/>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2">
       <c r="A38" s="63"/>
       <c r="B38" s="63"/>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2">
       <c r="A39" s="63"/>
       <c r="B39" s="63"/>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2">
       <c r="A40" s="63"/>
       <c r="B40" s="63"/>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2">
       <c r="A41" s="63"/>
       <c r="B41" s="63"/>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2">
       <c r="A42" s="63"/>
       <c r="B42" s="63"/>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2">
       <c r="A43" s="63"/>
       <c r="B43" s="63"/>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2">
       <c r="A44" s="63"/>
       <c r="B44" s="63"/>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2">
       <c r="A45" s="63"/>
     </row>
   </sheetData>
@@ -5012,11 +5012,11 @@
   </sheetPr>
   <dimension ref="A1:X16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.5703125" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" customWidth="1"/>
@@ -5043,7 +5043,7 @@
     <col min="24" max="24" width="37.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5054,7 +5054,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" ht="30">
       <c r="A2" s="68" t="s">
         <v>3</v>
       </c>
@@ -5128,7 +5128,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" ht="15" customHeight="1" thickBot="1">
       <c r="A3" s="79">
         <v>45911</v>
       </c>
@@ -5184,7 +5184,7 @@
       <c r="W3" s="46"/>
       <c r="X3" s="44"/>
     </row>
-    <row r="4" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" ht="15" customHeight="1">
       <c r="A4" s="79">
         <v>45917</v>
       </c>
@@ -5232,7 +5232,7 @@
       <c r="W4" s="15"/>
       <c r="X4" s="13"/>
     </row>
-    <row r="5" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" ht="15.75" customHeight="1">
       <c r="A5" s="79">
         <v>45926</v>
       </c>
@@ -5283,7 +5283,7 @@
       <c r="W5" s="15"/>
       <c r="X5" s="13"/>
     </row>
-    <row r="6" spans="1:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" ht="16.5" customHeight="1">
       <c r="A6" s="79">
         <v>45939</v>
       </c>
@@ -5334,7 +5334,7 @@
       <c r="W6" s="15"/>
       <c r="X6" s="13"/>
     </row>
-    <row r="7" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" ht="15.75" customHeight="1">
       <c r="A7" s="79">
         <v>45946</v>
       </c>
@@ -5382,7 +5382,7 @@
       <c r="W7" s="15"/>
       <c r="X7" s="13"/>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24">
       <c r="A8" s="79">
         <v>45953</v>
       </c>
@@ -5433,7 +5433,7 @@
       <c r="W8" s="15"/>
       <c r="X8" s="13"/>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24">
       <c r="A9" s="79">
         <v>45967</v>
       </c>
@@ -5482,7 +5482,7 @@
       <c r="W9" s="15"/>
       <c r="X9" s="13"/>
     </row>
-    <row r="10" spans="1:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" ht="18.75" customHeight="1">
       <c r="A10" s="79">
         <v>45974</v>
       </c>
@@ -5532,7 +5532,7 @@
       <c r="W10" s="15"/>
       <c r="X10" s="13"/>
     </row>
-    <row r="11" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" ht="19.5" customHeight="1">
       <c r="A11" s="79">
         <v>45981</v>
       </c>
@@ -5583,7 +5583,7 @@
       <c r="W11" s="15"/>
       <c r="X11" s="13"/>
     </row>
-    <row r="12" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" ht="19.5" customHeight="1">
       <c r="A12" s="79">
         <v>45995</v>
       </c>
@@ -5612,10 +5612,10 @@
         <v>91</v>
       </c>
       <c r="I12" s="101" t="s">
-        <v>322</v>
+        <v>273</v>
       </c>
       <c r="J12" s="136" t="s">
-        <v>323</v>
+        <v>274</v>
       </c>
       <c r="K12" s="106"/>
       <c r="L12" s="5"/>
@@ -5634,24 +5634,24 @@
       <c r="W12" s="15"/>
       <c r="X12" s="13"/>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24">
       <c r="A13" s="26"/>
       <c r="B13" s="26"/>
       <c r="C13" s="26"/>
       <c r="W13" s="20"/>
       <c r="X13" s="18"/>
     </row>
-    <row r="14" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" ht="12.75" customHeight="1">
       <c r="A14" s="26"/>
       <c r="B14" s="26"/>
       <c r="C14" s="26"/>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24">
       <c r="A15" s="26"/>
       <c r="B15" s="26"/>
       <c r="C15" s="26"/>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24">
       <c r="A16" s="26"/>
       <c r="B16" s="26"/>
       <c r="C16" s="26"/>
@@ -5679,7 +5679,7 @@
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.5703125" customWidth="1"/>
     <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1"/>
@@ -5706,7 +5706,7 @@
     <col min="24" max="24" width="37.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" ht="15.75" thickBot="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5717,7 +5717,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" ht="30.75" thickBot="1">
       <c r="A2" s="68" t="s">
         <v>3</v>
       </c>
@@ -5791,7 +5791,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" ht="15" customHeight="1">
       <c r="A3" s="79">
         <v>46051</v>
       </c>
@@ -5810,7 +5810,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="G3" s="14" t="s">
         <v>250</v>
@@ -5843,7 +5843,7 @@
       <c r="W3" s="46"/>
       <c r="X3" s="44"/>
     </row>
-    <row r="4" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" ht="15.75" customHeight="1">
       <c r="A4" s="79">
         <f>A3+14</f>
         <v>46065</v>
@@ -5864,7 +5864,7 @@
         <v>3</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="G4" s="14" t="s">
         <v>250</v>
@@ -5895,7 +5895,7 @@
       <c r="W4" s="15"/>
       <c r="X4" s="13"/>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24">
       <c r="A5" s="79">
         <f t="shared" ref="A5:A9" si="2">A4+14</f>
         <v>46079</v>
@@ -5916,7 +5916,7 @@
         <v>5</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="G5" s="14" t="s">
         <v>250</v>
@@ -5947,7 +5947,7 @@
       <c r="W5" s="15"/>
       <c r="X5" s="13"/>
     </row>
-    <row r="6" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" ht="15.75" customHeight="1">
       <c r="A6" s="79">
         <f t="shared" si="2"/>
         <v>46093</v>
@@ -5968,7 +5968,7 @@
         <v>7</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="G6" s="14" t="s">
         <v>250</v>
@@ -5999,7 +5999,7 @@
       <c r="W6" s="15"/>
       <c r="X6" s="13"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24">
       <c r="A7" s="79">
         <f t="shared" si="2"/>
         <v>46107</v>
@@ -6020,7 +6020,7 @@
         <v>9</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="G7" s="14" t="s">
         <v>250</v>
@@ -6051,7 +6051,7 @@
       <c r="W7" s="15"/>
       <c r="X7" s="13"/>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24">
       <c r="A8" s="79">
         <f t="shared" si="2"/>
         <v>46121</v>
@@ -6072,7 +6072,7 @@
         <v>11</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="G8" s="14" t="s">
         <v>250</v>
@@ -6101,7 +6101,7 @@
       <c r="W8" s="15"/>
       <c r="X8" s="13"/>
     </row>
-    <row r="9" spans="1:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" ht="18.75" customHeight="1">
       <c r="A9" s="79">
         <f t="shared" si="2"/>
         <v>46135</v>
@@ -6122,7 +6122,7 @@
         <v>13</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="G9" s="14" t="s">
         <v>250</v>
@@ -6153,24 +6153,24 @@
       <c r="W9" s="15"/>
       <c r="X9" s="13"/>
     </row>
-    <row r="10" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" ht="15.75" thickBot="1">
       <c r="A10" s="26"/>
       <c r="B10" s="26"/>
       <c r="C10" s="26"/>
       <c r="W10" s="20"/>
       <c r="X10" s="18"/>
     </row>
-    <row r="11" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" ht="12.75" customHeight="1">
       <c r="A11" s="26"/>
       <c r="B11" s="26"/>
       <c r="C11" s="26"/>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24">
       <c r="A12" s="26"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24">
       <c r="A13" s="26"/>
       <c r="B13" s="26"/>
       <c r="C13" s="26"/>
@@ -6195,231 +6195,231 @@
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="31.28515625" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
     <col min="3" max="3" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="57" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="B2" s="56" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="C2" s="56" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="140" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B3" s="141"/>
       <c r="C3" s="142" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="5" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="B4" s="54"/>
       <c r="C4" s="52" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" s="54" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="B5" s="54"/>
       <c r="C5" s="52" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="54" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="B6" s="54" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="C6" s="52" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" s="54" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="B7" s="54" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="C7" s="52" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" s="54" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="B8" s="54" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="C8" s="52" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" s="54" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="B9" s="54"/>
       <c r="C9" s="52"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" s="54" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="B10" s="54" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="C10" s="52" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" s="54" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="B11" s="54" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="C11" s="52" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" s="54" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="B12" s="54" t="s">
+        <v>298</v>
+      </c>
+      <c r="C12" s="52" t="s">
         <v>296</v>
       </c>
-      <c r="C12" s="52" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" s="54" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="B13" s="54" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="C13" s="52" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" s="54" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="B14" s="54" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="C14" s="52" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" s="54" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="B15" s="54" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="C15" s="52" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" s="141" t="s">
         <v>271</v>
       </c>
       <c r="B16" s="141" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="C16" s="143" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" s="54" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="B17" s="54" t="s">
+        <v>308</v>
+      </c>
+      <c r="C17" s="52" t="s">
         <v>306</v>
       </c>
-      <c r="C17" s="52" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" s="54" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="B18" s="54" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="C18" s="52" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="A19" s="55" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="B19" s="55" t="s">
         <v>218</v>
       </c>
       <c r="C19" s="53" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>307</v>
-      </c>
       <c r="B24" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="C24" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="B25" t="s">
         <v>218</v>
       </c>
       <c r="C25" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
     </row>
   </sheetData>
@@ -6440,24 +6440,24 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
     <col min="6" max="6" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1">
       <c r="A1" s="139" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="135" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="C1" s="134" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" thickTop="1">
       <c r="A2" s="137">
         <v>45911</v>
       </c>
@@ -6465,7 +6465,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="138" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="F2" s="79">
         <v>45911</v>
@@ -6485,7 +6485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="137">
         <f>A2+7</f>
         <v>45918</v>
@@ -6495,7 +6495,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="138" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="F3" s="79">
         <v>45926</v>
@@ -6516,7 +6516,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="137">
         <f t="shared" ref="A4:A12" si="0">A3+7</f>
         <v>45925</v>
@@ -6526,7 +6526,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="138" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="F4" s="79">
         <v>45939</v>
@@ -6547,7 +6547,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="137">
         <f t="shared" si="0"/>
         <v>45932</v>
@@ -6557,7 +6557,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="138" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="F5" s="79">
         <v>45946</v>
@@ -6575,7 +6575,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="137">
         <f t="shared" si="0"/>
         <v>45939</v>
@@ -6585,7 +6585,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="138" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="F6" s="79">
         <v>45953</v>
@@ -6606,7 +6606,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" s="137">
         <f t="shared" si="0"/>
         <v>45946</v>
@@ -6616,7 +6616,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="138" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="F7" s="79">
         <v>45967</v>
@@ -6637,7 +6637,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" s="137">
         <f t="shared" si="0"/>
         <v>45953</v>
@@ -6647,7 +6647,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="138" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="F8" s="79">
         <v>45974</v>
@@ -6667,7 +6667,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9" s="137">
         <f t="shared" si="0"/>
         <v>45960</v>
@@ -6677,7 +6677,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="138" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="F9" s="79">
         <v>45981</v>
@@ -6698,7 +6698,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10" s="137">
         <f t="shared" si="0"/>
         <v>45967</v>
@@ -6708,7 +6708,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="138" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="F10" s="79">
         <v>45995</v>
@@ -6729,7 +6729,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" s="137">
         <f t="shared" si="0"/>
         <v>45974</v>
@@ -6739,10 +6739,10 @@
         <v>10</v>
       </c>
       <c r="C11" s="138" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="137">
         <f t="shared" si="0"/>
         <v>45981</v>
@@ -6752,10 +6752,10 @@
         <v>11</v>
       </c>
       <c r="C12" s="138" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" s="137">
         <f t="shared" ref="A13:A14" si="6">A12+7</f>
         <v>45988</v>
@@ -6765,10 +6765,10 @@
         <v>12</v>
       </c>
       <c r="C13" s="138" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" s="137">
         <f t="shared" si="6"/>
         <v>45995</v>
@@ -6778,15 +6778,15 @@
         <v>13</v>
       </c>
       <c r="C14" s="138" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" s="137"/>
       <c r="B15" s="138"/>
       <c r="C15" s="138"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="G16" s="26"/>
     </row>
   </sheetData>
@@ -6817,7 +6817,7 @@
       <selection activeCell="F8" sqref="F8:H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.42578125" customWidth="1"/>
     <col min="2" max="2" width="9.140625" customWidth="1"/>
@@ -6829,17 +6829,17 @@
     <col min="9" max="9" width="64.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="23.25">
       <c r="A2" s="95" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="18.75">
       <c r="A3" s="83" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="37.5" x14ac:dyDescent="0.25">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="37.5">
       <c r="A5" s="84" t="s">
         <v>3</v>
       </c>
@@ -6862,13 +6862,13 @@
         <v>9</v>
       </c>
       <c r="H5" s="86" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="I5" s="85" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="18.75">
       <c r="A6" s="96">
         <v>45694</v>
       </c>
@@ -6895,7 +6895,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="18.75">
       <c r="A7" s="87">
         <v>45708</v>
       </c>
@@ -6924,7 +6924,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="18.75">
       <c r="A8" s="87">
         <v>45722</v>
       </c>
@@ -6951,7 +6951,7 @@
       </c>
       <c r="I8" s="90"/>
     </row>
-    <row r="9" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="18.75">
       <c r="A9" s="87">
         <v>45735</v>
       </c>
@@ -6962,7 +6962,7 @@
         <v>186</v>
       </c>
       <c r="D9" s="98" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="E9" s="98">
         <v>8</v>
@@ -6980,7 +6980,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="18.75">
       <c r="A10" s="87">
         <v>45744</v>
       </c>
@@ -7007,7 +7007,7 @@
       </c>
       <c r="I10" s="90"/>
     </row>
-    <row r="11" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="18.75">
       <c r="A11" s="87">
         <v>45750</v>
       </c>
@@ -7024,7 +7024,7 @@
         <v>10</v>
       </c>
       <c r="F11" s="91" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="G11" s="91" t="s">
         <v>179</v>
@@ -7034,7 +7034,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="18.75">
       <c r="A12" s="87">
         <v>45758</v>
       </c>
@@ -7063,7 +7063,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="18.75">
       <c r="A13" s="87">
         <v>45764</v>
       </c>
@@ -7080,13 +7080,13 @@
         <v>12</v>
       </c>
       <c r="F13" s="91" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="G13" s="91"/>
       <c r="H13" s="91"/>
       <c r="I13" s="90"/>
     </row>
-    <row r="14" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="18.75">
       <c r="A14" s="92">
         <v>45771</v>
       </c>
@@ -7103,7 +7103,7 @@
         <v>13</v>
       </c>
       <c r="F14" s="94" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="G14" s="94" t="s">
         <v>143</v>
@@ -7115,7 +7115,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="20" spans="8:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="20" spans="8:8" ht="18.75">
       <c r="H20" s="83"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added MK title and abs
</commit_message>
<xml_diff>
--- a/data/MACSI seminar series.xlsx
+++ b/data/MACSI seminar series.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ulcampus-my.sharepoint.com/personal/david_osullivan_ul_ie/Documents/Academic_work/_Misc/MACSI_Seminars/macsi-seminars.github.io/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2386" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8A9DB52D-8063-43F8-A830-61E7396B1785}"/>
+  <xr:revisionPtr revIDLastSave="2389" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{93A4A704-73F9-40D0-AD98-57F2C22CB133}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AY2023-2024 Sem 2" sheetId="3" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="824" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="327">
   <si>
     <t>Fill in as much of the green boxes as possible. Ideally, this would be before you have finished your visitors travel dates (just to avoid double booking).</t>
   </si>
@@ -844,7 +844,13 @@
     <t>Padraig McCarron</t>
   </si>
   <si>
-    <t>TBC</t>
+    <t>Behaviour-driven epidemic phenomena in heterogeneous populations and networks</t>
+  </si>
+  <si>
+    <t>While realistic approaches have become increasingly important in epidemic modelling, behavioural factors and individual differences have historically been overlooked due to the lack of high-resolution data and appropriate mathematical methods. This gap became particularly evident during the recent pandemic, highlighting the need for large-scale data collection on individual-level epidemic-related behaviours across representative populations. These advancements have revealed several new and interesting spreading phenomena that challenge our previous understandings. In this talk, we will focus on a few examples of such new insights, derived from data-driven and behaviour-informed epidemic models. We will explore the effects of seeding strategies and input-output inequalities in spreading dynamics, and the paradoxical effects of awareness-driven adaptive behaviour on epidemic outcomes. These findings highlight the importance of data-driven models incorporating behavioural factors, offering a more accurate understanding and modelling of real-world epidemic scenarios.</t>
+  </si>
+  <si>
+    <t>https://scholar.google.com/citations?user=Pl9cdEYAAAAJ&amp;hl=en</t>
   </si>
   <si>
     <t>3pm</t>
@@ -879,6 +885,9 @@
   </si>
   <si>
     <t>Advances in Robust Mixed Effects Modelling</t>
+  </si>
+  <si>
+    <t>TBC</t>
   </si>
   <si>
     <t>Oct</t>
@@ -2177,8 +2186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7958562-D4BB-4776-9668-682A6F2E2AD0}">
   <dimension ref="A1:X20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5012,8 +5021,8 @@
   </sheetPr>
   <dimension ref="A1:X16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5215,9 +5224,11 @@
         <v>250</v>
       </c>
       <c r="J4" s="102" t="s">
-        <v>250</v>
-      </c>
-      <c r="K4" s="77"/>
+        <v>251</v>
+      </c>
+      <c r="K4" s="77" t="s">
+        <v>252</v>
+      </c>
       <c r="L4" s="5"/>
       <c r="M4" s="16"/>
       <c r="N4" s="35"/>
@@ -5237,7 +5248,7 @@
         <v>45926</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C5" s="26" t="str">
         <f>TEXT(A5, "mmm")</f>
@@ -5252,19 +5263,19 @@
         <v>3</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>194</v>
       </c>
       <c r="I5" s="102" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="J5" s="102" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="K5" s="106"/>
       <c r="L5" s="5"/>
@@ -5303,19 +5314,19 @@
         <v>5</v>
       </c>
       <c r="F6" s="105" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>69</v>
       </c>
       <c r="I6" s="100" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="J6" s="104" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="K6" s="106"/>
       <c r="L6" s="5"/>
@@ -5342,16 +5353,16 @@
         <v>177</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="E7">
         <v>6</v>
       </c>
       <c r="F7" s="105" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="G7" s="14" t="s">
         <v>179</v>
@@ -5360,10 +5371,10 @@
         <v>29</v>
       </c>
       <c r="I7" s="101" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="J7" s="104" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="K7" s="106"/>
       <c r="L7" s="5"/>
@@ -5402,19 +5413,19 @@
         <v>7</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="H8" s="5" t="s">
         <v>29</v>
       </c>
       <c r="I8" s="101" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="J8" s="102" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="K8" s="106"/>
       <c r="L8" s="5"/>
@@ -5453,19 +5464,19 @@
         <v>9</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="H9" s="5" t="s">
         <v>188</v>
       </c>
       <c r="I9" s="101" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="J9" s="101" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="K9" s="106"/>
       <c r="L9" s="5"/>
@@ -5501,19 +5512,19 @@
         <v>10</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="H10" s="5" t="s">
         <v>113</v>
       </c>
       <c r="I10" s="101" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="J10" s="101" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="K10" s="106"/>
       <c r="L10" s="5"/>
@@ -5552,7 +5563,7 @@
         <v>11</v>
       </c>
       <c r="F11" s="16" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="G11" s="14" t="s">
         <v>179</v>
@@ -5561,10 +5572,10 @@
         <v>91</v>
       </c>
       <c r="I11" s="101" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="J11" s="104" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="K11" s="14"/>
       <c r="L11" s="5"/>
@@ -5603,19 +5614,19 @@
         <v>13</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="G12" s="14" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="H12" s="5" t="s">
         <v>91</v>
       </c>
       <c r="I12" s="101" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="J12" s="136" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="K12" s="106"/>
       <c r="L12" s="5"/>
@@ -5666,6 +5677,7 @@
   </protectedRanges>
   <hyperlinks>
     <hyperlink ref="K3" r:id="rId1" xr:uid="{CC4847BF-5CC0-41D9-9E80-86D0D78BEFCD}"/>
+    <hyperlink ref="K4" r:id="rId2" xr:uid="{7DFE3762-8F5E-4F84-9CA0-19AC05FFD4B0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5810,19 +5822,19 @@
         <v>1</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="I3" s="102" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="J3" s="102" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="K3" s="77"/>
       <c r="L3" s="40"/>
@@ -5864,19 +5876,19 @@
         <v>3</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="I4" s="102" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="J4" s="102" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="K4" s="106"/>
       <c r="L4" s="5"/>
@@ -5916,19 +5928,19 @@
         <v>5</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="I5" s="102" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="J5" s="102" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="K5" s="106"/>
       <c r="L5" s="5"/>
@@ -5968,19 +5980,19 @@
         <v>7</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="I6" s="102" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="J6" s="102" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="K6" s="106"/>
       <c r="L6" s="5"/>
@@ -6020,19 +6032,19 @@
         <v>9</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="I7" s="102" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="J7" s="102" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="K7" s="106"/>
       <c r="L7" s="5"/>
@@ -6072,19 +6084,19 @@
         <v>11</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="I8" s="102" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="J8" s="102" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="K8" s="106"/>
       <c r="L8" s="5"/>
@@ -6122,19 +6134,19 @@
         <v>13</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="I9" s="102" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="J9" s="102" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="K9" s="106"/>
       <c r="L9" s="5"/>
@@ -6204,23 +6216,23 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="57" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="B2" s="56" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="C2" s="56" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="140" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="B3" s="141"/>
       <c r="C3" s="142" t="s">
@@ -6229,7 +6241,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="5" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="B4" s="54"/>
       <c r="C4" s="52" t="s">
@@ -6238,19 +6250,19 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="54" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="B5" s="54"/>
       <c r="C5" s="52" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="54" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="B6" s="54" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="C6" s="52" t="s">
         <v>78</v>
@@ -6258,10 +6270,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="54" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="B7" s="54" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="C7" s="52" t="s">
         <v>78</v>
@@ -6269,10 +6281,10 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="54" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="B8" s="54" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="C8" s="52" t="s">
         <v>91</v>
@@ -6280,105 +6292,105 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="54" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="B9" s="54"/>
       <c r="C9" s="52"/>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="54" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="B10" s="54" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="C10" s="52" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="54" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="B11" s="54" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="C11" s="52" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="54" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="B12" s="54" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="C12" s="52" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="54" t="s">
+        <v>302</v>
+      </c>
+      <c r="B13" s="54" t="s">
+        <v>303</v>
+      </c>
+      <c r="C13" s="52" t="s">
         <v>299</v>
-      </c>
-      <c r="B13" s="54" t="s">
-        <v>300</v>
-      </c>
-      <c r="C13" s="52" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="54" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="B14" s="54" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="C14" s="52" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="54" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="B15" s="54" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="C15" s="52" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="141" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="B16" s="141" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="C16" s="143" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="54" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="B17" s="54" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="C17" s="52" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="54" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="B18" s="54" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="C18" s="52" t="s">
         <v>78</v>
@@ -6386,26 +6398,26 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="55" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="B19" s="55" t="s">
         <v>218</v>
       </c>
       <c r="C19" s="53" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="B24" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="C24" t="s">
         <v>78</v>
@@ -6413,13 +6425,13 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="B25" t="s">
         <v>218</v>
       </c>
       <c r="C25" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
     </row>
   </sheetData>
@@ -6451,10 +6463,10 @@
         <v>3</v>
       </c>
       <c r="B1" s="135" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="C1" s="134" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickTop="1">
@@ -6465,7 +6477,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="138" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="F2" s="79">
         <v>45911</v>
@@ -6495,13 +6507,13 @@
         <v>2</v>
       </c>
       <c r="C3" s="138" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="F3" s="79">
         <v>45926</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="H3" s="26" t="str">
         <f>TEXT(F3, "mmm")</f>
@@ -6526,7 +6538,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="138" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="F4" s="79">
         <v>45939</v>
@@ -6557,7 +6569,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="138" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="F5" s="79">
         <v>45946</v>
@@ -6566,10 +6578,10 @@
         <v>177</v>
       </c>
       <c r="H5" s="26" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="I5" s="27" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="J5">
         <v>6</v>
@@ -6585,7 +6597,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="138" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="F6" s="79">
         <v>45953</v>
@@ -6616,7 +6628,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="138" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="F7" s="79">
         <v>45967</v>
@@ -6647,7 +6659,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="138" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="F8" s="79">
         <v>45974</v>
@@ -6677,7 +6689,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="138" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="F9" s="79">
         <v>45981</v>
@@ -6708,7 +6720,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="138" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="F10" s="79">
         <v>45995</v>
@@ -6739,7 +6751,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="138" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -6752,7 +6764,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="138" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -6765,7 +6777,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="138" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -6778,7 +6790,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="138" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -6831,12 +6843,12 @@
   <sheetData>
     <row r="2" spans="1:9" ht="23.25">
       <c r="A2" s="95" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="18.75">
       <c r="A3" s="83" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="37.5">
@@ -6862,7 +6874,7 @@
         <v>9</v>
       </c>
       <c r="H5" s="86" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="I5" s="85" t="s">
         <v>11</v>
@@ -6879,7 +6891,7 @@
         <v>178</v>
       </c>
       <c r="D6" s="97" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="E6" s="97">
         <v>2</v>
@@ -6892,7 +6904,7 @@
       </c>
       <c r="H6" s="89"/>
       <c r="I6" s="88" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="18.75">
@@ -6906,7 +6918,7 @@
         <v>178</v>
       </c>
       <c r="D7" s="98" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="E7" s="98">
         <v>4</v>
@@ -6935,7 +6947,7 @@
         <v>186</v>
       </c>
       <c r="D8" s="98" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="E8" s="98">
         <v>6</v>
@@ -6962,7 +6974,7 @@
         <v>186</v>
       </c>
       <c r="D9" s="98" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="E9" s="98">
         <v>8</v>
@@ -6977,7 +6989,7 @@
         <v>194</v>
       </c>
       <c r="I9" s="90" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="18.75">
@@ -7018,20 +7030,20 @@
         <v>197</v>
       </c>
       <c r="D11" s="98" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="E11" s="98">
         <v>10</v>
       </c>
       <c r="F11" s="91" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="G11" s="91" t="s">
         <v>179</v>
       </c>
       <c r="H11" s="91"/>
       <c r="I11" s="90" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="18.75">
@@ -7060,7 +7072,7 @@
         <v>29</v>
       </c>
       <c r="I12" s="90" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="18.75">
@@ -7074,13 +7086,13 @@
         <v>197</v>
       </c>
       <c r="D13" s="98" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="E13" s="98">
         <v>12</v>
       </c>
       <c r="F13" s="91" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="G13" s="91"/>
       <c r="H13" s="91"/>
@@ -7097,13 +7109,13 @@
         <v>197</v>
       </c>
       <c r="D14" s="99" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="E14" s="99">
         <v>13</v>
       </c>
       <c r="F14" s="94" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="G14" s="94" t="s">
         <v>143</v>

</xml_diff>

<commit_message>
added missing afil. to old seminars
</commit_message>
<xml_diff>
--- a/data/MACSI seminar series.xlsx
+++ b/data/MACSI seminar series.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ulcampus-my.sharepoint.com/personal/david_osullivan_ul_ie/Documents/Academic_work/_Misc/MACSI_Seminars/macsi-seminars.github.io/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2392" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{07BDB391-EE8A-4841-9FD8-31891226EB75}"/>
+  <xr:revisionPtr revIDLastSave="2412" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{59E04407-FAAB-4631-B150-69445DBC0BD7}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AY2023-2024 Sem 2" sheetId="3" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="843" uniqueCount="338">
   <si>
     <t>Fill in as much of the green boxes as possible. Ideally, this would be before you have finished your visitors travel dates (just to avoid double booking).</t>
   </si>
@@ -1088,6 +1088,36 @@
   <si>
     <t>Leornard Henckel</t>
   </si>
+  <si>
+    <t>Universidade Federal de Minas Gerais</t>
+  </si>
+  <si>
+    <t>Heriot-Watt University</t>
+  </si>
+  <si>
+    <t>University of Bristol</t>
+  </si>
+  <si>
+    <t>University of Leeds</t>
+  </si>
+  <si>
+    <t>University College Cork</t>
+  </si>
+  <si>
+    <t>UCL Centre for Artificial Intelligence</t>
+  </si>
+  <si>
+    <t>University of Huddersfield</t>
+  </si>
+  <si>
+    <t>University of Rochester</t>
+  </si>
+  <si>
+    <t>Murdoch University, Perth, Australia</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> York University</t>
+  </si>
 </sst>
 </file>
 
@@ -1096,7 +1126,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1891,9 +1921,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1931,7 +1961,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2037,7 +2067,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2179,7 +2209,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2190,10 +2220,10 @@
   <dimension ref="A1:X20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:G4"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="11.140625" customWidth="1"/>
@@ -2218,7 +2248,7 @@
     <col min="24" max="24" width="37.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15.75" thickBot="1">
+    <row r="1" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2229,7 +2259,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="15.75" thickBot="1">
+    <row r="2" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -2303,7 +2333,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="13.5" customHeight="1">
+    <row r="3" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>45317</v>
       </c>
@@ -2324,7 +2354,9 @@
       <c r="F3" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="14"/>
+      <c r="G3" s="14" t="s">
+        <v>328</v>
+      </c>
       <c r="H3" s="5" t="s">
         <v>29</v>
       </c>
@@ -2367,7 +2399,7 @@
       <c r="W3" s="13"/>
       <c r="X3" s="13"/>
     </row>
-    <row r="4" spans="1:24" ht="13.5" customHeight="1">
+    <row r="4" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>45323</v>
       </c>
@@ -2388,7 +2420,9 @@
       <c r="F4" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="G4" s="14"/>
+      <c r="G4" s="14" t="s">
+        <v>329</v>
+      </c>
       <c r="H4" s="5" t="s">
         <v>37</v>
       </c>
@@ -2427,7 +2461,7 @@
       <c r="W4" s="13"/>
       <c r="X4" s="13"/>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>45324</v>
       </c>
@@ -2448,7 +2482,9 @@
       <c r="F5" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="14"/>
+      <c r="G5" s="14" t="s">
+        <v>334</v>
+      </c>
       <c r="H5" s="5" t="s">
         <v>43</v>
       </c>
@@ -2485,7 +2521,7 @@
       <c r="W5" s="13"/>
       <c r="X5" s="13"/>
     </row>
-    <row r="6" spans="1:24" ht="12.75" customHeight="1">
+    <row r="6" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>45331</v>
       </c>
@@ -2506,7 +2542,9 @@
       <c r="F6" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="G6" s="14"/>
+      <c r="G6" s="14" t="s">
+        <v>330</v>
+      </c>
       <c r="H6" s="5" t="s">
         <v>43</v>
       </c>
@@ -2549,7 +2587,7 @@
       <c r="W6" s="13"/>
       <c r="X6" s="13"/>
     </row>
-    <row r="7" spans="1:24">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>45338</v>
       </c>
@@ -2570,7 +2608,9 @@
       <c r="F7" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="G7" s="14"/>
+      <c r="G7" s="14" t="s">
+        <v>331</v>
+      </c>
       <c r="H7" s="5" t="s">
         <v>54</v>
       </c>
@@ -2615,7 +2655,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="15" customHeight="1">
+    <row r="8" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>45345</v>
       </c>
@@ -2636,7 +2676,9 @@
       <c r="F8" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="G8" s="14"/>
+      <c r="G8" s="14" t="s">
+        <v>179</v>
+      </c>
       <c r="H8" s="5" t="s">
         <v>29</v>
       </c>
@@ -2679,7 +2721,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:24">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>45359</v>
       </c>
@@ -2700,7 +2742,9 @@
       <c r="F9" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="G9" s="14"/>
+      <c r="G9" s="14" t="s">
+        <v>332</v>
+      </c>
       <c r="H9" s="5" t="s">
         <v>29</v>
       </c>
@@ -2729,7 +2773,7 @@
       <c r="W9" s="13"/>
       <c r="X9" s="13"/>
     </row>
-    <row r="10" spans="1:24">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>45366</v>
       </c>
@@ -2750,7 +2794,9 @@
       <c r="F10" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="G10" s="14"/>
+      <c r="G10" s="14" t="s">
+        <v>143</v>
+      </c>
       <c r="H10" s="5" t="s">
         <v>69</v>
       </c>
@@ -2795,7 +2841,7 @@
       <c r="W10" s="13"/>
       <c r="X10" s="13"/>
     </row>
-    <row r="11" spans="1:24" ht="15" customHeight="1">
+    <row r="11" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>45379</v>
       </c>
@@ -2816,7 +2862,9 @@
       <c r="F11" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="G11" s="14"/>
+      <c r="G11" s="14" t="s">
+        <v>143</v>
+      </c>
       <c r="H11" s="5" t="s">
         <v>78</v>
       </c>
@@ -2853,7 +2901,7 @@
       <c r="W11" s="13"/>
       <c r="X11" s="13"/>
     </row>
-    <row r="12" spans="1:24" ht="13.5" customHeight="1">
+    <row r="12" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>45386</v>
       </c>
@@ -2874,7 +2922,9 @@
       <c r="F12" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="G12" s="14"/>
+      <c r="G12" s="14" t="s">
+        <v>333</v>
+      </c>
       <c r="H12" s="5" t="s">
         <v>85</v>
       </c>
@@ -2913,7 +2963,7 @@
       <c r="W12" s="13"/>
       <c r="X12" s="13"/>
     </row>
-    <row r="13" spans="1:24" ht="16.5" customHeight="1">
+    <row r="13" spans="1:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>45387</v>
       </c>
@@ -2934,7 +2984,9 @@
       <c r="F13" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="G13" s="14"/>
+      <c r="G13" s="14" t="s">
+        <v>332</v>
+      </c>
       <c r="H13" s="5" t="s">
         <v>91</v>
       </c>
@@ -2979,7 +3031,7 @@
       <c r="W13" s="13"/>
       <c r="X13" s="13"/>
     </row>
-    <row r="14" spans="1:24" ht="15.75" customHeight="1">
+    <row r="14" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>45394</v>
       </c>
@@ -3000,7 +3052,9 @@
       <c r="F14" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="G14" s="14"/>
+      <c r="G14" s="14" t="s">
+        <v>334</v>
+      </c>
       <c r="H14" s="5" t="s">
         <v>43</v>
       </c>
@@ -3037,7 +3091,7 @@
       <c r="W14" s="13"/>
       <c r="X14" s="13"/>
     </row>
-    <row r="15" spans="1:24" ht="17.25" customHeight="1">
+    <row r="15" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>45398</v>
       </c>
@@ -3058,7 +3112,9 @@
       <c r="F15" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="G15" s="14"/>
+      <c r="G15" s="14" t="s">
+        <v>335</v>
+      </c>
       <c r="H15" s="5" t="s">
         <v>101</v>
       </c>
@@ -3103,7 +3159,7 @@
       <c r="W15" s="13"/>
       <c r="X15" s="13"/>
     </row>
-    <row r="16" spans="1:24" ht="15.75" thickBot="1">
+    <row r="16" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>45401</v>
       </c>
@@ -3124,7 +3180,9 @@
       <c r="F16" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="G16" s="19"/>
+      <c r="G16" s="19" t="s">
+        <v>143</v>
+      </c>
       <c r="H16" s="17" t="s">
         <v>91</v>
       </c>
@@ -3163,7 +3221,7 @@
       <c r="W16" s="18"/>
       <c r="X16" s="18"/>
     </row>
-    <row r="17" spans="1:24">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>45421</v>
       </c>
@@ -3184,7 +3242,9 @@
       <c r="F17" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="G17" s="19"/>
+      <c r="G17" s="19" t="s">
+        <v>143</v>
+      </c>
       <c r="H17" s="17" t="s">
         <v>113</v>
       </c>
@@ -3231,7 +3291,7 @@
       <c r="W17" s="18"/>
       <c r="X17" s="18"/>
     </row>
-    <row r="18" spans="1:24" ht="15.75" thickBot="1">
+    <row r="18" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="26">
         <v>45474</v>
       </c>
@@ -3252,7 +3312,9 @@
       <c r="F18" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="G18" s="19"/>
+      <c r="G18" s="19" t="s">
+        <v>336</v>
+      </c>
       <c r="H18" s="17" t="s">
         <v>85</v>
       </c>
@@ -3279,7 +3341,7 @@
       <c r="W18" s="18"/>
       <c r="X18" s="18"/>
     </row>
-    <row r="19" spans="1:24" ht="17.25" customHeight="1" thickBot="1">
+    <row r="19" spans="1:24" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="26">
         <v>45505</v>
       </c>
@@ -3300,7 +3362,9 @@
       <c r="F19" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="G19" s="19"/>
+      <c r="G19" s="19" t="s">
+        <v>337</v>
+      </c>
       <c r="H19" s="17" t="s">
         <v>78</v>
       </c>
@@ -3327,7 +3391,7 @@
       <c r="W19" s="18"/>
       <c r="X19" s="18"/>
     </row>
-    <row r="20" spans="1:24">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="26"/>
       <c r="B20" s="26"/>
       <c r="C20" s="26"/>
@@ -3373,7 +3437,7 @@
       <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="11.140625" customWidth="1"/>
@@ -3398,7 +3462,7 @@
     <col min="24" max="24" width="37.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15.75" thickBot="1">
+    <row r="1" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3409,7 +3473,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="30.75" thickBot="1">
+    <row r="2" spans="1:24" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="149" t="s">
         <v>3</v>
       </c>
@@ -3483,7 +3547,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="13.5" customHeight="1">
+    <row r="3" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>45548</v>
       </c>
@@ -3547,7 +3611,7 @@
       <c r="W3" s="46"/>
       <c r="X3" s="44"/>
     </row>
-    <row r="4" spans="1:24" ht="13.5" customHeight="1">
+    <row r="4" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>45555</v>
       </c>
@@ -3595,7 +3659,7 @@
       <c r="W4" s="15"/>
       <c r="X4" s="13"/>
     </row>
-    <row r="5" spans="1:24" ht="14.25" customHeight="1">
+    <row r="5" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>45562</v>
       </c>
@@ -3643,7 +3707,7 @@
       <c r="W5" s="15"/>
       <c r="X5" s="13"/>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>45576</v>
       </c>
@@ -3691,7 +3755,7 @@
       <c r="W6" s="15"/>
       <c r="X6" s="13"/>
     </row>
-    <row r="7" spans="1:24" ht="15" customHeight="1">
+    <row r="7" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>45583</v>
       </c>
@@ -3739,7 +3803,7 @@
       <c r="W7" s="15"/>
       <c r="X7" s="13"/>
     </row>
-    <row r="8" spans="1:24" ht="14.25" customHeight="1">
+    <row r="8" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>45596</v>
       </c>
@@ -3787,7 +3851,7 @@
       <c r="W8" s="15"/>
       <c r="X8" s="13"/>
     </row>
-    <row r="9" spans="1:24">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>45604</v>
       </c>
@@ -3835,7 +3899,7 @@
       <c r="W9" s="15"/>
       <c r="X9" s="13"/>
     </row>
-    <row r="10" spans="1:24">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>45611</v>
       </c>
@@ -3883,7 +3947,7 @@
       <c r="W10" s="15"/>
       <c r="X10" s="13"/>
     </row>
-    <row r="11" spans="1:24" ht="13.5" customHeight="1">
+    <row r="11" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>45625</v>
       </c>
@@ -3931,7 +3995,7 @@
       <c r="W11" s="15"/>
       <c r="X11" s="13"/>
     </row>
-    <row r="12" spans="1:24" ht="16.5" customHeight="1" thickBot="1">
+    <row r="12" spans="1:24" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>45632</v>
       </c>
@@ -3987,20 +4051,20 @@
       <c r="W12" s="20"/>
       <c r="X12" s="18"/>
     </row>
-    <row r="13" spans="1:24">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="26"/>
       <c r="B13" s="26"/>
       <c r="C13" s="26"/>
       <c r="D13" s="26"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:24">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="26"/>
       <c r="B14" s="26"/>
       <c r="C14" s="26"/>
       <c r="D14" s="26"/>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="64"/>
       <c r="B29" s="64"/>
       <c r="C29" s="64"/>
@@ -4012,59 +4076,59 @@
       <c r="I29" s="64"/>
       <c r="J29" s="64"/>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="63"/>
       <c r="B31" s="63"/>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="63"/>
       <c r="B32" s="63"/>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="63"/>
       <c r="B33" s="63"/>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="63"/>
       <c r="B34" s="63"/>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="63"/>
       <c r="B35" s="63"/>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="63"/>
       <c r="B36" s="63"/>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="63"/>
       <c r="B37" s="63"/>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="63"/>
       <c r="B38" s="63"/>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="63"/>
       <c r="B39" s="63"/>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="63"/>
       <c r="B40" s="63"/>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="63"/>
       <c r="B41" s="63"/>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="63"/>
       <c r="B42" s="63"/>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="63"/>
       <c r="B43" s="63"/>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="63"/>
       <c r="B44" s="63"/>
     </row>
@@ -4097,7 +4161,7 @@
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" customWidth="1"/>
     <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1"/>
@@ -4125,7 +4189,7 @@
     <col min="24" max="24" width="37.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15.75" thickBot="1">
+    <row r="1" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4136,7 +4200,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="27.75" customHeight="1" thickBot="1">
+    <row r="2" spans="1:24" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="68" t="s">
         <v>3</v>
       </c>
@@ -4210,7 +4274,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="15" customHeight="1">
+    <row r="3" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>45694</v>
       </c>
@@ -4259,7 +4323,7 @@
       <c r="W3" s="46"/>
       <c r="X3" s="44"/>
     </row>
-    <row r="4" spans="1:24" ht="14.25" customHeight="1">
+    <row r="4" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>45708</v>
       </c>
@@ -4316,7 +4380,7 @@
       <c r="W4" s="15"/>
       <c r="X4" s="13"/>
     </row>
-    <row r="5" spans="1:24" ht="14.25" customHeight="1">
+    <row r="5" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>45722</v>
       </c>
@@ -4371,7 +4435,7 @@
       <c r="W5" s="15"/>
       <c r="X5" s="13"/>
     </row>
-    <row r="6" spans="1:24" ht="16.5" customHeight="1">
+    <row r="6" spans="1:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>45735</v>
       </c>
@@ -4426,7 +4490,7 @@
       <c r="W6" s="15"/>
       <c r="X6" s="13"/>
     </row>
-    <row r="7" spans="1:24" ht="18" customHeight="1">
+    <row r="7" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>45750</v>
       </c>
@@ -4479,7 +4543,7 @@
       <c r="W7" s="15"/>
       <c r="X7" s="13"/>
     </row>
-    <row r="8" spans="1:24" ht="16.5" customHeight="1">
+    <row r="8" spans="1:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>45751</v>
       </c>
@@ -4537,7 +4601,7 @@
       <c r="W8" s="15"/>
       <c r="X8" s="13"/>
     </row>
-    <row r="9" spans="1:24" ht="15.75" customHeight="1">
+    <row r="9" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>45757</v>
       </c>
@@ -4598,7 +4662,7 @@
       <c r="W9" s="15"/>
       <c r="X9" s="13"/>
     </row>
-    <row r="10" spans="1:24" ht="15.75" customHeight="1">
+    <row r="10" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>45758</v>
       </c>
@@ -4651,7 +4715,7 @@
       <c r="W10" s="20"/>
       <c r="X10" s="18"/>
     </row>
-    <row r="11" spans="1:24" ht="15.75" customHeight="1">
+    <row r="11" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>45764</v>
       </c>
@@ -4710,7 +4774,7 @@
       <c r="W11" s="35"/>
       <c r="X11" s="35"/>
     </row>
-    <row r="12" spans="1:24" ht="15.75" customHeight="1">
+    <row r="12" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>45771</v>
       </c>
@@ -4770,7 +4834,7 @@
       <c r="W12" s="35"/>
       <c r="X12" s="35"/>
     </row>
-    <row r="13" spans="1:24" ht="15.75" customHeight="1">
+    <row r="13" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>45785</v>
       </c>
@@ -4822,7 +4886,7 @@
       <c r="W13" s="35"/>
       <c r="X13" s="35"/>
     </row>
-    <row r="14" spans="1:24" ht="15.75" customHeight="1">
+    <row r="14" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>45799</v>
       </c>
@@ -4868,7 +4932,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:24" ht="15.75" customHeight="1">
+    <row r="15" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>45805</v>
       </c>
@@ -4902,101 +4966,101 @@
         <v>238</v>
       </c>
     </row>
-    <row r="16" spans="1:24" ht="15.75" customHeight="1">
+    <row r="16" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="79"/>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="26"/>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="26"/>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="26"/>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="79"/>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="26"/>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="79"/>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="26"/>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="26"/>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="26"/>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="26"/>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="26"/>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="26"/>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B31" s="63"/>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="63"/>
       <c r="B32" s="63"/>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="63"/>
       <c r="B33" s="63"/>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="63"/>
       <c r="B34" s="63"/>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="63"/>
       <c r="B35" s="63"/>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="63"/>
       <c r="B36" s="63"/>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="63"/>
       <c r="B37" s="63"/>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="63"/>
       <c r="B38" s="63"/>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="63"/>
       <c r="B39" s="63"/>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="63"/>
       <c r="B40" s="63"/>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="63"/>
       <c r="B41" s="63"/>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="63"/>
       <c r="B42" s="63"/>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="63"/>
       <c r="B43" s="63"/>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="63"/>
       <c r="B44" s="63"/>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="63"/>
     </row>
   </sheetData>
@@ -5024,11 +5088,11 @@
   </sheetPr>
   <dimension ref="A1:X16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11:I11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" customWidth="1"/>
@@ -5055,7 +5119,7 @@
     <col min="24" max="24" width="37.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5066,7 +5130,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="30.75">
+    <row r="2" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="68" t="s">
         <v>3</v>
       </c>
@@ -5140,7 +5204,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="15" customHeight="1">
+    <row r="3" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="79">
         <v>45911</v>
       </c>
@@ -5196,7 +5260,7 @@
       <c r="W3" s="46"/>
       <c r="X3" s="44"/>
     </row>
-    <row r="4" spans="1:24" ht="15" customHeight="1">
+    <row r="4" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="79">
         <v>45917</v>
       </c>
@@ -5248,7 +5312,7 @@
       <c r="W4" s="15"/>
       <c r="X4" s="13"/>
     </row>
-    <row r="5" spans="1:24" ht="15.75" customHeight="1">
+    <row r="5" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="79">
         <v>45926</v>
       </c>
@@ -5299,7 +5363,7 @@
       <c r="W5" s="15"/>
       <c r="X5" s="13"/>
     </row>
-    <row r="6" spans="1:24" ht="16.5" customHeight="1">
+    <row r="6" spans="1:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="79">
         <v>45939</v>
       </c>
@@ -5350,7 +5414,7 @@
       <c r="W6" s="15"/>
       <c r="X6" s="13"/>
     </row>
-    <row r="7" spans="1:24" ht="15.75" customHeight="1">
+    <row r="7" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="79">
         <v>45946</v>
       </c>
@@ -5398,7 +5462,7 @@
       <c r="W7" s="15"/>
       <c r="X7" s="13"/>
     </row>
-    <row r="8" spans="1:24">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="79">
         <v>45953</v>
       </c>
@@ -5449,7 +5513,7 @@
       <c r="W8" s="15"/>
       <c r="X8" s="13"/>
     </row>
-    <row r="9" spans="1:24">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="79">
         <v>45967</v>
       </c>
@@ -5498,7 +5562,7 @@
       <c r="W9" s="15"/>
       <c r="X9" s="13"/>
     </row>
-    <row r="10" spans="1:24" ht="18.75" customHeight="1">
+    <row r="10" spans="1:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="79">
         <v>45974</v>
       </c>
@@ -5548,7 +5612,7 @@
       <c r="W10" s="15"/>
       <c r="X10" s="13"/>
     </row>
-    <row r="11" spans="1:24" ht="19.5" customHeight="1">
+    <row r="11" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="79">
         <v>45981</v>
       </c>
@@ -5599,7 +5663,7 @@
       <c r="W11" s="15"/>
       <c r="X11" s="13"/>
     </row>
-    <row r="12" spans="1:24" ht="19.5" customHeight="1">
+    <row r="12" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="79">
         <v>45995</v>
       </c>
@@ -5650,24 +5714,24 @@
       <c r="W12" s="15"/>
       <c r="X12" s="13"/>
     </row>
-    <row r="13" spans="1:24">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="26"/>
       <c r="B13" s="26"/>
       <c r="C13" s="26"/>
       <c r="W13" s="20"/>
       <c r="X13" s="18"/>
     </row>
-    <row r="14" spans="1:24" ht="12.75" customHeight="1">
+    <row r="14" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="26"/>
       <c r="B14" s="26"/>
       <c r="C14" s="26"/>
     </row>
-    <row r="15" spans="1:24">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="26"/>
       <c r="B15" s="26"/>
       <c r="C15" s="26"/>
     </row>
-    <row r="16" spans="1:24">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="26"/>
       <c r="B16" s="26"/>
       <c r="C16" s="26"/>
@@ -5696,7 +5760,7 @@
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" customWidth="1"/>
     <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1"/>
@@ -5723,7 +5787,7 @@
     <col min="24" max="24" width="37.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15.75" thickBot="1">
+    <row r="1" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5734,7 +5798,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="30.75" thickBot="1">
+    <row r="2" spans="1:24" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="68" t="s">
         <v>3</v>
       </c>
@@ -5808,7 +5872,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="15" customHeight="1">
+    <row r="3" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="79">
         <v>46051</v>
       </c>
@@ -5860,7 +5924,7 @@
       <c r="W3" s="46"/>
       <c r="X3" s="44"/>
     </row>
-    <row r="4" spans="1:24" ht="15.75" customHeight="1">
+    <row r="4" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="79">
         <f>A3+14</f>
         <v>46065</v>
@@ -5912,7 +5976,7 @@
       <c r="W4" s="15"/>
       <c r="X4" s="13"/>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="79">
         <f t="shared" ref="A5:A9" si="2">A4+14</f>
         <v>46079</v>
@@ -5964,7 +6028,7 @@
       <c r="W5" s="15"/>
       <c r="X5" s="13"/>
     </row>
-    <row r="6" spans="1:24" ht="15.75" customHeight="1">
+    <row r="6" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="79">
         <f t="shared" si="2"/>
         <v>46093</v>
@@ -6016,7 +6080,7 @@
       <c r="W6" s="15"/>
       <c r="X6" s="13"/>
     </row>
-    <row r="7" spans="1:24">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="79">
         <f t="shared" si="2"/>
         <v>46107</v>
@@ -6068,7 +6132,7 @@
       <c r="W7" s="15"/>
       <c r="X7" s="13"/>
     </row>
-    <row r="8" spans="1:24">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="79">
         <f t="shared" si="2"/>
         <v>46121</v>
@@ -6118,7 +6182,7 @@
       <c r="W8" s="15"/>
       <c r="X8" s="13"/>
     </row>
-    <row r="9" spans="1:24" ht="18.75" customHeight="1">
+    <row r="9" spans="1:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="79">
         <f t="shared" si="2"/>
         <v>46135</v>
@@ -6170,24 +6234,24 @@
       <c r="W9" s="15"/>
       <c r="X9" s="13"/>
     </row>
-    <row r="10" spans="1:24" ht="15.75" thickBot="1">
+    <row r="10" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="26"/>
       <c r="B10" s="26"/>
       <c r="C10" s="26"/>
       <c r="W10" s="20"/>
       <c r="X10" s="18"/>
     </row>
-    <row r="11" spans="1:24" ht="12.75" customHeight="1">
+    <row r="11" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="26"/>
       <c r="B11" s="26"/>
       <c r="C11" s="26"/>
     </row>
-    <row r="12" spans="1:24">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="26"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
     </row>
-    <row r="13" spans="1:24">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="26"/>
       <c r="B13" s="26"/>
       <c r="C13" s="26"/>
@@ -6208,23 +6272,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AEC079F-155A-491D-9189-1418FC903287}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.28515625" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
     <col min="3" max="3" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="57" t="s">
         <v>281</v>
       </c>
@@ -6235,7 +6299,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="140" t="s">
         <v>284</v>
       </c>
@@ -6244,7 +6308,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>285</v>
       </c>
@@ -6253,7 +6317,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="54" t="s">
         <v>286</v>
       </c>
@@ -6262,7 +6326,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="54" t="s">
         <v>288</v>
       </c>
@@ -6273,7 +6337,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="54" t="s">
         <v>290</v>
       </c>
@@ -6284,7 +6348,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="54" t="s">
         <v>292</v>
       </c>
@@ -6295,14 +6359,14 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="54" t="s">
         <v>294</v>
       </c>
       <c r="B9" s="54"/>
       <c r="C9" s="52"/>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="54" t="s">
         <v>295</v>
       </c>
@@ -6313,7 +6377,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="54" t="s">
         <v>298</v>
       </c>
@@ -6324,7 +6388,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="54" t="s">
         <v>301</v>
       </c>
@@ -6335,7 +6399,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="54" t="s">
         <v>303</v>
       </c>
@@ -6346,7 +6410,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="54" t="s">
         <v>305</v>
       </c>
@@ -6357,7 +6421,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="54" t="s">
         <v>307</v>
       </c>
@@ -6368,7 +6432,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="141" t="s">
         <v>275</v>
       </c>
@@ -6379,7 +6443,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="54" t="s">
         <v>311</v>
       </c>
@@ -6390,7 +6454,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="54" t="s">
         <v>313</v>
       </c>
@@ -6401,7 +6465,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="55" t="s">
         <v>314</v>
       </c>
@@ -6412,12 +6476,12 @@
         <v>315</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>313</v>
       </c>
@@ -6428,7 +6492,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>314</v>
       </c>
@@ -6457,13 +6521,13 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
     <col min="6" max="6" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="139" t="s">
         <v>3</v>
       </c>
@@ -6474,7 +6538,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickTop="1">
+    <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="137">
         <v>45911</v>
       </c>
@@ -6502,7 +6566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="137">
         <f>A2+7</f>
         <v>45918</v>
@@ -6533,7 +6597,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="137">
         <f t="shared" ref="A4:A12" si="0">A3+7</f>
         <v>45925</v>
@@ -6564,7 +6628,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="137">
         <f t="shared" si="0"/>
         <v>45932</v>
@@ -6592,7 +6656,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="137">
         <f t="shared" si="0"/>
         <v>45939</v>
@@ -6623,7 +6687,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="137">
         <f t="shared" si="0"/>
         <v>45946</v>
@@ -6654,7 +6718,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="137">
         <f t="shared" si="0"/>
         <v>45953</v>
@@ -6684,7 +6748,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="137">
         <f t="shared" si="0"/>
         <v>45960</v>
@@ -6715,7 +6779,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="137">
         <f t="shared" si="0"/>
         <v>45967</v>
@@ -6746,7 +6810,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="137">
         <f t="shared" si="0"/>
         <v>45974</v>
@@ -6759,7 +6823,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="137">
         <f t="shared" si="0"/>
         <v>45981</v>
@@ -6772,7 +6836,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="137">
         <f t="shared" ref="A13:A14" si="6">A12+7</f>
         <v>45988</v>
@@ -6785,7 +6849,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="137">
         <f t="shared" si="6"/>
         <v>45995</v>
@@ -6798,12 +6862,12 @@
         <v>319</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="137"/>
       <c r="B15" s="138"/>
       <c r="C15" s="138"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G16" s="26"/>
     </row>
   </sheetData>
@@ -6834,7 +6898,7 @@
       <selection activeCell="F8" sqref="F8:H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.42578125" customWidth="1"/>
     <col min="2" max="2" width="9.140625" customWidth="1"/>
@@ -6846,17 +6910,17 @@
     <col min="9" max="9" width="64.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" ht="23.25">
+    <row r="2" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="95" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="18.75">
+    <row r="3" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="83" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="37.5">
+    <row r="5" spans="1:9" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A5" s="84" t="s">
         <v>3</v>
       </c>
@@ -6885,7 +6949,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="18.75">
+    <row r="6" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="96">
         <v>45694</v>
       </c>
@@ -6912,7 +6976,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="18.75">
+    <row r="7" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="87">
         <v>45708</v>
       </c>
@@ -6941,7 +7005,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="18.75">
+    <row r="8" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="87">
         <v>45722</v>
       </c>
@@ -6968,7 +7032,7 @@
       </c>
       <c r="I8" s="90"/>
     </row>
-    <row r="9" spans="1:9" ht="18.75">
+    <row r="9" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="87">
         <v>45735</v>
       </c>
@@ -6997,7 +7061,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="18.75">
+    <row r="10" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="87">
         <v>45744</v>
       </c>
@@ -7024,7 +7088,7 @@
       </c>
       <c r="I10" s="90"/>
     </row>
-    <row r="11" spans="1:9" ht="18.75">
+    <row r="11" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="87">
         <v>45750</v>
       </c>
@@ -7051,7 +7115,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="18.75">
+    <row r="12" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="87">
         <v>45758</v>
       </c>
@@ -7080,7 +7144,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="18.75">
+    <row r="13" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="87">
         <v>45764</v>
       </c>
@@ -7103,7 +7167,7 @@
       <c r="H13" s="91"/>
       <c r="I13" s="90"/>
     </row>
-    <row r="14" spans="1:9" ht="18.75">
+    <row r="14" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="92">
         <v>45771</v>
       </c>
@@ -7132,7 +7196,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="20" spans="8:8" ht="18.75">
+    <row r="20" spans="8:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="H20" s="83"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update MK seminar time
</commit_message>
<xml_diff>
--- a/data/MACSI seminar series.xlsx
+++ b/data/MACSI seminar series.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ulcampus-my.sharepoint.com/personal/david_osullivan_ul_ie/Documents/Academic_work/_Misc/MACSI_Seminars/macsi-seminars.github.io/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2429" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E2E1881E-28F8-4E8E-8FD4-A08EC9909AE9}"/>
+  <xr:revisionPtr revIDLastSave="2481" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9AF711EC-13E3-4E99-8D47-6AA442AE42CD}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AY2023-2024 Sem 2" sheetId="3" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="879" uniqueCount="342">
   <si>
     <t>Fill in as much of the green boxes as possible. Ideally, this would be before you have finished your visitors travel dates (just to avoid double booking).</t>
   </si>
@@ -1120,6 +1120,15 @@
   </si>
   <si>
     <t>Synthetic Aperture Radar (SAR) imaging has proven an invaluable all-weather day and night remote sensing information source, increasingly provided by monostatic SAR satellite constellations. Future developments will include multistatic SAR constellations (with a mix of separated transmitter and receiver platforms) for more timely or simultaneous multiple collections for interferometric modes, for example for 3D imaging or more basic terrain height determination, as well as for sensitive change detection amongst others. This presentation will provide an overview of multistatic SAR processing and show highlight results from the Ground-Based SAR laboratory based at Cranfield University, which has allowed the exploration and validation of multistatic SAR sensing concepts amongst others.</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>16th</t>
+  </si>
+  <si>
+    <t>0</t>
   </si>
 </sst>
 </file>
@@ -5109,8 +5118,11 @@
   </sheetPr>
   <dimension ref="A1:X23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="7" ySplit="16" topLeftCell="H17" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
+      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5264,18 +5276,24 @@
       <c r="L3" s="59" t="s">
         <v>244</v>
       </c>
-      <c r="M3" s="38"/>
+      <c r="M3" s="38" t="s">
+        <v>33</v>
+      </c>
       <c r="N3" s="35" t="s">
         <v>33</v>
       </c>
       <c r="O3" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="P3" s="40"/>
+      <c r="P3" s="40" t="s">
+        <v>341</v>
+      </c>
       <c r="Q3" s="40"/>
       <c r="R3" s="38"/>
       <c r="S3" s="35"/>
-      <c r="T3" s="40"/>
+      <c r="T3" s="40" t="s">
+        <v>35</v>
+      </c>
       <c r="U3" s="40"/>
       <c r="V3" s="40"/>
       <c r="W3" s="46"/>
@@ -5320,14 +5338,30 @@
       <c r="L4" s="25" t="s">
         <v>252</v>
       </c>
-      <c r="M4" s="16"/>
-      <c r="N4" s="35"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="5"/>
-      <c r="R4" s="16"/>
-      <c r="S4" s="35"/>
-      <c r="T4" s="5"/>
+      <c r="M4" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="N4" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="O4" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P4" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q4" s="5" t="s">
+        <v>340</v>
+      </c>
+      <c r="R4" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="S4" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="T4" s="5" t="s">
+        <v>35</v>
+      </c>
       <c r="U4" s="5"/>
       <c r="V4" s="5"/>
       <c r="W4" s="15"/>
@@ -5369,16 +5403,22 @@
       </c>
       <c r="K5" s="157"/>
       <c r="L5" s="25"/>
-      <c r="M5" s="16"/>
+      <c r="M5" s="16" t="s">
+        <v>33</v>
+      </c>
       <c r="N5" s="35"/>
       <c r="O5" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="P5" s="5"/>
+      <c r="P5" s="5" t="s">
+        <v>341</v>
+      </c>
       <c r="Q5" s="5"/>
       <c r="R5" s="16"/>
       <c r="S5" s="35"/>
-      <c r="T5" s="5"/>
+      <c r="T5" s="5" t="s">
+        <v>35</v>
+      </c>
       <c r="U5" s="5"/>
       <c r="V5" s="5"/>
       <c r="W5" s="15"/>
@@ -5420,16 +5460,26 @@
       </c>
       <c r="K6" s="157"/>
       <c r="L6" s="25"/>
-      <c r="M6" s="16"/>
-      <c r="N6" s="35"/>
+      <c r="M6" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="N6" s="35" t="s">
+        <v>41</v>
+      </c>
       <c r="O6" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="P6" s="5"/>
+      <c r="P6" s="5" t="s">
+        <v>58</v>
+      </c>
       <c r="Q6" s="5"/>
       <c r="R6" s="16"/>
-      <c r="S6" s="35"/>
-      <c r="T6" s="5"/>
+      <c r="S6" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="T6" s="5" t="s">
+        <v>64</v>
+      </c>
       <c r="U6" s="5"/>
       <c r="V6" s="5"/>
       <c r="W6" s="15"/>
@@ -5468,16 +5518,22 @@
       </c>
       <c r="K7" s="157"/>
       <c r="L7" s="25"/>
-      <c r="M7" s="16"/>
+      <c r="M7" s="16" t="s">
+        <v>33</v>
+      </c>
       <c r="N7" s="35"/>
       <c r="O7" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="P7" s="5"/>
+      <c r="P7" s="5" t="s">
+        <v>341</v>
+      </c>
       <c r="Q7" s="5"/>
       <c r="R7" s="16"/>
       <c r="S7" s="35"/>
-      <c r="T7" s="5"/>
+      <c r="T7" s="5" t="s">
+        <v>35</v>
+      </c>
       <c r="U7" s="5"/>
       <c r="V7" s="5"/>
       <c r="W7" s="15"/>
@@ -5519,7 +5575,9 @@
       </c>
       <c r="K8" s="157"/>
       <c r="L8" s="25"/>
-      <c r="M8" s="16"/>
+      <c r="M8" s="16" t="s">
+        <v>41</v>
+      </c>
       <c r="N8" s="35"/>
       <c r="O8" s="5" t="s">
         <v>41</v>
@@ -5528,7 +5586,9 @@
       <c r="Q8" s="5"/>
       <c r="R8" s="16"/>
       <c r="S8" s="35"/>
-      <c r="T8" s="5"/>
+      <c r="T8" s="5" t="s">
+        <v>64</v>
+      </c>
       <c r="U8" s="5"/>
       <c r="V8" s="5"/>
       <c r="W8" s="15"/>
@@ -5618,16 +5678,24 @@
       </c>
       <c r="K10" s="157"/>
       <c r="L10" s="25"/>
-      <c r="M10" s="16"/>
+      <c r="M10" s="16" t="s">
+        <v>41</v>
+      </c>
       <c r="N10" s="35"/>
       <c r="O10" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="P10" s="5"/>
+      <c r="P10" s="5" t="s">
+        <v>339</v>
+      </c>
       <c r="Q10" s="5"/>
       <c r="R10" s="16"/>
-      <c r="S10" s="35"/>
-      <c r="T10" s="5"/>
+      <c r="S10" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="T10" s="5" t="s">
+        <v>64</v>
+      </c>
       <c r="U10" s="5"/>
       <c r="V10" s="5"/>
       <c r="W10" s="15"/>
@@ -5669,16 +5737,22 @@
       </c>
       <c r="K11" s="107"/>
       <c r="L11" s="25"/>
-      <c r="M11" s="16"/>
+      <c r="M11" s="16" t="s">
+        <v>33</v>
+      </c>
       <c r="N11" s="35"/>
       <c r="O11" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="P11" s="5"/>
+      <c r="P11" s="5" t="s">
+        <v>341</v>
+      </c>
       <c r="Q11" s="5"/>
       <c r="R11" s="16"/>
       <c r="S11" s="35"/>
-      <c r="T11" s="5"/>
+      <c r="T11" s="5" t="s">
+        <v>64</v>
+      </c>
       <c r="U11" s="5"/>
       <c r="V11" s="5"/>
       <c r="W11" s="15"/>
@@ -5720,16 +5794,24 @@
       </c>
       <c r="K12" s="157"/>
       <c r="L12" s="25"/>
-      <c r="M12" s="16"/>
+      <c r="M12" s="16" t="s">
+        <v>41</v>
+      </c>
       <c r="N12" s="35"/>
       <c r="O12" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="P12" s="5"/>
+      <c r="P12" s="5" t="s">
+        <v>58</v>
+      </c>
       <c r="Q12" s="5"/>
       <c r="R12" s="16"/>
-      <c r="S12" s="35"/>
-      <c r="T12" s="5"/>
+      <c r="S12" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="T12" s="5" t="s">
+        <v>64</v>
+      </c>
       <c r="U12" s="5"/>
       <c r="V12" s="5"/>
       <c r="W12" s="15"/>
@@ -5784,7 +5866,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F62D4156-0A06-4DBF-B1E7-3E12580121CB}">
   <dimension ref="A1:X13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add AOC title and abs
</commit_message>
<xml_diff>
--- a/data/MACSI seminar series.xlsx
+++ b/data/MACSI seminar series.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ulcampus-my.sharepoint.com/personal/david_osullivan_ul_ie/Documents/Academic_work/_Misc/MACSI_Seminars/macsi-seminars.github.io/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2481" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9AF711EC-13E3-4E99-8D47-6AA442AE42CD}"/>
+  <xr:revisionPtr revIDLastSave="2491" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{456F8772-F5F4-4216-92AD-7F479810E203}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AY2023-2024 Sem 2" sheetId="3" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="879" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="885" uniqueCount="350">
   <si>
     <t>Fill in as much of the green boxes as possible. Ideally, this would be before you have finished your visitors travel dates (just to avoid double booking).</t>
   </si>
@@ -132,6 +132,9 @@
     <t>Marcos Prates</t>
   </si>
   <si>
+    <t>Universidade Federal de Minas Gerais</t>
+  </si>
+  <si>
     <t>James Sweeney</t>
   </si>
   <si>
@@ -154,6 +157,9 @@
   </si>
   <si>
     <t>Emmanuil H. Georgoulis</t>
+  </si>
+  <si>
+    <t>Heriot-Watt University</t>
   </si>
   <si>
     <t>Natalia Kopteva</t>
@@ -175,6 +181,9 @@
     <t>William Lee</t>
   </si>
   <si>
+    <t>University of Huddersfield</t>
+  </si>
+  <si>
     <t>Kevin Moroney</t>
   </si>
   <si>
@@ -188,6 +197,9 @@
   </si>
   <si>
     <t>Cameron Hall</t>
+  </si>
+  <si>
+    <t>University of Bristol</t>
   </si>
   <si>
     <t>Opportunities and challenges in optimising power grid stability</t>
@@ -209,6 +221,9 @@
     <t>Srikanth Toppaladoddi</t>
   </si>
   <si>
+    <t>University of Leeds</t>
+  </si>
+  <si>
     <t>Anthony Bonfils</t>
   </si>
   <si>
@@ -231,6 +246,9 @@
   </si>
   <si>
     <t>Maeve Upton</t>
+  </si>
+  <si>
+    <t>University of Limerick</t>
   </si>
   <si>
     <t xml:space="preserve"> Bayesian generalised additive models for quantifying sea-level change.</t>
@@ -246,6 +264,9 @@
     <t xml:space="preserve">Ben Taylor </t>
   </si>
   <si>
+    <t>University College Cork</t>
+  </si>
+  <si>
     <t>Modelling and inference for Spatial Processes Under Aggregation and Change of Support</t>
   </si>
   <si>
@@ -253,6 +274,9 @@
   </si>
   <si>
     <t>Michael Fop</t>
+  </si>
+  <si>
+    <t>University College Dublin</t>
   </si>
   <si>
     <t>Shirin Moghaddam</t>
@@ -302,6 +326,9 @@
   </si>
   <si>
     <t>Dan Giles</t>
+  </si>
+  <si>
+    <t>UCL Centre for Artificial Intelligence</t>
   </si>
   <si>
     <t>James Gleeson</t>
@@ -357,6 +384,9 @@
     <t>Allan Greenleaf</t>
   </si>
   <si>
+    <t>University of Rochester</t>
+  </si>
+  <si>
     <t>Cliff Nolan</t>
   </si>
   <si>
@@ -411,6 +441,9 @@
     <t>Graeme Hocking</t>
   </si>
   <si>
+    <t>Murdoch University, Perth, Australia</t>
+  </si>
+  <si>
     <t>Splashes, waves and bores - unsteady, free-surface flows</t>
   </si>
   <si>
@@ -418,6 +451,9 @@
   </si>
   <si>
     <t>Laura Keane</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> York University</t>
   </si>
   <si>
     <t>Simulation and analysis of double charge layers in electrolyte models for Lithium-ion batteries</t>
@@ -490,9 +526,6 @@
     <t>Graham Benham</t>
   </si>
   <si>
-    <t>University College Dublin</t>
-  </si>
-  <si>
     <t>Wave-driven propulsion occurs when a floating body, driven into oscillations at the fluid interface, is propelled by the waves generated by its own motion. Wave-driven propulsion has been observed in the case of the waves generated by a honeybee trapped on the surface of water, in the case of “SurferBot”, a centimeter-scale interfacial robot that was inspired by the stricken honeybee, and at much larger scales, in the case of the waves generated by jumping up and down on a canoe, also known as “gunwale bobbing”.
 In this seminar I will present a new theory for wave-driven propulsion based on coupling the equations of motion of a floating raft to a quasi-potential flow model of the fluid. Using this model, expressions are derived for the drift speed and propulsive thrust of the raft which in turn are shown to be consistent with global momentum conservation. The validity of the model is explored by describing the motion of SurferBot, demonstrating close agreement with the experimentally determined drift speed and oscillatory dynamics. The efficiency of wave-driven propulsion is then computed as a function of driving oscillation frequency and the forcing location, revealing optimal values for both of these parameters which await confirmation in experiments.</t>
   </si>
@@ -585,6 +618,12 @@
     <t xml:space="preserve">Cranfield University </t>
   </si>
   <si>
+    <t>Multistatic Synthetic Aperture Radar Imaging and Coherence</t>
+  </si>
+  <si>
+    <t>Synthetic Aperture Radar (SAR) imaging has proven an invaluable all-weather day and night remote sensing information source, increasingly provided by monostatic SAR satellite constellations. Future developments will include multistatic SAR constellations (with a mix of separated transmitter and receiver platforms) for more timely or simultaneous multiple collections for interferometric modes, for example for 3D imaging or more basic terrain height determination, as well as for sensitive change detection amongst others. This presentation will provide an overview of multistatic SAR processing and show highlight results from the Ground-Based SAR laboratory based at Cranfield University, which has allowed the exploration and validation of multistatic SAR sensing concepts amongst others.</t>
+  </si>
+  <si>
     <t>December 5</t>
   </si>
   <si>
@@ -598,9 +637,6 @@
   </si>
   <si>
     <t>Feb</t>
-  </si>
-  <si>
-    <t>University of Limerick</t>
   </si>
   <si>
     <t xml:space="preserve">Fractional differential equations: gentle introduction and gentle numerical analysis
@@ -829,6 +865,9 @@
     <t xml:space="preserve"> https://arxiv.org/abs/2508.09647</t>
   </si>
   <si>
+    <t>0</t>
+  </si>
+  <si>
     <t>4pm</t>
   </si>
   <si>
@@ -851,6 +890,9 @@
   </si>
   <si>
     <t>https://doi.org/10.1038/s41467-024-48332-y ; https://doi.org/10.1126/sciadv.adk4606 ; https://doi.org/10.1103/PhysRevResearch.7.L012061</t>
+  </si>
+  <si>
+    <t>16th</t>
   </si>
   <si>
     <t>3pm</t>
@@ -890,6 +932,9 @@
     <t>TBC</t>
   </si>
   <si>
+    <t>https://scholar.google.com/citations?user=j2CypRIAAAAJ&amp;hl=en</t>
+  </si>
+  <si>
     <t>Oct</t>
   </si>
   <si>
@@ -902,6 +947,9 @@
     <t>A wavelet lifting approach for spatial/network data</t>
   </si>
   <si>
+    <t>https://scholar.google.com/citations?user=paf72YcAAAAJ&amp;hl=en</t>
+  </si>
+  <si>
     <t>Theresa Smith</t>
   </si>
   <si>
@@ -911,6 +959,19 @@
     <t>Yanghong Huang</t>
   </si>
   <si>
+    <t xml:space="preserve">Finite Difference Methods for fractional Laplacian of radial functions 
+</t>
+  </si>
+  <si>
+    <t>Numerical evaluation of nonlocal operators like the fractional Laplacian is more computationally intensive because of the dependence on the underlying function over the whole space. On the other hand, many solutions to the fractional counterparts of classical semi-linear PDEs, especially ground states obtained via variational methods, are radial. In this talk, fractional Laplacian of radial functions in general dimensions will be considered with a kernel represented by a Gauss hypergeometric function of the radial variables.  The singular part of the kernel is isolated and then treated with effective methods well studied in the one-dimensional context, while the regular part can be evaluated with by classical quadrature. The method can be extended to general non-radial functions that can be expanded using spherical harmonics, making it effective in the numerical study of fractional equations and complementing existing theoretical investigations.</t>
+  </si>
+  <si>
+    <t>4th Nov</t>
+  </si>
+  <si>
+    <t>6th Nov</t>
+  </si>
+  <si>
     <t>Lea Kaufmann</t>
   </si>
   <si>
@@ -921,6 +982,9 @@
   </si>
   <si>
     <t>In the last decades, high-dimensional problems in a regression-type context including a large number of explanatory variables arise in a huge variety of application fields. Specifically considering categorical explanatory variables, i.e., factors, the dummy-coding scheme introduces one (dummy) variable for each factor level, thus the dimension of the parameter space grows rapidly, even for a moderate number of factors. To simultaneously obtain the estimates of the regression coefficients and reducing the dimension of the parameter space, penalized regression is known to be a suitable tool. In this talk, I will discuss the characteristics that a penalization technique needs to fulfil to be suitable for the application to factors, as it is not only important to select those having an influence on the response variable (factor selection), but also to fuse those levels of a factor having a similar influence (levels fusion). A new penalization technique, called L0-Fused Group Lasso (L0-FGL), is introduced, tailored for the needs of factors. The quality of this new method is underlined by its theoretical properties, e.g.,  root-n-consistency and asymptotic normality, as well as by its performance in simulation studies.</t>
+  </si>
+  <si>
+    <t>5</t>
   </si>
   <si>
     <t>Alison O'Connor</t>
@@ -1086,49 +1150,18 @@
     <t>Leornard Henckel</t>
   </si>
   <si>
-    <t>Universidade Federal de Minas Gerais</t>
-  </si>
-  <si>
-    <t>Heriot-Watt University</t>
-  </si>
-  <si>
-    <t>University of Bristol</t>
-  </si>
-  <si>
-    <t>University of Leeds</t>
-  </si>
-  <si>
-    <t>University College Cork</t>
-  </si>
-  <si>
-    <t>UCL Centre for Artificial Intelligence</t>
-  </si>
-  <si>
-    <t>University of Huddersfield</t>
-  </si>
-  <si>
-    <t>University of Rochester</t>
-  </si>
-  <si>
-    <t>Murdoch University, Perth, Australia</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> York University</t>
-  </si>
-  <si>
-    <t>Multistatic Synthetic Aperture Radar Imaging and Coherence</t>
-  </si>
-  <si>
-    <t>Synthetic Aperture Radar (SAR) imaging has proven an invaluable all-weather day and night remote sensing information source, increasingly provided by monostatic SAR satellite constellations. Future developments will include multistatic SAR constellations (with a mix of separated transmitter and receiver platforms) for more timely or simultaneous multiple collections for interferometric modes, for example for 3D imaging or more basic terrain height determination, as well as for sensitive change detection amongst others. This presentation will provide an overview of multistatic SAR processing and show highlight results from the Ground-Based SAR laboratory based at Cranfield University, which has allowed the exploration and validation of multistatic SAR sensing concepts amongst others.</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>16th</t>
-  </si>
-  <si>
-    <t>0</t>
+    <t>Hip Fractures Trends in Older Adults in Ireland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">European healthcare systems are under pressure from rapidly ageing populations, with hip fractures representing one of the most costly and impactful injuries among older adults (1,2). Ireland faces the dual challenge of both a rapidly growing ageing population and one of the highest European rates in hip fracture incidence (3,4). Irish standards require admission to orthopaedic care within four hours, yet national audits show this target is rarely achieved (5). Improving hip fracture services requires not just clinical reform but also new ways of leveraging data.
+In this talk, we show how publicly available datasets can be used to uncover correlations and trends in hip fracture demand. When combined with national audit records we show how population health interacts with environmental pressures. Our findings suggest that extreme weather is a strong national indicator of surges in hip fractures with some regions experiencing more pressure than others. This creates opportunities not only for predictive modelling and smarter resource allocation, but also for preventative strategies where timely information can be used to warn and protect at-risk groups.
+References
+1.	Looi MK. The European healthcare workforce crisis: how bad is it? BMJ. 2024 Jan 19;384:q8. 
+2.	EUROSTAT. Ageing Europe - statistics on population developments. Eurostat; 2020. Report No.: 80393. 
+3.	CSO. Central Statistics Office (CSO). Central Statistics Office; 2022 [cited 2024 Sep 23]. Society Measuring Ireland’s Progress 2022 - Central Statistics Office. Available from: https://www.cso.ie/en/releasesandpublications/ep/p-mip/measuringirelandsprogress2022/society/
+4.	Walsh ME, Ferris H, Coughlan T, Hurson C, Ahern E, Sorensen J, et al. Trends in hip fracture care in the Republic of Ireland from 2013 to 2018: results from the Irish Hip Fracture Database. Osteoporos Int. 2021 Apr 1;32(4):727–36. 
+5.	Kelly P, Horan B, Murphy T, Ahern E, Brent L, Kelly F, et al. Irish Hip Fracture Database National Report 2022 [Internet]. National Office of Clinical Audit (NOCA); 2022 p. 1–88. Available from: https://d7g406zpx7bgk.cloudfront.net/38cf762d5b/irish_hip_fracture_database_national_report_2022_final.pdf
+</t>
   </si>
 </sst>
 </file>
@@ -2383,45 +2416,45 @@
         <v>28</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>327</v>
+        <v>29</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="L3" s="5"/>
       <c r="M3" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="N3" s="13" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="O3" s="14" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="P3" s="16"/>
       <c r="Q3" s="14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="S3" s="15" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="T3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="U3" s="16" t="s">
         <v>35</v>
-      </c>
-      <c r="U3" s="16" t="s">
-        <v>34</v>
       </c>
       <c r="V3" s="14"/>
       <c r="W3" s="13"/>
@@ -2446,44 +2479,44 @@
         <v>1</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>328</v>
+        <v>38</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="J4" s="25" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="K4" s="12" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="L4" s="5"/>
       <c r="M4" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="N4" s="13" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="O4" s="14" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="P4" s="16"/>
       <c r="Q4" s="14"/>
       <c r="R4" s="5"/>
       <c r="S4" s="15" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="T4" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="U4" s="16" t="s">
         <v>35</v>
-      </c>
-      <c r="U4" s="16" t="s">
-        <v>34</v>
       </c>
       <c r="V4" s="14"/>
       <c r="W4" s="13"/>
@@ -2508,41 +2541,41 @@
         <v>1</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>333</v>
+        <v>45</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="L5" s="5"/>
       <c r="M5" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="N5" s="13" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="O5" s="14" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="P5" s="16"/>
       <c r="Q5" s="14"/>
       <c r="R5" s="5"/>
       <c r="S5" s="15" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="T5" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="U5" s="16"/>
       <c r="V5" s="14"/>
@@ -2568,48 +2601,48 @@
         <v>2</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>329</v>
+        <v>51</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="J6" s="25" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="L6" s="5"/>
       <c r="M6" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="N6" s="13" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="O6" s="14" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="P6" s="16"/>
       <c r="Q6" s="14" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="R6" s="5" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="S6" s="15" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="T6" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="U6" s="16" t="s">
         <v>35</v>
-      </c>
-      <c r="U6" s="16" t="s">
-        <v>34</v>
       </c>
       <c r="V6" s="14"/>
       <c r="W6" s="13"/>
@@ -2634,53 +2667,53 @@
         <v>3</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>330</v>
+        <v>58</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="L7" s="5"/>
       <c r="M7" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="N7" s="13"/>
       <c r="O7" s="14" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="P7" s="16" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="Q7" s="14" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="R7" s="5" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="S7" s="15" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="T7" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="U7" s="16"/>
       <c r="V7" s="14"/>
       <c r="W7" s="13" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="X7" s="13" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2702,51 +2735,51 @@
         <v>4</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>178</v>
+        <v>67</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="J8" s="25" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
       <c r="M8" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="N8" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="O8" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="O8" s="14" t="s">
-        <v>33</v>
-      </c>
       <c r="P8" s="16" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="Q8" s="14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="R8" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="S8" s="15" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="T8" s="5" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="U8" s="16"/>
       <c r="V8" s="14"/>
       <c r="W8" s="13"/>
       <c r="X8" s="13" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2768,24 +2801,24 @@
         <v>6</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>331</v>
+        <v>72</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="J9" s="25" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
       <c r="M9" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="N9" s="13"/>
       <c r="O9" s="14"/>
@@ -2794,7 +2827,7 @@
       <c r="R9" s="5"/>
       <c r="S9" s="15"/>
       <c r="T9" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="U9" s="16"/>
       <c r="V9" s="14"/>
@@ -2820,51 +2853,51 @@
         <v>7</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>143</v>
+        <v>76</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="K10" s="24" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="L10" s="5"/>
       <c r="M10" s="5" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="N10" s="13"/>
       <c r="O10" s="14" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="P10" s="16" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="Q10" s="14" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="R10" s="5" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="S10" s="15" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="T10" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="U10" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="V10" s="14" t="s">
         <v>35</v>
-      </c>
-      <c r="U10" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="V10" s="14" t="s">
-        <v>34</v>
       </c>
       <c r="W10" s="13"/>
       <c r="X10" s="13"/>
@@ -2888,41 +2921,41 @@
         <v>9</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>143</v>
+        <v>76</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="J11" s="25" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="K11" s="24" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
       <c r="N11" s="13"/>
       <c r="O11" s="14" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="P11" s="16" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="Q11" s="14" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="R11" s="5" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="S11" s="15"/>
       <c r="T11" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="U11" s="16"/>
       <c r="V11" s="14"/>
@@ -2948,43 +2981,43 @@
         <v>10</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="G12" s="14" t="s">
-        <v>332</v>
+        <v>93</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="J12" s="30" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="K12" s="12"/>
       <c r="L12" s="12"/>
       <c r="M12" s="5" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="N12" s="13" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="O12" s="14" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="P12" s="16" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="Q12" s="14" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="R12" s="5" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="S12" s="15"/>
       <c r="T12" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="U12" s="16"/>
       <c r="V12" s="14"/>
@@ -3010,50 +3043,50 @@
         <v>10</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="G13" s="14" t="s">
-        <v>331</v>
+        <v>72</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="K13" s="12" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="L13" s="12" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="M13" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="N13" s="13"/>
       <c r="O13" s="14" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="P13" s="16" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="Q13" s="14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="R13" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="S13" s="15" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="T13" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="U13" s="16" t="s">
         <v>35</v>
-      </c>
-      <c r="U13" s="16" t="s">
-        <v>34</v>
       </c>
       <c r="V13" s="14"/>
       <c r="W13" s="13"/>
@@ -3078,42 +3111,42 @@
         <v>11</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="G14" s="14" t="s">
-        <v>333</v>
+        <v>45</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="I14" s="32" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="J14" s="32" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="K14" s="24" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="L14" s="5"/>
       <c r="M14" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="N14" s="13"/>
       <c r="O14" s="14" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="P14" s="16" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="Q14" s="14"/>
       <c r="R14" s="5"/>
       <c r="S14" s="15"/>
       <c r="T14" s="5" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="U14" s="16" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="V14" s="14"/>
       <c r="W14" s="13"/>
@@ -3138,51 +3171,51 @@
         <v>12</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="G15" s="14" t="s">
-        <v>334</v>
+        <v>110</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="I15" s="33" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="J15" s="33" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="K15" s="31" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="L15" s="5"/>
       <c r="M15" s="5" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="N15" s="13"/>
       <c r="O15" s="14" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="P15" s="16" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="Q15" s="14" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="R15" s="5" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="S15" s="15" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="T15" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="U15" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="U15" s="16" t="s">
-        <v>34</v>
-      </c>
       <c r="V15" s="14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="W15" s="13"/>
       <c r="X15" s="13"/>
@@ -3206,45 +3239,45 @@
         <v>12</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="G16" s="19" t="s">
-        <v>143</v>
+        <v>76</v>
       </c>
       <c r="H16" s="17" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="I16" s="34" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="J16" s="34" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="K16" s="23"/>
       <c r="L16" s="17"/>
       <c r="M16" s="17" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="N16" s="18"/>
       <c r="O16" s="19" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="P16" s="21"/>
       <c r="Q16" s="19" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="R16" s="17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="S16" s="20"/>
       <c r="T16" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="U16" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="U16" s="21" t="s">
-        <v>34</v>
-      </c>
       <c r="V16" s="19" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="W16" s="18"/>
       <c r="X16" s="18"/>
@@ -3268,53 +3301,53 @@
         <v>15</v>
       </c>
       <c r="F17" s="19" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="G17" s="19" t="s">
-        <v>143</v>
+        <v>76</v>
       </c>
       <c r="H17" s="17" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="I17" s="34" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="J17" s="34" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="K17" s="23" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="L17" s="17"/>
       <c r="M17" s="17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="N17" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="O17" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="O17" s="19" t="s">
-        <v>33</v>
-      </c>
       <c r="P17" s="21" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="Q17" s="19" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="R17" s="17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="S17" s="20" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="T17" s="17" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="U17" s="21" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="V17" s="19" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="W17" s="18"/>
       <c r="X17" s="18"/>
@@ -3338,19 +3371,19 @@
         <v>16</v>
       </c>
       <c r="F18" s="19" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="G18" s="19" t="s">
-        <v>335</v>
+        <v>129</v>
       </c>
       <c r="H18" s="17" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="I18" s="34" t="s">
-        <v>119</v>
+        <v>130</v>
       </c>
       <c r="J18" s="34" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="K18" s="23"/>
       <c r="L18" s="17"/>
@@ -3362,7 +3395,7 @@
       <c r="R18" s="17"/>
       <c r="S18" s="20"/>
       <c r="T18" s="17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="U18" s="21"/>
       <c r="V18" s="19"/>
@@ -3388,19 +3421,19 @@
         <v>19</v>
       </c>
       <c r="F19" s="19" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
       <c r="G19" s="19" t="s">
-        <v>336</v>
+        <v>133</v>
       </c>
       <c r="H19" s="17" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="I19" s="34" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
       <c r="J19" s="56" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
       <c r="K19" s="23"/>
       <c r="L19" s="17"/>
@@ -3412,7 +3445,7 @@
       <c r="R19" s="17"/>
       <c r="S19" s="20"/>
       <c r="T19" s="17" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="U19" s="21"/>
       <c r="V19" s="19"/>
@@ -3512,7 +3545,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="148" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="E2" s="149" t="s">
         <v>7</v>
@@ -3566,7 +3599,7 @@
         <v>23</v>
       </c>
       <c r="V2" s="39" t="s">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="W2" s="45" t="s">
         <v>25</v>
@@ -3580,7 +3613,7 @@
         <v>45548</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="C3" s="26" t="str">
         <f t="shared" ref="C3:C10" si="0">TEXT(A3, "mmm")</f>
@@ -3594,47 +3627,47 @@
         <v>1</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="G3" s="40" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
       <c r="H3" s="40" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="I3" s="154" t="s">
-        <v>129</v>
+        <v>141</v>
       </c>
       <c r="J3" s="59" t="s">
-        <v>130</v>
+        <v>142</v>
       </c>
       <c r="K3" s="42" t="s">
-        <v>131</v>
+        <v>143</v>
       </c>
       <c r="L3" s="40"/>
       <c r="M3" s="38" t="s">
-        <v>132</v>
+        <v>144</v>
       </c>
       <c r="N3" s="35"/>
       <c r="O3" s="40" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="P3" s="40" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="Q3" s="40" t="s">
-        <v>135</v>
+        <v>147</v>
       </c>
       <c r="R3" s="38" t="s">
-        <v>136</v>
+        <v>148</v>
       </c>
       <c r="S3" s="35"/>
       <c r="T3" s="40" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="U3" s="40"/>
       <c r="V3" s="40" t="s">
-        <v>137</v>
+        <v>149</v>
       </c>
       <c r="W3" s="46"/>
       <c r="X3" s="44"/>
@@ -3644,7 +3677,7 @@
         <v>45555</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="C4" s="26" t="str">
         <f t="shared" si="0"/>
@@ -3658,19 +3691,19 @@
         <v>2</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>138</v>
+        <v>150</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>139</v>
+        <v>151</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="I4" s="101" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
       <c r="J4" s="25" t="s">
-        <v>141</v>
+        <v>153</v>
       </c>
       <c r="K4" s="12"/>
       <c r="L4" s="5"/>
@@ -3692,7 +3725,7 @@
         <v>45562</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="C5" s="26" t="str">
         <f t="shared" si="0"/>
@@ -3706,19 +3739,19 @@
         <v>3</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>142</v>
+        <v>154</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>143</v>
+        <v>76</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="I5" s="101" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="J5" s="25" t="s">
-        <v>144</v>
+        <v>155</v>
       </c>
       <c r="K5" s="12"/>
       <c r="L5" s="5"/>
@@ -3740,7 +3773,7 @@
         <v>45576</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="C6" s="26" t="str">
         <f t="shared" si="0"/>
@@ -3754,19 +3787,19 @@
         <v>5</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>145</v>
+        <v>156</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>146</v>
+        <v>157</v>
       </c>
       <c r="H6" t="s">
-        <v>147</v>
+        <v>158</v>
       </c>
       <c r="I6" s="129" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="J6" s="25" t="s">
-        <v>149</v>
+        <v>160</v>
       </c>
       <c r="K6" s="12"/>
       <c r="L6" s="5"/>
@@ -3788,7 +3821,7 @@
         <v>45583</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="C7" s="26" t="str">
         <f t="shared" si="0"/>
@@ -3802,19 +3835,19 @@
         <v>6</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>151</v>
+        <v>162</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>152</v>
+        <v>163</v>
       </c>
       <c r="I7" s="101" t="s">
-        <v>153</v>
+        <v>164</v>
       </c>
       <c r="J7" s="25" t="s">
-        <v>154</v>
+        <v>165</v>
       </c>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
@@ -3836,7 +3869,7 @@
         <v>45596</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="C8" s="26" t="str">
         <f t="shared" si="0"/>
@@ -3850,19 +3883,19 @@
         <v>8</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>155</v>
+        <v>166</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="I8" s="101" t="s">
-        <v>157</v>
+        <v>168</v>
       </c>
       <c r="J8" s="25" t="s">
-        <v>158</v>
+        <v>169</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -3884,7 +3917,7 @@
         <v>45604</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="C9" s="26" t="str">
         <f t="shared" si="0"/>
@@ -3898,19 +3931,19 @@
         <v>9</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>159</v>
+        <v>170</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="I9" s="150" t="s">
-        <v>161</v>
+        <v>172</v>
       </c>
       <c r="J9" s="150" t="s">
-        <v>162</v>
+        <v>173</v>
       </c>
       <c r="K9" s="24"/>
       <c r="L9" s="5"/>
@@ -3932,7 +3965,7 @@
         <v>45611</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="C10" s="26" t="str">
         <f t="shared" si="0"/>
@@ -3946,19 +3979,19 @@
         <v>10</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>163</v>
+        <v>174</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="I10" s="151" t="s">
-        <v>165</v>
+        <v>176</v>
       </c>
       <c r="J10" s="151" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
@@ -3980,7 +4013,7 @@
         <v>45625</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="C11" s="26" t="str">
         <f t="shared" ref="C11" si="2">TEXT(A11, "mmm")</f>
@@ -3994,19 +4027,19 @@
         <v>12</v>
       </c>
       <c r="F11" s="57" t="s">
-        <v>167</v>
+        <v>178</v>
       </c>
       <c r="G11" s="58" t="s">
-        <v>168</v>
+        <v>179</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="I11" s="152" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
       <c r="J11" s="152" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="K11" s="12"/>
       <c r="L11" s="12"/>
@@ -4028,7 +4061,7 @@
         <v>45632</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="C12" s="47" t="str">
         <f>TEXT(A12, "mmm")</f>
@@ -4042,35 +4075,35 @@
         <v>13</v>
       </c>
       <c r="F12" s="17" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="H12" s="17" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="I12" s="155" t="s">
-        <v>337</v>
+        <v>184</v>
       </c>
       <c r="J12" s="153" t="s">
-        <v>338</v>
+        <v>185</v>
       </c>
       <c r="K12" s="48"/>
       <c r="L12" s="48"/>
       <c r="M12" s="21"/>
       <c r="N12" s="49"/>
       <c r="O12" s="17" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="P12" s="17" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="Q12" s="17" t="s">
-        <v>173</v>
+        <v>186</v>
       </c>
       <c r="R12" s="21" t="s">
-        <v>174</v>
+        <v>187</v>
       </c>
       <c r="S12" s="49"/>
       <c r="T12" s="17"/>
@@ -4239,10 +4272,10 @@
         <v>5</v>
       </c>
       <c r="D2" s="78" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="E2" s="64" t="s">
-        <v>175</v>
+        <v>188</v>
       </c>
       <c r="F2" s="140" t="s">
         <v>8</v>
@@ -4293,7 +4326,7 @@
         <v>23</v>
       </c>
       <c r="V2" s="66" t="s">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="W2" s="70" t="s">
         <v>25</v>
@@ -4307,10 +4340,10 @@
         <v>45694</v>
       </c>
       <c r="B3" s="126" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="C3" s="120" t="s">
-        <v>177</v>
+        <v>190</v>
       </c>
       <c r="D3" s="104" t="str">
         <f>TEXT(A3, "dddd")</f>
@@ -4320,33 +4353,33 @@
         <v>2</v>
       </c>
       <c r="F3" s="62" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G3" s="38" t="s">
-        <v>178</v>
+        <v>67</v>
       </c>
       <c r="H3" s="108" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="I3" s="113" t="s">
-        <v>179</v>
+        <v>191</v>
       </c>
       <c r="J3" s="99" t="s">
-        <v>180</v>
+        <v>192</v>
       </c>
       <c r="K3" s="71"/>
       <c r="L3" s="40"/>
       <c r="M3" s="38"/>
       <c r="N3" s="35"/>
       <c r="O3" s="40" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="P3" s="40"/>
       <c r="Q3" s="40"/>
       <c r="R3" s="38"/>
       <c r="S3" s="35"/>
       <c r="T3" s="40" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="U3" s="40"/>
       <c r="V3" s="40"/>
@@ -4358,10 +4391,10 @@
         <v>45708</v>
       </c>
       <c r="B4" s="127" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="C4" s="121" t="s">
-        <v>177</v>
+        <v>190</v>
       </c>
       <c r="D4" s="103" t="str">
         <f t="shared" ref="D4:D7" si="0">TEXT(A4, "dddd")</f>
@@ -4371,39 +4404,39 @@
         <v>4</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>181</v>
+        <v>193</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>182</v>
+        <v>194</v>
       </c>
       <c r="H4" s="109" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="I4" s="114" t="s">
-        <v>183</v>
+        <v>195</v>
       </c>
       <c r="J4" s="98" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="K4" s="72"/>
       <c r="L4" s="5"/>
       <c r="M4" s="16" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="N4" s="35"/>
       <c r="O4" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="P4" s="5" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="Q4" s="5"/>
       <c r="R4" s="16"/>
       <c r="S4" s="35" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="T4" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="U4" s="5"/>
       <c r="V4" s="5"/>
@@ -4415,10 +4448,10 @@
         <v>45722</v>
       </c>
       <c r="B5" s="127" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="C5" s="121" t="s">
-        <v>185</v>
+        <v>197</v>
       </c>
       <c r="D5" s="103" t="str">
         <f t="shared" si="0"/>
@@ -4428,37 +4461,37 @@
         <v>6</v>
       </c>
       <c r="F5" s="107" t="s">
-        <v>186</v>
+        <v>198</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>178</v>
+        <v>67</v>
       </c>
       <c r="H5" s="109" t="s">
-        <v>187</v>
+        <v>199</v>
       </c>
       <c r="I5" s="115" t="s">
-        <v>188</v>
+        <v>200</v>
       </c>
       <c r="J5" s="100" t="s">
-        <v>189</v>
+        <v>201</v>
       </c>
       <c r="K5" s="72" t="s">
-        <v>190</v>
+        <v>202</v>
       </c>
       <c r="L5" s="5"/>
       <c r="M5" s="16" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="N5" s="35"/>
       <c r="O5" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
       <c r="R5" s="16"/>
       <c r="S5" s="35"/>
       <c r="T5" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="U5" s="5"/>
       <c r="V5" s="5"/>
@@ -4470,10 +4503,10 @@
         <v>45735</v>
       </c>
       <c r="B6" s="127" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="C6" s="121" t="s">
-        <v>185</v>
+        <v>197</v>
       </c>
       <c r="D6" s="103" t="str">
         <f t="shared" si="0"/>
@@ -4483,37 +4516,37 @@
         <v>8</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>191</v>
+        <v>203</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>192</v>
+        <v>204</v>
       </c>
       <c r="H6" s="109" t="s">
-        <v>193</v>
+        <v>205</v>
       </c>
       <c r="I6" s="115" t="s">
-        <v>194</v>
+        <v>206</v>
       </c>
       <c r="J6" s="98" t="s">
-        <v>195</v>
+        <v>207</v>
       </c>
       <c r="K6" s="72"/>
       <c r="L6" s="5"/>
       <c r="M6" s="16" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="N6" s="35" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="O6" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="P6" s="5"/>
       <c r="Q6" s="5"/>
       <c r="R6" s="16"/>
       <c r="S6" s="35"/>
       <c r="T6" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="U6" s="5"/>
       <c r="V6" s="5"/>
@@ -4525,10 +4558,10 @@
         <v>45750</v>
       </c>
       <c r="B7" s="127" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="C7" s="121" t="s">
-        <v>196</v>
+        <v>208</v>
       </c>
       <c r="D7" s="103" t="str">
         <f t="shared" si="0"/>
@@ -4538,35 +4571,35 @@
         <v>10</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>197</v>
+        <v>209</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>178</v>
+        <v>67</v>
       </c>
       <c r="H7" s="109" t="s">
-        <v>198</v>
+        <v>210</v>
       </c>
       <c r="I7" s="115" t="s">
-        <v>199</v>
+        <v>211</v>
       </c>
       <c r="J7" s="98" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
       <c r="K7" s="73"/>
       <c r="L7" s="5"/>
       <c r="M7" s="16" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="N7" s="35"/>
       <c r="O7" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="P7" s="5"/>
       <c r="Q7" s="5"/>
       <c r="R7" s="16"/>
       <c r="S7" s="35"/>
       <c r="T7" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="U7" s="5"/>
       <c r="V7" s="5"/>
@@ -4578,53 +4611,53 @@
         <v>45751</v>
       </c>
       <c r="B8" s="127" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="C8" s="122" t="s">
-        <v>196</v>
+        <v>208</v>
       </c>
       <c r="D8" s="103" t="s">
-        <v>201</v>
+        <v>213</v>
       </c>
       <c r="E8" s="103">
         <v>10</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>202</v>
+        <v>214</v>
       </c>
       <c r="G8" s="16" t="s">
-        <v>203</v>
+        <v>215</v>
       </c>
       <c r="H8" s="109" t="s">
-        <v>204</v>
+        <v>216</v>
       </c>
       <c r="I8" s="116" t="s">
-        <v>205</v>
+        <v>217</v>
       </c>
       <c r="J8" s="16" t="s">
-        <v>206</v>
+        <v>218</v>
       </c>
       <c r="K8" s="14"/>
       <c r="L8" s="5"/>
       <c r="M8" s="16" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="N8" s="35"/>
       <c r="O8" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="P8" s="5" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="Q8" s="5" t="s">
-        <v>207</v>
+        <v>219</v>
       </c>
       <c r="R8" s="16" t="s">
-        <v>208</v>
+        <v>220</v>
       </c>
       <c r="S8" s="35"/>
       <c r="T8" s="5" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="U8" s="5"/>
       <c r="V8" s="5"/>
@@ -4636,10 +4669,10 @@
         <v>45757</v>
       </c>
       <c r="B9" s="127" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="C9" s="121" t="s">
-        <v>196</v>
+        <v>208</v>
       </c>
       <c r="D9" s="103" t="str">
         <f>TEXT(A10, "dddd")</f>
@@ -4649,43 +4682,43 @@
         <v>11</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>209</v>
+        <v>221</v>
       </c>
       <c r="G9" s="16" t="s">
-        <v>210</v>
+        <v>222</v>
       </c>
       <c r="H9" s="109" t="s">
-        <v>211</v>
+        <v>223</v>
       </c>
       <c r="I9" s="115" t="s">
-        <v>212</v>
+        <v>224</v>
       </c>
       <c r="J9" s="98" t="s">
-        <v>213</v>
+        <v>225</v>
       </c>
       <c r="K9" s="73"/>
       <c r="L9" s="5"/>
       <c r="M9" s="16" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="N9" s="35"/>
       <c r="O9" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="P9" s="5" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="Q9" s="5" t="s">
-        <v>214</v>
+        <v>226</v>
       </c>
       <c r="R9" s="16" t="s">
-        <v>215</v>
+        <v>227</v>
       </c>
       <c r="S9" s="35" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="T9" s="5" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="U9" s="5"/>
       <c r="V9" s="5"/>
@@ -4700,7 +4733,7 @@
         <v>27</v>
       </c>
       <c r="C10" s="121" t="s">
-        <v>196</v>
+        <v>208</v>
       </c>
       <c r="D10" s="103" t="str">
         <f t="shared" ref="D10:D15" si="1">TEXT(A10, "dddd")</f>
@@ -4710,35 +4743,35 @@
         <v>11</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>216</v>
+        <v>228</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>217</v>
+        <v>229</v>
       </c>
       <c r="H10" s="109" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I10" s="115" t="s">
-        <v>218</v>
+        <v>230</v>
       </c>
       <c r="J10" s="98" t="s">
-        <v>219</v>
+        <v>231</v>
       </c>
       <c r="K10" s="74"/>
       <c r="L10" s="48"/>
       <c r="M10" s="21" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="N10" s="49"/>
       <c r="O10" s="17" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="P10" s="17"/>
       <c r="Q10" s="17"/>
       <c r="R10" s="21"/>
       <c r="S10" s="49"/>
       <c r="T10" s="17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="U10" s="17"/>
       <c r="V10" s="17"/>
@@ -4750,10 +4783,10 @@
         <v>45764</v>
       </c>
       <c r="B11" s="128" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="C11" s="123" t="s">
-        <v>196</v>
+        <v>208</v>
       </c>
       <c r="D11" s="105" t="str">
         <f t="shared" si="1"/>
@@ -4763,41 +4796,41 @@
         <v>12</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>220</v>
+        <v>232</v>
       </c>
       <c r="G11" s="21" t="s">
-        <v>221</v>
+        <v>233</v>
       </c>
       <c r="H11" s="110" t="s">
-        <v>222</v>
+        <v>234</v>
       </c>
       <c r="I11" s="117" t="s">
-        <v>223</v>
+        <v>235</v>
       </c>
       <c r="J11" s="112" t="s">
-        <v>224</v>
+        <v>236</v>
       </c>
       <c r="K11" s="72"/>
       <c r="L11" s="72"/>
       <c r="M11" s="14" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="N11" s="35" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="O11" s="14" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="P11" s="14" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="Q11" s="14"/>
       <c r="R11" s="14"/>
       <c r="S11" s="35" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="T11" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="U11" s="14"/>
       <c r="V11" s="14"/>
@@ -4809,7 +4842,7 @@
         <v>45771</v>
       </c>
       <c r="B12" s="128" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="C12" s="124" t="str">
         <f>TEXT(A12,"mmm")</f>
@@ -4823,41 +4856,41 @@
         <v>13</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>225</v>
+        <v>237</v>
       </c>
       <c r="G12" s="16" t="s">
-        <v>143</v>
+        <v>76</v>
       </c>
       <c r="H12" s="109" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="I12" s="114" t="s">
-        <v>226</v>
+        <v>238</v>
       </c>
       <c r="J12" s="98" t="s">
-        <v>227</v>
+        <v>239</v>
       </c>
       <c r="K12" s="72"/>
       <c r="L12" s="72"/>
       <c r="M12" s="14" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="N12" s="35" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="O12" s="14" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="P12" s="14" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="Q12" s="14"/>
       <c r="R12" s="14"/>
       <c r="S12" s="35" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="T12" s="14" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="U12" s="14"/>
       <c r="V12" s="14"/>
@@ -4869,7 +4902,7 @@
         <v>45785</v>
       </c>
       <c r="B13" s="128" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="C13" s="124" t="str">
         <f>TEXT(A13,"mmm")</f>
@@ -4883,33 +4916,33 @@
         <v>15</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>228</v>
+        <v>240</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>143</v>
+        <v>76</v>
       </c>
       <c r="H13" s="109" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="I13" s="114" t="s">
-        <v>229</v>
+        <v>241</v>
       </c>
       <c r="J13" s="98" t="s">
-        <v>230</v>
+        <v>242</v>
       </c>
       <c r="K13" s="72"/>
       <c r="L13" s="72"/>
       <c r="M13" s="14"/>
       <c r="N13" s="35"/>
       <c r="O13" s="14" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="P13" s="14"/>
       <c r="Q13" s="14"/>
       <c r="R13" s="14"/>
       <c r="S13" s="35"/>
       <c r="T13" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="U13" s="14"/>
       <c r="V13" s="14"/>
@@ -4921,7 +4954,7 @@
         <v>45799</v>
       </c>
       <c r="B14" s="119" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="C14" s="125" t="str">
         <f>TEXT(A14,"mmm")</f>
@@ -4935,31 +4968,31 @@
         <v>17</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>231</v>
+        <v>243</v>
       </c>
       <c r="G14" s="21" t="s">
-        <v>232</v>
+        <v>244</v>
       </c>
       <c r="H14" s="111" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="I14" s="118" t="s">
-        <v>233</v>
+        <v>245</v>
       </c>
       <c r="J14" s="112" t="s">
-        <v>234</v>
+        <v>246</v>
       </c>
       <c r="M14" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="O14" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="P14">
         <v>2</v>
       </c>
       <c r="T14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4981,19 +5014,19 @@
         <v>18</v>
       </c>
       <c r="F15" t="s">
-        <v>235</v>
+        <v>247</v>
       </c>
       <c r="G15" t="s">
-        <v>139</v>
+        <v>151</v>
       </c>
       <c r="H15" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="I15" t="s">
-        <v>236</v>
+        <v>248</v>
       </c>
       <c r="J15" s="129" t="s">
-        <v>237</v>
+        <v>249</v>
       </c>
     </row>
     <row r="16" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5122,7 +5155,7 @@
       <pane xSplit="7" ySplit="16" topLeftCell="H17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomRight" activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5174,10 +5207,10 @@
         <v>5</v>
       </c>
       <c r="D2" s="78" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="E2" s="64" t="s">
-        <v>175</v>
+        <v>188</v>
       </c>
       <c r="F2" s="140" t="s">
         <v>8</v>
@@ -5228,7 +5261,7 @@
         <v>23</v>
       </c>
       <c r="V2" s="66" t="s">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="W2" s="70" t="s">
         <v>25</v>
@@ -5242,7 +5275,7 @@
         <v>45911</v>
       </c>
       <c r="B3" s="77" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="C3" s="29" t="str">
         <f>TEXT(A3, "mmm")</f>
@@ -5256,43 +5289,43 @@
         <v>1</v>
       </c>
       <c r="F3" s="101" t="s">
-        <v>238</v>
+        <v>250</v>
       </c>
       <c r="G3" s="107" t="s">
-        <v>239</v>
+        <v>251</v>
       </c>
       <c r="H3" s="25" t="s">
-        <v>240</v>
+        <v>252</v>
       </c>
       <c r="I3" s="98" t="s">
-        <v>241</v>
+        <v>253</v>
       </c>
       <c r="J3" s="98" t="s">
-        <v>242</v>
+        <v>254</v>
       </c>
       <c r="K3" s="156" t="s">
-        <v>243</v>
+        <v>255</v>
       </c>
       <c r="L3" s="59" t="s">
-        <v>244</v>
+        <v>256</v>
       </c>
       <c r="M3" s="38" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="N3" s="35" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="O3" s="40" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="P3" s="40" t="s">
-        <v>341</v>
+        <v>257</v>
       </c>
       <c r="Q3" s="40"/>
       <c r="R3" s="38"/>
       <c r="S3" s="35"/>
       <c r="T3" s="40" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="U3" s="40"/>
       <c r="V3" s="40"/>
@@ -5304,7 +5337,7 @@
         <v>45917</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>245</v>
+        <v>258</v>
       </c>
       <c r="C4" s="29" t="str">
         <f>TEXT(A4, "mmm")</f>
@@ -5318,49 +5351,49 @@
         <v>2</v>
       </c>
       <c r="F4" s="101" t="s">
-        <v>246</v>
+        <v>259</v>
       </c>
       <c r="G4" s="107" t="s">
-        <v>247</v>
+        <v>260</v>
       </c>
       <c r="H4" s="25" t="s">
-        <v>248</v>
+        <v>261</v>
       </c>
       <c r="I4" s="98" t="s">
-        <v>249</v>
+        <v>262</v>
       </c>
       <c r="J4" s="98" t="s">
-        <v>250</v>
+        <v>263</v>
       </c>
       <c r="K4" s="156" t="s">
-        <v>251</v>
+        <v>264</v>
       </c>
       <c r="L4" s="25" t="s">
-        <v>252</v>
+        <v>265</v>
       </c>
       <c r="M4" s="16" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="N4" s="35" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="O4" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="P4" s="5" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="Q4" s="5" t="s">
-        <v>340</v>
+        <v>266</v>
       </c>
       <c r="R4" s="16" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="S4" s="35" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="T4" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="U4" s="5"/>
       <c r="V4" s="5"/>
@@ -5372,7 +5405,7 @@
         <v>45926</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>253</v>
+        <v>267</v>
       </c>
       <c r="C5" s="26" t="str">
         <f>TEXT(A5, "mmm")</f>
@@ -5387,37 +5420,37 @@
         <v>3</v>
       </c>
       <c r="F5" s="101" t="s">
-        <v>254</v>
+        <v>268</v>
       </c>
       <c r="G5" s="107" t="s">
-        <v>255</v>
+        <v>269</v>
       </c>
       <c r="H5" s="25" t="s">
-        <v>193</v>
+        <v>205</v>
       </c>
       <c r="I5" s="98" t="s">
-        <v>256</v>
+        <v>270</v>
       </c>
       <c r="J5" s="98" t="s">
-        <v>257</v>
+        <v>271</v>
       </c>
       <c r="K5" s="157"/>
       <c r="L5" s="25"/>
       <c r="M5" s="16" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="N5" s="35"/>
       <c r="O5" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="P5" s="5" t="s">
-        <v>341</v>
+        <v>257</v>
       </c>
       <c r="Q5" s="5"/>
       <c r="R5" s="16"/>
       <c r="S5" s="35"/>
       <c r="T5" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="U5" s="5"/>
       <c r="V5" s="5"/>
@@ -5429,7 +5462,7 @@
         <v>45939</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="C6" s="26" t="str">
         <f t="shared" ref="C6" si="0">TEXT(A6, "mmm")</f>
@@ -5444,41 +5477,43 @@
         <v>5</v>
       </c>
       <c r="F6" s="101" t="s">
-        <v>258</v>
+        <v>272</v>
       </c>
       <c r="G6" s="107" t="s">
-        <v>259</v>
+        <v>273</v>
       </c>
       <c r="H6" s="25" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="I6" s="96" t="s">
-        <v>260</v>
+        <v>274</v>
       </c>
       <c r="J6" s="98" t="s">
-        <v>261</v>
-      </c>
-      <c r="K6" s="157"/>
+        <v>275</v>
+      </c>
+      <c r="K6" s="157" t="s">
+        <v>276</v>
+      </c>
       <c r="L6" s="25"/>
       <c r="M6" s="16" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="N6" s="35" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="O6" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="P6" s="5" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="Q6" s="5"/>
       <c r="R6" s="16"/>
       <c r="S6" s="35" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="T6" s="5" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="U6" s="5"/>
       <c r="V6" s="5"/>
@@ -5490,49 +5525,51 @@
         <v>45946</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>263</v>
+        <v>278</v>
       </c>
       <c r="E7">
         <v>6</v>
       </c>
       <c r="F7" s="101" t="s">
-        <v>264</v>
+        <v>279</v>
       </c>
       <c r="G7" s="107" t="s">
-        <v>178</v>
+        <v>67</v>
       </c>
       <c r="H7" s="25" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I7" s="97" t="s">
-        <v>265</v>
+        <v>280</v>
       </c>
       <c r="J7" s="98" t="s">
-        <v>261</v>
-      </c>
-      <c r="K7" s="157"/>
+        <v>275</v>
+      </c>
+      <c r="K7" s="157" t="s">
+        <v>281</v>
+      </c>
       <c r="L7" s="25"/>
       <c r="M7" s="16" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="N7" s="35"/>
       <c r="O7" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="P7" s="5" t="s">
-        <v>341</v>
+        <v>257</v>
       </c>
       <c r="Q7" s="5"/>
       <c r="R7" s="16"/>
       <c r="S7" s="35"/>
       <c r="T7" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="U7" s="5"/>
       <c r="V7" s="5"/>
@@ -5544,7 +5581,7 @@
         <v>45953</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="C8" s="26" t="str">
         <f>TEXT(A8, "mmm")</f>
@@ -5559,35 +5596,35 @@
         <v>7</v>
       </c>
       <c r="F8" s="101" t="s">
-        <v>266</v>
+        <v>282</v>
       </c>
       <c r="G8" s="107" t="s">
-        <v>267</v>
+        <v>283</v>
       </c>
       <c r="H8" s="25" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I8" s="97" t="s">
-        <v>261</v>
+        <v>275</v>
       </c>
       <c r="J8" s="98" t="s">
-        <v>261</v>
+        <v>275</v>
       </c>
       <c r="K8" s="157"/>
       <c r="L8" s="25"/>
       <c r="M8" s="16" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="N8" s="35"/>
       <c r="O8" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="P8" s="5"/>
       <c r="Q8" s="5"/>
       <c r="R8" s="16"/>
       <c r="S8" s="35"/>
       <c r="T8" s="5" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="U8" s="5"/>
       <c r="V8" s="5"/>
@@ -5599,7 +5636,7 @@
         <v>45967</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="C9" s="26" t="str">
         <f>TEXT(A9, "mmm")</f>
@@ -5614,28 +5651,36 @@
         <v>9</v>
       </c>
       <c r="F9" s="101" t="s">
-        <v>268</v>
+        <v>284</v>
       </c>
       <c r="G9" s="107" t="s">
-        <v>255</v>
+        <v>269</v>
       </c>
       <c r="H9" s="25" t="s">
-        <v>187</v>
+        <v>199</v>
       </c>
       <c r="I9" s="97" t="s">
-        <v>261</v>
+        <v>285</v>
       </c>
       <c r="J9" s="97" t="s">
-        <v>261</v>
+        <v>286</v>
       </c>
       <c r="K9" s="157"/>
       <c r="L9" s="25"/>
       <c r="M9" s="16"/>
       <c r="N9" s="35"/>
-      <c r="O9" s="5"/>
-      <c r="P9" s="5"/>
-      <c r="Q9" s="5"/>
-      <c r="R9" s="16"/>
+      <c r="O9" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="P9" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q9" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="R9" s="16" t="s">
+        <v>288</v>
+      </c>
       <c r="S9" s="35"/>
       <c r="T9" s="5"/>
       <c r="U9" s="5"/>
@@ -5648,7 +5693,7 @@
         <v>45974</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="C10" s="26" t="str">
         <f>TEXT(A10, "mmm")</f>
@@ -5662,39 +5707,39 @@
         <v>10</v>
       </c>
       <c r="F10" s="101" t="s">
-        <v>269</v>
+        <v>289</v>
       </c>
       <c r="G10" s="107" t="s">
-        <v>270</v>
+        <v>290</v>
       </c>
       <c r="H10" s="25" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="I10" s="97" t="s">
-        <v>271</v>
+        <v>291</v>
       </c>
       <c r="J10" s="97" t="s">
-        <v>272</v>
+        <v>292</v>
       </c>
       <c r="K10" s="157"/>
       <c r="L10" s="25"/>
       <c r="M10" s="16" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="N10" s="35"/>
       <c r="O10" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="P10" s="5" t="s">
-        <v>339</v>
+        <v>293</v>
       </c>
       <c r="Q10" s="5"/>
       <c r="R10" s="16"/>
       <c r="S10" s="35" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="T10" s="5" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="U10" s="5"/>
       <c r="V10" s="5"/>
@@ -5706,7 +5751,7 @@
         <v>45981</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="C11" s="26" t="str">
         <f>TEXT(A11, "mmm")</f>
@@ -5721,37 +5766,37 @@
         <v>11</v>
       </c>
       <c r="F11" s="101" t="s">
-        <v>273</v>
+        <v>294</v>
       </c>
       <c r="G11" s="107" t="s">
-        <v>178</v>
+        <v>67</v>
       </c>
       <c r="H11" s="25" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="I11" s="97" t="s">
-        <v>261</v>
+        <v>348</v>
       </c>
       <c r="J11" s="98" t="s">
-        <v>261</v>
+        <v>349</v>
       </c>
       <c r="K11" s="107"/>
       <c r="L11" s="25"/>
       <c r="M11" s="16" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="N11" s="35"/>
       <c r="O11" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="P11" s="5" t="s">
-        <v>341</v>
+        <v>257</v>
       </c>
       <c r="Q11" s="5"/>
       <c r="R11" s="16"/>
       <c r="S11" s="35"/>
       <c r="T11" s="5" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="U11" s="5"/>
       <c r="V11" s="5"/>
@@ -5763,7 +5808,7 @@
         <v>45995</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="C12" s="26" t="str">
         <f>TEXT(A12, "mmm")</f>
@@ -5778,39 +5823,39 @@
         <v>13</v>
       </c>
       <c r="F12" s="101" t="s">
-        <v>274</v>
+        <v>295</v>
       </c>
       <c r="G12" s="107" t="s">
-        <v>275</v>
+        <v>296</v>
       </c>
       <c r="H12" s="25" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="I12" s="97" t="s">
-        <v>276</v>
+        <v>297</v>
       </c>
       <c r="J12" s="132" t="s">
-        <v>277</v>
+        <v>298</v>
       </c>
       <c r="K12" s="157"/>
       <c r="L12" s="25"/>
       <c r="M12" s="16" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="N12" s="35"/>
       <c r="O12" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="P12" s="5" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="Q12" s="5"/>
       <c r="R12" s="16"/>
       <c r="S12" s="35" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="T12" s="5" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="U12" s="5"/>
       <c r="V12" s="5"/>
@@ -5857,6 +5902,8 @@
   <hyperlinks>
     <hyperlink ref="K3" r:id="rId1" xr:uid="{CC4847BF-5CC0-41D9-9E80-86D0D78BEFCD}"/>
     <hyperlink ref="K4" r:id="rId2" xr:uid="{7DFE3762-8F5E-4F84-9CA0-19AC05FFD4B0}"/>
+    <hyperlink ref="K6" r:id="rId3" xr:uid="{B9C6041F-ED68-4E30-9696-976A7A7C59D6}"/>
+    <hyperlink ref="K7" r:id="rId4" xr:uid="{7120277C-1705-4DE0-ADA5-C41C5441CF52}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5919,10 +5966,10 @@
         <v>5</v>
       </c>
       <c r="D2" s="78" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="E2" s="64" t="s">
-        <v>175</v>
+        <v>188</v>
       </c>
       <c r="F2" s="140" t="s">
         <v>8</v>
@@ -5973,7 +6020,7 @@
         <v>23</v>
       </c>
       <c r="V2" s="66" t="s">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="W2" s="70" t="s">
         <v>25</v>
@@ -5987,7 +6034,7 @@
         <v>46051</v>
       </c>
       <c r="B3" s="77" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="C3" s="29" t="str">
         <f>TEXT(A3, "mmm")</f>
@@ -6001,28 +6048,28 @@
         <v>1</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>278</v>
+        <v>299</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>261</v>
+        <v>275</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>261</v>
+        <v>275</v>
       </c>
       <c r="I3" s="98" t="s">
-        <v>261</v>
+        <v>275</v>
       </c>
       <c r="J3" s="98" t="s">
-        <v>261</v>
+        <v>275</v>
       </c>
       <c r="K3" s="73"/>
       <c r="L3" s="40"/>
       <c r="M3" s="38"/>
       <c r="N3" s="35" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="O3" s="40" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="P3" s="40"/>
       <c r="Q3" s="40"/>
@@ -6040,7 +6087,7 @@
         <v>46065</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="C4" s="26" t="str">
         <f t="shared" ref="C4:C9" si="0">TEXT(A4, "mmm")</f>
@@ -6055,26 +6102,26 @@
         <v>3</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>278</v>
+        <v>299</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>261</v>
+        <v>275</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>261</v>
+        <v>275</v>
       </c>
       <c r="I4" s="98" t="s">
-        <v>261</v>
+        <v>275</v>
       </c>
       <c r="J4" s="98" t="s">
-        <v>261</v>
+        <v>275</v>
       </c>
       <c r="K4" s="102"/>
       <c r="L4" s="5"/>
       <c r="M4" s="16"/>
       <c r="N4" s="35"/>
       <c r="O4" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="P4" s="5"/>
       <c r="Q4" s="5"/>
@@ -6092,7 +6139,7 @@
         <v>46079</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="C5" s="26" t="str">
         <f t="shared" si="0"/>
@@ -6107,26 +6154,26 @@
         <v>5</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>278</v>
+        <v>299</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>261</v>
+        <v>275</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>261</v>
+        <v>275</v>
       </c>
       <c r="I5" s="98" t="s">
-        <v>261</v>
+        <v>275</v>
       </c>
       <c r="J5" s="98" t="s">
-        <v>261</v>
+        <v>275</v>
       </c>
       <c r="K5" s="102"/>
       <c r="L5" s="5"/>
       <c r="M5" s="16"/>
       <c r="N5" s="35"/>
       <c r="O5" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
@@ -6144,7 +6191,7 @@
         <v>46093</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="C6" s="26" t="str">
         <f t="shared" si="0"/>
@@ -6159,26 +6206,26 @@
         <v>7</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>278</v>
+        <v>299</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>261</v>
+        <v>275</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>261</v>
+        <v>275</v>
       </c>
       <c r="I6" s="98" t="s">
-        <v>261</v>
+        <v>275</v>
       </c>
       <c r="J6" s="98" t="s">
-        <v>261</v>
+        <v>275</v>
       </c>
       <c r="K6" s="102"/>
       <c r="L6" s="5"/>
       <c r="M6" s="16"/>
       <c r="N6" s="35"/>
       <c r="O6" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="P6" s="5"/>
       <c r="Q6" s="5"/>
@@ -6196,7 +6243,7 @@
         <v>46107</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="C7" s="26" t="str">
         <f t="shared" si="0"/>
@@ -6211,26 +6258,26 @@
         <v>9</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>278</v>
+        <v>299</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>261</v>
+        <v>275</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>261</v>
+        <v>275</v>
       </c>
       <c r="I7" s="98" t="s">
-        <v>261</v>
+        <v>275</v>
       </c>
       <c r="J7" s="98" t="s">
-        <v>261</v>
+        <v>275</v>
       </c>
       <c r="K7" s="102"/>
       <c r="L7" s="5"/>
       <c r="M7" s="16"/>
       <c r="N7" s="35"/>
       <c r="O7" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="P7" s="5"/>
       <c r="Q7" s="5"/>
@@ -6248,7 +6295,7 @@
         <v>46121</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="C8" s="26" t="str">
         <f t="shared" si="0"/>
@@ -6263,19 +6310,19 @@
         <v>11</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>278</v>
+        <v>299</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>261</v>
+        <v>275</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>261</v>
+        <v>275</v>
       </c>
       <c r="I8" s="98" t="s">
-        <v>261</v>
+        <v>275</v>
       </c>
       <c r="J8" s="98" t="s">
-        <v>261</v>
+        <v>275</v>
       </c>
       <c r="K8" s="102"/>
       <c r="L8" s="5"/>
@@ -6298,7 +6345,7 @@
         <v>46135</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="C9" s="26" t="str">
         <f t="shared" si="0"/>
@@ -6313,26 +6360,26 @@
         <v>13</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>278</v>
+        <v>299</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>261</v>
+        <v>275</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>261</v>
+        <v>275</v>
       </c>
       <c r="I9" s="98" t="s">
-        <v>261</v>
+        <v>275</v>
       </c>
       <c r="J9" s="98" t="s">
-        <v>261</v>
+        <v>275</v>
       </c>
       <c r="K9" s="102"/>
       <c r="L9" s="5"/>
       <c r="M9" s="16"/>
       <c r="N9" s="35"/>
       <c r="O9" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="P9" s="5"/>
       <c r="Q9" s="5"/>
@@ -6395,222 +6442,222 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>279</v>
+        <v>300</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="55" t="s">
-        <v>280</v>
+        <v>301</v>
       </c>
       <c r="B2" s="54" t="s">
-        <v>281</v>
+        <v>302</v>
       </c>
       <c r="C2" s="54" t="s">
-        <v>282</v>
+        <v>303</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="136" t="s">
-        <v>283</v>
+        <v>304</v>
       </c>
       <c r="B3" s="137"/>
       <c r="C3" s="138" t="s">
-        <v>211</v>
+        <v>223</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>284</v>
+        <v>305</v>
       </c>
       <c r="B4" s="52"/>
       <c r="C4" s="50" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="52" t="s">
-        <v>285</v>
+        <v>306</v>
       </c>
       <c r="B5" s="52"/>
       <c r="C5" s="50" t="s">
-        <v>286</v>
+        <v>307</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="52" t="s">
-        <v>287</v>
+        <v>308</v>
       </c>
       <c r="B6" s="52" t="s">
-        <v>288</v>
+        <v>309</v>
       </c>
       <c r="C6" s="50" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="52" t="s">
-        <v>289</v>
+        <v>310</v>
       </c>
       <c r="B7" s="52" t="s">
-        <v>290</v>
+        <v>311</v>
       </c>
       <c r="C7" s="50" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="52" t="s">
-        <v>291</v>
+        <v>312</v>
       </c>
       <c r="B8" s="52" t="s">
-        <v>292</v>
+        <v>313</v>
       </c>
       <c r="C8" s="50" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="52" t="s">
-        <v>293</v>
+        <v>314</v>
       </c>
       <c r="B9" s="52"/>
       <c r="C9" s="50"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="52" t="s">
-        <v>294</v>
+        <v>315</v>
       </c>
       <c r="B10" s="52" t="s">
-        <v>295</v>
+        <v>316</v>
       </c>
       <c r="C10" s="50" t="s">
-        <v>296</v>
+        <v>317</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="52" t="s">
-        <v>297</v>
+        <v>318</v>
       </c>
       <c r="B11" s="52" t="s">
-        <v>298</v>
+        <v>319</v>
       </c>
       <c r="C11" s="50" t="s">
-        <v>299</v>
+        <v>320</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="52" t="s">
-        <v>300</v>
+        <v>321</v>
       </c>
       <c r="B12" s="52" t="s">
-        <v>301</v>
+        <v>322</v>
       </c>
       <c r="C12" s="50" t="s">
-        <v>299</v>
+        <v>320</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="52" t="s">
-        <v>302</v>
+        <v>323</v>
       </c>
       <c r="B13" s="52" t="s">
-        <v>303</v>
+        <v>324</v>
       </c>
       <c r="C13" s="50" t="s">
-        <v>299</v>
+        <v>320</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="52" t="s">
-        <v>304</v>
+        <v>325</v>
       </c>
       <c r="B14" s="52" t="s">
-        <v>305</v>
+        <v>326</v>
       </c>
       <c r="C14" s="50" t="s">
-        <v>299</v>
+        <v>320</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="52" t="s">
-        <v>306</v>
+        <v>327</v>
       </c>
       <c r="B15" s="52" t="s">
-        <v>307</v>
+        <v>328</v>
       </c>
       <c r="C15" s="50" t="s">
-        <v>299</v>
+        <v>320</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="137" t="s">
-        <v>274</v>
+        <v>295</v>
       </c>
       <c r="B16" s="137" t="s">
-        <v>308</v>
+        <v>329</v>
       </c>
       <c r="C16" s="139" t="s">
-        <v>309</v>
+        <v>330</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="52" t="s">
-        <v>310</v>
+        <v>331</v>
       </c>
       <c r="B17" s="52" t="s">
-        <v>311</v>
+        <v>332</v>
       </c>
       <c r="C17" s="50" t="s">
-        <v>309</v>
+        <v>330</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="52" t="s">
-        <v>312</v>
+        <v>333</v>
       </c>
       <c r="B18" s="52" t="s">
-        <v>288</v>
+        <v>309</v>
       </c>
       <c r="C18" s="50" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="53" t="s">
-        <v>313</v>
+        <v>334</v>
       </c>
       <c r="B19" s="53" t="s">
-        <v>217</v>
+        <v>229</v>
       </c>
       <c r="C19" s="51" t="s">
-        <v>314</v>
+        <v>335</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>315</v>
+        <v>336</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>312</v>
+        <v>333</v>
       </c>
       <c r="B24" t="s">
-        <v>288</v>
+        <v>309</v>
       </c>
       <c r="C24" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>313</v>
+        <v>334</v>
       </c>
       <c r="B25" t="s">
-        <v>217</v>
+        <v>229</v>
       </c>
       <c r="C25" t="s">
-        <v>314</v>
+        <v>335</v>
       </c>
     </row>
   </sheetData>
@@ -6642,10 +6689,10 @@
         <v>3</v>
       </c>
       <c r="B1" s="131" t="s">
-        <v>316</v>
+        <v>337</v>
       </c>
       <c r="C1" s="130" t="s">
-        <v>317</v>
+        <v>338</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -6656,13 +6703,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="134" t="s">
-        <v>318</v>
+        <v>339</v>
       </c>
       <c r="F2" s="75">
         <v>45911</v>
       </c>
       <c r="G2" s="77" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="H2" s="29" t="str">
         <f>TEXT(F2, "mmm")</f>
@@ -6686,13 +6733,13 @@
         <v>2</v>
       </c>
       <c r="C3" s="134" t="s">
-        <v>318</v>
+        <v>339</v>
       </c>
       <c r="F3" s="75">
         <v>45926</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>253</v>
+        <v>267</v>
       </c>
       <c r="H3" s="26" t="str">
         <f>TEXT(F3, "mmm")</f>
@@ -6717,13 +6764,13 @@
         <v>3</v>
       </c>
       <c r="C4" s="134" t="s">
-        <v>318</v>
+        <v>339</v>
       </c>
       <c r="F4" s="75">
         <v>45939</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="H4" s="26" t="str">
         <f t="shared" ref="H4" si="2">TEXT(F4, "mmm")</f>
@@ -6748,19 +6795,19 @@
         <v>4</v>
       </c>
       <c r="C5" s="134" t="s">
-        <v>318</v>
+        <v>339</v>
       </c>
       <c r="F5" s="75">
         <v>45946</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="H5" s="26" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="I5" s="27" t="s">
-        <v>263</v>
+        <v>278</v>
       </c>
       <c r="J5">
         <v>6</v>
@@ -6776,13 +6823,13 @@
         <v>5</v>
       </c>
       <c r="C6" s="134" t="s">
-        <v>318</v>
+        <v>339</v>
       </c>
       <c r="F6" s="75">
         <v>45953</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="H6" s="26" t="str">
         <f>TEXT(F6, "mmm")</f>
@@ -6807,13 +6854,13 @@
         <v>6</v>
       </c>
       <c r="C7" s="134" t="s">
-        <v>278</v>
+        <v>299</v>
       </c>
       <c r="F7" s="75">
         <v>45967</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="H7" s="26" t="str">
         <f>TEXT(F7, "mmm")</f>
@@ -6838,13 +6885,13 @@
         <v>7</v>
       </c>
       <c r="C8" s="134" t="s">
-        <v>319</v>
+        <v>340</v>
       </c>
       <c r="F8" s="75">
         <v>45974</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="H8" s="26" t="str">
         <f>TEXT(F8, "mmm")</f>
@@ -6868,13 +6915,13 @@
         <v>8</v>
       </c>
       <c r="C9" s="134" t="s">
-        <v>318</v>
+        <v>339</v>
       </c>
       <c r="F9" s="75">
         <v>45981</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="H9" s="26" t="str">
         <f>TEXT(F9, "mmm")</f>
@@ -6899,13 +6946,13 @@
         <v>9</v>
       </c>
       <c r="C10" s="134" t="s">
-        <v>319</v>
+        <v>340</v>
       </c>
       <c r="F10" s="75">
         <v>45995</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="H10" s="26" t="str">
         <f>TEXT(F10, "mmm")</f>
@@ -6930,7 +6977,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="134" t="s">
-        <v>318</v>
+        <v>339</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -6943,7 +6990,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="134" t="s">
-        <v>318</v>
+        <v>339</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -6956,7 +7003,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="134" t="s">
-        <v>278</v>
+        <v>299</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -6969,7 +7016,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="134" t="s">
-        <v>318</v>
+        <v>339</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -7022,12 +7069,12 @@
   <sheetData>
     <row r="2" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="91" t="s">
-        <v>320</v>
+        <v>341</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="79" t="s">
-        <v>321</v>
+        <v>342</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="37.5" x14ac:dyDescent="0.25">
@@ -7041,10 +7088,10 @@
         <v>5</v>
       </c>
       <c r="D5" s="80" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="E5" s="80" t="s">
-        <v>175</v>
+        <v>188</v>
       </c>
       <c r="F5" s="80" t="s">
         <v>8</v>
@@ -7053,7 +7100,7 @@
         <v>9</v>
       </c>
       <c r="H5" s="82" t="s">
-        <v>322</v>
+        <v>343</v>
       </c>
       <c r="I5" s="81" t="s">
         <v>11</v>
@@ -7064,26 +7111,26 @@
         <v>45694</v>
       </c>
       <c r="B6" s="92" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="C6" s="92" t="s">
-        <v>177</v>
+        <v>190</v>
       </c>
       <c r="D6" s="93" t="s">
-        <v>263</v>
+        <v>278</v>
       </c>
       <c r="E6" s="93">
         <v>2</v>
       </c>
       <c r="F6" s="85" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G6" s="85" t="s">
-        <v>178</v>
+        <v>67</v>
       </c>
       <c r="H6" s="85"/>
       <c r="I6" s="84" t="s">
-        <v>261</v>
+        <v>275</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
@@ -7091,28 +7138,28 @@
         <v>45708</v>
       </c>
       <c r="B7" s="83" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="C7" s="83" t="s">
-        <v>177</v>
+        <v>190</v>
       </c>
       <c r="D7" s="94" t="s">
-        <v>263</v>
+        <v>278</v>
       </c>
       <c r="E7" s="94">
         <v>4</v>
       </c>
       <c r="F7" s="87" t="s">
-        <v>181</v>
+        <v>193</v>
       </c>
       <c r="G7" s="87" t="s">
-        <v>182</v>
+        <v>194</v>
       </c>
       <c r="H7" s="87" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="I7" s="86" t="s">
-        <v>183</v>
+        <v>195</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
@@ -7120,25 +7167,25 @@
         <v>45722</v>
       </c>
       <c r="B8" s="83" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="C8" s="83" t="s">
-        <v>185</v>
+        <v>197</v>
       </c>
       <c r="D8" s="94" t="s">
-        <v>263</v>
+        <v>278</v>
       </c>
       <c r="E8" s="94">
         <v>6</v>
       </c>
       <c r="F8" s="87" t="s">
-        <v>186</v>
+        <v>198</v>
       </c>
       <c r="G8" s="87" t="s">
-        <v>178</v>
+        <v>67</v>
       </c>
       <c r="H8" s="87" t="s">
-        <v>187</v>
+        <v>199</v>
       </c>
       <c r="I8" s="86"/>
     </row>
@@ -7147,28 +7194,28 @@
         <v>45735</v>
       </c>
       <c r="B9" s="83" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="C9" s="83" t="s">
-        <v>185</v>
+        <v>197</v>
       </c>
       <c r="D9" s="94" t="s">
-        <v>323</v>
+        <v>344</v>
       </c>
       <c r="E9" s="94">
         <v>8</v>
       </c>
       <c r="F9" s="87" t="s">
-        <v>191</v>
+        <v>203</v>
       </c>
       <c r="G9" s="87" t="s">
-        <v>192</v>
+        <v>204</v>
       </c>
       <c r="H9" s="87" t="s">
-        <v>193</v>
+        <v>205</v>
       </c>
       <c r="I9" s="86" t="s">
-        <v>261</v>
+        <v>275</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
@@ -7176,25 +7223,25 @@
         <v>45744</v>
       </c>
       <c r="B10" s="83" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="C10" s="83" t="s">
-        <v>185</v>
+        <v>197</v>
       </c>
       <c r="D10" s="94" t="s">
-        <v>201</v>
+        <v>213</v>
       </c>
       <c r="E10" s="94">
         <v>9</v>
       </c>
       <c r="F10" s="87" t="s">
-        <v>209</v>
+        <v>221</v>
       </c>
       <c r="G10" s="87" t="s">
-        <v>210</v>
+        <v>222</v>
       </c>
       <c r="H10" s="87" t="s">
-        <v>211</v>
+        <v>223</v>
       </c>
       <c r="I10" s="86"/>
     </row>
@@ -7203,26 +7250,26 @@
         <v>45750</v>
       </c>
       <c r="B11" s="83" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="C11" s="83" t="s">
-        <v>196</v>
+        <v>208</v>
       </c>
       <c r="D11" s="94" t="s">
-        <v>263</v>
+        <v>278</v>
       </c>
       <c r="E11" s="94">
         <v>10</v>
       </c>
       <c r="F11" s="87" t="s">
-        <v>324</v>
+        <v>345</v>
       </c>
       <c r="G11" s="87" t="s">
-        <v>178</v>
+        <v>67</v>
       </c>
       <c r="H11" s="87"/>
       <c r="I11" s="86" t="s">
-        <v>261</v>
+        <v>275</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
@@ -7233,25 +7280,25 @@
         <v>27</v>
       </c>
       <c r="C12" s="83" t="s">
-        <v>196</v>
+        <v>208</v>
       </c>
       <c r="D12" s="94" t="s">
-        <v>201</v>
+        <v>213</v>
       </c>
       <c r="E12" s="94">
         <v>11</v>
       </c>
       <c r="F12" s="87" t="s">
-        <v>216</v>
+        <v>228</v>
       </c>
       <c r="G12" s="87" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="H12" s="87" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I12" s="86" t="s">
-        <v>261</v>
+        <v>275</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
@@ -7259,19 +7306,19 @@
         <v>45764</v>
       </c>
       <c r="B13" s="83" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="C13" s="83" t="s">
-        <v>196</v>
+        <v>208</v>
       </c>
       <c r="D13" s="94" t="s">
-        <v>263</v>
+        <v>278</v>
       </c>
       <c r="E13" s="94">
         <v>12</v>
       </c>
       <c r="F13" s="87" t="s">
-        <v>325</v>
+        <v>346</v>
       </c>
       <c r="G13" s="87"/>
       <c r="H13" s="87"/>
@@ -7282,28 +7329,28 @@
         <v>45771</v>
       </c>
       <c r="B14" s="88" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="C14" s="88" t="s">
-        <v>196</v>
+        <v>208</v>
       </c>
       <c r="D14" s="95" t="s">
-        <v>263</v>
+        <v>278</v>
       </c>
       <c r="E14" s="95">
         <v>13</v>
       </c>
       <c r="F14" s="90" t="s">
-        <v>326</v>
+        <v>347</v>
       </c>
       <c r="G14" s="90" t="s">
-        <v>143</v>
+        <v>76</v>
       </c>
       <c r="H14" s="90" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="I14" s="89" t="s">
-        <v>226</v>
+        <v>238</v>
       </c>
     </row>
     <row r="20" spans="8:8" ht="18.75" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
fix paragraph issue in old seminars
</commit_message>
<xml_diff>
--- a/data/MACSI seminar series.xlsx
+++ b/data/MACSI seminar series.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ulcampus-my.sharepoint.com/personal/david_osullivan_ul_ie/Documents/Academic_work/_Misc/MACSI_Seminars/macsi-seminars.github.io/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2495" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E6A7292-0199-4105-A415-9AF6D3B45CEC}"/>
+  <xr:revisionPtr revIDLastSave="2497" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{994866AB-1CAF-4008-B678-59E24FA32A5B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AY2023-2024 Sem 2" sheetId="3" r:id="rId1"/>
@@ -728,22 +728,6 @@
     <t>One, Two, Many (or a dozen reasons why mathematics isn’t as easy as 1,2,3)</t>
   </si>
   <si>
-    <t>Are there really primitive tribes whose system of counting goes: "One, Two, Many", indicating that
-from three on it’s more or less a blur? Maybe we modern humans are such a tribe. Despite the
-sophistication we see in ourselves compared with our less advanced ancestors from times long past,
-it’s surprising how little progress we’ve made in addressing some basic problems in 3D or beyond, or
-when solving seemingly simple equations in 3 or more variables. For despite our astonishing mastery
-of some ABCs, such as Air (flight, weather prediction), Biology (medical breakthroughs, DNA) and
-Communications (phone, video, email), we often struggle to get past 1, 2, 3 in other domains. Or
-sometimes even to get to 3. We'll survey a dozen fun topics in shapes and numbers and patterns
-whose basics and generalization can be explored with little mathematical background, and which
-speedily lead to "what if" questions ranging from easy to tricky to "we just don't know." Coins, cakes,
-fruit, bagels, cubes, squares and primes will all make an appearance. The late Martin Gardner, whose writings  turned  so many  on to maths, knew all too well that such playful queries
-can both excite students about mathematics and lead to real research at the frontiers of the subject.
-There will be satisfying Aha! moments, there will be room for innovative ideas, and million dollar
-prizes will be discussed.</t>
-  </si>
-  <si>
     <t>9th of April</t>
   </si>
   <si>
@@ -905,6 +889,252 @@
   </si>
   <si>
     <t>Coupling rheology and segregation in granular flows</t>
+  </si>
+  <si>
+    <t>Lisa McFetridge</t>
+  </si>
+  <si>
+    <t>Queen's University Belfast</t>
+  </si>
+  <si>
+    <t>Advances in Robust Mixed Effects Modelling</t>
+  </si>
+  <si>
+    <t>TBC</t>
+  </si>
+  <si>
+    <t>https://scholar.google.com/citations?user=j2CypRIAAAAJ&amp;hl=en</t>
+  </si>
+  <si>
+    <t>Oct</t>
+  </si>
+  <si>
+    <t>Thursday</t>
+  </si>
+  <si>
+    <t>Dingjia Cao</t>
+  </si>
+  <si>
+    <t>A wavelet lifting approach for spatial/network data</t>
+  </si>
+  <si>
+    <t>https://scholar.google.com/citations?user=paf72YcAAAAJ&amp;hl=en</t>
+  </si>
+  <si>
+    <t>Theresa Smith</t>
+  </si>
+  <si>
+    <t>University of Bath</t>
+  </si>
+  <si>
+    <t>Yanghong Huang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finite Difference Methods for fractional Laplacian of radial functions 
+</t>
+  </si>
+  <si>
+    <t>Numerical evaluation of nonlocal operators like the fractional Laplacian is more computationally intensive because of the dependence on the underlying function over the whole space. On the other hand, many solutions to the fractional counterparts of classical semi-linear PDEs, especially ground states obtained via variational methods, are radial. In this talk, fractional Laplacian of radial functions in general dimensions will be considered with a kernel represented by a Gauss hypergeometric function of the radial variables.  The singular part of the kernel is isolated and then treated with effective methods well studied in the one-dimensional context, while the regular part can be evaluated with by classical quadrature. The method can be extended to general non-radial functions that can be expanded using spherical harmonics, making it effective in the numerical study of fractional equations and complementing existing theoretical investigations.</t>
+  </si>
+  <si>
+    <t>4th Nov</t>
+  </si>
+  <si>
+    <t>6th Nov</t>
+  </si>
+  <si>
+    <t>Lea Kaufmann</t>
+  </si>
+  <si>
+    <t>RWTH Aachen University</t>
+  </si>
+  <si>
+    <t>Factor Selection and Levels Fusion in High-Dimensional Logistic Regression</t>
+  </si>
+  <si>
+    <t>In the last decades, high-dimensional problems in a regression-type context including a large number of explanatory variables arise in a huge variety of application fields. Specifically considering categorical explanatory variables, i.e., factors, the dummy-coding scheme introduces one (dummy) variable for each factor level, thus the dimension of the parameter space grows rapidly, even for a moderate number of factors. To simultaneously obtain the estimates of the regression coefficients and reducing the dimension of the parameter space, penalized regression is known to be a suitable tool. In this talk, I will discuss the characteristics that a penalization technique needs to fulfil to be suitable for the application to factors, as it is not only important to select those having an influence on the response variable (factor selection), but also to fuse those levels of a factor having a similar influence (levels fusion). A new penalization technique, called L0-Fused Group Lasso (L0-FGL), is introduced, tailored for the needs of factors. The quality of this new method is underlined by its theoretical properties, e.g.,  root-n-consistency and asymptotic normality, as well as by its performance in simulation studies.</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Alison O'Connor</t>
+  </si>
+  <si>
+    <t>Silvia D'Angelo</t>
+  </si>
+  <si>
+    <t>Trinity College Dublin</t>
+  </si>
+  <si>
+    <t>Clustering high-dimensional discrete data: a compressed approach</t>
+  </si>
+  <si>
+    <t>Custering high-dimensional data is a challenging task, typically addressed in the context of continuous numerical data. Recent literature is exploring strategies to cluster high-dimensional categorical and discrete data, which finds numerous applications, such as RNA sequencing and text data analysis. We propose a fast and easy-to-implement approach to cluster high-dimensional discrete data, scalable to datasets with thousands of dimensions where other strategies may be computationally unfeasible. Our approach relies on reducing the dimension of the data by performing a deterministic compression to a drastically lower dimension. The method employs a lossy compression that reduces the data to a collection of continuous features.
+We demonstrate that such compressed features can be treated as approximately normally distributed, allowing the application of standard finite Gaussian mixture models for model-based clustering. We discuss the approach and study its performance on a series of simulated scenarios with different dimensions and levels of complexity, involving both categorical and count data. Additionally, we illustrate the method on real-world data.</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>This is a just a place for those who are interested but that dont have a specific date in mind. (Ideally, a couple of these are people that we could invite with relatively short notice to fill missing slots.)</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Where are they from?</t>
+  </si>
+  <si>
+    <t>Adacemic Host</t>
+  </si>
+  <si>
+    <t>Colm</t>
+  </si>
+  <si>
+    <t>Niamh Cahill</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Niall Madden </t>
+  </si>
+  <si>
+    <t>Mehakpreet</t>
+  </si>
+  <si>
+    <t>Paul Weaver (invitation sent)</t>
+  </si>
+  <si>
+    <t>UL (Bernal)</t>
+  </si>
+  <si>
+    <t>Eleanor Doman</t>
+  </si>
+  <si>
+    <t>Manchester</t>
+  </si>
+  <si>
+    <t>Connor Hacket</t>
+  </si>
+  <si>
+    <t>MU</t>
+  </si>
+  <si>
+    <t>David Henry (?)</t>
+  </si>
+  <si>
+    <t>Jess Enright</t>
+  </si>
+  <si>
+    <t>Glasgow</t>
+  </si>
+  <si>
+    <t>JS/Networks</t>
+  </si>
+  <si>
+    <t>Ben Swallows</t>
+  </si>
+  <si>
+    <t>St Andrews</t>
+  </si>
+  <si>
+    <t>JS</t>
+  </si>
+  <si>
+    <t>Andrew Finlay</t>
+  </si>
+  <si>
+    <t>Uni Michigan</t>
+  </si>
+  <si>
+    <t>Denis Allard</t>
+  </si>
+  <si>
+    <t>INRAE</t>
+  </si>
+  <si>
+    <t>Nicholas J Clark</t>
+  </si>
+  <si>
+    <t>University of Queensland</t>
+  </si>
+  <si>
+    <t>Andrew Zammit Mangion</t>
+  </si>
+  <si>
+    <t>University of Wollongong</t>
+  </si>
+  <si>
+    <t>Trinity</t>
+  </si>
+  <si>
+    <t>DOS</t>
+  </si>
+  <si>
+    <t>Catherine Higgins</t>
+  </si>
+  <si>
+    <t>UCD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paul Weaver </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suzanne Fielding </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Doireann O'Kiely and Anthony </t>
+  </si>
+  <si>
+    <t>Possible speaker for next semester</t>
+  </si>
+  <si>
+    <t>Week</t>
+  </si>
+  <si>
+    <t>Speaker</t>
+  </si>
+  <si>
+    <t>Taken</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Taken </t>
+  </si>
+  <si>
+    <t>Seminar Series AY2024-25 Sem 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact david.osullivan@ul.ie &amp; mehakpreet.singh@ul.ie to book a speaker in. </t>
+  </si>
+  <si>
+    <t>Deptartmental contact</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>Robery Garvey</t>
+  </si>
+  <si>
+    <t>Tentative speaker</t>
+  </si>
+  <si>
+    <t>Leornard Henckel</t>
+  </si>
+  <si>
+    <t>Hip Fractures Trends in Older Adults in Ireland</t>
+  </si>
+  <si>
+    <t>https://scholar.google.com/citations?user=cbz4D-gAAAAJ&amp;hl=en</t>
+  </si>
+  <si>
+    <t>European healthcare systems are under pressure from rapidly ageing populations, with hip fractures representing one of the most costly and impactful injuries among older adults (1,2). Ireland faces the dual challenge of both a rapidly growing ageing population and one of the highest European rates in hip fracture incidence (3,4). Irish standards require admission to orthopaedic care within four hours, yet national audits show this target is rarely achieved (5). Improving hip fracture services requires not just clinical reform but also new ways of leveraging data.
+In this talk, we show how publicly available datasets can be used to uncover correlations and trends in hip fracture demand. When combined with national audit records we show how population health interacts with environmental pressures. Our findings suggest that extreme weather is a strong national indicator of surges in hip fractures with some regions experiencing more pressure than others. This creates opportunities not only for predictive modelling and smarter resource allocation, but also for preventative strategies where timely information can be used to warn and protect at-risk groups.
+References
+1. Looi MK. The European healthcare workforce crisis: how bad is it? BMJ. 2024 Jan 19;384:q8. 
+2. EUROSTAT. Ageing Europe - statistics on population developments. Eurostat; 2020. Report No.: 80393. 
+3. CSO. Central Statistics Office (CSO). Central Statistics Office; 2022 [cited 2024 Sep 23]. Society Measuring Ireland’s Progress 2022 - Central Statistics Office. Available from: https://www.cso.ie/en/releasesandpublications/ep/p-mip/measuringirelandsprogress2022/society/
+4. Walsh ME, Ferris H, Coughlan T, Hurson C, Ahern E, Sorensen J, et al. Trends in hip fracture care in the Republic of Ireland from 2013 to 2018: results from the Irish Hip Fracture Database. Osteoporos Int. 2021 Apr 1;32(4):727–36. 
+5. Kelly P, Horan B, Murphy T, Ahern E, Brent L, Kelly F, et al. Irish Hip Fracture Database National Report 2022 [Internet]. National Office of Clinical Audit (NOCA); 2022 p. 1–88. Available from: https://d7g406zpx7bgk.cloudfront.net/38cf762d5b/irish_hip_fracture_database_national_report_2022_final.pdf</t>
   </si>
   <si>
     <t>During the last fifteen years there has been a paradigm shift in the continuum modelling of granular materials; most notably with the development of rheological models, such as the  μ(I)-rheology (where μ is the friction and I is the inertial number), but also with significant advances in theories for particle segregation. This paper details theoretical and numerical frameworks (based on OpenFOAM) which unify these currently disconnected endeavours. Coupling the segregation with the flow, and vice versa, is not only vital for a complete theory of granular materials, but is also beneficial for developing numerical methods to handle evolving free surfaces. This general approach is based on the partially regularized incompressible-rheology, which is coupled to the gravity-driven segregation theory of Gray &amp; Ancey (J. Fluid Mech., vol. 678, 2011, pp. 353-588). These advection-diffusion-segregation equations describe the evolving concentrations of the constituents, which then couple back to the variable viscosity in the incompressible Navier-Stokes equations. A novel feature of this approach is that any number of differently sized phases may be included, which may have disparate frictional properties. Further inclusion of an excess air phase, which segregates away from the granular material, then allows the complex evolution of the free surface to be captured simultaneously. Three primary coupling mechanisms are identified: (i) advection of the particle concentrations by the bulk velocity, (ii) feedback of the particle-size and/or frictional properties on the bulk flow field and (iii) influence of the shear rate, pressure, gravity, particle size and particle-size ratio on the locally evolving segregation and diffusion rates. The numerical method is extensively tested in one-way coupled computations, before the fully coupled model is compared with the discrete element method simulations of Tripathi &amp; Khakhar (Phys. Fluids, vol. 23, 2011, 113302) and used to compute the petal-like segregation pattern that spontaneously develops in a square and triangular rotating drums.
@@ -920,250 +1150,7 @@
 T. Barker &amp; J. M. N. T. Gray (2017) J. Fluid Mech. 828, 5--32.   (movies)</t>
   </si>
   <si>
-    <t>Lisa McFetridge</t>
-  </si>
-  <si>
-    <t>Queen's University Belfast</t>
-  </si>
-  <si>
-    <t>Advances in Robust Mixed Effects Modelling</t>
-  </si>
-  <si>
-    <t>TBC</t>
-  </si>
-  <si>
-    <t>https://scholar.google.com/citations?user=j2CypRIAAAAJ&amp;hl=en</t>
-  </si>
-  <si>
-    <t>Oct</t>
-  </si>
-  <si>
-    <t>Thursday</t>
-  </si>
-  <si>
-    <t>Dingjia Cao</t>
-  </si>
-  <si>
-    <t>A wavelet lifting approach for spatial/network data</t>
-  </si>
-  <si>
-    <t>https://scholar.google.com/citations?user=paf72YcAAAAJ&amp;hl=en</t>
-  </si>
-  <si>
-    <t>Theresa Smith</t>
-  </si>
-  <si>
-    <t>University of Bath</t>
-  </si>
-  <si>
-    <t>Yanghong Huang</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Finite Difference Methods for fractional Laplacian of radial functions 
-</t>
-  </si>
-  <si>
-    <t>Numerical evaluation of nonlocal operators like the fractional Laplacian is more computationally intensive because of the dependence on the underlying function over the whole space. On the other hand, many solutions to the fractional counterparts of classical semi-linear PDEs, especially ground states obtained via variational methods, are radial. In this talk, fractional Laplacian of radial functions in general dimensions will be considered with a kernel represented by a Gauss hypergeometric function of the radial variables.  The singular part of the kernel is isolated and then treated with effective methods well studied in the one-dimensional context, while the regular part can be evaluated with by classical quadrature. The method can be extended to general non-radial functions that can be expanded using spherical harmonics, making it effective in the numerical study of fractional equations and complementing existing theoretical investigations.</t>
-  </si>
-  <si>
-    <t>4th Nov</t>
-  </si>
-  <si>
-    <t>6th Nov</t>
-  </si>
-  <si>
-    <t>Lea Kaufmann</t>
-  </si>
-  <si>
-    <t>RWTH Aachen University</t>
-  </si>
-  <si>
-    <t>Factor Selection and Levels Fusion in High-Dimensional Logistic Regression</t>
-  </si>
-  <si>
-    <t>In the last decades, high-dimensional problems in a regression-type context including a large number of explanatory variables arise in a huge variety of application fields. Specifically considering categorical explanatory variables, i.e., factors, the dummy-coding scheme introduces one (dummy) variable for each factor level, thus the dimension of the parameter space grows rapidly, even for a moderate number of factors. To simultaneously obtain the estimates of the regression coefficients and reducing the dimension of the parameter space, penalized regression is known to be a suitable tool. In this talk, I will discuss the characteristics that a penalization technique needs to fulfil to be suitable for the application to factors, as it is not only important to select those having an influence on the response variable (factor selection), but also to fuse those levels of a factor having a similar influence (levels fusion). A new penalization technique, called L0-Fused Group Lasso (L0-FGL), is introduced, tailored for the needs of factors. The quality of this new method is underlined by its theoretical properties, e.g.,  root-n-consistency and asymptotic normality, as well as by its performance in simulation studies.</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>Alison O'Connor</t>
-  </si>
-  <si>
-    <t>Silvia D'Angelo</t>
-  </si>
-  <si>
-    <t>Trinity College Dublin</t>
-  </si>
-  <si>
-    <t>Clustering high-dimensional discrete data: a compressed approach</t>
-  </si>
-  <si>
-    <t>Custering high-dimensional data is a challenging task, typically addressed in the context of continuous numerical data. Recent literature is exploring strategies to cluster high-dimensional categorical and discrete data, which finds numerous applications, such as RNA sequencing and text data analysis. We propose a fast and easy-to-implement approach to cluster high-dimensional discrete data, scalable to datasets with thousands of dimensions where other strategies may be computationally unfeasible. Our approach relies on reducing the dimension of the data by performing a deterministic compression to a drastically lower dimension. The method employs a lossy compression that reduces the data to a collection of continuous features.
-We demonstrate that such compressed features can be treated as approximately normally distributed, allowing the application of standard finite Gaussian mixture models for model-based clustering. We discuss the approach and study its performance on a series of simulated scenarios with different dimensions and levels of complexity, involving both categorical and count data. Additionally, we illustrate the method on real-world data.</t>
-  </si>
-  <si>
-    <t>Open</t>
-  </si>
-  <si>
-    <t>This is a just a place for those who are interested but that dont have a specific date in mind. (Ideally, a couple of these are people that we could invite with relatively short notice to fill missing slots.)</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Where are they from?</t>
-  </si>
-  <si>
-    <t>Adacemic Host</t>
-  </si>
-  <si>
-    <t>Colm</t>
-  </si>
-  <si>
-    <t>Niamh Cahill</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Niall Madden </t>
-  </si>
-  <si>
-    <t>Mehakpreet</t>
-  </si>
-  <si>
-    <t>Paul Weaver (invitation sent)</t>
-  </si>
-  <si>
-    <t>UL (Bernal)</t>
-  </si>
-  <si>
-    <t>Eleanor Doman</t>
-  </si>
-  <si>
-    <t>Manchester</t>
-  </si>
-  <si>
-    <t>Connor Hacket</t>
-  </si>
-  <si>
-    <t>MU</t>
-  </si>
-  <si>
-    <t>David Henry (?)</t>
-  </si>
-  <si>
-    <t>Jess Enright</t>
-  </si>
-  <si>
-    <t>Glasgow</t>
-  </si>
-  <si>
-    <t>JS/Networks</t>
-  </si>
-  <si>
-    <t>Ben Swallows</t>
-  </si>
-  <si>
-    <t>St Andrews</t>
-  </si>
-  <si>
-    <t>JS</t>
-  </si>
-  <si>
-    <t>Andrew Finlay</t>
-  </si>
-  <si>
-    <t>Uni Michigan</t>
-  </si>
-  <si>
-    <t>Denis Allard</t>
-  </si>
-  <si>
-    <t>INRAE</t>
-  </si>
-  <si>
-    <t>Nicholas J Clark</t>
-  </si>
-  <si>
-    <t>University of Queensland</t>
-  </si>
-  <si>
-    <t>Andrew Zammit Mangion</t>
-  </si>
-  <si>
-    <t>University of Wollongong</t>
-  </si>
-  <si>
-    <t>Trinity</t>
-  </si>
-  <si>
-    <t>DOS</t>
-  </si>
-  <si>
-    <t>Catherine Higgins</t>
-  </si>
-  <si>
-    <t>UCD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paul Weaver </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Suzanne Fielding </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Doireann O'Kiely and Anthony </t>
-  </si>
-  <si>
-    <t>Possible speaker for next semester</t>
-  </si>
-  <si>
-    <t>Week</t>
-  </si>
-  <si>
-    <t>Speaker</t>
-  </si>
-  <si>
-    <t>Taken</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Taken </t>
-  </si>
-  <si>
-    <t>Seminar Series AY2024-25 Sem 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contact david.osullivan@ul.ie &amp; mehakpreet.singh@ul.ie to book a speaker in. </t>
-  </si>
-  <si>
-    <t>Deptartmental contact</t>
-  </si>
-  <si>
-    <t>Wednesday</t>
-  </si>
-  <si>
-    <t>Robery Garvey</t>
-  </si>
-  <si>
-    <t>Tentative speaker</t>
-  </si>
-  <si>
-    <t>Leornard Henckel</t>
-  </si>
-  <si>
-    <t>Hip Fractures Trends in Older Adults in Ireland</t>
-  </si>
-  <si>
-    <t>https://scholar.google.com/citations?user=cbz4D-gAAAAJ&amp;hl=en</t>
-  </si>
-  <si>
-    <t>European healthcare systems are under pressure from rapidly ageing populations, with hip fractures representing one of the most costly and impactful injuries among older adults (1,2). Ireland faces the dual challenge of both a rapidly growing ageing population and one of the highest European rates in hip fracture incidence (3,4). Irish standards require admission to orthopaedic care within four hours, yet national audits show this target is rarely achieved (5). Improving hip fracture services requires not just clinical reform but also new ways of leveraging data.
-In this talk, we show how publicly available datasets can be used to uncover correlations and trends in hip fracture demand. When combined with national audit records we show how population health interacts with environmental pressures. Our findings suggest that extreme weather is a strong national indicator of surges in hip fractures with some regions experiencing more pressure than others. This creates opportunities not only for predictive modelling and smarter resource allocation, but also for preventative strategies where timely information can be used to warn and protect at-risk groups.
-References
-1. Looi MK. The European healthcare workforce crisis: how bad is it? BMJ. 2024 Jan 19;384:q8. 
-2. EUROSTAT. Ageing Europe - statistics on population developments. Eurostat; 2020. Report No.: 80393. 
-3. CSO. Central Statistics Office (CSO). Central Statistics Office; 2022 [cited 2024 Sep 23]. Society Measuring Ireland’s Progress 2022 - Central Statistics Office. Available from: https://www.cso.ie/en/releasesandpublications/ep/p-mip/measuringirelandsprogress2022/society/
-4. Walsh ME, Ferris H, Coughlan T, Hurson C, Ahern E, Sorensen J, et al. Trends in hip fracture care in the Republic of Ireland from 2013 to 2018: results from the Irish Hip Fracture Database. Osteoporos Int. 2021 Apr 1;32(4):727–36. 
-5. Kelly P, Horan B, Murphy T, Ahern E, Brent L, Kelly F, et al. Irish Hip Fracture Database National Report 2022 [Internet]. National Office of Clinical Audit (NOCA); 2022 p. 1–88. Available from: https://d7g406zpx7bgk.cloudfront.net/38cf762d5b/irish_hip_fracture_database_national_report_2022_final.pdf</t>
+    <t>Are there really primitive tribes whose system of counting goes: "One, Two, Many", indicating that from three on it’s more or less a blur? Maybe we modern humans are such a tribe. Despite the sophistication we see in ourselves compared with our less advanced ancestors from times long past, it’s surprising how little progress we’ve made in addressing some basic problems in 3D or beyond, or when solving seemingly simple equations in 3 or more variables. For despite our astonishing mastery of some ABCs, such as Air (flight, weather prediction), Biology (medical breakthroughs, DNA) and Communications (phone, video, email), we often struggle to get past 1, 2, 3 in other domains. Or sometimes even to get to 3. We'll survey a dozen fun topics in shapes and numbers and patterns whose basics and generalization can be explored with little mathematical background, and which speedily lead to "what if" questions ranging from easy to tricky to "we just don't know." Coins, cakes, fruit, bagels, cubes, squares and primes will all make an appearance. The late Martin Gardner, whose writings  turned  so many  on to maths, knew all too well that such playful queries can both excite students about mathematics and lead to real research at the frontiers of the subject. There will be satisfying Aha! moments, there will be room for innovative ideas, and million dollar prizes will be discussed.</t>
   </si>
 </sst>
 </file>
@@ -1983,10 +1970,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
@@ -4224,8 +4207,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12299A9A-6C0C-4F92-957E-FBFCB6211744}">
   <dimension ref="A1:X45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4641,7 +4624,7 @@
         <v>217</v>
       </c>
       <c r="J8" s="16" t="s">
-        <v>218</v>
+        <v>350</v>
       </c>
       <c r="K8" s="14"/>
       <c r="L8" s="5"/>
@@ -4656,10 +4639,10 @@
         <v>146</v>
       </c>
       <c r="Q8" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="R8" s="16" t="s">
         <v>219</v>
-      </c>
-      <c r="R8" s="16" t="s">
-        <v>220</v>
       </c>
       <c r="S8" s="35"/>
       <c r="T8" s="5" t="s">
@@ -4688,19 +4671,19 @@
         <v>11</v>
       </c>
       <c r="F9" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="G9" s="16" t="s">
         <v>221</v>
       </c>
-      <c r="G9" s="16" t="s">
+      <c r="H9" s="109" t="s">
         <v>222</v>
       </c>
-      <c r="H9" s="109" t="s">
+      <c r="I9" s="115" t="s">
         <v>223</v>
       </c>
-      <c r="I9" s="115" t="s">
+      <c r="J9" s="98" t="s">
         <v>224</v>
-      </c>
-      <c r="J9" s="98" t="s">
-        <v>225</v>
       </c>
       <c r="K9" s="73"/>
       <c r="L9" s="5"/>
@@ -4715,10 +4698,10 @@
         <v>146</v>
       </c>
       <c r="Q9" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="R9" s="16" t="s">
         <v>226</v>
-      </c>
-      <c r="R9" s="16" t="s">
-        <v>227</v>
       </c>
       <c r="S9" s="35" t="s">
         <v>43</v>
@@ -4749,19 +4732,19 @@
         <v>11</v>
       </c>
       <c r="F10" s="14" t="s">
+        <v>227</v>
+      </c>
+      <c r="G10" s="16" t="s">
         <v>228</v>
-      </c>
-      <c r="G10" s="16" t="s">
-        <v>229</v>
       </c>
       <c r="H10" s="109" t="s">
         <v>30</v>
       </c>
       <c r="I10" s="115" t="s">
+        <v>229</v>
+      </c>
+      <c r="J10" s="98" t="s">
         <v>230</v>
-      </c>
-      <c r="J10" s="98" t="s">
-        <v>231</v>
       </c>
       <c r="K10" s="74"/>
       <c r="L10" s="48"/>
@@ -4802,19 +4785,19 @@
         <v>12</v>
       </c>
       <c r="F11" s="19" t="s">
+        <v>231</v>
+      </c>
+      <c r="G11" s="21" t="s">
         <v>232</v>
       </c>
-      <c r="G11" s="21" t="s">
+      <c r="H11" s="110" t="s">
         <v>233</v>
       </c>
-      <c r="H11" s="110" t="s">
+      <c r="I11" s="117" t="s">
         <v>234</v>
       </c>
-      <c r="I11" s="117" t="s">
+      <c r="J11" s="112" t="s">
         <v>235</v>
-      </c>
-      <c r="J11" s="112" t="s">
-        <v>236</v>
       </c>
       <c r="K11" s="72"/>
       <c r="L11" s="72"/>
@@ -4862,7 +4845,7 @@
         <v>13</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G12" s="16" t="s">
         <v>76</v>
@@ -4871,10 +4854,10 @@
         <v>123</v>
       </c>
       <c r="I12" s="114" t="s">
+        <v>237</v>
+      </c>
+      <c r="J12" s="98" t="s">
         <v>238</v>
-      </c>
-      <c r="J12" s="98" t="s">
-        <v>239</v>
       </c>
       <c r="K12" s="72"/>
       <c r="L12" s="72"/>
@@ -4922,7 +4905,7 @@
         <v>15</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G13" s="16" t="s">
         <v>76</v>
@@ -4931,10 +4914,10 @@
         <v>100</v>
       </c>
       <c r="I13" s="114" t="s">
+        <v>240</v>
+      </c>
+      <c r="J13" s="98" t="s">
         <v>241</v>
-      </c>
-      <c r="J13" s="98" t="s">
-        <v>242</v>
       </c>
       <c r="K13" s="72"/>
       <c r="L13" s="72"/>
@@ -4974,19 +4957,19 @@
         <v>17</v>
       </c>
       <c r="F14" s="19" t="s">
+        <v>242</v>
+      </c>
+      <c r="G14" s="21" t="s">
         <v>243</v>
-      </c>
-      <c r="G14" s="21" t="s">
-        <v>244</v>
       </c>
       <c r="H14" s="111" t="s">
         <v>94</v>
       </c>
       <c r="I14" s="118" t="s">
+        <v>244</v>
+      </c>
+      <c r="J14" s="112" t="s">
         <v>245</v>
-      </c>
-      <c r="J14" s="112" t="s">
-        <v>246</v>
       </c>
       <c r="M14" t="s">
         <v>43</v>
@@ -5020,7 +5003,7 @@
         <v>18</v>
       </c>
       <c r="F15" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G15" t="s">
         <v>151</v>
@@ -5029,10 +5012,10 @@
         <v>100</v>
       </c>
       <c r="I15" t="s">
+        <v>247</v>
+      </c>
+      <c r="J15" s="129" t="s">
         <v>248</v>
-      </c>
-      <c r="J15" s="129" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="16" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5157,11 +5140,11 @@
   </sheetPr>
   <dimension ref="A1:X23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="7" ySplit="16" topLeftCell="H17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="J11" sqref="J11"/>
+      <selection pane="bottomRight" activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5295,25 +5278,25 @@
         <v>1</v>
       </c>
       <c r="F3" s="101" t="s">
+        <v>249</v>
+      </c>
+      <c r="G3" s="107" t="s">
         <v>250</v>
       </c>
-      <c r="G3" s="107" t="s">
+      <c r="H3" s="25" t="s">
         <v>251</v>
       </c>
-      <c r="H3" s="25" t="s">
+      <c r="I3" s="98" t="s">
         <v>252</v>
       </c>
-      <c r="I3" s="98" t="s">
+      <c r="J3" s="98" t="s">
         <v>253</v>
       </c>
-      <c r="J3" s="98" t="s">
+      <c r="K3" s="156" t="s">
         <v>254</v>
       </c>
-      <c r="K3" s="156" t="s">
+      <c r="L3" s="59" t="s">
         <v>255</v>
-      </c>
-      <c r="L3" s="59" t="s">
-        <v>256</v>
       </c>
       <c r="M3" s="38" t="s">
         <v>34</v>
@@ -5325,7 +5308,7 @@
         <v>34</v>
       </c>
       <c r="P3" s="40" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="Q3" s="40"/>
       <c r="R3" s="38"/>
@@ -5343,7 +5326,7 @@
         <v>45917</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C4" s="29" t="str">
         <f>TEXT(A4, "mmm")</f>
@@ -5357,25 +5340,25 @@
         <v>2</v>
       </c>
       <c r="F4" s="101" t="s">
+        <v>258</v>
+      </c>
+      <c r="G4" s="107" t="s">
         <v>259</v>
       </c>
-      <c r="G4" s="107" t="s">
+      <c r="H4" s="25" t="s">
         <v>260</v>
       </c>
-      <c r="H4" s="25" t="s">
+      <c r="I4" s="98" t="s">
         <v>261</v>
       </c>
-      <c r="I4" s="98" t="s">
+      <c r="J4" s="98" t="s">
         <v>262</v>
       </c>
-      <c r="J4" s="98" t="s">
+      <c r="K4" s="156" t="s">
         <v>263</v>
       </c>
-      <c r="K4" s="156" t="s">
+      <c r="L4" s="25" t="s">
         <v>264</v>
-      </c>
-      <c r="L4" s="25" t="s">
-        <v>265</v>
       </c>
       <c r="M4" s="16" t="s">
         <v>43</v>
@@ -5390,7 +5373,7 @@
         <v>63</v>
       </c>
       <c r="Q4" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="R4" s="16" t="s">
         <v>65</v>
@@ -5411,7 +5394,7 @@
         <v>45926</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C5" s="26" t="str">
         <f>TEXT(A5, "mmm")</f>
@@ -5426,19 +5409,19 @@
         <v>3</v>
       </c>
       <c r="F5" s="101" t="s">
+        <v>267</v>
+      </c>
+      <c r="G5" s="107" t="s">
         <v>268</v>
-      </c>
-      <c r="G5" s="107" t="s">
-        <v>269</v>
       </c>
       <c r="H5" s="25" t="s">
         <v>205</v>
       </c>
       <c r="I5" s="98" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="J5" s="98" t="s">
-        <v>271</v>
+        <v>349</v>
       </c>
       <c r="K5" s="157"/>
       <c r="L5" s="25"/>
@@ -5450,7 +5433,7 @@
         <v>34</v>
       </c>
       <c r="P5" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="Q5" s="5"/>
       <c r="R5" s="16"/>
@@ -5483,22 +5466,22 @@
         <v>5</v>
       </c>
       <c r="F6" s="101" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G6" s="107" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="H6" s="25" t="s">
         <v>77</v>
       </c>
       <c r="I6" s="96" t="s">
+        <v>272</v>
+      </c>
+      <c r="J6" s="98" t="s">
+        <v>273</v>
+      </c>
+      <c r="K6" s="157" t="s">
         <v>274</v>
-      </c>
-      <c r="J6" s="98" t="s">
-        <v>275</v>
-      </c>
-      <c r="K6" s="157" t="s">
-        <v>276</v>
       </c>
       <c r="L6" s="25"/>
       <c r="M6" s="16" t="s">
@@ -5534,16 +5517,16 @@
         <v>189</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E7">
         <v>6</v>
       </c>
       <c r="F7" s="101" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="G7" s="107" t="s">
         <v>67</v>
@@ -5552,13 +5535,13 @@
         <v>30</v>
       </c>
       <c r="I7" s="97" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="J7" s="98" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="K7" s="157" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="L7" s="25"/>
       <c r="M7" s="16" t="s">
@@ -5569,7 +5552,7 @@
         <v>34</v>
       </c>
       <c r="P7" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="Q7" s="5"/>
       <c r="R7" s="16"/>
@@ -5602,19 +5585,19 @@
         <v>7</v>
       </c>
       <c r="F8" s="101" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="G8" s="107" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="H8" s="25" t="s">
         <v>30</v>
       </c>
       <c r="I8" s="97" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="J8" s="98" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="K8" s="157"/>
       <c r="L8" s="25"/>
@@ -5657,22 +5640,22 @@
         <v>9</v>
       </c>
       <c r="F9" s="101" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="G9" s="107" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="H9" s="25" t="s">
         <v>199</v>
       </c>
       <c r="I9" s="97" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="J9" s="97" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="K9" s="157" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="L9" s="25"/>
       <c r="M9" s="16"/>
@@ -5684,10 +5667,10 @@
         <v>63</v>
       </c>
       <c r="Q9" s="5" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="R9" s="16" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="S9" s="35"/>
       <c r="T9" s="5" t="s">
@@ -5717,19 +5700,19 @@
         <v>10</v>
       </c>
       <c r="F10" s="101" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="G10" s="107" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="H10" s="25" t="s">
         <v>123</v>
       </c>
       <c r="I10" s="97" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="J10" s="97" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="K10" s="157"/>
       <c r="L10" s="25"/>
@@ -5741,7 +5724,7 @@
         <v>43</v>
       </c>
       <c r="P10" s="5" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="Q10" s="5"/>
       <c r="R10" s="16"/>
@@ -5776,7 +5759,7 @@
         <v>11</v>
       </c>
       <c r="F11" s="101" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="G11" s="107" t="s">
         <v>67</v>
@@ -5785,10 +5768,10 @@
         <v>100</v>
       </c>
       <c r="I11" s="97" t="s">
+        <v>346</v>
+      </c>
+      <c r="J11" s="98" t="s">
         <v>348</v>
-      </c>
-      <c r="J11" s="98" t="s">
-        <v>350</v>
       </c>
       <c r="K11" s="107"/>
       <c r="L11" s="25"/>
@@ -5800,7 +5783,7 @@
         <v>34</v>
       </c>
       <c r="P11" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="Q11" s="5"/>
       <c r="R11" s="16"/>
@@ -5833,19 +5816,19 @@
         <v>13</v>
       </c>
       <c r="F12" s="101" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="G12" s="107" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="H12" s="25" t="s">
         <v>100</v>
       </c>
       <c r="I12" s="97" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="J12" s="132" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="K12" s="157"/>
       <c r="L12" s="25"/>
@@ -6059,19 +6042,19 @@
         <v>1</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="I3" s="98" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="J3" s="98" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="K3" s="73"/>
       <c r="L3" s="40"/>
@@ -6113,19 +6096,19 @@
         <v>3</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="I4" s="98" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="J4" s="98" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="K4" s="102"/>
       <c r="L4" s="5"/>
@@ -6165,19 +6148,19 @@
         <v>5</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="I5" s="98" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="J5" s="98" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="K5" s="102"/>
       <c r="L5" s="5"/>
@@ -6217,19 +6200,19 @@
         <v>7</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="I6" s="98" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="J6" s="98" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="K6" s="102"/>
       <c r="L6" s="5"/>
@@ -6269,19 +6252,19 @@
         <v>9</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="I7" s="98" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="J7" s="98" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="K7" s="102"/>
       <c r="L7" s="5"/>
@@ -6321,19 +6304,19 @@
         <v>11</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="I8" s="98" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="J8" s="98" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="K8" s="102"/>
       <c r="L8" s="5"/>
@@ -6371,19 +6354,19 @@
         <v>13</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="I9" s="98" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="J9" s="98" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="K9" s="102"/>
       <c r="L9" s="5"/>
@@ -6453,32 +6436,32 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="55" t="s">
+        <v>299</v>
+      </c>
+      <c r="B2" s="54" t="s">
+        <v>300</v>
+      </c>
+      <c r="C2" s="54" t="s">
         <v>301</v>
-      </c>
-      <c r="B2" s="54" t="s">
-        <v>302</v>
-      </c>
-      <c r="C2" s="54" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="136" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B3" s="137"/>
       <c r="C3" s="138" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B4" s="52"/>
       <c r="C4" s="50" t="s">
@@ -6487,19 +6470,19 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="52" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B5" s="52"/>
       <c r="C5" s="50" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="52" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B6" s="52" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C6" s="50" t="s">
         <v>86</v>
@@ -6507,10 +6490,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="52" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B7" s="52" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C7" s="50" t="s">
         <v>86</v>
@@ -6518,10 +6501,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="52" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B8" s="52" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C8" s="50" t="s">
         <v>100</v>
@@ -6529,105 +6512,105 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="52" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B9" s="52"/>
       <c r="C9" s="50"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="52" t="s">
+        <v>313</v>
+      </c>
+      <c r="B10" s="52" t="s">
+        <v>314</v>
+      </c>
+      <c r="C10" s="50" t="s">
         <v>315</v>
-      </c>
-      <c r="B10" s="52" t="s">
-        <v>316</v>
-      </c>
-      <c r="C10" s="50" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="52" t="s">
+        <v>316</v>
+      </c>
+      <c r="B11" s="52" t="s">
+        <v>317</v>
+      </c>
+      <c r="C11" s="50" t="s">
         <v>318</v>
-      </c>
-      <c r="B11" s="52" t="s">
-        <v>319</v>
-      </c>
-      <c r="C11" s="50" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="52" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B12" s="52" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C12" s="50" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="52" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B13" s="52" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C13" s="50" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="52" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B14" s="52" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C14" s="50" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="52" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B15" s="52" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C15" s="50" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="137" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B16" s="137" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C16" s="139" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="52" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B17" s="52" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C17" s="50" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="52" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B18" s="52" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C18" s="50" t="s">
         <v>86</v>
@@ -6635,26 +6618,26 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="53" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B19" s="53" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C19" s="51" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B24" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C24" t="s">
         <v>86</v>
@@ -6662,13 +6645,13 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B25" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C25" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
   </sheetData>
@@ -6700,10 +6683,10 @@
         <v>3</v>
       </c>
       <c r="B1" s="131" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C1" s="130" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -6714,7 +6697,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="134" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="F2" s="75">
         <v>45911</v>
@@ -6744,13 +6727,13 @@
         <v>2</v>
       </c>
       <c r="C3" s="134" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="F3" s="75">
         <v>45926</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="H3" s="26" t="str">
         <f>TEXT(F3, "mmm")</f>
@@ -6775,7 +6758,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="134" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="F4" s="75">
         <v>45939</v>
@@ -6806,7 +6789,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="134" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="F5" s="75">
         <v>45946</v>
@@ -6815,10 +6798,10 @@
         <v>189</v>
       </c>
       <c r="H5" s="26" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="I5" s="27" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="J5">
         <v>6</v>
@@ -6834,7 +6817,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="134" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="F6" s="75">
         <v>45953</v>
@@ -6865,7 +6848,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="134" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="F7" s="75">
         <v>45967</v>
@@ -6896,7 +6879,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="134" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="F8" s="75">
         <v>45974</v>
@@ -6926,7 +6909,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="134" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="F9" s="75">
         <v>45981</v>
@@ -6957,7 +6940,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="134" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="F10" s="75">
         <v>45995</v>
@@ -6988,7 +6971,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="134" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -7001,7 +6984,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="134" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -7014,7 +6997,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="134" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -7027,7 +7010,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="134" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -7080,12 +7063,12 @@
   <sheetData>
     <row r="2" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="91" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="79" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="37.5" x14ac:dyDescent="0.25">
@@ -7111,7 +7094,7 @@
         <v>9</v>
       </c>
       <c r="H5" s="82" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="I5" s="81" t="s">
         <v>11</v>
@@ -7128,7 +7111,7 @@
         <v>190</v>
       </c>
       <c r="D6" s="93" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E6" s="93">
         <v>2</v>
@@ -7141,7 +7124,7 @@
       </c>
       <c r="H6" s="85"/>
       <c r="I6" s="84" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
@@ -7155,7 +7138,7 @@
         <v>190</v>
       </c>
       <c r="D7" s="94" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E7" s="94">
         <v>4</v>
@@ -7184,7 +7167,7 @@
         <v>197</v>
       </c>
       <c r="D8" s="94" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E8" s="94">
         <v>6</v>
@@ -7211,7 +7194,7 @@
         <v>197</v>
       </c>
       <c r="D9" s="94" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E9" s="94">
         <v>8</v>
@@ -7226,7 +7209,7 @@
         <v>205</v>
       </c>
       <c r="I9" s="86" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
@@ -7246,13 +7229,13 @@
         <v>9</v>
       </c>
       <c r="F10" s="87" t="s">
+        <v>220</v>
+      </c>
+      <c r="G10" s="87" t="s">
         <v>221</v>
       </c>
-      <c r="G10" s="87" t="s">
+      <c r="H10" s="87" t="s">
         <v>222</v>
-      </c>
-      <c r="H10" s="87" t="s">
-        <v>223</v>
       </c>
       <c r="I10" s="86"/>
     </row>
@@ -7267,20 +7250,20 @@
         <v>208</v>
       </c>
       <c r="D11" s="94" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E11" s="94">
         <v>10</v>
       </c>
       <c r="F11" s="87" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="G11" s="87" t="s">
         <v>67</v>
       </c>
       <c r="H11" s="87"/>
       <c r="I11" s="86" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
@@ -7300,7 +7283,7 @@
         <v>11</v>
       </c>
       <c r="F12" s="87" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G12" s="87" t="s">
         <v>171</v>
@@ -7309,7 +7292,7 @@
         <v>30</v>
       </c>
       <c r="I12" s="86" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
@@ -7323,13 +7306,13 @@
         <v>208</v>
       </c>
       <c r="D13" s="94" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E13" s="94">
         <v>12</v>
       </c>
       <c r="F13" s="87" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="G13" s="87"/>
       <c r="H13" s="87"/>
@@ -7346,13 +7329,13 @@
         <v>208</v>
       </c>
       <c r="D14" s="95" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E14" s="95">
         <v>13</v>
       </c>
       <c r="F14" s="90" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="G14" s="90" t="s">
         <v>76</v>
@@ -7361,7 +7344,7 @@
         <v>123</v>
       </c>
       <c r="I14" s="89" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="20" spans="8:8" ht="18.75" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
fix MK time, moved to 3pm
</commit_message>
<xml_diff>
--- a/data/MACSI seminar series.xlsx
+++ b/data/MACSI seminar series.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ulcampus-my.sharepoint.com/personal/david_osullivan_ul_ie/Documents/Academic_work/_Misc/MACSI_Seminars/macsi-seminars.github.io/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2497" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{994866AB-1CAF-4008-B678-59E24FA32A5B}"/>
+  <xr:revisionPtr revIDLastSave="2498" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8ABC1665-85A3-4193-87B1-B425E6344C18}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AY2023-2024 Sem 2" sheetId="3" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="350">
   <si>
     <t>Fill in as much of the green boxes as possible. Ideally, this would be before you have finished your visitors travel dates (just to avoid double booking).</t>
   </si>
@@ -850,9 +850,6 @@
   </si>
   <si>
     <t>0</t>
-  </si>
-  <si>
-    <t>4pm</t>
   </si>
   <si>
     <t>Márton Karsai</t>
@@ -4207,7 +4204,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12299A9A-6C0C-4F92-957E-FBFCB6211744}">
   <dimension ref="A1:X45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
@@ -4624,7 +4621,7 @@
         <v>217</v>
       </c>
       <c r="J8" s="16" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="K8" s="14"/>
       <c r="L8" s="5"/>
@@ -5140,11 +5137,11 @@
   </sheetPr>
   <dimension ref="A1:X23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="7" ySplit="16" topLeftCell="H17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="L4" sqref="L4"/>
+      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5326,7 +5323,7 @@
         <v>45917</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="C4" s="29" t="str">
         <f>TEXT(A4, "mmm")</f>
@@ -5340,25 +5337,25 @@
         <v>2</v>
       </c>
       <c r="F4" s="101" t="s">
+        <v>257</v>
+      </c>
+      <c r="G4" s="107" t="s">
         <v>258</v>
       </c>
-      <c r="G4" s="107" t="s">
+      <c r="H4" s="25" t="s">
         <v>259</v>
       </c>
-      <c r="H4" s="25" t="s">
+      <c r="I4" s="98" t="s">
         <v>260</v>
       </c>
-      <c r="I4" s="98" t="s">
+      <c r="J4" s="98" t="s">
         <v>261</v>
       </c>
-      <c r="J4" s="98" t="s">
+      <c r="K4" s="156" t="s">
         <v>262</v>
       </c>
-      <c r="K4" s="156" t="s">
+      <c r="L4" s="25" t="s">
         <v>263</v>
-      </c>
-      <c r="L4" s="25" t="s">
-        <v>264</v>
       </c>
       <c r="M4" s="16" t="s">
         <v>43</v>
@@ -5373,7 +5370,7 @@
         <v>63</v>
       </c>
       <c r="Q4" s="5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="R4" s="16" t="s">
         <v>65</v>
@@ -5394,7 +5391,7 @@
         <v>45926</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C5" s="26" t="str">
         <f>TEXT(A5, "mmm")</f>
@@ -5409,19 +5406,19 @@
         <v>3</v>
       </c>
       <c r="F5" s="101" t="s">
+        <v>266</v>
+      </c>
+      <c r="G5" s="107" t="s">
         <v>267</v>
-      </c>
-      <c r="G5" s="107" t="s">
-        <v>268</v>
       </c>
       <c r="H5" s="25" t="s">
         <v>205</v>
       </c>
       <c r="I5" s="98" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="J5" s="98" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="K5" s="157"/>
       <c r="L5" s="25"/>
@@ -5466,22 +5463,22 @@
         <v>5</v>
       </c>
       <c r="F6" s="101" t="s">
+        <v>269</v>
+      </c>
+      <c r="G6" s="107" t="s">
         <v>270</v>
-      </c>
-      <c r="G6" s="107" t="s">
-        <v>271</v>
       </c>
       <c r="H6" s="25" t="s">
         <v>77</v>
       </c>
       <c r="I6" s="96" t="s">
+        <v>271</v>
+      </c>
+      <c r="J6" s="98" t="s">
         <v>272</v>
       </c>
-      <c r="J6" s="98" t="s">
+      <c r="K6" s="157" t="s">
         <v>273</v>
-      </c>
-      <c r="K6" s="157" t="s">
-        <v>274</v>
       </c>
       <c r="L6" s="25"/>
       <c r="M6" s="16" t="s">
@@ -5517,16 +5514,16 @@
         <v>189</v>
       </c>
       <c r="C7" s="26" t="s">
+        <v>274</v>
+      </c>
+      <c r="D7" s="27" t="s">
         <v>275</v>
-      </c>
-      <c r="D7" s="27" t="s">
-        <v>276</v>
       </c>
       <c r="E7">
         <v>6</v>
       </c>
       <c r="F7" s="101" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G7" s="107" t="s">
         <v>67</v>
@@ -5535,13 +5532,13 @@
         <v>30</v>
       </c>
       <c r="I7" s="97" t="s">
+        <v>277</v>
+      </c>
+      <c r="J7" s="98" t="s">
+        <v>272</v>
+      </c>
+      <c r="K7" s="157" t="s">
         <v>278</v>
-      </c>
-      <c r="J7" s="98" t="s">
-        <v>273</v>
-      </c>
-      <c r="K7" s="157" t="s">
-        <v>279</v>
       </c>
       <c r="L7" s="25"/>
       <c r="M7" s="16" t="s">
@@ -5585,19 +5582,19 @@
         <v>7</v>
       </c>
       <c r="F8" s="101" t="s">
+        <v>279</v>
+      </c>
+      <c r="G8" s="107" t="s">
         <v>280</v>
-      </c>
-      <c r="G8" s="107" t="s">
-        <v>281</v>
       </c>
       <c r="H8" s="25" t="s">
         <v>30</v>
       </c>
       <c r="I8" s="97" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="J8" s="98" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="K8" s="157"/>
       <c r="L8" s="25"/>
@@ -5640,22 +5637,22 @@
         <v>9</v>
       </c>
       <c r="F9" s="101" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G9" s="107" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="H9" s="25" t="s">
         <v>199</v>
       </c>
       <c r="I9" s="97" t="s">
+        <v>282</v>
+      </c>
+      <c r="J9" s="97" t="s">
         <v>283</v>
       </c>
-      <c r="J9" s="97" t="s">
-        <v>284</v>
-      </c>
       <c r="K9" s="157" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="L9" s="25"/>
       <c r="M9" s="16"/>
@@ -5667,10 +5664,10 @@
         <v>63</v>
       </c>
       <c r="Q9" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="R9" s="16" t="s">
         <v>285</v>
-      </c>
-      <c r="R9" s="16" t="s">
-        <v>286</v>
       </c>
       <c r="S9" s="35"/>
       <c r="T9" s="5" t="s">
@@ -5700,19 +5697,19 @@
         <v>10</v>
       </c>
       <c r="F10" s="101" t="s">
+        <v>286</v>
+      </c>
+      <c r="G10" s="107" t="s">
         <v>287</v>
-      </c>
-      <c r="G10" s="107" t="s">
-        <v>288</v>
       </c>
       <c r="H10" s="25" t="s">
         <v>123</v>
       </c>
       <c r="I10" s="97" t="s">
+        <v>288</v>
+      </c>
+      <c r="J10" s="97" t="s">
         <v>289</v>
-      </c>
-      <c r="J10" s="97" t="s">
-        <v>290</v>
       </c>
       <c r="K10" s="157"/>
       <c r="L10" s="25"/>
@@ -5724,7 +5721,7 @@
         <v>43</v>
       </c>
       <c r="P10" s="5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="Q10" s="5"/>
       <c r="R10" s="16"/>
@@ -5759,7 +5756,7 @@
         <v>11</v>
       </c>
       <c r="F11" s="101" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="G11" s="107" t="s">
         <v>67</v>
@@ -5768,10 +5765,10 @@
         <v>100</v>
       </c>
       <c r="I11" s="97" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="J11" s="98" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="K11" s="107"/>
       <c r="L11" s="25"/>
@@ -5816,19 +5813,19 @@
         <v>13</v>
       </c>
       <c r="F12" s="101" t="s">
+        <v>292</v>
+      </c>
+      <c r="G12" s="107" t="s">
         <v>293</v>
-      </c>
-      <c r="G12" s="107" t="s">
-        <v>294</v>
       </c>
       <c r="H12" s="25" t="s">
         <v>100</v>
       </c>
       <c r="I12" s="97" t="s">
+        <v>294</v>
+      </c>
+      <c r="J12" s="132" t="s">
         <v>295</v>
-      </c>
-      <c r="J12" s="132" t="s">
-        <v>296</v>
       </c>
       <c r="K12" s="157"/>
       <c r="L12" s="25"/>
@@ -6042,19 +6039,19 @@
         <v>1</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="I3" s="98" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="J3" s="98" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="K3" s="73"/>
       <c r="L3" s="40"/>
@@ -6096,19 +6093,19 @@
         <v>3</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="I4" s="98" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="J4" s="98" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="K4" s="102"/>
       <c r="L4" s="5"/>
@@ -6148,19 +6145,19 @@
         <v>5</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="I5" s="98" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="J5" s="98" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="K5" s="102"/>
       <c r="L5" s="5"/>
@@ -6200,19 +6197,19 @@
         <v>7</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="I6" s="98" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="J6" s="98" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="K6" s="102"/>
       <c r="L6" s="5"/>
@@ -6252,19 +6249,19 @@
         <v>9</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="I7" s="98" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="J7" s="98" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="K7" s="102"/>
       <c r="L7" s="5"/>
@@ -6304,19 +6301,19 @@
         <v>11</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="I8" s="98" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="J8" s="98" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="K8" s="102"/>
       <c r="L8" s="5"/>
@@ -6354,19 +6351,19 @@
         <v>13</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="I9" s="98" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="J9" s="98" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="K9" s="102"/>
       <c r="L9" s="5"/>
@@ -6436,23 +6433,23 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="55" t="s">
+        <v>298</v>
+      </c>
+      <c r="B2" s="54" t="s">
         <v>299</v>
       </c>
-      <c r="B2" s="54" t="s">
+      <c r="C2" s="54" t="s">
         <v>300</v>
-      </c>
-      <c r="C2" s="54" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="136" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B3" s="137"/>
       <c r="C3" s="138" t="s">
@@ -6461,7 +6458,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B4" s="52"/>
       <c r="C4" s="50" t="s">
@@ -6470,19 +6467,19 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="52" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B5" s="52"/>
       <c r="C5" s="50" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="52" t="s">
+        <v>305</v>
+      </c>
+      <c r="B6" s="52" t="s">
         <v>306</v>
-      </c>
-      <c r="B6" s="52" t="s">
-        <v>307</v>
       </c>
       <c r="C6" s="50" t="s">
         <v>86</v>
@@ -6490,10 +6487,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="52" t="s">
+        <v>307</v>
+      </c>
+      <c r="B7" s="52" t="s">
         <v>308</v>
-      </c>
-      <c r="B7" s="52" t="s">
-        <v>309</v>
       </c>
       <c r="C7" s="50" t="s">
         <v>86</v>
@@ -6501,10 +6498,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="52" t="s">
+        <v>309</v>
+      </c>
+      <c r="B8" s="52" t="s">
         <v>310</v>
-      </c>
-      <c r="B8" s="52" t="s">
-        <v>311</v>
       </c>
       <c r="C8" s="50" t="s">
         <v>100</v>
@@ -6512,105 +6509,105 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="52" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B9" s="52"/>
       <c r="C9" s="50"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="52" t="s">
+        <v>312</v>
+      </c>
+      <c r="B10" s="52" t="s">
         <v>313</v>
       </c>
-      <c r="B10" s="52" t="s">
+      <c r="C10" s="50" t="s">
         <v>314</v>
-      </c>
-      <c r="C10" s="50" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="52" t="s">
+        <v>315</v>
+      </c>
+      <c r="B11" s="52" t="s">
         <v>316</v>
       </c>
-      <c r="B11" s="52" t="s">
+      <c r="C11" s="50" t="s">
         <v>317</v>
-      </c>
-      <c r="C11" s="50" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="52" t="s">
+        <v>318</v>
+      </c>
+      <c r="B12" s="52" t="s">
         <v>319</v>
       </c>
-      <c r="B12" s="52" t="s">
-        <v>320</v>
-      </c>
       <c r="C12" s="50" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="52" t="s">
+        <v>320</v>
+      </c>
+      <c r="B13" s="52" t="s">
         <v>321</v>
       </c>
-      <c r="B13" s="52" t="s">
-        <v>322</v>
-      </c>
       <c r="C13" s="50" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="52" t="s">
+        <v>322</v>
+      </c>
+      <c r="B14" s="52" t="s">
         <v>323</v>
       </c>
-      <c r="B14" s="52" t="s">
-        <v>324</v>
-      </c>
       <c r="C14" s="50" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="52" t="s">
+        <v>324</v>
+      </c>
+      <c r="B15" s="52" t="s">
         <v>325</v>
       </c>
-      <c r="B15" s="52" t="s">
-        <v>326</v>
-      </c>
       <c r="C15" s="50" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="137" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B16" s="137" t="s">
+        <v>326</v>
+      </c>
+      <c r="C16" s="139" t="s">
         <v>327</v>
-      </c>
-      <c r="C16" s="139" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="52" t="s">
+        <v>328</v>
+      </c>
+      <c r="B17" s="52" t="s">
         <v>329</v>
       </c>
-      <c r="B17" s="52" t="s">
-        <v>330</v>
-      </c>
       <c r="C17" s="50" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="52" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B18" s="52" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C18" s="50" t="s">
         <v>86</v>
@@ -6618,26 +6615,26 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="53" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B19" s="53" t="s">
         <v>228</v>
       </c>
       <c r="C19" s="51" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B24" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C24" t="s">
         <v>86</v>
@@ -6645,13 +6642,13 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B25" t="s">
         <v>228</v>
       </c>
       <c r="C25" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
   </sheetData>
@@ -6683,10 +6680,10 @@
         <v>3</v>
       </c>
       <c r="B1" s="131" t="s">
+        <v>334</v>
+      </c>
+      <c r="C1" s="130" t="s">
         <v>335</v>
-      </c>
-      <c r="C1" s="130" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -6697,7 +6694,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="134" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F2" s="75">
         <v>45911</v>
@@ -6727,13 +6724,13 @@
         <v>2</v>
       </c>
       <c r="C3" s="134" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F3" s="75">
         <v>45926</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="H3" s="26" t="str">
         <f>TEXT(F3, "mmm")</f>
@@ -6758,7 +6755,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="134" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F4" s="75">
         <v>45939</v>
@@ -6789,7 +6786,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="134" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F5" s="75">
         <v>45946</v>
@@ -6798,10 +6795,10 @@
         <v>189</v>
       </c>
       <c r="H5" s="26" t="s">
+        <v>274</v>
+      </c>
+      <c r="I5" s="27" t="s">
         <v>275</v>
-      </c>
-      <c r="I5" s="27" t="s">
-        <v>276</v>
       </c>
       <c r="J5">
         <v>6</v>
@@ -6817,7 +6814,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="134" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F6" s="75">
         <v>45953</v>
@@ -6848,7 +6845,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="134" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F7" s="75">
         <v>45967</v>
@@ -6879,7 +6876,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="134" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F8" s="75">
         <v>45974</v>
@@ -6909,7 +6906,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="134" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F9" s="75">
         <v>45981</v>
@@ -6940,7 +6937,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="134" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F10" s="75">
         <v>45995</v>
@@ -6971,7 +6968,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="134" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -6984,7 +6981,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="134" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -6997,7 +6994,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="134" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -7010,7 +7007,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="134" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -7063,12 +7060,12 @@
   <sheetData>
     <row r="2" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="91" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="79" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="37.5" x14ac:dyDescent="0.25">
@@ -7094,7 +7091,7 @@
         <v>9</v>
       </c>
       <c r="H5" s="82" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="I5" s="81" t="s">
         <v>11</v>
@@ -7111,7 +7108,7 @@
         <v>190</v>
       </c>
       <c r="D6" s="93" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E6" s="93">
         <v>2</v>
@@ -7124,7 +7121,7 @@
       </c>
       <c r="H6" s="85"/>
       <c r="I6" s="84" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
@@ -7138,7 +7135,7 @@
         <v>190</v>
       </c>
       <c r="D7" s="94" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E7" s="94">
         <v>4</v>
@@ -7167,7 +7164,7 @@
         <v>197</v>
       </c>
       <c r="D8" s="94" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E8" s="94">
         <v>6</v>
@@ -7194,7 +7191,7 @@
         <v>197</v>
       </c>
       <c r="D9" s="94" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E9" s="94">
         <v>8</v>
@@ -7209,7 +7206,7 @@
         <v>205</v>
       </c>
       <c r="I9" s="86" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
@@ -7250,20 +7247,20 @@
         <v>208</v>
       </c>
       <c r="D11" s="94" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E11" s="94">
         <v>10</v>
       </c>
       <c r="F11" s="87" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G11" s="87" t="s">
         <v>67</v>
       </c>
       <c r="H11" s="87"/>
       <c r="I11" s="86" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
@@ -7292,7 +7289,7 @@
         <v>30</v>
       </c>
       <c r="I12" s="86" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
@@ -7306,13 +7303,13 @@
         <v>208</v>
       </c>
       <c r="D13" s="94" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E13" s="94">
         <v>12</v>
       </c>
       <c r="F13" s="87" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G13" s="87"/>
       <c r="H13" s="87"/>
@@ -7329,13 +7326,13 @@
         <v>208</v>
       </c>
       <c r="D14" s="95" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E14" s="95">
         <v>13</v>
       </c>
       <c r="F14" s="90" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G14" s="90" t="s">
         <v>76</v>

</xml_diff>

<commit_message>
added LK for next year
</commit_message>
<xml_diff>
--- a/data/MACSI seminar series.xlsx
+++ b/data/MACSI seminar series.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ulcampus-my.sharepoint.com/personal/david_osullivan_ul_ie/Documents/Academic_work/_Misc/MACSI_Seminars/macsi-seminars.github.io/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2499" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67B4DC84-C187-43A6-830E-50F3AEA5B7DE}"/>
+  <xr:revisionPtr revIDLastSave="2502" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{462168E1-F0EC-4305-A466-926D38CA642F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AY2023-2024 Sem 2" sheetId="3" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="352">
   <si>
     <t>Fill in as much of the green boxes as possible. Ideally, this would be before you have finished your visitors travel dates (just to avoid double booking).</t>
   </si>
@@ -1152,6 +1152,9 @@
   <si>
     <t>Leornard Henckel</t>
   </si>
+  <si>
+    <t>Leah Keating</t>
+  </si>
 </sst>
 </file>
 
@@ -1160,7 +1163,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1971,9 +1974,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2011,7 +2014,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2117,7 +2120,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2259,7 +2262,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2273,7 +2276,7 @@
       <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="11.140625" customWidth="1"/>
@@ -2298,7 +2301,7 @@
     <col min="24" max="24" width="37.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15.75" thickBot="1">
+    <row r="1" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2309,7 +2312,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="15.75" thickBot="1">
+    <row r="2" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -2383,7 +2386,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="13.5" customHeight="1">
+    <row r="3" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>45317</v>
       </c>
@@ -2449,7 +2452,7 @@
       <c r="W3" s="13"/>
       <c r="X3" s="13"/>
     </row>
-    <row r="4" spans="1:24" ht="13.5" customHeight="1">
+    <row r="4" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>45323</v>
       </c>
@@ -2511,7 +2514,7 @@
       <c r="W4" s="13"/>
       <c r="X4" s="13"/>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>45324</v>
       </c>
@@ -2571,7 +2574,7 @@
       <c r="W5" s="13"/>
       <c r="X5" s="13"/>
     </row>
-    <row r="6" spans="1:24" ht="12.75" customHeight="1">
+    <row r="6" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>45331</v>
       </c>
@@ -2637,7 +2640,7 @@
       <c r="W6" s="13"/>
       <c r="X6" s="13"/>
     </row>
-    <row r="7" spans="1:24">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>45338</v>
       </c>
@@ -2705,7 +2708,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="15" customHeight="1">
+    <row r="8" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>45345</v>
       </c>
@@ -2771,7 +2774,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:24" ht="16.5" customHeight="1">
+    <row r="9" spans="1:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>45359</v>
       </c>
@@ -2823,7 +2826,7 @@
       <c r="W9" s="13"/>
       <c r="X9" s="13"/>
     </row>
-    <row r="10" spans="1:24">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>45366</v>
       </c>
@@ -2891,7 +2894,7 @@
       <c r="W10" s="13"/>
       <c r="X10" s="13"/>
     </row>
-    <row r="11" spans="1:24" ht="15" customHeight="1">
+    <row r="11" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>45379</v>
       </c>
@@ -2951,7 +2954,7 @@
       <c r="W11" s="13"/>
       <c r="X11" s="13"/>
     </row>
-    <row r="12" spans="1:24" ht="13.5" customHeight="1">
+    <row r="12" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>45386</v>
       </c>
@@ -3013,7 +3016,7 @@
       <c r="W12" s="13"/>
       <c r="X12" s="13"/>
     </row>
-    <row r="13" spans="1:24" ht="16.5" customHeight="1">
+    <row r="13" spans="1:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>45387</v>
       </c>
@@ -3081,7 +3084,7 @@
       <c r="W13" s="13"/>
       <c r="X13" s="13"/>
     </row>
-    <row r="14" spans="1:24" ht="15.75" customHeight="1">
+    <row r="14" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>45394</v>
       </c>
@@ -3141,7 +3144,7 @@
       <c r="W14" s="13"/>
       <c r="X14" s="13"/>
     </row>
-    <row r="15" spans="1:24" ht="17.25" customHeight="1">
+    <row r="15" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>45398</v>
       </c>
@@ -3209,7 +3212,7 @@
       <c r="W15" s="13"/>
       <c r="X15" s="13"/>
     </row>
-    <row r="16" spans="1:24" ht="15.75" thickBot="1">
+    <row r="16" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>45401</v>
       </c>
@@ -3271,7 +3274,7 @@
       <c r="W16" s="18"/>
       <c r="X16" s="18"/>
     </row>
-    <row r="17" spans="1:24">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>45421</v>
       </c>
@@ -3341,7 +3344,7 @@
       <c r="W17" s="18"/>
       <c r="X17" s="18"/>
     </row>
-    <row r="18" spans="1:24" ht="15.75" thickBot="1">
+    <row r="18" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="26">
         <v>45474</v>
       </c>
@@ -3391,7 +3394,7 @@
       <c r="W18" s="18"/>
       <c r="X18" s="18"/>
     </row>
-    <row r="19" spans="1:24" ht="17.25" customHeight="1" thickBot="1">
+    <row r="19" spans="1:24" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="26">
         <v>45505</v>
       </c>
@@ -3441,7 +3444,7 @@
       <c r="W19" s="18"/>
       <c r="X19" s="18"/>
     </row>
-    <row r="20" spans="1:24">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="26"/>
       <c r="B20" s="26"/>
       <c r="C20" s="26"/>
@@ -3487,7 +3490,7 @@
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="11.140625" customWidth="1"/>
@@ -3512,7 +3515,7 @@
     <col min="24" max="24" width="37.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15.75" thickBot="1">
+    <row r="1" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3523,7 +3526,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="30.75" thickBot="1">
+    <row r="2" spans="1:24" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="145" t="s">
         <v>3</v>
       </c>
@@ -3597,7 +3600,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="15" customHeight="1">
+    <row r="3" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>45548</v>
       </c>
@@ -3661,7 +3664,7 @@
       <c r="W3" s="46"/>
       <c r="X3" s="44"/>
     </row>
-    <row r="4" spans="1:24" ht="15" customHeight="1">
+    <row r="4" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>45555</v>
       </c>
@@ -3709,7 +3712,7 @@
       <c r="W4" s="15"/>
       <c r="X4" s="13"/>
     </row>
-    <row r="5" spans="1:24" ht="15" customHeight="1">
+    <row r="5" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>45562</v>
       </c>
@@ -3757,7 +3760,7 @@
       <c r="W5" s="15"/>
       <c r="X5" s="13"/>
     </row>
-    <row r="6" spans="1:24" ht="15" customHeight="1">
+    <row r="6" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>45576</v>
       </c>
@@ -3805,7 +3808,7 @@
       <c r="W6" s="15"/>
       <c r="X6" s="13"/>
     </row>
-    <row r="7" spans="1:24" ht="15" customHeight="1">
+    <row r="7" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>45583</v>
       </c>
@@ -3853,7 +3856,7 @@
       <c r="W7" s="15"/>
       <c r="X7" s="13"/>
     </row>
-    <row r="8" spans="1:24" ht="15" customHeight="1">
+    <row r="8" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>45596</v>
       </c>
@@ -3901,7 +3904,7 @@
       <c r="W8" s="15"/>
       <c r="X8" s="13"/>
     </row>
-    <row r="9" spans="1:24" ht="15" customHeight="1">
+    <row r="9" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>45604</v>
       </c>
@@ -3949,7 +3952,7 @@
       <c r="W9" s="15"/>
       <c r="X9" s="13"/>
     </row>
-    <row r="10" spans="1:24" ht="15" customHeight="1">
+    <row r="10" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>45611</v>
       </c>
@@ -3997,7 +4000,7 @@
       <c r="W10" s="15"/>
       <c r="X10" s="13"/>
     </row>
-    <row r="11" spans="1:24" ht="15" customHeight="1">
+    <row r="11" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>45625</v>
       </c>
@@ -4045,7 +4048,7 @@
       <c r="W11" s="15"/>
       <c r="X11" s="13"/>
     </row>
-    <row r="12" spans="1:24" ht="15" customHeight="1" thickBot="1">
+    <row r="12" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>45632</v>
       </c>
@@ -4101,20 +4104,20 @@
       <c r="W12" s="20"/>
       <c r="X12" s="18"/>
     </row>
-    <row r="13" spans="1:24">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="26"/>
       <c r="B13" s="26"/>
       <c r="C13" s="26"/>
       <c r="D13" s="26"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:24">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="26"/>
       <c r="B14" s="26"/>
       <c r="C14" s="26"/>
       <c r="D14" s="26"/>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="61"/>
       <c r="B29" s="61"/>
       <c r="C29" s="61"/>
@@ -4126,59 +4129,59 @@
       <c r="I29" s="61"/>
       <c r="J29" s="61"/>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="60"/>
       <c r="B31" s="60"/>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="60"/>
       <c r="B32" s="60"/>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="60"/>
       <c r="B33" s="60"/>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="60"/>
       <c r="B34" s="60"/>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="60"/>
       <c r="B35" s="60"/>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="60"/>
       <c r="B36" s="60"/>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="60"/>
       <c r="B37" s="60"/>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="60"/>
       <c r="B38" s="60"/>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="60"/>
       <c r="B39" s="60"/>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="60"/>
       <c r="B40" s="60"/>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="60"/>
       <c r="B41" s="60"/>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="60"/>
       <c r="B42" s="60"/>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="60"/>
       <c r="B43" s="60"/>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="60"/>
       <c r="B44" s="60"/>
     </row>
@@ -4211,7 +4214,7 @@
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" customWidth="1"/>
     <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1"/>
@@ -4239,7 +4242,7 @@
     <col min="24" max="24" width="37.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15.75" thickBot="1">
+    <row r="1" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4250,7 +4253,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="27.75" customHeight="1" thickBot="1">
+    <row r="2" spans="1:24" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="64" t="s">
         <v>3</v>
       </c>
@@ -4324,7 +4327,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="15" customHeight="1">
+    <row r="3" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>45694</v>
       </c>
@@ -4375,7 +4378,7 @@
       <c r="W3" s="46"/>
       <c r="X3" s="44"/>
     </row>
-    <row r="4" spans="1:24" ht="14.25" customHeight="1">
+    <row r="4" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>45708</v>
       </c>
@@ -4432,7 +4435,7 @@
       <c r="W4" s="15"/>
       <c r="X4" s="13"/>
     </row>
-    <row r="5" spans="1:24" ht="14.25" customHeight="1">
+    <row r="5" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>45722</v>
       </c>
@@ -4487,7 +4490,7 @@
       <c r="W5" s="15"/>
       <c r="X5" s="13"/>
     </row>
-    <row r="6" spans="1:24" ht="16.5" customHeight="1">
+    <row r="6" spans="1:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>45735</v>
       </c>
@@ -4542,7 +4545,7 @@
       <c r="W6" s="15"/>
       <c r="X6" s="13"/>
     </row>
-    <row r="7" spans="1:24" ht="18" customHeight="1">
+    <row r="7" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>45750</v>
       </c>
@@ -4595,7 +4598,7 @@
       <c r="W7" s="15"/>
       <c r="X7" s="13"/>
     </row>
-    <row r="8" spans="1:24" ht="16.5" customHeight="1">
+    <row r="8" spans="1:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>45751</v>
       </c>
@@ -4653,7 +4656,7 @@
       <c r="W8" s="15"/>
       <c r="X8" s="13"/>
     </row>
-    <row r="9" spans="1:24" ht="15.75" customHeight="1">
+    <row r="9" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>45757</v>
       </c>
@@ -4714,7 +4717,7 @@
       <c r="W9" s="15"/>
       <c r="X9" s="13"/>
     </row>
-    <row r="10" spans="1:24" ht="15.75" customHeight="1">
+    <row r="10" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>45758</v>
       </c>
@@ -4767,7 +4770,7 @@
       <c r="W10" s="20"/>
       <c r="X10" s="18"/>
     </row>
-    <row r="11" spans="1:24" ht="15.75" customHeight="1">
+    <row r="11" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>45764</v>
       </c>
@@ -4826,7 +4829,7 @@
       <c r="W11" s="35"/>
       <c r="X11" s="35"/>
     </row>
-    <row r="12" spans="1:24" ht="15.75" customHeight="1">
+    <row r="12" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>45771</v>
       </c>
@@ -4886,7 +4889,7 @@
       <c r="W12" s="35"/>
       <c r="X12" s="35"/>
     </row>
-    <row r="13" spans="1:24" ht="15.75" customHeight="1">
+    <row r="13" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>45785</v>
       </c>
@@ -4938,7 +4941,7 @@
       <c r="W13" s="35"/>
       <c r="X13" s="35"/>
     </row>
-    <row r="14" spans="1:24" ht="15.75" customHeight="1">
+    <row r="14" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>45799</v>
       </c>
@@ -4984,7 +4987,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:24" ht="15.75" customHeight="1">
+    <row r="15" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>45805</v>
       </c>
@@ -5018,101 +5021,101 @@
         <v>249</v>
       </c>
     </row>
-    <row r="16" spans="1:24" ht="15.75" customHeight="1">
+    <row r="16" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="75"/>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="26"/>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="26"/>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="26"/>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="75"/>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="26"/>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="75"/>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="26"/>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="26"/>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="26"/>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="26"/>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="26"/>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="26"/>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B31" s="60"/>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="60"/>
       <c r="B32" s="60"/>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="60"/>
       <c r="B33" s="60"/>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="60"/>
       <c r="B34" s="60"/>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="60"/>
       <c r="B35" s="60"/>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="60"/>
       <c r="B36" s="60"/>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="60"/>
       <c r="B37" s="60"/>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="60"/>
       <c r="B38" s="60"/>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="60"/>
       <c r="B39" s="60"/>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="60"/>
       <c r="B40" s="60"/>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="60"/>
       <c r="B41" s="60"/>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="60"/>
       <c r="B42" s="60"/>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="60"/>
       <c r="B43" s="60"/>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="60"/>
       <c r="B44" s="60"/>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="60"/>
     </row>
   </sheetData>
@@ -5140,14 +5143,14 @@
   </sheetPr>
   <dimension ref="A1:X23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="7" ySplit="16" topLeftCell="H17" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
       <selection pane="bottomRight" activeCell="I16" sqref="I16"/>
-      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="topRight" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" customWidth="1"/>
@@ -5174,7 +5177,7 @@
     <col min="24" max="24" width="37.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5185,7 +5188,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="30">
+    <row r="2" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="64" t="s">
         <v>3</v>
       </c>
@@ -5259,7 +5262,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="15" customHeight="1">
+    <row r="3" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="75">
         <v>45911</v>
       </c>
@@ -5321,7 +5324,7 @@
       <c r="W3" s="46"/>
       <c r="X3" s="44"/>
     </row>
-    <row r="4" spans="1:24" ht="15" customHeight="1">
+    <row r="4" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="75">
         <v>45917</v>
       </c>
@@ -5389,7 +5392,7 @@
       <c r="W4" s="15"/>
       <c r="X4" s="13"/>
     </row>
-    <row r="5" spans="1:24" ht="15" customHeight="1">
+    <row r="5" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="75">
         <v>45926</v>
       </c>
@@ -5446,7 +5449,7 @@
       <c r="W5" s="15"/>
       <c r="X5" s="13"/>
     </row>
-    <row r="6" spans="1:24" ht="15" customHeight="1">
+    <row r="6" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="75">
         <v>45939</v>
       </c>
@@ -5509,7 +5512,7 @@
       <c r="W6" s="15"/>
       <c r="X6" s="13"/>
     </row>
-    <row r="7" spans="1:24" ht="15" customHeight="1">
+    <row r="7" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="75">
         <v>45946</v>
       </c>
@@ -5565,7 +5568,7 @@
       <c r="W7" s="15"/>
       <c r="X7" s="13"/>
     </row>
-    <row r="8" spans="1:24" ht="15" customHeight="1">
+    <row r="8" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="75">
         <v>45953</v>
       </c>
@@ -5620,7 +5623,7 @@
       <c r="W8" s="15"/>
       <c r="X8" s="13"/>
     </row>
-    <row r="9" spans="1:24" ht="15" customHeight="1">
+    <row r="9" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="75">
         <v>45967</v>
       </c>
@@ -5681,7 +5684,7 @@
       <c r="W9" s="15"/>
       <c r="X9" s="13"/>
     </row>
-    <row r="10" spans="1:24" ht="15" customHeight="1">
+    <row r="10" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="75">
         <v>45974</v>
       </c>
@@ -5739,7 +5742,7 @@
       <c r="W10" s="15"/>
       <c r="X10" s="13"/>
     </row>
-    <row r="11" spans="1:24" ht="15" customHeight="1">
+    <row r="11" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="75">
         <v>45981</v>
       </c>
@@ -5796,7 +5799,7 @@
       <c r="W11" s="15"/>
       <c r="X11" s="13"/>
     </row>
-    <row r="12" spans="1:24" ht="15" customHeight="1">
+    <row r="12" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="75">
         <v>45995</v>
       </c>
@@ -5855,35 +5858,35 @@
       <c r="W12" s="15"/>
       <c r="X12" s="13"/>
     </row>
-    <row r="13" spans="1:24" ht="15" customHeight="1">
+    <row r="13" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="26"/>
       <c r="B13" s="26"/>
       <c r="C13" s="26"/>
       <c r="W13" s="20"/>
       <c r="X13" s="18"/>
     </row>
-    <row r="14" spans="1:24" ht="15" customHeight="1">
+    <row r="14" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="26"/>
       <c r="B14" s="26"/>
       <c r="C14" s="26"/>
     </row>
-    <row r="15" spans="1:24" ht="15" customHeight="1">
+    <row r="15" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="26"/>
       <c r="B15" s="26"/>
       <c r="C15" s="26"/>
     </row>
-    <row r="16" spans="1:24" ht="15" customHeight="1">
+    <row r="16" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="26"/>
       <c r="B16" s="26"/>
       <c r="C16" s="26"/>
     </row>
-    <row r="17" ht="15" customHeight="1"/>
-    <row r="18" ht="15" customHeight="1"/>
-    <row r="19" ht="15" customHeight="1"/>
-    <row r="20" ht="15" customHeight="1"/>
-    <row r="21" ht="15" customHeight="1"/>
-    <row r="22" ht="15" customHeight="1"/>
-    <row r="23" ht="15" customHeight="1"/>
+    <row r="17" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <protectedRanges>
     <protectedRange algorithmName="SHA-512" hashValue="pQyTzP/d7t5ThMimBt5mu8gGozgAm1OwF6BMILsn5/kmtZ5mZf81NMi09wwU8mvtItxf0EVNWa6V4MCa0DKeSQ==" saltValue="NzZBiAQ1yFjat+SeIqh2Uw==" spinCount="100000" sqref="A3:E16" name="Range3_1"/>
@@ -5907,11 +5910,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F62D4156-0A06-4DBF-B1E7-3E12580121CB}">
   <dimension ref="A1:X13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" customWidth="1"/>
     <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1"/>
@@ -5938,7 +5941,7 @@
     <col min="24" max="24" width="37.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15.75" thickBot="1">
+    <row r="1" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5949,7 +5952,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="30.75" thickBot="1">
+    <row r="2" spans="1:24" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="64" t="s">
         <v>3</v>
       </c>
@@ -6023,7 +6026,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="15" customHeight="1">
+    <row r="3" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="75">
         <v>46051</v>
       </c>
@@ -6075,7 +6078,7 @@
       <c r="W3" s="46"/>
       <c r="X3" s="44"/>
     </row>
-    <row r="4" spans="1:24" ht="15.75" customHeight="1">
+    <row r="4" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="75">
         <f>A3+14</f>
         <v>46065</v>
@@ -6127,7 +6130,7 @@
       <c r="W4" s="15"/>
       <c r="X4" s="13"/>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="75">
         <f t="shared" ref="A5:A9" si="2">A4+14</f>
         <v>46079</v>
@@ -6179,7 +6182,7 @@
       <c r="W5" s="15"/>
       <c r="X5" s="13"/>
     </row>
-    <row r="6" spans="1:24" ht="15.75" customHeight="1">
+    <row r="6" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="75">
         <f t="shared" si="2"/>
         <v>46093</v>
@@ -6200,13 +6203,13 @@
         <v>7</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>302</v>
+        <v>351</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>274</v>
+        <v>151</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>274</v>
+        <v>94</v>
       </c>
       <c r="I6" s="98" t="s">
         <v>274</v>
@@ -6231,7 +6234,7 @@
       <c r="W6" s="15"/>
       <c r="X6" s="13"/>
     </row>
-    <row r="7" spans="1:24">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="75">
         <f t="shared" si="2"/>
         <v>46107</v>
@@ -6283,7 +6286,7 @@
       <c r="W7" s="15"/>
       <c r="X7" s="13"/>
     </row>
-    <row r="8" spans="1:24">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="75">
         <f t="shared" si="2"/>
         <v>46121</v>
@@ -6333,7 +6336,7 @@
       <c r="W8" s="15"/>
       <c r="X8" s="13"/>
     </row>
-    <row r="9" spans="1:24" ht="18.75" customHeight="1">
+    <row r="9" spans="1:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="75">
         <f t="shared" si="2"/>
         <v>46135</v>
@@ -6385,24 +6388,24 @@
       <c r="W9" s="15"/>
       <c r="X9" s="13"/>
     </row>
-    <row r="10" spans="1:24" ht="15.75" thickBot="1">
+    <row r="10" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="26"/>
       <c r="B10" s="26"/>
       <c r="C10" s="26"/>
       <c r="W10" s="20"/>
       <c r="X10" s="18"/>
     </row>
-    <row r="11" spans="1:24" ht="12.75" customHeight="1">
+    <row r="11" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="26"/>
       <c r="B11" s="26"/>
       <c r="C11" s="26"/>
     </row>
-    <row r="12" spans="1:24">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="26"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
     </row>
-    <row r="13" spans="1:24">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="26"/>
       <c r="B13" s="26"/>
       <c r="C13" s="26"/>
@@ -6427,19 +6430,19 @@
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.28515625" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
     <col min="3" max="3" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="55" t="s">
         <v>304</v>
       </c>
@@ -6450,7 +6453,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="136" t="s">
         <v>307</v>
       </c>
@@ -6459,7 +6462,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>308</v>
       </c>
@@ -6468,7 +6471,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="52" t="s">
         <v>309</v>
       </c>
@@ -6477,7 +6480,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="52" t="s">
         <v>311</v>
       </c>
@@ -6488,7 +6491,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="52" t="s">
         <v>313</v>
       </c>
@@ -6499,7 +6502,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="52" t="s">
         <v>315</v>
       </c>
@@ -6510,14 +6513,14 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="52" t="s">
         <v>317</v>
       </c>
       <c r="B9" s="52"/>
       <c r="C9" s="50"/>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="52" t="s">
         <v>318</v>
       </c>
@@ -6528,7 +6531,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="52" t="s">
         <v>321</v>
       </c>
@@ -6539,7 +6542,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="52" t="s">
         <v>324</v>
       </c>
@@ -6550,7 +6553,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="52" t="s">
         <v>326</v>
       </c>
@@ -6561,7 +6564,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="52" t="s">
         <v>328</v>
       </c>
@@ -6572,7 +6575,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="52" t="s">
         <v>330</v>
       </c>
@@ -6583,7 +6586,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="137" t="s">
         <v>298</v>
       </c>
@@ -6594,7 +6597,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="52" t="s">
         <v>334</v>
       </c>
@@ -6605,7 +6608,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="52" t="s">
         <v>336</v>
       </c>
@@ -6616,7 +6619,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="53" t="s">
         <v>337</v>
       </c>
@@ -6627,12 +6630,12 @@
         <v>338</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>336</v>
       </c>
@@ -6643,7 +6646,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>337</v>
       </c>
@@ -6672,13 +6675,13 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
     <col min="6" max="6" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="135" t="s">
         <v>3</v>
       </c>
@@ -6689,7 +6692,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickTop="1">
+    <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="133">
         <v>45911</v>
       </c>
@@ -6717,7 +6720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="133">
         <f>A2+7</f>
         <v>45918</v>
@@ -6748,7 +6751,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="133">
         <f t="shared" ref="A4:A12" si="0">A3+7</f>
         <v>45925</v>
@@ -6779,7 +6782,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="133">
         <f t="shared" si="0"/>
         <v>45932</v>
@@ -6807,7 +6810,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="133">
         <f t="shared" si="0"/>
         <v>45939</v>
@@ -6838,7 +6841,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="133">
         <f t="shared" si="0"/>
         <v>45946</v>
@@ -6869,7 +6872,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="133">
         <f t="shared" si="0"/>
         <v>45953</v>
@@ -6899,7 +6902,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="133">
         <f t="shared" si="0"/>
         <v>45960</v>
@@ -6930,7 +6933,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="133">
         <f t="shared" si="0"/>
         <v>45967</v>
@@ -6961,7 +6964,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="133">
         <f t="shared" si="0"/>
         <v>45974</v>
@@ -6974,7 +6977,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="133">
         <f t="shared" si="0"/>
         <v>45981</v>
@@ -6987,7 +6990,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="133">
         <f t="shared" ref="A13:A14" si="6">A12+7</f>
         <v>45988</v>
@@ -7000,7 +7003,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="133">
         <f t="shared" si="6"/>
         <v>45995</v>
@@ -7013,12 +7016,12 @@
         <v>342</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="133"/>
       <c r="B15" s="134"/>
       <c r="C15" s="134"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G16" s="26"/>
     </row>
   </sheetData>
@@ -7049,7 +7052,7 @@
       <selection activeCell="F8" sqref="F8:H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.42578125" customWidth="1"/>
     <col min="2" max="2" width="9.140625" customWidth="1"/>
@@ -7061,17 +7064,17 @@
     <col min="9" max="9" width="64.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" ht="23.25">
+    <row r="2" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="91" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="18.75">
+    <row r="3" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="79" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="37.5">
+    <row r="5" spans="1:9" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A5" s="80" t="s">
         <v>3</v>
       </c>
@@ -7100,7 +7103,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="18.75">
+    <row r="6" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="92">
         <v>45694</v>
       </c>
@@ -7127,7 +7130,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="18.75">
+    <row r="7" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="83">
         <v>45708</v>
       </c>
@@ -7156,7 +7159,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="18.75">
+    <row r="8" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="83">
         <v>45722</v>
       </c>
@@ -7183,7 +7186,7 @@
       </c>
       <c r="I8" s="86"/>
     </row>
-    <row r="9" spans="1:9" ht="18.75">
+    <row r="9" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="83">
         <v>45735</v>
       </c>
@@ -7212,7 +7215,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="18.75">
+    <row r="10" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="83">
         <v>45744</v>
       </c>
@@ -7239,7 +7242,7 @@
       </c>
       <c r="I10" s="86"/>
     </row>
-    <row r="11" spans="1:9" ht="18.75">
+    <row r="11" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="83">
         <v>45750</v>
       </c>
@@ -7266,7 +7269,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="18.75">
+    <row r="12" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="83">
         <v>45758</v>
       </c>
@@ -7295,7 +7298,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="18.75">
+    <row r="13" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="83">
         <v>45764</v>
       </c>
@@ -7318,7 +7321,7 @@
       <c r="H13" s="87"/>
       <c r="I13" s="86"/>
     </row>
-    <row r="14" spans="1:9" ht="18.75">
+    <row r="14" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="88">
         <v>45771</v>
       </c>
@@ -7347,7 +7350,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="20" spans="8:8" ht="18.75">
+    <row r="20" spans="8:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="H20" s="79"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change time for DC
</commit_message>
<xml_diff>
--- a/data/MACSI seminar series.xlsx
+++ b/data/MACSI seminar series.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ulcampus-my.sharepoint.com/personal/david_osullivan_ul_ie/Documents/Academic_work/_Misc/MACSI_Seminars/macsi-seminars.github.io/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2508" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6DE9EA38-2D4B-4B9F-815F-61388D0897A5}"/>
+  <xr:revisionPtr revIDLastSave="2509" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D3F863A8-13BB-4AFE-876B-C95D2F685A72}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AY2023-2024 Sem 2" sheetId="3" r:id="rId1"/>
@@ -5161,7 +5161,7 @@
       <pane xSplit="7" ySplit="16" topLeftCell="H19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="F19" sqref="F19"/>
+      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5531,7 +5531,7 @@
         <v>45946</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>189</v>
+        <v>258</v>
       </c>
       <c r="C7" s="26" t="s">
         <v>276</v>

</xml_diff>

<commit_message>
added abs for TS
</commit_message>
<xml_diff>
--- a/data/MACSI seminar series.xlsx
+++ b/data/MACSI seminar series.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ulcampus-my.sharepoint.com/personal/david_osullivan_ul_ie/Documents/Academic_work/_Misc/MACSI_Seminars/macsi-seminars.github.io/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2509" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D3F863A8-13BB-4AFE-876B-C95D2F685A72}"/>
+  <xr:revisionPtr revIDLastSave="2510" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8AFFD790-BAC8-4A5A-BFEF-0823DB0A523E}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="888" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="888" uniqueCount="356">
   <si>
     <t>Fill in as much of the green boxes as possible. Ideally, this would be before you have finished your visitors travel dates (just to avoid double booking).</t>
   </si>
@@ -934,7 +934,9 @@
     <t>A wavelet lifting approach for spatial/network data</t>
   </si>
   <si>
-    <t>TBC</t>
+    <t>As an emerging research area, analysing functions that arise from network (graph) structures attracts researchers in both statistics and signal processing communities. Data collected over graphs can be modelled as noisy observations of an unknown function over the vertices of a graph structure, fully described by its vertices and their connections, the edges.
+While current literature is rich when data are collected from the graph vertex space, the data collected from graph edges call for new techniques, and in its turn reaches across many application fields, from traffic networks to neuroscience and hydrology. Wavelets can be powerful tools for understanding the behaviour of the underlying (edge) functions due to their computational efficiency and robust performance in the presence of discontinuities.
+In this talk, we will begin by tracing the ‘evolution’ of wavelet methods, from classical wavelets to second-generation wavelets (constructed via the lifting scheme), and then to a variant that allows us to handle a broader class of data (such as spatial data). We will then move on to construct some new wavelet bases that can represent and perform nonparametric regression for functions defined on both the vertex and edge sets of graphs.</t>
   </si>
   <si>
     <t>https://scholar.google.com/citations?user=paf72YcAAAAJ&amp;hl=en</t>
@@ -947,6 +949,9 @@
   </si>
   <si>
     <t>Multi-output gaussian process models for pollution in river networks</t>
+  </si>
+  <si>
+    <t>The impact of human activity on the quality of surface waters, particularly rivers, has recently received considerable attention. Statistical models aimed at characterizing the spatiotemporal distribution of biological and chemical indicators across river networks must address several unique challenges not typically encountered in standard spatial modelling. In this seminar, I will present a class of spatiotemporal models designed for multivariate data sampled on river networks. These models build upon the framework introduced by Ver Hoef et al. (2006), which replaces traditional Euclidean distances with stream distance metrics to better represent spatial relationships in river systems. We extend this approach to incorporate temporal dynamics and multivariate dependencies, while also addressing practical aspects of water quality monitoring such as censoring limits and intermittent sampling. Finally, I will introduce a variational inference framework for fitting these models efficiently and share results from simulation experiments comparing our proposed approach with more conventional Gaussian Process models.</t>
   </si>
   <si>
     <t>https://scholar.google.com/citations?user=pglQgmQAAAAJ&amp;hl=en</t>
@@ -1018,6 +1023,9 @@
     <t>Open</t>
   </si>
   <si>
+    <t>TBC</t>
+  </si>
+  <si>
     <t>Leah Keating</t>
   </si>
   <si>
@@ -1163,11 +1171,6 @@
   </si>
   <si>
     <t>Leornard Henckel</t>
-  </si>
-  <si>
-    <t>As an emerging research area, analysing functions that arise from network (graph) structures attracts researchers in both statistics and signal processing communities. Data collected over graphs can be modelled as noisy observations of an unknown function over the vertices of a graph structure, fully described by its vertices and their connections, the edges.
-While current literature is rich when data are collected from the graph vertex space, the data collected from graph edges call for new techniques, and in its turn reaches across many application fields, from traffic networks to neuroscience and hydrology. Wavelets can be powerful tools for understanding the behaviour of the underlying (edge) functions due to their computational efficiency and robust performance in the presence of discontinuities.
-In this talk, we will begin by tracing the ‘evolution’ of wavelet methods, from classical wavelets to second-generation wavelets (constructed via the lifting scheme), and then to a variant that allows us to handle a broader class of data (such as spatial data). We will then move on to construct some new wavelet bases that can represent and perform nonparametric regression for functions defined on both the vertex and edge sets of graphs.</t>
   </si>
 </sst>
 </file>
@@ -1177,7 +1180,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1988,9 +1991,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2028,7 +2031,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2134,7 +2137,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2276,7 +2279,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2290,7 +2293,7 @@
       <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="11.140625" customWidth="1"/>
@@ -2315,7 +2318,7 @@
     <col min="24" max="24" width="37.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" ht="15.75" thickBot="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2326,7 +2329,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" ht="15.75" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -2400,7 +2403,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" ht="13.5" customHeight="1">
       <c r="A3" s="2">
         <v>45317</v>
       </c>
@@ -2466,7 +2469,7 @@
       <c r="W3" s="13"/>
       <c r="X3" s="13"/>
     </row>
-    <row r="4" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" ht="13.5" customHeight="1">
       <c r="A4" s="2">
         <v>45323</v>
       </c>
@@ -2528,7 +2531,7 @@
       <c r="W4" s="13"/>
       <c r="X4" s="13"/>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24">
       <c r="A5" s="2">
         <v>45324</v>
       </c>
@@ -2588,7 +2591,7 @@
       <c r="W5" s="13"/>
       <c r="X5" s="13"/>
     </row>
-    <row r="6" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" ht="12.75" customHeight="1">
       <c r="A6" s="2">
         <v>45331</v>
       </c>
@@ -2654,7 +2657,7 @@
       <c r="W6" s="13"/>
       <c r="X6" s="13"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24">
       <c r="A7" s="2">
         <v>45338</v>
       </c>
@@ -2722,7 +2725,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" ht="15" customHeight="1">
       <c r="A8" s="2">
         <v>45345</v>
       </c>
@@ -2788,7 +2791,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" ht="16.5" customHeight="1">
       <c r="A9" s="2">
         <v>45359</v>
       </c>
@@ -2840,7 +2843,7 @@
       <c r="W9" s="13"/>
       <c r="X9" s="13"/>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24">
       <c r="A10" s="2">
         <v>45366</v>
       </c>
@@ -2908,7 +2911,7 @@
       <c r="W10" s="13"/>
       <c r="X10" s="13"/>
     </row>
-    <row r="11" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" ht="15" customHeight="1">
       <c r="A11" s="2">
         <v>45379</v>
       </c>
@@ -2968,7 +2971,7 @@
       <c r="W11" s="13"/>
       <c r="X11" s="13"/>
     </row>
-    <row r="12" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" ht="13.5" customHeight="1">
       <c r="A12" s="2">
         <v>45386</v>
       </c>
@@ -3030,7 +3033,7 @@
       <c r="W12" s="13"/>
       <c r="X12" s="13"/>
     </row>
-    <row r="13" spans="1:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" ht="16.5" customHeight="1">
       <c r="A13" s="2">
         <v>45387</v>
       </c>
@@ -3098,7 +3101,7 @@
       <c r="W13" s="13"/>
       <c r="X13" s="13"/>
     </row>
-    <row r="14" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" ht="15.75" customHeight="1">
       <c r="A14" s="2">
         <v>45394</v>
       </c>
@@ -3158,7 +3161,7 @@
       <c r="W14" s="13"/>
       <c r="X14" s="13"/>
     </row>
-    <row r="15" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" ht="17.25" customHeight="1">
       <c r="A15" s="2">
         <v>45398</v>
       </c>
@@ -3226,7 +3229,7 @@
       <c r="W15" s="13"/>
       <c r="X15" s="13"/>
     </row>
-    <row r="16" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" ht="15.75" thickBot="1">
       <c r="A16" s="2">
         <v>45401</v>
       </c>
@@ -3288,7 +3291,7 @@
       <c r="W16" s="18"/>
       <c r="X16" s="18"/>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24">
       <c r="A17" s="4">
         <v>45421</v>
       </c>
@@ -3358,7 +3361,7 @@
       <c r="W17" s="18"/>
       <c r="X17" s="18"/>
     </row>
-    <row r="18" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:24" ht="15.75" thickBot="1">
       <c r="A18" s="26">
         <v>45474</v>
       </c>
@@ -3408,7 +3411,7 @@
       <c r="W18" s="18"/>
       <c r="X18" s="18"/>
     </row>
-    <row r="19" spans="1:24" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:24" ht="17.25" customHeight="1" thickBot="1">
       <c r="A19" s="26">
         <v>45505</v>
       </c>
@@ -3458,7 +3461,7 @@
       <c r="W19" s="18"/>
       <c r="X19" s="18"/>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24">
       <c r="A20" s="26"/>
       <c r="B20" s="26"/>
       <c r="C20" s="26"/>
@@ -3504,7 +3507,7 @@
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="11.140625" customWidth="1"/>
@@ -3529,7 +3532,7 @@
     <col min="24" max="24" width="37.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" ht="15.75" thickBot="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3540,7 +3543,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" ht="30.75" thickBot="1">
       <c r="A2" s="145" t="s">
         <v>3</v>
       </c>
@@ -3614,7 +3617,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" ht="15" customHeight="1">
       <c r="A3" s="2">
         <v>45548</v>
       </c>
@@ -3678,7 +3681,7 @@
       <c r="W3" s="46"/>
       <c r="X3" s="44"/>
     </row>
-    <row r="4" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" ht="15" customHeight="1">
       <c r="A4" s="2">
         <v>45555</v>
       </c>
@@ -3726,7 +3729,7 @@
       <c r="W4" s="15"/>
       <c r="X4" s="13"/>
     </row>
-    <row r="5" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" ht="15" customHeight="1">
       <c r="A5" s="2">
         <v>45562</v>
       </c>
@@ -3774,7 +3777,7 @@
       <c r="W5" s="15"/>
       <c r="X5" s="13"/>
     </row>
-    <row r="6" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" ht="15" customHeight="1">
       <c r="A6" s="2">
         <v>45576</v>
       </c>
@@ -3822,7 +3825,7 @@
       <c r="W6" s="15"/>
       <c r="X6" s="13"/>
     </row>
-    <row r="7" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" ht="15" customHeight="1">
       <c r="A7" s="2">
         <v>45583</v>
       </c>
@@ -3870,7 +3873,7 @@
       <c r="W7" s="15"/>
       <c r="X7" s="13"/>
     </row>
-    <row r="8" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" ht="15" customHeight="1">
       <c r="A8" s="2">
         <v>45596</v>
       </c>
@@ -3918,7 +3921,7 @@
       <c r="W8" s="15"/>
       <c r="X8" s="13"/>
     </row>
-    <row r="9" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" ht="15" customHeight="1">
       <c r="A9" s="2">
         <v>45604</v>
       </c>
@@ -3966,7 +3969,7 @@
       <c r="W9" s="15"/>
       <c r="X9" s="13"/>
     </row>
-    <row r="10" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" ht="15" customHeight="1">
       <c r="A10" s="2">
         <v>45611</v>
       </c>
@@ -4014,7 +4017,7 @@
       <c r="W10" s="15"/>
       <c r="X10" s="13"/>
     </row>
-    <row r="11" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" ht="15" customHeight="1">
       <c r="A11" s="2">
         <v>45625</v>
       </c>
@@ -4062,7 +4065,7 @@
       <c r="W11" s="15"/>
       <c r="X11" s="13"/>
     </row>
-    <row r="12" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" ht="15" customHeight="1" thickBot="1">
       <c r="A12" s="4">
         <v>45632</v>
       </c>
@@ -4118,20 +4121,20 @@
       <c r="W12" s="20"/>
       <c r="X12" s="18"/>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24">
       <c r="A13" s="26"/>
       <c r="B13" s="26"/>
       <c r="C13" s="26"/>
       <c r="D13" s="26"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24">
       <c r="A14" s="26"/>
       <c r="B14" s="26"/>
       <c r="C14" s="26"/>
       <c r="D14" s="26"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10">
       <c r="A29" s="61"/>
       <c r="B29" s="61"/>
       <c r="C29" s="61"/>
@@ -4143,59 +4146,59 @@
       <c r="I29" s="61"/>
       <c r="J29" s="61"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10">
       <c r="A31" s="60"/>
       <c r="B31" s="60"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10">
       <c r="A32" s="60"/>
       <c r="B32" s="60"/>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2">
       <c r="A33" s="60"/>
       <c r="B33" s="60"/>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2">
       <c r="A34" s="60"/>
       <c r="B34" s="60"/>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2">
       <c r="A35" s="60"/>
       <c r="B35" s="60"/>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2">
       <c r="A36" s="60"/>
       <c r="B36" s="60"/>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2">
       <c r="A37" s="60"/>
       <c r="B37" s="60"/>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2">
       <c r="A38" s="60"/>
       <c r="B38" s="60"/>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2">
       <c r="A39" s="60"/>
       <c r="B39" s="60"/>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2">
       <c r="A40" s="60"/>
       <c r="B40" s="60"/>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2">
       <c r="A41" s="60"/>
       <c r="B41" s="60"/>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2">
       <c r="A42" s="60"/>
       <c r="B42" s="60"/>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2">
       <c r="A43" s="60"/>
       <c r="B43" s="60"/>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2">
       <c r="A44" s="60"/>
       <c r="B44" s="60"/>
     </row>
@@ -4228,7 +4231,7 @@
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.5703125" customWidth="1"/>
     <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1"/>
@@ -4256,7 +4259,7 @@
     <col min="24" max="24" width="37.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" ht="15.75" thickBot="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4267,7 +4270,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" ht="27.75" customHeight="1" thickBot="1">
       <c r="A2" s="64" t="s">
         <v>3</v>
       </c>
@@ -4341,7 +4344,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" ht="15" customHeight="1">
       <c r="A3" s="2">
         <v>45694</v>
       </c>
@@ -4392,7 +4395,7 @@
       <c r="W3" s="46"/>
       <c r="X3" s="44"/>
     </row>
-    <row r="4" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" ht="14.25" customHeight="1">
       <c r="A4" s="2">
         <v>45708</v>
       </c>
@@ -4449,7 +4452,7 @@
       <c r="W4" s="15"/>
       <c r="X4" s="13"/>
     </row>
-    <row r="5" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" ht="14.25" customHeight="1">
       <c r="A5" s="2">
         <v>45722</v>
       </c>
@@ -4504,7 +4507,7 @@
       <c r="W5" s="15"/>
       <c r="X5" s="13"/>
     </row>
-    <row r="6" spans="1:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" ht="16.5" customHeight="1">
       <c r="A6" s="2">
         <v>45735</v>
       </c>
@@ -4559,7 +4562,7 @@
       <c r="W6" s="15"/>
       <c r="X6" s="13"/>
     </row>
-    <row r="7" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" ht="18" customHeight="1">
       <c r="A7" s="2">
         <v>45750</v>
       </c>
@@ -4612,7 +4615,7 @@
       <c r="W7" s="15"/>
       <c r="X7" s="13"/>
     </row>
-    <row r="8" spans="1:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" ht="16.5" customHeight="1">
       <c r="A8" s="2">
         <v>45751</v>
       </c>
@@ -4670,7 +4673,7 @@
       <c r="W8" s="15"/>
       <c r="X8" s="13"/>
     </row>
-    <row r="9" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" ht="15.75" customHeight="1">
       <c r="A9" s="2">
         <v>45757</v>
       </c>
@@ -4731,7 +4734,7 @@
       <c r="W9" s="15"/>
       <c r="X9" s="13"/>
     </row>
-    <row r="10" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" ht="15.75" customHeight="1">
       <c r="A10" s="2">
         <v>45758</v>
       </c>
@@ -4784,7 +4787,7 @@
       <c r="W10" s="20"/>
       <c r="X10" s="18"/>
     </row>
-    <row r="11" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" ht="15.75" customHeight="1">
       <c r="A11" s="4">
         <v>45764</v>
       </c>
@@ -4843,7 +4846,7 @@
       <c r="W11" s="35"/>
       <c r="X11" s="35"/>
     </row>
-    <row r="12" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" ht="15.75" customHeight="1">
       <c r="A12" s="4">
         <v>45771</v>
       </c>
@@ -4903,7 +4906,7 @@
       <c r="W12" s="35"/>
       <c r="X12" s="35"/>
     </row>
-    <row r="13" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" ht="15.75" customHeight="1">
       <c r="A13" s="2">
         <v>45785</v>
       </c>
@@ -4955,7 +4958,7 @@
       <c r="W13" s="35"/>
       <c r="X13" s="35"/>
     </row>
-    <row r="14" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" ht="15.75" customHeight="1">
       <c r="A14" s="4">
         <v>45799</v>
       </c>
@@ -5001,7 +5004,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" ht="15.75" customHeight="1">
       <c r="A15" s="4">
         <v>45805</v>
       </c>
@@ -5035,101 +5038,101 @@
         <v>249</v>
       </c>
     </row>
-    <row r="16" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" ht="15.75" customHeight="1">
       <c r="A16" s="75"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="A17" s="26"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2">
       <c r="A18" s="26"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2">
       <c r="A19" s="26"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2">
       <c r="A20" s="75"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2">
       <c r="A21" s="26"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2">
       <c r="A22" s="75"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2">
       <c r="A23" s="26"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2">
       <c r="A24" s="26"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2">
       <c r="A25" s="26"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2">
       <c r="A26" s="26"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2">
       <c r="A27" s="26"/>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2">
       <c r="A28" s="26"/>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2">
       <c r="B31" s="60"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2">
       <c r="A32" s="60"/>
       <c r="B32" s="60"/>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2">
       <c r="A33" s="60"/>
       <c r="B33" s="60"/>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2">
       <c r="A34" s="60"/>
       <c r="B34" s="60"/>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2">
       <c r="A35" s="60"/>
       <c r="B35" s="60"/>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2">
       <c r="A36" s="60"/>
       <c r="B36" s="60"/>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2">
       <c r="A37" s="60"/>
       <c r="B37" s="60"/>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2">
       <c r="A38" s="60"/>
       <c r="B38" s="60"/>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2">
       <c r="A39" s="60"/>
       <c r="B39" s="60"/>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2">
       <c r="A40" s="60"/>
       <c r="B40" s="60"/>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2">
       <c r="A41" s="60"/>
       <c r="B41" s="60"/>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2">
       <c r="A42" s="60"/>
       <c r="B42" s="60"/>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2">
       <c r="A43" s="60"/>
       <c r="B43" s="60"/>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2">
       <c r="A44" s="60"/>
       <c r="B44" s="60"/>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2">
       <c r="A45" s="60"/>
     </row>
   </sheetData>
@@ -5159,12 +5162,12 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="7" ySplit="16" topLeftCell="H19" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="I8" sqref="I8"/>
+      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.5703125" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" customWidth="1"/>
@@ -5191,7 +5194,7 @@
     <col min="24" max="24" width="37.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5202,7 +5205,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" ht="30">
       <c r="A2" s="64" t="s">
         <v>3</v>
       </c>
@@ -5276,7 +5279,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" ht="15" customHeight="1">
       <c r="A3" s="75">
         <v>45911</v>
       </c>
@@ -5338,7 +5341,7 @@
       <c r="W3" s="46"/>
       <c r="X3" s="44"/>
     </row>
-    <row r="4" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" ht="15" customHeight="1">
       <c r="A4" s="75">
         <v>45917</v>
       </c>
@@ -5406,7 +5409,7 @@
       <c r="W4" s="15"/>
       <c r="X4" s="13"/>
     </row>
-    <row r="5" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" ht="15" customHeight="1">
       <c r="A5" s="75">
         <v>45926</v>
       </c>
@@ -5463,7 +5466,7 @@
       <c r="W5" s="15"/>
       <c r="X5" s="13"/>
     </row>
-    <row r="6" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" ht="15" customHeight="1">
       <c r="A6" s="75">
         <v>45939</v>
       </c>
@@ -5526,7 +5529,7 @@
       <c r="W6" s="15"/>
       <c r="X6" s="13"/>
     </row>
-    <row r="7" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" ht="15" customHeight="1">
       <c r="A7" s="75">
         <v>45946</v>
       </c>
@@ -5555,7 +5558,7 @@
         <v>279</v>
       </c>
       <c r="J7" s="98" t="s">
-        <v>354</v>
+        <v>280</v>
       </c>
       <c r="K7" s="157" t="s">
         <v>281</v>
@@ -5582,7 +5585,7 @@
       <c r="W7" s="15"/>
       <c r="X7" s="13"/>
     </row>
-    <row r="8" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" ht="15" customHeight="1">
       <c r="A8" s="75">
         <v>45953</v>
       </c>
@@ -5614,10 +5617,10 @@
         <v>284</v>
       </c>
       <c r="J8" s="98" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="K8" s="157" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="L8" s="25"/>
       <c r="M8" s="16" t="s">
@@ -5639,7 +5642,7 @@
       <c r="W8" s="15"/>
       <c r="X8" s="13"/>
     </row>
-    <row r="9" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" ht="15" customHeight="1">
       <c r="A9" s="75">
         <v>45967</v>
       </c>
@@ -5659,7 +5662,7 @@
         <v>9</v>
       </c>
       <c r="F9" s="101" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G9" s="107" t="s">
         <v>268</v>
@@ -5668,13 +5671,13 @@
         <v>199</v>
       </c>
       <c r="I9" s="97" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="J9" s="97" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="K9" s="157" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="L9" s="25"/>
       <c r="M9" s="16"/>
@@ -5686,10 +5689,10 @@
         <v>63</v>
       </c>
       <c r="Q9" s="5" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="R9" s="16" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="S9" s="35"/>
       <c r="T9" s="5" t="s">
@@ -5700,7 +5703,7 @@
       <c r="W9" s="15"/>
       <c r="X9" s="13"/>
     </row>
-    <row r="10" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" ht="15" customHeight="1">
       <c r="A10" s="75">
         <v>45974</v>
       </c>
@@ -5719,19 +5722,19 @@
         <v>10</v>
       </c>
       <c r="F10" s="101" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="G10" s="107" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="H10" s="25" t="s">
         <v>123</v>
       </c>
       <c r="I10" s="97" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="J10" s="97" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="K10" s="157"/>
       <c r="L10" s="25"/>
@@ -5743,7 +5746,7 @@
         <v>43</v>
       </c>
       <c r="P10" s="5" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="Q10" s="5"/>
       <c r="R10" s="16"/>
@@ -5758,7 +5761,7 @@
       <c r="W10" s="15"/>
       <c r="X10" s="13"/>
     </row>
-    <row r="11" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" ht="15" customHeight="1">
       <c r="A11" s="75">
         <v>45981</v>
       </c>
@@ -5778,7 +5781,7 @@
         <v>11</v>
       </c>
       <c r="F11" s="101" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="G11" s="107" t="s">
         <v>67</v>
@@ -5787,10 +5790,10 @@
         <v>100</v>
       </c>
       <c r="I11" s="97" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="J11" s="98" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="K11" s="107"/>
       <c r="L11" s="25"/>
@@ -5815,7 +5818,7 @@
       <c r="W11" s="15"/>
       <c r="X11" s="13"/>
     </row>
-    <row r="12" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" ht="15" customHeight="1">
       <c r="A12" s="75">
         <v>45995</v>
       </c>
@@ -5835,19 +5838,19 @@
         <v>13</v>
       </c>
       <c r="F12" s="101" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="G12" s="107" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="H12" s="25" t="s">
         <v>100</v>
       </c>
       <c r="I12" s="97" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="J12" s="132" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="K12" s="157"/>
       <c r="L12" s="25"/>
@@ -5874,35 +5877,35 @@
       <c r="W12" s="15"/>
       <c r="X12" s="13"/>
     </row>
-    <row r="13" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" ht="15" customHeight="1">
       <c r="A13" s="26"/>
       <c r="B13" s="26"/>
       <c r="C13" s="26"/>
       <c r="W13" s="20"/>
       <c r="X13" s="18"/>
     </row>
-    <row r="14" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" ht="15" customHeight="1">
       <c r="A14" s="26"/>
       <c r="B14" s="26"/>
       <c r="C14" s="26"/>
     </row>
-    <row r="15" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" ht="15" customHeight="1">
       <c r="A15" s="26"/>
       <c r="B15" s="26"/>
       <c r="C15" s="26"/>
     </row>
-    <row r="16" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" ht="15" customHeight="1">
       <c r="A16" s="26"/>
       <c r="B16" s="26"/>
       <c r="C16" s="26"/>
     </row>
-    <row r="17" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="15" customHeight="1"/>
+    <row r="18" ht="15" customHeight="1"/>
+    <row r="19" ht="15" customHeight="1"/>
+    <row r="20" ht="15" customHeight="1"/>
+    <row r="21" ht="15" customHeight="1"/>
+    <row r="22" ht="15" customHeight="1"/>
+    <row r="23" ht="15" customHeight="1"/>
   </sheetData>
   <protectedRanges>
     <protectedRange algorithmName="SHA-512" hashValue="pQyTzP/d7t5ThMimBt5mu8gGozgAm1OwF6BMILsn5/kmtZ5mZf81NMi09wwU8mvtItxf0EVNWa6V4MCa0DKeSQ==" saltValue="NzZBiAQ1yFjat+SeIqh2Uw==" spinCount="100000" sqref="A3:E16" name="Range3_1"/>
@@ -5931,7 +5934,7 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.5703125" customWidth="1"/>
     <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1"/>
@@ -5958,7 +5961,7 @@
     <col min="24" max="24" width="37.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" ht="15.75" thickBot="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5969,7 +5972,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" ht="30.75" thickBot="1">
       <c r="A2" s="64" t="s">
         <v>3</v>
       </c>
@@ -6043,7 +6046,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" ht="15" customHeight="1">
       <c r="A3" s="75">
         <v>46051</v>
       </c>
@@ -6062,19 +6065,19 @@
         <v>1</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>280</v>
+        <v>306</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>280</v>
+        <v>306</v>
       </c>
       <c r="I3" s="98" t="s">
-        <v>280</v>
+        <v>306</v>
       </c>
       <c r="J3" s="98" t="s">
-        <v>280</v>
+        <v>306</v>
       </c>
       <c r="K3" s="73"/>
       <c r="L3" s="40"/>
@@ -6095,7 +6098,7 @@
       <c r="W3" s="46"/>
       <c r="X3" s="44"/>
     </row>
-    <row r="4" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" ht="15.75" customHeight="1">
       <c r="A4" s="75">
         <f>A3+14</f>
         <v>46065</v>
@@ -6116,19 +6119,19 @@
         <v>3</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>280</v>
+        <v>306</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>280</v>
+        <v>306</v>
       </c>
       <c r="I4" s="98" t="s">
-        <v>280</v>
+        <v>306</v>
       </c>
       <c r="J4" s="98" t="s">
-        <v>280</v>
+        <v>306</v>
       </c>
       <c r="K4" s="102"/>
       <c r="L4" s="5"/>
@@ -6147,7 +6150,7 @@
       <c r="W4" s="15"/>
       <c r="X4" s="13"/>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24">
       <c r="A5" s="75">
         <f t="shared" ref="A5:A9" si="2">A4+14</f>
         <v>46079</v>
@@ -6168,19 +6171,19 @@
         <v>5</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>280</v>
+        <v>306</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>280</v>
+        <v>306</v>
       </c>
       <c r="I5" s="98" t="s">
-        <v>280</v>
+        <v>306</v>
       </c>
       <c r="J5" s="98" t="s">
-        <v>280</v>
+        <v>306</v>
       </c>
       <c r="K5" s="102"/>
       <c r="L5" s="5"/>
@@ -6199,7 +6202,7 @@
       <c r="W5" s="15"/>
       <c r="X5" s="13"/>
     </row>
-    <row r="6" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" ht="15.75" customHeight="1">
       <c r="A6" s="75">
         <f>A5+14</f>
         <v>46093</v>
@@ -6220,7 +6223,7 @@
         <v>7</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="G6" s="14" t="s">
         <v>151</v>
@@ -6229,10 +6232,10 @@
         <v>94</v>
       </c>
       <c r="I6" s="98" t="s">
-        <v>280</v>
+        <v>306</v>
       </c>
       <c r="J6" s="98" t="s">
-        <v>280</v>
+        <v>306</v>
       </c>
       <c r="K6" s="102"/>
       <c r="L6" s="5"/>
@@ -6251,7 +6254,7 @@
       <c r="W6" s="15"/>
       <c r="X6" s="13"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24">
       <c r="A7" s="75">
         <f t="shared" si="2"/>
         <v>46107</v>
@@ -6272,19 +6275,19 @@
         <v>9</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>280</v>
+        <v>306</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>280</v>
+        <v>306</v>
       </c>
       <c r="I7" s="98" t="s">
-        <v>280</v>
+        <v>306</v>
       </c>
       <c r="J7" s="98" t="s">
-        <v>280</v>
+        <v>306</v>
       </c>
       <c r="K7" s="102"/>
       <c r="L7" s="5"/>
@@ -6303,7 +6306,7 @@
       <c r="W7" s="15"/>
       <c r="X7" s="13"/>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24">
       <c r="A8" s="75">
         <f t="shared" si="2"/>
         <v>46121</v>
@@ -6324,19 +6327,19 @@
         <v>11</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>280</v>
+        <v>306</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>280</v>
+        <v>306</v>
       </c>
       <c r="I8" s="98" t="s">
-        <v>280</v>
+        <v>306</v>
       </c>
       <c r="J8" s="98" t="s">
-        <v>280</v>
+        <v>306</v>
       </c>
       <c r="K8" s="102"/>
       <c r="L8" s="5"/>
@@ -6353,7 +6356,7 @@
       <c r="W8" s="15"/>
       <c r="X8" s="13"/>
     </row>
-    <row r="9" spans="1:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" ht="18.75" customHeight="1">
       <c r="A9" s="75">
         <f t="shared" si="2"/>
         <v>46135</v>
@@ -6374,19 +6377,19 @@
         <v>13</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>280</v>
+        <v>306</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>280</v>
+        <v>306</v>
       </c>
       <c r="I9" s="98" t="s">
-        <v>280</v>
+        <v>306</v>
       </c>
       <c r="J9" s="98" t="s">
-        <v>280</v>
+        <v>306</v>
       </c>
       <c r="K9" s="102"/>
       <c r="L9" s="5"/>
@@ -6405,24 +6408,24 @@
       <c r="W9" s="15"/>
       <c r="X9" s="13"/>
     </row>
-    <row r="10" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" ht="15.75" thickBot="1">
       <c r="A10" s="26"/>
       <c r="B10" s="26"/>
       <c r="C10" s="26"/>
       <c r="W10" s="20"/>
       <c r="X10" s="18"/>
     </row>
-    <row r="11" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" ht="12.75" customHeight="1">
       <c r="A11" s="26"/>
       <c r="B11" s="26"/>
       <c r="C11" s="26"/>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24">
       <c r="A12" s="26"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24">
       <c r="A13" s="26"/>
       <c r="B13" s="26"/>
       <c r="C13" s="26"/>
@@ -6447,231 +6450,231 @@
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="31.28515625" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
     <col min="3" max="3" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="55" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="B2" s="54" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="C2" s="54" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="136" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="B3" s="137"/>
       <c r="C3" s="138" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="5" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="B4" s="52"/>
       <c r="C4" s="50" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" s="52" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="B5" s="52"/>
       <c r="C5" s="50" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="52" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="B6" s="52" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="C6" s="50" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" s="52" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="B7" s="52" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="C7" s="50" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" s="52" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="B8" s="52" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="C8" s="50" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" s="52" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="B9" s="52"/>
       <c r="C9" s="50"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" s="52" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="B10" s="52" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="C10" s="50" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" s="52" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="B11" s="52" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="C11" s="50" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" s="52" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="B12" s="52" t="s">
+        <v>330</v>
+      </c>
+      <c r="C12" s="50" t="s">
         <v>328</v>
       </c>
-      <c r="C12" s="50" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" s="52" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="B13" s="52" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="C13" s="50" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" s="52" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="B14" s="52" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="C14" s="50" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" s="52" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="B15" s="52" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="C15" s="50" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" s="137" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B16" s="137" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="C16" s="139" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" s="52" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="B17" s="52" t="s">
+        <v>340</v>
+      </c>
+      <c r="C17" s="50" t="s">
         <v>338</v>
       </c>
-      <c r="C17" s="50" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" s="52" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="B18" s="52" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="C18" s="50" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="A19" s="53" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="B19" s="53" t="s">
         <v>229</v>
       </c>
       <c r="C19" s="51" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>339</v>
-      </c>
       <c r="B24" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="C24" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="B25" t="s">
         <v>229</v>
       </c>
       <c r="C25" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
     </row>
   </sheetData>
@@ -6692,24 +6695,24 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
     <col min="6" max="6" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1">
       <c r="A1" s="135" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="131" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="C1" s="130" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" thickTop="1">
       <c r="A2" s="133">
         <v>45911</v>
       </c>
@@ -6717,7 +6720,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="134" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="F2" s="75">
         <v>45911</v>
@@ -6737,7 +6740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="133">
         <f>A2+7</f>
         <v>45918</v>
@@ -6747,7 +6750,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="134" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="F3" s="75">
         <v>45926</v>
@@ -6768,7 +6771,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="133">
         <f t="shared" ref="A4:A12" si="0">A3+7</f>
         <v>45925</v>
@@ -6778,7 +6781,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="134" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="F4" s="75">
         <v>45939</v>
@@ -6799,7 +6802,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="133">
         <f t="shared" si="0"/>
         <v>45932</v>
@@ -6809,7 +6812,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="134" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="F5" s="75">
         <v>45946</v>
@@ -6827,7 +6830,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="133">
         <f t="shared" si="0"/>
         <v>45939</v>
@@ -6837,7 +6840,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="134" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="F6" s="75">
         <v>45953</v>
@@ -6858,7 +6861,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" s="133">
         <f t="shared" si="0"/>
         <v>45946</v>
@@ -6868,7 +6871,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="134" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="F7" s="75">
         <v>45967</v>
@@ -6889,7 +6892,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" s="133">
         <f t="shared" si="0"/>
         <v>45953</v>
@@ -6899,7 +6902,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="134" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="F8" s="75">
         <v>45974</v>
@@ -6919,7 +6922,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9" s="133">
         <f t="shared" si="0"/>
         <v>45960</v>
@@ -6929,7 +6932,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="134" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="F9" s="75">
         <v>45981</v>
@@ -6950,7 +6953,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10" s="133">
         <f t="shared" si="0"/>
         <v>45967</v>
@@ -6960,7 +6963,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="134" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="F10" s="75">
         <v>45995</v>
@@ -6981,7 +6984,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" s="133">
         <f t="shared" si="0"/>
         <v>45974</v>
@@ -6991,10 +6994,10 @@
         <v>10</v>
       </c>
       <c r="C11" s="134" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="133">
         <f t="shared" si="0"/>
         <v>45981</v>
@@ -7004,10 +7007,10 @@
         <v>11</v>
       </c>
       <c r="C12" s="134" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" s="133">
         <f t="shared" ref="A13:A14" si="6">A12+7</f>
         <v>45988</v>
@@ -7017,10 +7020,10 @@
         <v>12</v>
       </c>
       <c r="C13" s="134" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" s="133">
         <f t="shared" si="6"/>
         <v>45995</v>
@@ -7030,15 +7033,15 @@
         <v>13</v>
       </c>
       <c r="C14" s="134" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" s="133"/>
       <c r="B15" s="134"/>
       <c r="C15" s="134"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="G16" s="26"/>
     </row>
   </sheetData>
@@ -7069,7 +7072,7 @@
       <selection activeCell="F8" sqref="F8:H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.42578125" customWidth="1"/>
     <col min="2" max="2" width="9.140625" customWidth="1"/>
@@ -7081,17 +7084,17 @@
     <col min="9" max="9" width="64.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="23.25">
       <c r="A2" s="91" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="18.75">
       <c r="A3" s="79" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="37.5" x14ac:dyDescent="0.25">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="37.5">
       <c r="A5" s="80" t="s">
         <v>3</v>
       </c>
@@ -7114,13 +7117,13 @@
         <v>9</v>
       </c>
       <c r="H5" s="82" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="I5" s="81" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="18.75">
       <c r="A6" s="92">
         <v>45694</v>
       </c>
@@ -7144,10 +7147,10 @@
       </c>
       <c r="H6" s="85"/>
       <c r="I6" s="84" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="18.75">
       <c r="A7" s="83">
         <v>45708</v>
       </c>
@@ -7176,7 +7179,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="18.75">
       <c r="A8" s="83">
         <v>45722</v>
       </c>
@@ -7203,7 +7206,7 @@
       </c>
       <c r="I8" s="86"/>
     </row>
-    <row r="9" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="18.75">
       <c r="A9" s="83">
         <v>45735</v>
       </c>
@@ -7214,7 +7217,7 @@
         <v>197</v>
       </c>
       <c r="D9" s="94" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="E9" s="94">
         <v>8</v>
@@ -7229,10 +7232,10 @@
         <v>205</v>
       </c>
       <c r="I9" s="86" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="18.75">
       <c r="A10" s="83">
         <v>45744</v>
       </c>
@@ -7259,7 +7262,7 @@
       </c>
       <c r="I10" s="86"/>
     </row>
-    <row r="11" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="18.75">
       <c r="A11" s="83">
         <v>45750</v>
       </c>
@@ -7276,17 +7279,17 @@
         <v>10</v>
       </c>
       <c r="F11" s="87" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="G11" s="87" t="s">
         <v>67</v>
       </c>
       <c r="H11" s="87"/>
       <c r="I11" s="86" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="18.75">
       <c r="A12" s="83">
         <v>45758</v>
       </c>
@@ -7312,10 +7315,10 @@
         <v>30</v>
       </c>
       <c r="I12" s="86" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="18.75">
       <c r="A13" s="83">
         <v>45764</v>
       </c>
@@ -7332,13 +7335,13 @@
         <v>12</v>
       </c>
       <c r="F13" s="87" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="G13" s="87"/>
       <c r="H13" s="87"/>
       <c r="I13" s="86"/>
     </row>
-    <row r="14" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="18.75">
       <c r="A14" s="88">
         <v>45771</v>
       </c>
@@ -7355,7 +7358,7 @@
         <v>13</v>
       </c>
       <c r="F14" s="90" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="G14" s="90" t="s">
         <v>76</v>
@@ -7367,7 +7370,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="20" spans="8:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="20" spans="8:8" ht="18.75">
       <c r="H20" s="79"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DOK speaker AY25-26 sem2
</commit_message>
<xml_diff>
--- a/data/MACSI seminar series.xlsx
+++ b/data/MACSI seminar series.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ulcampus-my.sharepoint.com/personal/david_osullivan_ul_ie/Documents/Academic_work/_Misc/MACSI_Seminars/macsi-seminars.github.io/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="88" documentId="13_ncr:1_{12BE53B5-C8C7-44FE-8280-19C653D9122E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{01B6E111-3255-4725-96AA-55590E349AE4}"/>
+  <xr:revisionPtr revIDLastSave="91" documentId="13_ncr:1_{12BE53B5-C8C7-44FE-8280-19C653D9122E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C1CE96E5-5729-4F1A-8515-221E4968858F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AY2023-2024 Sem 2" sheetId="3" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="379">
   <si>
     <t>Fill in as much of the green boxes as possible. Ideally, this would be before you have finished your visitors travel dates (just to avoid double booking).</t>
   </si>
@@ -1072,10 +1072,16 @@
     <t>https://www.tcd.ie/scss/people/academic-staff/dangelos/ ; https://sites.google.com/view/silviadangelo/home</t>
   </si>
   <si>
+    <t>Eoin O’Brien</t>
+  </si>
+  <si>
+    <t>Maynooth University</t>
+  </si>
+  <si>
+    <t>TBC</t>
+  </si>
+  <si>
     <t>Open</t>
-  </si>
-  <si>
-    <t>TBC</t>
   </si>
   <si>
     <t>Philip Pearce</t>
@@ -5298,7 +5304,7 @@
   </sheetPr>
   <dimension ref="A1:Y25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="7" ySplit="18" topLeftCell="H27" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="I31" sqref="I31"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
@@ -6181,8 +6187,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F62D4156-0A06-4DBF-B1E7-3E12580121CB}">
   <dimension ref="A1:Y13"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6325,13 +6331,13 @@
         <v>323</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>323</v>
+        <v>87</v>
       </c>
       <c r="I3" s="98" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="J3" s="98" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="K3" s="73"/>
       <c r="L3" s="40"/>
@@ -6370,19 +6376,19 @@
         <v>3</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="I4" s="98" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="J4" s="98" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="K4" s="102"/>
       <c r="L4" s="5"/>
@@ -6421,29 +6427,29 @@
         <v>5</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>87</v>
       </c>
       <c r="I5" s="98" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="J5" s="98" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="K5" s="102"/>
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
       <c r="N5" s="16"/>
       <c r="O5" s="35" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="P5" s="5" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="Q5" s="5"/>
       <c r="R5" s="5"/>
@@ -6476,7 +6482,7 @@
         <v>7</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="G6" s="14" t="s">
         <v>152</v>
@@ -6485,10 +6491,10 @@
         <v>95</v>
       </c>
       <c r="I6" s="98" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="J6" s="98" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="K6" s="102"/>
       <c r="L6" s="5"/>
@@ -6527,19 +6533,19 @@
         <v>9</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="I7" s="98" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="J7" s="98" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="K7" s="102"/>
       <c r="L7" s="5"/>
@@ -6578,19 +6584,19 @@
         <v>11</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="I8" s="98" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="J8" s="98" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="K8" s="102"/>
       <c r="L8" s="5"/>
@@ -6629,19 +6635,19 @@
         <v>13</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="I9" s="98" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="J9" s="98" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="K9" s="102"/>
       <c r="L9" s="5"/>
@@ -6711,23 +6717,23 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="55" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="B2" s="54" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="C2" s="54" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="136" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="B3" s="137"/>
       <c r="C3" s="138" t="s">
@@ -6736,7 +6742,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="5" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="B4" s="52"/>
       <c r="C4" s="50" t="s">
@@ -6745,19 +6751,19 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="52" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="B5" s="52"/>
       <c r="C5" s="50" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="52" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="B6" s="52" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="C6" s="50" t="s">
         <v>87</v>
@@ -6765,10 +6771,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="52" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="B7" s="52" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="C7" s="50" t="s">
         <v>87</v>
@@ -6776,10 +6782,10 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="52" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="B8" s="52" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="C8" s="50" t="s">
         <v>101</v>
@@ -6787,75 +6793,75 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="52" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="B9" s="52"/>
       <c r="C9" s="50"/>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="52" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="B10" s="52" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="C10" s="50" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="52" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="B11" s="52" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="C11" s="50" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="52" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="B12" s="52" t="s">
+        <v>353</v>
+      </c>
+      <c r="C12" s="50" t="s">
         <v>351</v>
-      </c>
-      <c r="C12" s="50" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="52" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="B13" s="52" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="C13" s="50" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="52" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="B14" s="52" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="C14" s="50" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="52" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="B15" s="52" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="C15" s="50" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -6863,29 +6869,29 @@
         <v>316</v>
       </c>
       <c r="B16" s="137" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="C16" s="139" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="52" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="B17" s="52" t="s">
+        <v>363</v>
+      </c>
+      <c r="C17" s="50" t="s">
         <v>361</v>
-      </c>
-      <c r="C17" s="50" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="52" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="B18" s="52" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="C18" s="50" t="s">
         <v>87</v>
@@ -6893,26 +6899,26 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="53" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="B19" s="53" t="s">
         <v>230</v>
       </c>
       <c r="C19" s="51" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="B24" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="C24" t="s">
         <v>87</v>
@@ -6920,13 +6926,13 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="B25" t="s">
         <v>230</v>
       </c>
       <c r="C25" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
     </row>
   </sheetData>
@@ -6958,10 +6964,10 @@
         <v>3</v>
       </c>
       <c r="B1" s="131" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="C1" s="130" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickTop="1">
@@ -6972,7 +6978,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="134" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="F2" s="75">
         <v>45911</v>
@@ -7002,7 +7008,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="134" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="F3" s="75">
         <v>45926</v>
@@ -7033,7 +7039,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="134" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="F4" s="75">
         <v>45939</v>
@@ -7064,7 +7070,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="134" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="F5" s="75">
         <v>45946</v>
@@ -7092,7 +7098,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="134" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="F6" s="75">
         <v>45953</v>
@@ -7123,7 +7129,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="134" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="F7" s="75">
         <v>45967</v>
@@ -7154,7 +7160,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="134" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="F8" s="75">
         <v>45974</v>
@@ -7184,7 +7190,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="134" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="F9" s="75">
         <v>45981</v>
@@ -7215,7 +7221,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="134" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="F10" s="75">
         <v>45995</v>
@@ -7246,7 +7252,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="134" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -7259,7 +7265,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="134" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -7272,7 +7278,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="134" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -7285,7 +7291,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="134" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -7338,12 +7344,12 @@
   <sheetData>
     <row r="2" spans="1:9" ht="23.25">
       <c r="A2" s="91" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="18.75">
       <c r="A3" s="79" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="37.5">
@@ -7369,7 +7375,7 @@
         <v>9</v>
       </c>
       <c r="H5" s="82" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="I5" s="81" t="s">
         <v>11</v>
@@ -7399,7 +7405,7 @@
       </c>
       <c r="H6" s="85"/>
       <c r="I6" s="84" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="18.75">
@@ -7469,7 +7475,7 @@
         <v>198</v>
       </c>
       <c r="D9" s="94" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="E9" s="94">
         <v>8</v>
@@ -7484,7 +7490,7 @@
         <v>206</v>
       </c>
       <c r="I9" s="86" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="18.75">
@@ -7531,14 +7537,14 @@
         <v>10</v>
       </c>
       <c r="F11" s="87" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="G11" s="87" t="s">
         <v>68</v>
       </c>
       <c r="H11" s="87"/>
       <c r="I11" s="86" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="18.75">
@@ -7567,7 +7573,7 @@
         <v>31</v>
       </c>
       <c r="I12" s="86" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="18.75">
@@ -7587,7 +7593,7 @@
         <v>12</v>
       </c>
       <c r="F13" s="87" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="G13" s="87"/>
       <c r="H13" s="87"/>
@@ -7610,7 +7616,7 @@
         <v>13</v>
       </c>
       <c r="F14" s="90" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="G14" s="90" t="s">
         <v>77</v>

</xml_diff>

<commit_message>
updated with DOK speaker
</commit_message>
<xml_diff>
--- a/data/MACSI seminar series.xlsx
+++ b/data/MACSI seminar series.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ulcampus-my.sharepoint.com/personal/david_osullivan_ul_ie/Documents/Academic_work/_Misc/MACSI_Seminars/macsi-seminars.github.io/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="91" documentId="13_ncr:1_{12BE53B5-C8C7-44FE-8280-19C653D9122E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C1CE96E5-5729-4F1A-8515-221E4968858F}"/>
+  <xr:revisionPtr revIDLastSave="109" documentId="13_ncr:1_{12BE53B5-C8C7-44FE-8280-19C653D9122E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{383F70AF-182B-4084-86F3-806EB002AE46}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AY2023-2024 Sem 2" sheetId="3" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="383">
   <si>
     <t>Fill in as much of the green boxes as possible. Ideally, this would be before you have finished your visitors travel dates (just to avoid double booking).</t>
   </si>
@@ -1006,241 +1006,255 @@
     <t>Hip Fractures Trends in Older Adults in Ireland</t>
   </si>
   <si>
+    <t>https://scholar.google.com/citations?user=dIpyVmAAAAAJ&amp;hl=en&amp;oi=ao</t>
+  </si>
+  <si>
+    <t>Nov</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>Christos Xenophontos</t>
+  </si>
+  <si>
+    <t>University of Cyprus</t>
+  </si>
+  <si>
+    <t>Neural Networks for singular perturbations</t>
+  </si>
+  <si>
+    <t>In this talk we will give an introduction to Neural Networks (NNs) and describe how they can be used for emulating the solution to singularly perturbed problems. In addition, we will present results on the expressivity rate bounds for solution sets of a model class of singularly perturbed, elliptic two-point boundary value problems, in Sobolev norms, on the bounded interval (-1,1). The expression rate bounds in Sobolev norms in terms of the NN size are robust, i.e. uniform with respect to the singular perturbation parameter for several classes of DNN architectures. In particular, ReLU NNs, tanh- and sigmoid-activated NNs. The latter activations can represent “exponential boundary layer solution features” explicitly, in the last hidden layer of the DNN, i.e. in a shallow subnetwork, and afford improved robust expression rate bounds in terms of the NN size.</t>
+  </si>
+  <si>
+    <t>Hugo Luiz Oliveira</t>
+  </si>
+  <si>
+    <t>University of Campinas (Unicamp), Brazil</t>
+  </si>
+  <si>
+    <t>Numerical and computational modelling of the Wheatley aortic valve</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recent studies have indicated an increase in cardiovascular diseases in developing countries, particularly valvular disorders caused by rheumatic fever, which are affecting younger populations. In severe cases, when the natural valve cannot be repaired, replacing it with a prosthetic valve may be the most effective way to ensure the patient's survival. Existing artificial valves have limitations, such as early deterioration and the risk of clot formation. To address these issues, the Wheatley Valve introduces an innovative S-shaped leaflet design that enhances the washout effect in the aortic root, thereby reducing the risk of thrombus formation and the need for extensive antiplatelet therapy. In this talk, we will discuss the main elements needed to build a fluid-structure interaction computational model able to represent the real behaviour of the Wheatley valve and which can be readily extended to other valve designs.
+</t>
+  </si>
+  <si>
+    <t>https://scholar.google.com/citations?user=nfeQtPQAAAAJ&amp;hl=pt-BR</t>
+  </si>
+  <si>
+    <t>Silvia D'Angelo</t>
+  </si>
+  <si>
+    <t>Trinity College Dublin</t>
+  </si>
+  <si>
+    <t>Clustering high-dimensional discrete data: a compressed approach</t>
+  </si>
+  <si>
+    <t>Custering high-dimensional data is a challenging task, typically addressed in the context of continuous numerical data. Recent literature is exploring strategies to cluster high-dimensional categorical and discrete data, which finds numerous applications, such as RNA sequencing and text data analysis. We propose a fast and easy-to-implement approach to cluster high-dimensional discrete data, scalable to datasets with thousands of dimensions where other strategies may be computationally unfeasible. Our approach relies on reducing the dimension of the data by performing a deterministic compression to a drastically lower dimension. The method employs a lossy compression that reduces the data to a collection of continuous features.
+We demonstrate that such compressed features can be treated as approximately normally distributed, allowing the application of standard finite Gaussian mixture models for model-based clustering. We discuss the approach and study its performance on a series of simulated scenarios with different dimensions and levels of complexity, involving both categorical and count data. Additionally, we illustrate the method on real-world data.</t>
+  </si>
+  <si>
+    <t>https://scholar.google.com/citations?user=d-Wde0EAAAAJ&amp;hl=en</t>
+  </si>
+  <si>
+    <t>https://www.tcd.ie/scss/people/academic-staff/dangelos/ ; https://sites.google.com/view/silviadangelo/home</t>
+  </si>
+  <si>
+    <t>Eoin O’Brien</t>
+  </si>
+  <si>
+    <t>Maynooth University</t>
+  </si>
+  <si>
+    <t>TBC</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>Philip Pearce</t>
+  </si>
+  <si>
+    <t>University College London</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>Email sent to Castltroy park hotel on 13 NOv 2025</t>
+  </si>
+  <si>
+    <t>Leah Keating</t>
+  </si>
+  <si>
+    <t>This is a just a place for those who are interested but that dont have a specific date in mind. (Ideally, a couple of these are people that we could invite with relatively short notice to fill missing slots.)</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Where are they from?</t>
+  </si>
+  <si>
+    <t>Adacemic Host</t>
+  </si>
+  <si>
+    <t>Colm</t>
+  </si>
+  <si>
+    <t>Niamh Cahill</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Niall Madden </t>
+  </si>
+  <si>
+    <t>Mehakpreet</t>
+  </si>
+  <si>
+    <t>Paul Weaver (invitation sent)</t>
+  </si>
+  <si>
+    <t>UL (Bernal)</t>
+  </si>
+  <si>
+    <t>Eleanor Doman</t>
+  </si>
+  <si>
+    <t>Manchester</t>
+  </si>
+  <si>
+    <t>Connor Hacket</t>
+  </si>
+  <si>
+    <t>MU</t>
+  </si>
+  <si>
+    <t>David Henry (?)</t>
+  </si>
+  <si>
+    <t>Jess Enright</t>
+  </si>
+  <si>
+    <t>Glasgow</t>
+  </si>
+  <si>
+    <t>JS/Networks</t>
+  </si>
+  <si>
+    <t>Ben Swallows</t>
+  </si>
+  <si>
+    <t>St Andrews</t>
+  </si>
+  <si>
+    <t>JS</t>
+  </si>
+  <si>
+    <t>Andrew Finlay</t>
+  </si>
+  <si>
+    <t>Uni Michigan</t>
+  </si>
+  <si>
+    <t>Denis Allard</t>
+  </si>
+  <si>
+    <t>INRAE</t>
+  </si>
+  <si>
+    <t>Nicholas J Clark</t>
+  </si>
+  <si>
+    <t>University of Queensland</t>
+  </si>
+  <si>
+    <t>Andrew Zammit Mangion</t>
+  </si>
+  <si>
+    <t>University of Wollongong</t>
+  </si>
+  <si>
+    <t>Trinity</t>
+  </si>
+  <si>
+    <t>DOS</t>
+  </si>
+  <si>
+    <t>Catherine Higgins</t>
+  </si>
+  <si>
+    <t>UCD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paul Weaver </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suzanne Fielding </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Doireann O'Kiely and Anthony </t>
+  </si>
+  <si>
+    <t>Possible speaker for next semester</t>
+  </si>
+  <si>
+    <t>Week</t>
+  </si>
+  <si>
+    <t>Speaker</t>
+  </si>
+  <si>
+    <t>Taken</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Taken </t>
+  </si>
+  <si>
+    <t>Seminar Series AY2024-25 Sem 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact david.osullivan@ul.ie &amp; mehakpreet.singh@ul.ie to book a speaker in. </t>
+  </si>
+  <si>
+    <t>Deptartmental contact</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>Robery Garvey</t>
+  </si>
+  <si>
+    <t>Tentative speaker</t>
+  </si>
+  <si>
+    <t>Leornard Henckel</t>
+  </si>
+  <si>
+    <t>12:30pm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shresh Jain </t>
+  </si>
+  <si>
+    <t>Investigating Material Nonlinearities in Coke Cans and Plastic Holey Columns</t>
+  </si>
+  <si>
+    <t>Most real-world buckling problems, from Coke cans to metamaterials, involve metals or other hard materials that deform plastically. Yet, many studies focus primarily on geometric nonlinearities, often neglecting the material nonlinearities that play a crucial role in determining post-buckling behaviour. In this talk, we examine two systems in which we incorporate these effects through semi-empirical modelling of material nonlinearities: hard holey columns and the sequential ring-buckling of fluid-filled Coke cans.
+By including material nonlinearities in our models, we show that intuitive, mechanics-based approaches can successfully capture the complex behaviour observed in the buckling of hard materials.</t>
+  </si>
+  <si>
     <t>European healthcare systems are under pressure from rapidly ageing populations, with hip fractures representing one of the most costly and impactful injuries among older adults (1,2). Ireland faces the dual challenge of both a rapidly growing ageing population and one of the highest European rates in hip fracture incidence (3,4). Irish standards require admission to orthopaedic care within four hours, yet national audits show this target is rarely achieved (5). Improving hip fracture services requires not just clinical reform but also new ways of leveraging data.
 In this talk, we show how publicly available datasets can be used to uncover correlations and trends in hip fracture demand. When combined with national audit records we show how population health interacts with environmental pressures. Our findings suggest that extreme weather is a strong national indicator of surges in hip fractures with some regions experiencing more pressure than others. This creates opportunities not only for predictive modelling and smarter resource allocation, but also for preventative strategies where timely information can be used to warn and protect at-risk groups.
 References
-1. Looi MK. The European healthcare workforce crisis: how bad is it? BMJ. 2024 Jan 19;384:q8. 
-2. EUROSTAT. Ageing Europe - statistics on population developments. Eurostat; 2020. Report No.: 80393. 
+1. Looi MK. The European healthcare workforce crisis: how bad is it? BMJ. 2024 Jan 19;384:q8.
+2. EUROSTAT. Ageing Europe - statistics on population developments. Eurostat; 2020. Report No.: 80393.
 3. CSO. Central Statistics Office (CSO). Central Statistics Office; 2022 [cited 2024 Sep 23]. Society Measuring Ireland’s Progress 2022 - Central Statistics Office. Available from: https://www.cso.ie/en/releasesandpublications/ep/p-mip/measuringirelandsprogress2022/society/
-4. Walsh ME, Ferris H, Coughlan T, Hurson C, Ahern E, Sorensen J, et al. Trends in hip fracture care in the Republic of Ireland from 2013 to 2018: results from the Irish Hip Fracture Database. Osteoporos Int. 2021 Apr 1;32(4):727–36. 
-5. Kelly P, Horan B, Murphy T, Ahern E, Brent L, Kelly F, et al. Irish Hip Fracture Database National Report 2022 [Internet]. National Office of Clinical Audit (NOCA); 2022 p. 1–88. Available from: https://d7g406zpx7bgk.cloudfront.net/38cf762d5b/irish_hip_fracture_database_national_report_2022_final.pdf</t>
-  </si>
-  <si>
-    <t>https://scholar.google.com/citations?user=dIpyVmAAAAAJ&amp;hl=en&amp;oi=ao</t>
-  </si>
-  <si>
-    <t>Nov</t>
-  </si>
-  <si>
-    <t>Tuesday</t>
-  </si>
-  <si>
-    <t>Christos Xenophontos</t>
-  </si>
-  <si>
-    <t>University of Cyprus</t>
-  </si>
-  <si>
-    <t>Neural Networks for singular perturbations</t>
-  </si>
-  <si>
-    <t>In this talk we will give an introduction to Neural Networks (NNs) and describe how they can be used for emulating the solution to singularly perturbed problems. In addition, we will present results on the expressivity rate bounds for solution sets of a model class of singularly perturbed, elliptic two-point boundary value problems, in Sobolev norms, on the bounded interval (-1,1). The expression rate bounds in Sobolev norms in terms of the NN size are robust, i.e. uniform with respect to the singular perturbation parameter for several classes of DNN architectures. In particular, ReLU NNs, tanh- and sigmoid-activated NNs. The latter activations can represent “exponential boundary layer solution features” explicitly, in the last hidden layer of the DNN, i.e. in a shallow subnetwork, and afford improved robust expression rate bounds in terms of the NN size.</t>
-  </si>
-  <si>
-    <t>Hugo Luiz Oliveira</t>
-  </si>
-  <si>
-    <t>University of Campinas (Unicamp), Brazil</t>
-  </si>
-  <si>
-    <t>Numerical and computational modelling of the Wheatley aortic valve</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Recent studies have indicated an increase in cardiovascular diseases in developing countries, particularly valvular disorders caused by rheumatic fever, which are affecting younger populations. In severe cases, when the natural valve cannot be repaired, replacing it with a prosthetic valve may be the most effective way to ensure the patient's survival. Existing artificial valves have limitations, such as early deterioration and the risk of clot formation. To address these issues, the Wheatley Valve introduces an innovative S-shaped leaflet design that enhances the washout effect in the aortic root, thereby reducing the risk of thrombus formation and the need for extensive antiplatelet therapy. In this talk, we will discuss the main elements needed to build a fluid-structure interaction computational model able to represent the real behaviour of the Wheatley valve and which can be readily extended to other valve designs.
-</t>
-  </si>
-  <si>
-    <t>https://scholar.google.com/citations?user=nfeQtPQAAAAJ&amp;hl=pt-BR</t>
-  </si>
-  <si>
-    <t>Silvia D'Angelo</t>
-  </si>
-  <si>
-    <t>Trinity College Dublin</t>
-  </si>
-  <si>
-    <t>Clustering high-dimensional discrete data: a compressed approach</t>
-  </si>
-  <si>
-    <t>Custering high-dimensional data is a challenging task, typically addressed in the context of continuous numerical data. Recent literature is exploring strategies to cluster high-dimensional categorical and discrete data, which finds numerous applications, such as RNA sequencing and text data analysis. We propose a fast and easy-to-implement approach to cluster high-dimensional discrete data, scalable to datasets with thousands of dimensions where other strategies may be computationally unfeasible. Our approach relies on reducing the dimension of the data by performing a deterministic compression to a drastically lower dimension. The method employs a lossy compression that reduces the data to a collection of continuous features.
-We demonstrate that such compressed features can be treated as approximately normally distributed, allowing the application of standard finite Gaussian mixture models for model-based clustering. We discuss the approach and study its performance on a series of simulated scenarios with different dimensions and levels of complexity, involving both categorical and count data. Additionally, we illustrate the method on real-world data.</t>
-  </si>
-  <si>
-    <t>https://scholar.google.com/citations?user=d-Wde0EAAAAJ&amp;hl=en</t>
-  </si>
-  <si>
-    <t>https://www.tcd.ie/scss/people/academic-staff/dangelos/ ; https://sites.google.com/view/silviadangelo/home</t>
-  </si>
-  <si>
-    <t>Eoin O’Brien</t>
-  </si>
-  <si>
-    <t>Maynooth University</t>
-  </si>
-  <si>
-    <t>TBC</t>
-  </si>
-  <si>
-    <t>Open</t>
-  </si>
-  <si>
-    <t>Philip Pearce</t>
-  </si>
-  <si>
-    <t>University College London</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>Email sent to Castltroy park hotel on 13 NOv 2025</t>
-  </si>
-  <si>
-    <t>Leah Keating</t>
-  </si>
-  <si>
-    <t>This is a just a place for those who are interested but that dont have a specific date in mind. (Ideally, a couple of these are people that we could invite with relatively short notice to fill missing slots.)</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Where are they from?</t>
-  </si>
-  <si>
-    <t>Adacemic Host</t>
-  </si>
-  <si>
-    <t>Colm</t>
-  </si>
-  <si>
-    <t>Niamh Cahill</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Niall Madden </t>
-  </si>
-  <si>
-    <t>Mehakpreet</t>
-  </si>
-  <si>
-    <t>Paul Weaver (invitation sent)</t>
-  </si>
-  <si>
-    <t>UL (Bernal)</t>
-  </si>
-  <si>
-    <t>Eleanor Doman</t>
-  </si>
-  <si>
-    <t>Manchester</t>
-  </si>
-  <si>
-    <t>Connor Hacket</t>
-  </si>
-  <si>
-    <t>MU</t>
-  </si>
-  <si>
-    <t>David Henry (?)</t>
-  </si>
-  <si>
-    <t>Jess Enright</t>
-  </si>
-  <si>
-    <t>Glasgow</t>
-  </si>
-  <si>
-    <t>JS/Networks</t>
-  </si>
-  <si>
-    <t>Ben Swallows</t>
-  </si>
-  <si>
-    <t>St Andrews</t>
-  </si>
-  <si>
-    <t>JS</t>
-  </si>
-  <si>
-    <t>Andrew Finlay</t>
-  </si>
-  <si>
-    <t>Uni Michigan</t>
-  </si>
-  <si>
-    <t>Denis Allard</t>
-  </si>
-  <si>
-    <t>INRAE</t>
-  </si>
-  <si>
-    <t>Nicholas J Clark</t>
-  </si>
-  <si>
-    <t>University of Queensland</t>
-  </si>
-  <si>
-    <t>Andrew Zammit Mangion</t>
-  </si>
-  <si>
-    <t>University of Wollongong</t>
-  </si>
-  <si>
-    <t>Trinity</t>
-  </si>
-  <si>
-    <t>DOS</t>
-  </si>
-  <si>
-    <t>Catherine Higgins</t>
-  </si>
-  <si>
-    <t>UCD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paul Weaver </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Suzanne Fielding </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Doireann O'Kiely and Anthony </t>
-  </si>
-  <si>
-    <t>Possible speaker for next semester</t>
-  </si>
-  <si>
-    <t>Week</t>
-  </si>
-  <si>
-    <t>Speaker</t>
-  </si>
-  <si>
-    <t>Taken</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Taken </t>
-  </si>
-  <si>
-    <t>Seminar Series AY2024-25 Sem 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contact david.osullivan@ul.ie &amp; mehakpreet.singh@ul.ie to book a speaker in. </t>
-  </si>
-  <si>
-    <t>Deptartmental contact</t>
-  </si>
-  <si>
-    <t>Wednesday</t>
-  </si>
-  <si>
-    <t>Robery Garvey</t>
-  </si>
-  <si>
-    <t>Tentative speaker</t>
-  </si>
-  <si>
-    <t>Leornard Henckel</t>
+4. Walsh ME, Ferris H, Coughlan T, Hurson C, Ahern E, Sorensen J, et al. Trends in hip fracture care in the Republic of Ireland from 2013 to 2018: results from the Irish Hip Fracture Database. Osteoporos Int. 2021 Apr 1;32(4):727–36.
+5. Kelly P, Horan B, Murphy T, Ahern E, Brent L, Kelly F, et al. Irish Hip Fracture Database National Report 2022 [Internet]. National Office of Clinical Audit (NOCA); 2022 p. 1–88. Available from:
+https://d7g406zpx7bgk.cloudfront.net/38cf762d5b/irish_hip_fracture_database_national_report_2022_final.pdf</t>
   </si>
 </sst>
 </file>
@@ -1250,7 +1264,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1767,7 +1781,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="167">
+  <cellXfs count="169">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -2045,6 +2059,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2085,9 +2105,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2125,7 +2145,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2231,7 +2251,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2373,7 +2393,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2387,7 +2407,7 @@
       <selection activeCell="K1" sqref="K1:L1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="11.140625" customWidth="1"/>
@@ -2412,7 +2432,7 @@
     <col min="25" max="25" width="37.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2423,7 +2443,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="30.75">
+    <row r="2" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -2500,7 +2520,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="13.5" customHeight="1">
+    <row r="3" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>45317</v>
       </c>
@@ -2567,7 +2587,7 @@
       <c r="X3" s="13"/>
       <c r="Y3" s="13"/>
     </row>
-    <row r="4" spans="1:25" ht="13.5" customHeight="1">
+    <row r="4" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>45323</v>
       </c>
@@ -2630,7 +2650,7 @@
       <c r="X4" s="13"/>
       <c r="Y4" s="13"/>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>45324</v>
       </c>
@@ -2691,7 +2711,7 @@
       <c r="X5" s="13"/>
       <c r="Y5" s="13"/>
     </row>
-    <row r="6" spans="1:25" ht="12.75" customHeight="1">
+    <row r="6" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>45331</v>
       </c>
@@ -2758,7 +2778,7 @@
       <c r="X6" s="13"/>
       <c r="Y6" s="13"/>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>45338</v>
       </c>
@@ -2827,7 +2847,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="15" customHeight="1">
+    <row r="8" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>45345</v>
       </c>
@@ -2894,7 +2914,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="16.5" customHeight="1">
+    <row r="9" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>45359</v>
       </c>
@@ -2947,7 +2967,7 @@
       <c r="X9" s="13"/>
       <c r="Y9" s="13"/>
     </row>
-    <row r="10" spans="1:25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>45366</v>
       </c>
@@ -3016,7 +3036,7 @@
       <c r="X10" s="13"/>
       <c r="Y10" s="13"/>
     </row>
-    <row r="11" spans="1:25" ht="15" customHeight="1">
+    <row r="11" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>45379</v>
       </c>
@@ -3077,7 +3097,7 @@
       <c r="X11" s="13"/>
       <c r="Y11" s="13"/>
     </row>
-    <row r="12" spans="1:25" ht="13.5" customHeight="1">
+    <row r="12" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>45386</v>
       </c>
@@ -3140,7 +3160,7 @@
       <c r="X12" s="13"/>
       <c r="Y12" s="13"/>
     </row>
-    <row r="13" spans="1:25" ht="16.5" customHeight="1">
+    <row r="13" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>45387</v>
       </c>
@@ -3209,7 +3229,7 @@
       <c r="X13" s="13"/>
       <c r="Y13" s="13"/>
     </row>
-    <row r="14" spans="1:25" ht="15.75" customHeight="1">
+    <row r="14" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>45394</v>
       </c>
@@ -3270,7 +3290,7 @@
       <c r="X14" s="13"/>
       <c r="Y14" s="13"/>
     </row>
-    <row r="15" spans="1:25" ht="17.25" customHeight="1">
+    <row r="15" spans="1:25" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>45398</v>
       </c>
@@ -3339,7 +3359,7 @@
       <c r="X15" s="13"/>
       <c r="Y15" s="13"/>
     </row>
-    <row r="16" spans="1:25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>45401</v>
       </c>
@@ -3402,7 +3422,7 @@
       <c r="X16" s="18"/>
       <c r="Y16" s="18"/>
     </row>
-    <row r="17" spans="1:25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>45421</v>
       </c>
@@ -3473,7 +3493,7 @@
       <c r="X17" s="18"/>
       <c r="Y17" s="18"/>
     </row>
-    <row r="18" spans="1:25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" s="26">
         <v>45474</v>
       </c>
@@ -3524,7 +3544,7 @@
       <c r="X18" s="18"/>
       <c r="Y18" s="18"/>
     </row>
-    <row r="19" spans="1:25" ht="17.25" customHeight="1" thickBot="1">
+    <row r="19" spans="1:25" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="26">
         <v>45505</v>
       </c>
@@ -3575,7 +3595,7 @@
       <c r="X19" s="18"/>
       <c r="Y19" s="18"/>
     </row>
-    <row r="20" spans="1:25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" s="26"/>
       <c r="B20" s="26"/>
       <c r="C20" s="26"/>
@@ -3622,7 +3642,7 @@
       <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="11.140625" customWidth="1"/>
@@ -3647,7 +3667,7 @@
     <col min="25" max="25" width="37.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3658,7 +3678,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="30.75" thickBot="1">
+    <row r="2" spans="1:25" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="145" t="s">
         <v>3</v>
       </c>
@@ -3735,7 +3755,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="15" customHeight="1">
+    <row r="3" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>45548</v>
       </c>
@@ -3800,7 +3820,7 @@
       <c r="X3" s="46"/>
       <c r="Y3" s="44"/>
     </row>
-    <row r="4" spans="1:25" ht="15" customHeight="1">
+    <row r="4" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>45555</v>
       </c>
@@ -3849,7 +3869,7 @@
       <c r="X4" s="15"/>
       <c r="Y4" s="13"/>
     </row>
-    <row r="5" spans="1:25" ht="15" customHeight="1">
+    <row r="5" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>45562</v>
       </c>
@@ -3898,7 +3918,7 @@
       <c r="X5" s="15"/>
       <c r="Y5" s="13"/>
     </row>
-    <row r="6" spans="1:25" ht="15" customHeight="1">
+    <row r="6" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>45576</v>
       </c>
@@ -3947,7 +3967,7 @@
       <c r="X6" s="15"/>
       <c r="Y6" s="13"/>
     </row>
-    <row r="7" spans="1:25" ht="15" customHeight="1">
+    <row r="7" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>45583</v>
       </c>
@@ -3996,7 +4016,7 @@
       <c r="X7" s="15"/>
       <c r="Y7" s="13"/>
     </row>
-    <row r="8" spans="1:25" ht="15" customHeight="1">
+    <row r="8" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>45596</v>
       </c>
@@ -4045,7 +4065,7 @@
       <c r="X8" s="15"/>
       <c r="Y8" s="13"/>
     </row>
-    <row r="9" spans="1:25" ht="15" customHeight="1">
+    <row r="9" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>45604</v>
       </c>
@@ -4094,7 +4114,7 @@
       <c r="X9" s="15"/>
       <c r="Y9" s="13"/>
     </row>
-    <row r="10" spans="1:25" ht="15" customHeight="1">
+    <row r="10" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>45611</v>
       </c>
@@ -4143,7 +4163,7 @@
       <c r="X10" s="15"/>
       <c r="Y10" s="13"/>
     </row>
-    <row r="11" spans="1:25" ht="15" customHeight="1">
+    <row r="11" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>45625</v>
       </c>
@@ -4192,7 +4212,7 @@
       <c r="X11" s="15"/>
       <c r="Y11" s="13"/>
     </row>
-    <row r="12" spans="1:25" ht="15" customHeight="1" thickBot="1">
+    <row r="12" spans="1:25" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>45632</v>
       </c>
@@ -4249,20 +4269,20 @@
       <c r="X12" s="20"/>
       <c r="Y12" s="18"/>
     </row>
-    <row r="13" spans="1:25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="26"/>
       <c r="B13" s="26"/>
       <c r="C13" s="26"/>
       <c r="D13" s="26"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="26"/>
       <c r="B14" s="26"/>
       <c r="C14" s="26"/>
       <c r="D14" s="26"/>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="61"/>
       <c r="B29" s="61"/>
       <c r="C29" s="61"/>
@@ -4274,59 +4294,59 @@
       <c r="I29" s="61"/>
       <c r="J29" s="61"/>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="60"/>
       <c r="B31" s="60"/>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="60"/>
       <c r="B32" s="60"/>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="60"/>
       <c r="B33" s="60"/>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="60"/>
       <c r="B34" s="60"/>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="60"/>
       <c r="B35" s="60"/>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="60"/>
       <c r="B36" s="60"/>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="60"/>
       <c r="B37" s="60"/>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="60"/>
       <c r="B38" s="60"/>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="60"/>
       <c r="B39" s="60"/>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="60"/>
       <c r="B40" s="60"/>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="60"/>
       <c r="B41" s="60"/>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="60"/>
       <c r="B42" s="60"/>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="60"/>
       <c r="B43" s="60"/>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="60"/>
       <c r="B44" s="60"/>
     </row>
@@ -4360,7 +4380,7 @@
       <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" customWidth="1"/>
     <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1"/>
@@ -4388,7 +4408,7 @@
     <col min="25" max="25" width="37.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4399,7 +4419,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="27.75" customHeight="1" thickBot="1">
+    <row r="2" spans="1:25" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="64" t="s">
         <v>3</v>
       </c>
@@ -4476,7 +4496,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="15" customHeight="1">
+    <row r="3" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>45694</v>
       </c>
@@ -4528,7 +4548,7 @@
       <c r="X3" s="46"/>
       <c r="Y3" s="44"/>
     </row>
-    <row r="4" spans="1:25" ht="14.25" customHeight="1">
+    <row r="4" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>45708</v>
       </c>
@@ -4586,7 +4606,7 @@
       <c r="X4" s="15"/>
       <c r="Y4" s="13"/>
     </row>
-    <row r="5" spans="1:25" ht="14.25" customHeight="1">
+    <row r="5" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>45722</v>
       </c>
@@ -4642,7 +4662,7 @@
       <c r="X5" s="15"/>
       <c r="Y5" s="13"/>
     </row>
-    <row r="6" spans="1:25" ht="16.5" customHeight="1">
+    <row r="6" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>45735</v>
       </c>
@@ -4698,7 +4718,7 @@
       <c r="X6" s="15"/>
       <c r="Y6" s="13"/>
     </row>
-    <row r="7" spans="1:25" ht="18" customHeight="1">
+    <row r="7" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>45750</v>
       </c>
@@ -4752,7 +4772,7 @@
       <c r="X7" s="15"/>
       <c r="Y7" s="13"/>
     </row>
-    <row r="8" spans="1:25" ht="16.5" customHeight="1">
+    <row r="8" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>45751</v>
       </c>
@@ -4811,7 +4831,7 @@
       <c r="X8" s="15"/>
       <c r="Y8" s="13"/>
     </row>
-    <row r="9" spans="1:25" ht="15.75" customHeight="1">
+    <row r="9" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>45757</v>
       </c>
@@ -4873,7 +4893,7 @@
       <c r="X9" s="15"/>
       <c r="Y9" s="13"/>
     </row>
-    <row r="10" spans="1:25" ht="15.75" customHeight="1">
+    <row r="10" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>45758</v>
       </c>
@@ -4927,7 +4947,7 @@
       <c r="X10" s="20"/>
       <c r="Y10" s="18"/>
     </row>
-    <row r="11" spans="1:25" ht="15.75" customHeight="1">
+    <row r="11" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>45764</v>
       </c>
@@ -4987,7 +5007,7 @@
       <c r="X11" s="35"/>
       <c r="Y11" s="35"/>
     </row>
-    <row r="12" spans="1:25" ht="15.75" customHeight="1">
+    <row r="12" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>45771</v>
       </c>
@@ -5048,7 +5068,7 @@
       <c r="X12" s="35"/>
       <c r="Y12" s="35"/>
     </row>
-    <row r="13" spans="1:25" ht="15.75" customHeight="1">
+    <row r="13" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>45785</v>
       </c>
@@ -5101,7 +5121,7 @@
       <c r="X13" s="35"/>
       <c r="Y13" s="35"/>
     </row>
-    <row r="14" spans="1:25" ht="15.75" customHeight="1">
+    <row r="14" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>45799</v>
       </c>
@@ -5147,7 +5167,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="15.75" customHeight="1">
+    <row r="15" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>45805</v>
       </c>
@@ -5181,101 +5201,101 @@
         <v>250</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="15.75" customHeight="1">
+    <row r="16" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="75"/>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="26"/>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="26"/>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="26"/>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="75"/>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="26"/>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="75"/>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="26"/>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="26"/>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="26"/>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="26"/>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="26"/>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="26"/>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B31" s="60"/>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="60"/>
       <c r="B32" s="60"/>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="60"/>
       <c r="B33" s="60"/>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="60"/>
       <c r="B34" s="60"/>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="60"/>
       <c r="B35" s="60"/>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="60"/>
       <c r="B36" s="60"/>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="60"/>
       <c r="B37" s="60"/>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="60"/>
       <c r="B38" s="60"/>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="60"/>
       <c r="B39" s="60"/>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="60"/>
       <c r="B40" s="60"/>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="60"/>
       <c r="B41" s="60"/>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="60"/>
       <c r="B42" s="60"/>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="60"/>
       <c r="B43" s="60"/>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="60"/>
       <c r="B44" s="60"/>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="60"/>
     </row>
   </sheetData>
@@ -5302,16 +5322,16 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:Y25"/>
+  <dimension ref="A1:Y26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="7" ySplit="18" topLeftCell="H27" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="I31" sqref="I31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="7" ySplit="19" topLeftCell="H20" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="topRight" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomRight" activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" customWidth="1"/>
@@ -5338,7 +5358,7 @@
     <col min="25" max="25" width="37.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5349,7 +5369,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="30.75">
+    <row r="2" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="78" t="s">
         <v>3</v>
       </c>
@@ -5426,7 +5446,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="15" customHeight="1" thickBot="1">
+    <row r="3" spans="1:25" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="159">
         <v>45911</v>
       </c>
@@ -5489,7 +5509,7 @@
       <c r="X3" s="46"/>
       <c r="Y3" s="44"/>
     </row>
-    <row r="4" spans="1:25" ht="15" customHeight="1">
+    <row r="4" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="160">
         <v>45917</v>
       </c>
@@ -5558,7 +5578,7 @@
       <c r="X4" s="15"/>
       <c r="Y4" s="13"/>
     </row>
-    <row r="5" spans="1:25" ht="15" customHeight="1">
+    <row r="5" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="160">
         <v>45926</v>
       </c>
@@ -5616,7 +5636,7 @@
       <c r="X5" s="15"/>
       <c r="Y5" s="13"/>
     </row>
-    <row r="6" spans="1:25" ht="15" customHeight="1">
+    <row r="6" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="160">
         <v>45939</v>
       </c>
@@ -5680,7 +5700,7 @@
       <c r="X6" s="15"/>
       <c r="Y6" s="13"/>
     </row>
-    <row r="7" spans="1:25" ht="15" customHeight="1">
+    <row r="7" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="160">
         <v>45946</v>
       </c>
@@ -5737,7 +5757,7 @@
       <c r="X7" s="15"/>
       <c r="Y7" s="13"/>
     </row>
-    <row r="8" spans="1:25" ht="15" customHeight="1">
+    <row r="8" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="160">
         <v>45953</v>
       </c>
@@ -5745,11 +5765,11 @@
         <v>190</v>
       </c>
       <c r="C8" s="160" t="str">
-        <f t="shared" ref="C8:C11" si="2">TEXT(A8, "mmm")</f>
+        <f t="shared" ref="C8:C12" si="2">TEXT(A8, "mmm")</f>
         <v>Oct</v>
       </c>
       <c r="D8" s="103" t="str">
-        <f t="shared" ref="D8:D11" si="3">TEXT(A8, "dddd")</f>
+        <f t="shared" ref="D8:D12" si="3">TEXT(A8, "dddd")</f>
         <v>Thursday</v>
       </c>
       <c r="E8" s="103">
@@ -5795,7 +5815,7 @@
       <c r="X8" s="15"/>
       <c r="Y8" s="13"/>
     </row>
-    <row r="9" spans="1:25" ht="15" customHeight="1">
+    <row r="9" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="160">
         <v>45967</v>
       </c>
@@ -5857,7 +5877,7 @@
       <c r="X9" s="15"/>
       <c r="Y9" s="13"/>
     </row>
-    <row r="10" spans="1:25" ht="15" customHeight="1">
+    <row r="10" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="160">
         <v>45974</v>
       </c>
@@ -5920,191 +5940,182 @@
       <c r="X10" s="15"/>
       <c r="Y10" s="13"/>
     </row>
-    <row r="11" spans="1:25">
+    <row r="11" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="160">
+        <v>45980</v>
+      </c>
+      <c r="B11" s="160" t="s">
+        <v>378</v>
+      </c>
+      <c r="C11" s="160" t="str">
+        <f t="shared" si="2"/>
+        <v>Nov</v>
+      </c>
+      <c r="D11" s="103" t="str">
+        <f t="shared" si="3"/>
+        <v>Wednesday</v>
+      </c>
+      <c r="E11" s="103">
+        <v>11</v>
+      </c>
+      <c r="F11" s="107" t="s">
+        <v>379</v>
+      </c>
+      <c r="G11" s="107" t="s">
+        <v>269</v>
+      </c>
+      <c r="H11" s="107" t="s">
+        <v>87</v>
+      </c>
+      <c r="I11" s="167" t="s">
+        <v>380</v>
+      </c>
+      <c r="J11" s="167" t="s">
+        <v>381</v>
+      </c>
+      <c r="K11" s="157"/>
+      <c r="L11" s="156"/>
+      <c r="M11" s="156"/>
+      <c r="N11" s="14"/>
+      <c r="O11" s="35"/>
+      <c r="P11" s="14"/>
+      <c r="Q11" s="14"/>
+      <c r="R11" s="14"/>
+      <c r="S11" s="14"/>
+      <c r="T11" s="35"/>
+      <c r="U11" s="14"/>
+      <c r="V11" s="14"/>
+      <c r="W11" s="14"/>
+      <c r="X11" s="35"/>
+      <c r="Y11" s="35"/>
+    </row>
+    <row r="12" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="160">
         <f>A10+7</f>
         <v>45981</v>
       </c>
-      <c r="B11" s="103" t="s">
+      <c r="B12" s="103" t="s">
         <v>190</v>
       </c>
-      <c r="C11" s="103" t="str">
+      <c r="C12" s="103" t="str">
         <f t="shared" si="2"/>
         <v>Nov</v>
       </c>
-      <c r="D11" s="103" t="str">
+      <c r="D12" s="103" t="str">
         <f t="shared" si="3"/>
         <v>Thursday</v>
       </c>
-      <c r="E11" s="103">
+      <c r="E12" s="103">
         <f>E9+2</f>
         <v>11</v>
       </c>
-      <c r="F11" s="158" t="s">
+      <c r="F12" s="158" t="s">
         <v>301</v>
       </c>
-      <c r="G11" s="158" t="s">
+      <c r="G12" s="158" t="s">
         <v>68</v>
       </c>
-      <c r="H11" s="158" t="s">
+      <c r="H12" s="158" t="s">
         <v>101</v>
       </c>
-      <c r="I11" s="158" t="s">
+      <c r="I12" s="158" t="s">
         <v>302</v>
       </c>
-      <c r="J11" s="158" t="s">
+      <c r="J12" s="168" t="s">
+        <v>382</v>
+      </c>
+      <c r="K12" s="165" t="s">
         <v>303</v>
       </c>
-      <c r="K11" s="165" t="s">
-        <v>304</v>
-      </c>
-      <c r="L11" s="158"/>
-      <c r="M11" s="158"/>
-      <c r="N11" s="158" t="s">
-        <v>35</v>
-      </c>
-      <c r="P11" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>258</v>
-      </c>
-      <c r="U11" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25">
-      <c r="A12" s="160">
-        <v>45986</v>
-      </c>
-      <c r="B12" s="166" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="103" t="s">
-        <v>305</v>
-      </c>
-      <c r="D12" s="103" t="s">
-        <v>306</v>
-      </c>
-      <c r="E12" s="103">
-        <v>12</v>
-      </c>
-      <c r="F12" t="s">
-        <v>307</v>
-      </c>
-      <c r="G12" s="158" t="s">
-        <v>308</v>
-      </c>
-      <c r="H12" s="158" t="s">
-        <v>40</v>
-      </c>
-      <c r="I12" s="158" t="s">
-        <v>309</v>
-      </c>
-      <c r="J12" s="158" t="s">
-        <v>310</v>
-      </c>
-      <c r="K12" s="165"/>
       <c r="L12" s="158"/>
       <c r="M12" s="158"/>
-      <c r="N12" s="158"/>
-    </row>
-    <row r="13" spans="1:25" ht="15" customHeight="1">
+      <c r="N12" s="158" t="s">
+        <v>35</v>
+      </c>
+      <c r="P12" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>258</v>
+      </c>
+      <c r="U12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="160">
+        <v>45986</v>
+      </c>
+      <c r="B13" s="166" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="103" t="s">
+        <v>304</v>
+      </c>
+      <c r="D13" s="103" t="s">
+        <v>305</v>
+      </c>
+      <c r="E13" s="103">
+        <v>12</v>
+      </c>
+      <c r="F13" t="s">
+        <v>306</v>
+      </c>
+      <c r="G13" s="158" t="s">
+        <v>307</v>
+      </c>
+      <c r="H13" s="158" t="s">
+        <v>40</v>
+      </c>
+      <c r="I13" s="158" t="s">
+        <v>308</v>
+      </c>
+      <c r="J13" s="158" t="s">
+        <v>309</v>
+      </c>
+      <c r="K13" s="165"/>
+      <c r="L13" s="158"/>
+      <c r="M13" s="158"/>
+      <c r="N13" s="158"/>
+    </row>
+    <row r="14" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="160">
         <v>45988</v>
       </c>
-      <c r="B13" s="160" t="s">
-        <v>190</v>
-      </c>
-      <c r="C13" s="160" t="str">
-        <f>TEXT(A13, "mmm")</f>
+      <c r="B14" s="160" t="s">
+        <v>259</v>
+      </c>
+      <c r="C14" s="160" t="str">
+        <f>TEXT(A14, "mmm")</f>
         <v>Nov</v>
       </c>
-      <c r="D13" s="103" t="str">
-        <f>TEXT(A13, "dddd")</f>
-        <v>Thursday</v>
-      </c>
-      <c r="E13" s="103">
-        <v>13</v>
-      </c>
-      <c r="F13" s="164" t="s">
-        <v>311</v>
-      </c>
-      <c r="G13" s="107" t="s">
-        <v>312</v>
-      </c>
-      <c r="H13" s="25" t="s">
-        <v>211</v>
-      </c>
-      <c r="I13" s="97" t="s">
-        <v>313</v>
-      </c>
-      <c r="J13" s="97" t="s">
-        <v>314</v>
-      </c>
-      <c r="K13" s="157" t="s">
-        <v>315</v>
-      </c>
-      <c r="L13" s="25"/>
-      <c r="M13" s="25"/>
-      <c r="N13" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="O13" s="35"/>
-      <c r="P13" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q13" s="5"/>
-      <c r="R13" s="5"/>
-      <c r="S13" s="16"/>
-      <c r="T13" s="35"/>
-      <c r="U13" s="5"/>
-      <c r="V13" s="5"/>
-      <c r="W13" s="5"/>
-      <c r="X13" s="15"/>
-      <c r="Y13" s="13"/>
-    </row>
-    <row r="14" spans="1:25" ht="15" customHeight="1" thickBot="1">
-      <c r="A14" s="161">
-        <v>45995</v>
-      </c>
-      <c r="B14" s="161" t="s">
-        <v>190</v>
-      </c>
-      <c r="C14" s="161" t="str">
-        <f>TEXT(A14, "mmm")</f>
-        <v>Dec</v>
-      </c>
-      <c r="D14" s="106" t="str">
+      <c r="D14" s="103" t="str">
         <f>TEXT(A14, "dddd")</f>
         <v>Thursday</v>
       </c>
-      <c r="E14" s="106">
-        <f>E11+3</f>
-        <v>14</v>
+      <c r="E14" s="103">
+        <v>13</v>
       </c>
       <c r="F14" s="164" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="G14" s="107" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="H14" s="25" t="s">
-        <v>101</v>
+        <v>211</v>
       </c>
       <c r="I14" s="97" t="s">
-        <v>318</v>
-      </c>
-      <c r="J14" s="132" t="s">
-        <v>319</v>
+        <v>312</v>
+      </c>
+      <c r="J14" s="97" t="s">
+        <v>313</v>
       </c>
       <c r="K14" s="157" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="L14" s="25"/>
-      <c r="M14" s="31" t="s">
-        <v>321</v>
-      </c>
+      <c r="M14" s="25"/>
       <c r="N14" s="16" t="s">
         <v>44</v>
       </c>
@@ -6112,58 +6123,116 @@
       <c r="P14" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="Q14" s="5" t="s">
-        <v>64</v>
-      </c>
+      <c r="Q14" s="5"/>
       <c r="R14" s="5"/>
       <c r="S14" s="16"/>
-      <c r="T14" s="35" t="s">
-        <v>44</v>
-      </c>
-      <c r="U14" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="T14" s="35"/>
+      <c r="U14" s="5"/>
       <c r="V14" s="5"/>
       <c r="W14" s="5"/>
       <c r="X14" s="15"/>
       <c r="Y14" s="13"/>
     </row>
-    <row r="15" spans="1:25" ht="15" customHeight="1" thickBot="1">
-      <c r="A15" s="26"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="26"/>
-      <c r="X15" s="20"/>
-      <c r="Y15" s="18"/>
-    </row>
-    <row r="16" spans="1:25" ht="15" customHeight="1">
+    <row r="15" spans="1:25" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="161">
+        <v>45995</v>
+      </c>
+      <c r="B15" s="161" t="s">
+        <v>190</v>
+      </c>
+      <c r="C15" s="161" t="str">
+        <f>TEXT(A15, "mmm")</f>
+        <v>Dec</v>
+      </c>
+      <c r="D15" s="106" t="str">
+        <f>TEXT(A15, "dddd")</f>
+        <v>Thursday</v>
+      </c>
+      <c r="E15" s="106">
+        <f>E12+3</f>
+        <v>14</v>
+      </c>
+      <c r="F15" s="164" t="s">
+        <v>315</v>
+      </c>
+      <c r="G15" s="107" t="s">
+        <v>316</v>
+      </c>
+      <c r="H15" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="I15" s="97" t="s">
+        <v>317</v>
+      </c>
+      <c r="J15" s="132" t="s">
+        <v>318</v>
+      </c>
+      <c r="K15" s="157" t="s">
+        <v>319</v>
+      </c>
+      <c r="L15" s="25"/>
+      <c r="M15" s="31" t="s">
+        <v>320</v>
+      </c>
+      <c r="N15" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="O15" s="35"/>
+      <c r="P15" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q15" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="R15" s="5"/>
+      <c r="S15" s="16"/>
+      <c r="T15" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="U15" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="V15" s="5"/>
+      <c r="W15" s="5"/>
+      <c r="X15" s="15"/>
+      <c r="Y15" s="13"/>
+    </row>
+    <row r="16" spans="1:25" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="26"/>
       <c r="B16" s="26"/>
       <c r="C16" s="26"/>
-    </row>
-    <row r="17" spans="1:3" ht="15" customHeight="1">
+      <c r="X16" s="20"/>
+      <c r="Y16" s="18"/>
+    </row>
+    <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="26"/>
       <c r="B17" s="26"/>
       <c r="C17" s="26"/>
     </row>
-    <row r="18" spans="1:3" ht="15" customHeight="1">
+    <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="26"/>
       <c r="B18" s="26"/>
       <c r="C18" s="26"/>
     </row>
-    <row r="19" spans="1:3" ht="15" customHeight="1"/>
-    <row r="20" spans="1:3" ht="15" customHeight="1"/>
-    <row r="21" spans="1:3" ht="15" customHeight="1"/>
-    <row r="22" spans="1:3" ht="15" customHeight="1"/>
-    <row r="23" spans="1:3" ht="15" customHeight="1"/>
-    <row r="24" spans="1:3" ht="15" customHeight="1"/>
-    <row r="25" spans="1:3" ht="15" customHeight="1"/>
+    <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="26"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="26"/>
+    </row>
+    <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <protectedRanges>
-    <protectedRange algorithmName="SHA-512" hashValue="pQyTzP/d7t5ThMimBt5mu8gGozgAm1OwF6BMILsn5/kmtZ5mZf81NMi09wwU8mvtItxf0EVNWa6V4MCa0DKeSQ==" saltValue="NzZBiAQ1yFjat+SeIqh2Uw==" spinCount="100000" sqref="A3:E18" name="Range3_1"/>
+    <protectedRange algorithmName="SHA-512" hashValue="pQyTzP/d7t5ThMimBt5mu8gGozgAm1OwF6BMILsn5/kmtZ5mZf81NMi09wwU8mvtItxf0EVNWa6V4MCa0DKeSQ==" saltValue="NzZBiAQ1yFjat+SeIqh2Uw==" spinCount="100000" sqref="A3:E19" name="Range3_1"/>
     <protectedRange algorithmName="SHA-512" hashValue="JNB4nrqrfZD45ijUCOmyuk44ibTGOz2xPKKqUb8Fu6IzynfOW0Plt2J4MjvTXFpCm0cEkYqWWfoKwgUFnGztPw==" saltValue="gktf/myRKhBCN9s2pCislA==" spinCount="100000" sqref="A2:Y2" name="Range4_1"/>
-    <protectedRange algorithmName="SHA-512" hashValue="B/N8xqtMc7pXr3rfrr4k91A6IFAPX6lxEHUr9qsJ3yHA+MBnFuw+x27DjsTYKp86iL5C7QQh1TPFTQHueWpZbw==" saltValue="c0IR/echnZmip5yS1t29Rw==" spinCount="100000" sqref="T3:T14" name="Range6_1"/>
-    <protectedRange algorithmName="SHA-512" hashValue="BKDH3ki5lE3XQdc5qZnIH6o8wW8E0PkHgMZFCkv/XYDEa+b/qenui0oReDIqPDXHceUVJ+rEgU3I9CDBHraDYg==" saltValue="ruXqG4NOhhm7cSLor8wHfw==" spinCount="100000" sqref="O2:O14" name="Range7_1"/>
-    <protectedRange sqref="X15:Y15 F3:Y14" name="Range8_1"/>
+    <protectedRange algorithmName="SHA-512" hashValue="B/N8xqtMc7pXr3rfrr4k91A6IFAPX6lxEHUr9qsJ3yHA+MBnFuw+x27DjsTYKp86iL5C7QQh1TPFTQHueWpZbw==" saltValue="c0IR/echnZmip5yS1t29Rw==" spinCount="100000" sqref="T3:T15" name="Range6_1"/>
+    <protectedRange algorithmName="SHA-512" hashValue="BKDH3ki5lE3XQdc5qZnIH6o8wW8E0PkHgMZFCkv/XYDEa+b/qenui0oReDIqPDXHceUVJ+rEgU3I9CDBHraDYg==" saltValue="ruXqG4NOhhm7cSLor8wHfw==" spinCount="100000" sqref="O2:O15" name="Range7_1"/>
+    <protectedRange sqref="X16:Y16 F3:Y15" name="Range8_1"/>
   </protectedRanges>
   <hyperlinks>
     <hyperlink ref="K3" r:id="rId1" xr:uid="{CC4847BF-5CC0-41D9-9E80-86D0D78BEFCD}"/>
@@ -6172,14 +6241,15 @@
     <hyperlink ref="K7" r:id="rId4" xr:uid="{7120277C-1705-4DE0-ADA5-C41C5441CF52}"/>
     <hyperlink ref="K9" r:id="rId5" xr:uid="{4AC45F90-7175-4CE5-9D88-F653406BC232}"/>
     <hyperlink ref="K8" r:id="rId6" xr:uid="{5670CBAB-0F26-4CE3-B15B-6D1F054D4FCF}"/>
-    <hyperlink ref="K13" r:id="rId7" xr:uid="{22FAA2AA-5C27-49D1-BE58-6994B647E0B0}"/>
+    <hyperlink ref="K14" r:id="rId7" xr:uid="{22FAA2AA-5C27-49D1-BE58-6994B647E0B0}"/>
     <hyperlink ref="L10" r:id="rId8" xr:uid="{868EB6F0-D226-4BCB-8A71-EF764997CE08}"/>
     <hyperlink ref="M10" r:id="rId9" xr:uid="{294C464E-EF91-4638-871F-055BFBC562A3}"/>
-    <hyperlink ref="K11" r:id="rId10" xr:uid="{D6157109-0314-4E19-ABD9-5C3848013F5D}"/>
-    <hyperlink ref="M14" r:id="rId11" xr:uid="{D19FB516-A72C-4F26-B04A-D73126013BC5}"/>
-    <hyperlink ref="K14" r:id="rId12" xr:uid="{FAA02F49-DD76-40A9-9606-6A1BED9FFDD6}"/>
+    <hyperlink ref="K12" r:id="rId10" xr:uid="{D6157109-0314-4E19-ABD9-5C3848013F5D}"/>
+    <hyperlink ref="M15" r:id="rId11" xr:uid="{D19FB516-A72C-4F26-B04A-D73126013BC5}"/>
+    <hyperlink ref="K15" r:id="rId12" xr:uid="{FAA02F49-DD76-40A9-9606-6A1BED9FFDD6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
 
@@ -6187,11 +6257,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F62D4156-0A06-4DBF-B1E7-3E12580121CB}">
   <dimension ref="A1:Y13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" customWidth="1"/>
     <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1"/>
@@ -6218,7 +6288,7 @@
     <col min="25" max="25" width="37.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6229,7 +6299,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="30.75">
+    <row r="2" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="64" t="s">
         <v>3</v>
       </c>
@@ -6306,7 +6376,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="15" customHeight="1">
+    <row r="3" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="75">
         <v>46051</v>
       </c>
@@ -6325,19 +6395,19 @@
         <v>1</v>
       </c>
       <c r="F3" s="16" t="s">
+        <v>321</v>
+      </c>
+      <c r="G3" s="14" t="s">
         <v>322</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>323</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>87</v>
       </c>
       <c r="I3" s="98" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="J3" s="98" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="K3" s="73"/>
       <c r="L3" s="40"/>
@@ -6355,7 +6425,7 @@
       <c r="X3" s="46"/>
       <c r="Y3" s="44"/>
     </row>
-    <row r="4" spans="1:25" ht="15.75" customHeight="1">
+    <row r="4" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="75">
         <f>A3+14</f>
         <v>46065</v>
@@ -6376,19 +6446,19 @@
         <v>3</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="I4" s="98" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="J4" s="98" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="K4" s="102"/>
       <c r="L4" s="5"/>
@@ -6406,7 +6476,7 @@
       <c r="X4" s="15"/>
       <c r="Y4" s="13"/>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="75">
         <f t="shared" ref="A5:A9" si="2">A4+14</f>
         <v>46079</v>
@@ -6427,29 +6497,29 @@
         <v>5</v>
       </c>
       <c r="F5" s="16" t="s">
+        <v>325</v>
+      </c>
+      <c r="G5" s="14" t="s">
         <v>326</v>
-      </c>
-      <c r="G5" s="14" t="s">
-        <v>327</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>87</v>
       </c>
       <c r="I5" s="98" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="J5" s="98" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="K5" s="102"/>
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
       <c r="N5" s="16"/>
       <c r="O5" s="35" t="s">
+        <v>327</v>
+      </c>
+      <c r="P5" s="5" t="s">
         <v>328</v>
-      </c>
-      <c r="P5" s="5" t="s">
-        <v>329</v>
       </c>
       <c r="Q5" s="5"/>
       <c r="R5" s="5"/>
@@ -6461,7 +6531,7 @@
       <c r="X5" s="15"/>
       <c r="Y5" s="13"/>
     </row>
-    <row r="6" spans="1:25" ht="15.75" customHeight="1">
+    <row r="6" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="75">
         <f>A5+14</f>
         <v>46093</v>
@@ -6482,7 +6552,7 @@
         <v>7</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G6" s="14" t="s">
         <v>152</v>
@@ -6491,10 +6561,10 @@
         <v>95</v>
       </c>
       <c r="I6" s="98" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="J6" s="98" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="K6" s="102"/>
       <c r="L6" s="5"/>
@@ -6512,7 +6582,7 @@
       <c r="X6" s="15"/>
       <c r="Y6" s="13"/>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="75">
         <f t="shared" si="2"/>
         <v>46107</v>
@@ -6533,19 +6603,19 @@
         <v>9</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="I7" s="98" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="J7" s="98" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="K7" s="102"/>
       <c r="L7" s="5"/>
@@ -6563,7 +6633,7 @@
       <c r="X7" s="15"/>
       <c r="Y7" s="13"/>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="75">
         <f t="shared" si="2"/>
         <v>46121</v>
@@ -6584,19 +6654,19 @@
         <v>11</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="I8" s="98" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="J8" s="98" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="K8" s="102"/>
       <c r="L8" s="5"/>
@@ -6614,7 +6684,7 @@
       <c r="X8" s="15"/>
       <c r="Y8" s="13"/>
     </row>
-    <row r="9" spans="1:25" ht="18.75" customHeight="1">
+    <row r="9" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="75">
         <f t="shared" si="2"/>
         <v>46135</v>
@@ -6635,19 +6705,19 @@
         <v>13</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="I9" s="98" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="J9" s="98" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="K9" s="102"/>
       <c r="L9" s="5"/>
@@ -6665,24 +6735,24 @@
       <c r="X9" s="15"/>
       <c r="Y9" s="13"/>
     </row>
-    <row r="10" spans="1:25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="26"/>
       <c r="B10" s="26"/>
       <c r="C10" s="26"/>
       <c r="X10" s="20"/>
       <c r="Y10" s="18"/>
     </row>
-    <row r="11" spans="1:25" ht="12.75" customHeight="1">
+    <row r="11" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="26"/>
       <c r="B11" s="26"/>
       <c r="C11" s="26"/>
     </row>
-    <row r="12" spans="1:25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="26"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
     </row>
-    <row r="13" spans="1:25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="26"/>
       <c r="B13" s="26"/>
       <c r="C13" s="26"/>
@@ -6708,231 +6778,231 @@
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.28515625" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
     <col min="3" max="3" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="55" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="55" t="s">
+      <c r="B2" s="54" t="s">
         <v>332</v>
       </c>
-      <c r="B2" s="54" t="s">
+      <c r="C2" s="54" t="s">
         <v>333</v>
       </c>
-      <c r="C2" s="54" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="136" t="s">
         <v>334</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="136" t="s">
-        <v>335</v>
       </c>
       <c r="B3" s="137"/>
       <c r="C3" s="138" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B4" s="52"/>
       <c r="C4" s="50" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="52" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B5" s="52"/>
       <c r="C5" s="50" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="52" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="52" t="s">
+      <c r="B6" s="52" t="s">
         <v>339</v>
-      </c>
-      <c r="B6" s="52" t="s">
-        <v>340</v>
       </c>
       <c r="C6" s="50" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="52" t="s">
+        <v>340</v>
+      </c>
+      <c r="B7" s="52" t="s">
         <v>341</v>
-      </c>
-      <c r="B7" s="52" t="s">
-        <v>342</v>
       </c>
       <c r="C7" s="50" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="52" t="s">
+        <v>342</v>
+      </c>
+      <c r="B8" s="52" t="s">
         <v>343</v>
-      </c>
-      <c r="B8" s="52" t="s">
-        <v>344</v>
       </c>
       <c r="C8" s="50" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="52" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B9" s="52"/>
       <c r="C9" s="50"/>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="52" t="s">
+        <v>345</v>
+      </c>
+      <c r="B10" s="52" t="s">
         <v>346</v>
       </c>
-      <c r="B10" s="52" t="s">
+      <c r="C10" s="50" t="s">
         <v>347</v>
       </c>
-      <c r="C10" s="50" t="s">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="52" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="52" t="s">
+      <c r="B11" s="52" t="s">
         <v>349</v>
       </c>
-      <c r="B11" s="52" t="s">
+      <c r="C11" s="50" t="s">
         <v>350</v>
       </c>
-      <c r="C11" s="50" t="s">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="52" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="52" t="s">
+      <c r="B12" s="52" t="s">
         <v>352</v>
       </c>
-      <c r="B12" s="52" t="s">
+      <c r="C12" s="50" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="52" t="s">
         <v>353</v>
       </c>
-      <c r="C12" s="50" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="52" t="s">
+      <c r="B13" s="52" t="s">
         <v>354</v>
       </c>
-      <c r="B13" s="52" t="s">
+      <c r="C13" s="50" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="52" t="s">
         <v>355</v>
       </c>
-      <c r="C13" s="50" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="52" t="s">
+      <c r="B14" s="52" t="s">
         <v>356</v>
       </c>
-      <c r="B14" s="52" t="s">
+      <c r="C14" s="50" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="52" t="s">
         <v>357</v>
       </c>
-      <c r="C14" s="50" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="52" t="s">
+      <c r="B15" s="52" t="s">
         <v>358</v>
       </c>
-      <c r="B15" s="52" t="s">
+      <c r="C15" s="50" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="137" t="s">
+        <v>315</v>
+      </c>
+      <c r="B16" s="137" t="s">
         <v>359</v>
       </c>
-      <c r="C15" s="50" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="137" t="s">
-        <v>316</v>
-      </c>
-      <c r="B16" s="137" t="s">
+      <c r="C16" s="139" t="s">
         <v>360</v>
       </c>
-      <c r="C16" s="139" t="s">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="52" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="52" t="s">
+      <c r="B17" s="52" t="s">
         <v>362</v>
       </c>
-      <c r="B17" s="52" t="s">
+      <c r="C17" s="50" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="52" t="s">
         <v>363</v>
       </c>
-      <c r="C17" s="50" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="52" t="s">
-        <v>364</v>
-      </c>
       <c r="B18" s="52" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C18" s="50" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="53" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B19" s="53" t="s">
         <v>230</v>
       </c>
       <c r="C19" s="51" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
-      <c r="A23" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B24" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C24" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B25" t="s">
         <v>230</v>
       </c>
       <c r="C25" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
   </sheetData>
@@ -6953,24 +7023,24 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
     <col min="6" max="6" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="135" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="131" t="s">
+        <v>367</v>
+      </c>
+      <c r="C1" s="130" t="s">
         <v>368</v>
       </c>
-      <c r="C1" s="130" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="15.75" thickTop="1">
+    </row>
+    <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="133">
         <v>45911</v>
       </c>
@@ -6978,7 +7048,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="134" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F2" s="75">
         <v>45911</v>
@@ -6998,7 +7068,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="133">
         <f>A2+7</f>
         <v>45918</v>
@@ -7008,7 +7078,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="134" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F3" s="75">
         <v>45926</v>
@@ -7029,7 +7099,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="133">
         <f t="shared" ref="A4:A12" si="0">A3+7</f>
         <v>45925</v>
@@ -7039,7 +7109,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="134" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F4" s="75">
         <v>45939</v>
@@ -7060,7 +7130,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="133">
         <f t="shared" si="0"/>
         <v>45932</v>
@@ -7070,7 +7140,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="134" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F5" s="75">
         <v>45946</v>
@@ -7088,7 +7158,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="133">
         <f t="shared" si="0"/>
         <v>45939</v>
@@ -7098,7 +7168,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="134" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F6" s="75">
         <v>45953</v>
@@ -7119,7 +7189,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="133">
         <f t="shared" si="0"/>
         <v>45946</v>
@@ -7129,7 +7199,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="134" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="F7" s="75">
         <v>45967</v>
@@ -7150,7 +7220,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="133">
         <f t="shared" si="0"/>
         <v>45953</v>
@@ -7160,7 +7230,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="134" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F8" s="75">
         <v>45974</v>
@@ -7180,7 +7250,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="133">
         <f t="shared" si="0"/>
         <v>45960</v>
@@ -7190,7 +7260,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="134" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F9" s="75">
         <v>45981</v>
@@ -7211,7 +7281,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="133">
         <f t="shared" si="0"/>
         <v>45967</v>
@@ -7221,7 +7291,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="134" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F10" s="75">
         <v>45995</v>
@@ -7242,7 +7312,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="133">
         <f t="shared" si="0"/>
         <v>45974</v>
@@ -7252,10 +7322,10 @@
         <v>10</v>
       </c>
       <c r="C11" s="134" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="133">
         <f t="shared" si="0"/>
         <v>45981</v>
@@ -7265,10 +7335,10 @@
         <v>11</v>
       </c>
       <c r="C12" s="134" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="133">
         <f t="shared" ref="A13:A14" si="6">A12+7</f>
         <v>45988</v>
@@ -7278,10 +7348,10 @@
         <v>12</v>
       </c>
       <c r="C13" s="134" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="133">
         <f t="shared" si="6"/>
         <v>45995</v>
@@ -7291,15 +7361,15 @@
         <v>13</v>
       </c>
       <c r="C14" s="134" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="133"/>
       <c r="B15" s="134"/>
       <c r="C15" s="134"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G16" s="26"/>
     </row>
   </sheetData>
@@ -7330,7 +7400,7 @@
       <selection activeCell="F8" sqref="F8:H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.42578125" customWidth="1"/>
     <col min="2" max="2" width="9.140625" customWidth="1"/>
@@ -7342,17 +7412,17 @@
     <col min="9" max="9" width="64.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" ht="23.25">
+    <row r="2" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="91" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="79" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="18.75">
-      <c r="A3" s="79" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="37.5">
+    <row r="5" spans="1:9" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A5" s="80" t="s">
         <v>3</v>
       </c>
@@ -7375,13 +7445,13 @@
         <v>9</v>
       </c>
       <c r="H5" s="82" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="I5" s="81" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="18.75">
+    <row r="6" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="92">
         <v>45694</v>
       </c>
@@ -7405,10 +7475,10 @@
       </c>
       <c r="H6" s="85"/>
       <c r="I6" s="84" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="18.75">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="83">
         <v>45708</v>
       </c>
@@ -7437,7 +7507,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="18.75">
+    <row r="8" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="83">
         <v>45722</v>
       </c>
@@ -7464,7 +7534,7 @@
       </c>
       <c r="I8" s="86"/>
     </row>
-    <row r="9" spans="1:9" ht="18.75">
+    <row r="9" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="83">
         <v>45735</v>
       </c>
@@ -7475,7 +7545,7 @@
         <v>198</v>
       </c>
       <c r="D9" s="94" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E9" s="94">
         <v>8</v>
@@ -7490,10 +7560,10 @@
         <v>206</v>
       </c>
       <c r="I9" s="86" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="18.75">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="83">
         <v>45744</v>
       </c>
@@ -7520,7 +7590,7 @@
       </c>
       <c r="I10" s="86"/>
     </row>
-    <row r="11" spans="1:9" ht="18.75">
+    <row r="11" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="83">
         <v>45750</v>
       </c>
@@ -7537,17 +7607,17 @@
         <v>10</v>
       </c>
       <c r="F11" s="87" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="G11" s="87" t="s">
         <v>68</v>
       </c>
       <c r="H11" s="87"/>
       <c r="I11" s="86" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="18.75">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="83">
         <v>45758</v>
       </c>
@@ -7573,10 +7643,10 @@
         <v>31</v>
       </c>
       <c r="I12" s="86" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="18.75">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="83">
         <v>45764</v>
       </c>
@@ -7593,13 +7663,13 @@
         <v>12</v>
       </c>
       <c r="F13" s="87" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G13" s="87"/>
       <c r="H13" s="87"/>
       <c r="I13" s="86"/>
     </row>
-    <row r="14" spans="1:9" ht="18.75">
+    <row r="14" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="88">
         <v>45771</v>
       </c>
@@ -7616,7 +7686,7 @@
         <v>13</v>
       </c>
       <c r="F14" s="90" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G14" s="90" t="s">
         <v>77</v>
@@ -7628,7 +7698,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="20" spans="8:8" ht="18.75">
+    <row r="20" spans="8:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="H20" s="79"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added speakers; fixed week no.
</commit_message>
<xml_diff>
--- a/data/MACSI seminar series.xlsx
+++ b/data/MACSI seminar series.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29518"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ulcampus-my.sharepoint.com/personal/david_osullivan_ul_ie/Documents/Academic_work/_Misc/MACSI_Seminars/macsi-seminars.github.io/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="117" documentId="13_ncr:1_{12BE53B5-C8C7-44FE-8280-19C653D9122E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{64B9DAC9-E9DC-4C52-84B9-FF978EEBF022}"/>
+  <xr:revisionPtr revIDLastSave="119" documentId="13_ncr:1_{12BE53B5-C8C7-44FE-8280-19C653D9122E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5487EAA0-7362-4950-8DE5-5503B39B9EC1}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1000,239 +1000,6 @@
     <t>5</t>
   </si>
   <si>
-    <t>Alison O'Connor</t>
-  </si>
-  <si>
-    <t>Hip Fractures Trends in Older Adults in Ireland</t>
-  </si>
-  <si>
-    <t>https://scholar.google.com/citations?user=dIpyVmAAAAAJ&amp;hl=en&amp;oi=ao</t>
-  </si>
-  <si>
-    <t>Nov</t>
-  </si>
-  <si>
-    <t>Tuesday</t>
-  </si>
-  <si>
-    <t>Christos Xenophontos</t>
-  </si>
-  <si>
-    <t>University of Cyprus</t>
-  </si>
-  <si>
-    <t>Neural Networks for singular perturbations</t>
-  </si>
-  <si>
-    <t>In this talk we will give an introduction to Neural Networks (NNs) and describe how they can be used for emulating the solution to singularly perturbed problems. In addition, we will present results on the expressivity rate bounds for solution sets of a model class of singularly perturbed, elliptic two-point boundary value problems, in Sobolev norms, on the bounded interval (-1,1). The expression rate bounds in Sobolev norms in terms of the NN size are robust, i.e. uniform with respect to the singular perturbation parameter for several classes of DNN architectures. In particular, ReLU NNs, tanh- and sigmoid-activated NNs. The latter activations can represent “exponential boundary layer solution features” explicitly, in the last hidden layer of the DNN, i.e. in a shallow subnetwork, and afford improved robust expression rate bounds in terms of the NN size.</t>
-  </si>
-  <si>
-    <t>Hugo Luiz Oliveira</t>
-  </si>
-  <si>
-    <t>University of Campinas (Unicamp), Brazil</t>
-  </si>
-  <si>
-    <t>Numerical and computational modelling of the Wheatley aortic valve</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Recent studies have indicated an increase in cardiovascular diseases in developing countries, particularly valvular disorders caused by rheumatic fever, which are affecting younger populations. In severe cases, when the natural valve cannot be repaired, replacing it with a prosthetic valve may be the most effective way to ensure the patient's survival. Existing artificial valves have limitations, such as early deterioration and the risk of clot formation. To address these issues, the Wheatley Valve introduces an innovative S-shaped leaflet design that enhances the washout effect in the aortic root, thereby reducing the risk of thrombus formation and the need for extensive antiplatelet therapy. In this talk, we will discuss the main elements needed to build a fluid-structure interaction computational model able to represent the real behaviour of the Wheatley valve and which can be readily extended to other valve designs.
-</t>
-  </si>
-  <si>
-    <t>https://scholar.google.com/citations?user=nfeQtPQAAAAJ&amp;hl=pt-BR</t>
-  </si>
-  <si>
-    <t>Silvia D'Angelo</t>
-  </si>
-  <si>
-    <t>Trinity College Dublin</t>
-  </si>
-  <si>
-    <t>Clustering high-dimensional discrete data: a compressed approach</t>
-  </si>
-  <si>
-    <t>Custering high-dimensional data is a challenging task, typically addressed in the context of continuous numerical data. Recent literature is exploring strategies to cluster high-dimensional categorical and discrete data, which finds numerous applications, such as RNA sequencing and text data analysis. We propose a fast and easy-to-implement approach to cluster high-dimensional discrete data, scalable to datasets with thousands of dimensions where other strategies may be computationally unfeasible. Our approach relies on reducing the dimension of the data by performing a deterministic compression to a drastically lower dimension. The method employs a lossy compression that reduces the data to a collection of continuous features.
-We demonstrate that such compressed features can be treated as approximately normally distributed, allowing the application of standard finite Gaussian mixture models for model-based clustering. We discuss the approach and study its performance on a series of simulated scenarios with different dimensions and levels of complexity, involving both categorical and count data. Additionally, we illustrate the method on real-world data.</t>
-  </si>
-  <si>
-    <t>https://scholar.google.com/citations?user=d-Wde0EAAAAJ&amp;hl=en</t>
-  </si>
-  <si>
-    <t>https://www.tcd.ie/scss/people/academic-staff/dangelos/ ; https://sites.google.com/view/silviadangelo/home</t>
-  </si>
-  <si>
-    <t>Eoin O’Brien</t>
-  </si>
-  <si>
-    <t>Maynooth University</t>
-  </si>
-  <si>
-    <t>TBC</t>
-  </si>
-  <si>
-    <t>Open</t>
-  </si>
-  <si>
-    <t>Philip Pearce</t>
-  </si>
-  <si>
-    <t>University College London</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>Email sent to Castltroy park hotel on 13 NOv 2025</t>
-  </si>
-  <si>
-    <t>Leah Keating</t>
-  </si>
-  <si>
-    <t>This is a just a place for those who are interested but that dont have a specific date in mind. (Ideally, a couple of these are people that we could invite with relatively short notice to fill missing slots.)</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Where are they from?</t>
-  </si>
-  <si>
-    <t>Adacemic Host</t>
-  </si>
-  <si>
-    <t>Colm</t>
-  </si>
-  <si>
-    <t>Niamh Cahill</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Niall Madden </t>
-  </si>
-  <si>
-    <t>Mehakpreet</t>
-  </si>
-  <si>
-    <t>Paul Weaver (invitation sent)</t>
-  </si>
-  <si>
-    <t>UL (Bernal)</t>
-  </si>
-  <si>
-    <t>Eleanor Doman</t>
-  </si>
-  <si>
-    <t>Manchester</t>
-  </si>
-  <si>
-    <t>Connor Hacket</t>
-  </si>
-  <si>
-    <t>MU</t>
-  </si>
-  <si>
-    <t>David Henry (?)</t>
-  </si>
-  <si>
-    <t>Jess Enright</t>
-  </si>
-  <si>
-    <t>Glasgow</t>
-  </si>
-  <si>
-    <t>JS/Networks</t>
-  </si>
-  <si>
-    <t>Ben Swallows</t>
-  </si>
-  <si>
-    <t>St Andrews</t>
-  </si>
-  <si>
-    <t>JS</t>
-  </si>
-  <si>
-    <t>Andrew Finlay</t>
-  </si>
-  <si>
-    <t>Uni Michigan</t>
-  </si>
-  <si>
-    <t>Denis Allard</t>
-  </si>
-  <si>
-    <t>INRAE</t>
-  </si>
-  <si>
-    <t>Nicholas J Clark</t>
-  </si>
-  <si>
-    <t>University of Queensland</t>
-  </si>
-  <si>
-    <t>Andrew Zammit Mangion</t>
-  </si>
-  <si>
-    <t>University of Wollongong</t>
-  </si>
-  <si>
-    <t>Trinity</t>
-  </si>
-  <si>
-    <t>DOS</t>
-  </si>
-  <si>
-    <t>Catherine Higgins</t>
-  </si>
-  <si>
-    <t>UCD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paul Weaver </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Suzanne Fielding </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Doireann O'Kiely and Anthony </t>
-  </si>
-  <si>
-    <t>Possible speaker for next semester</t>
-  </si>
-  <si>
-    <t>Week</t>
-  </si>
-  <si>
-    <t>Speaker</t>
-  </si>
-  <si>
-    <t>Taken</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Taken </t>
-  </si>
-  <si>
-    <t>Seminar Series AY2024-25 Sem 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contact david.osullivan@ul.ie &amp; mehakpreet.singh@ul.ie to book a speaker in. </t>
-  </si>
-  <si>
-    <t>Deptartmental contact</t>
-  </si>
-  <si>
-    <t>Wednesday</t>
-  </si>
-  <si>
-    <t>Robery Garvey</t>
-  </si>
-  <si>
-    <t>Tentative speaker</t>
-  </si>
-  <si>
-    <t>Leornard Henckel</t>
-  </si>
-  <si>
     <t>12:30pm</t>
   </si>
   <si>
@@ -1244,6 +1011,15 @@
   <si>
     <t>Most real-world buckling problems, from Coke cans to metamaterials, involve metals or other hard materials that deform plastically. Yet, many studies focus primarily on geometric nonlinearities, often neglecting the material nonlinearities that play a crucial role in determining post-buckling behaviour. In this talk, we examine two systems in which we incorporate these effects through semi-empirical modelling of material nonlinearities: hard holey columns and the sequential ring-buckling of fluid-filled Coke cans.
 By including material nonlinearities in our models, we show that intuitive, mechanics-based approaches can successfully capture the complex behaviour observed in the buckling of hard materials.</t>
+  </si>
+  <si>
+    <t>https://orcid.org/0000-0002-8790-7654</t>
+  </si>
+  <si>
+    <t>Alison O'Connor</t>
+  </si>
+  <si>
+    <t>Hip Fractures Trends in Older Adults in Ireland</t>
   </si>
   <si>
     <t>European healthcare systems are under pressure from rapidly ageing populations, with hip fractures representing one of the most costly and impactful injuries among older adults (1,2). Ireland faces the dual challenge of both a rapidly growing ageing population and one of the highest European rates in hip fracture incidence (3,4). Irish standards require admission to orthopaedic care within four hours, yet national audits show this target is rarely achieved (5). Improving hip fracture services requires not just clinical reform but also new ways of leveraging data.
@@ -1257,7 +1033,231 @@
 https://d7g406zpx7bgk.cloudfront.net/38cf762d5b/irish_hip_fracture_database_national_report_2022_final.pdf</t>
   </si>
   <si>
-    <t>https://orcid.org/0000-0002-8790-7654</t>
+    <t>https://scholar.google.com/citations?user=dIpyVmAAAAAJ&amp;hl=en&amp;oi=ao</t>
+  </si>
+  <si>
+    <t>Nov</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>Christos Xenophontos</t>
+  </si>
+  <si>
+    <t>University of Cyprus</t>
+  </si>
+  <si>
+    <t>Neural Networks for singular perturbations</t>
+  </si>
+  <si>
+    <t>In this talk we will give an introduction to Neural Networks (NNs) and describe how they can be used for emulating the solution to singularly perturbed problems. In addition, we will present results on the expressivity rate bounds for solution sets of a model class of singularly perturbed, elliptic two-point boundary value problems, in Sobolev norms, on the bounded interval (-1,1). The expression rate bounds in Sobolev norms in terms of the NN size are robust, i.e. uniform with respect to the singular perturbation parameter for several classes of DNN architectures. In particular, ReLU NNs, tanh- and sigmoid-activated NNs. The latter activations can represent “exponential boundary layer solution features” explicitly, in the last hidden layer of the DNN, i.e. in a shallow subnetwork, and afford improved robust expression rate bounds in terms of the NN size.</t>
+  </si>
+  <si>
+    <t>Hugo Luiz Oliveira</t>
+  </si>
+  <si>
+    <t>University of Campinas (Unicamp), Brazil</t>
+  </si>
+  <si>
+    <t>Numerical and computational modelling of the Wheatley aortic valve</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recent studies have indicated an increase in cardiovascular diseases in developing countries, particularly valvular disorders caused by rheumatic fever, which are affecting younger populations. In severe cases, when the natural valve cannot be repaired, replacing it with a prosthetic valve may be the most effective way to ensure the patient's survival. Existing artificial valves have limitations, such as early deterioration and the risk of clot formation. To address these issues, the Wheatley Valve introduces an innovative S-shaped leaflet design that enhances the washout effect in the aortic root, thereby reducing the risk of thrombus formation and the need for extensive antiplatelet therapy. In this talk, we will discuss the main elements needed to build a fluid-structure interaction computational model able to represent the real behaviour of the Wheatley valve and which can be readily extended to other valve designs.
+</t>
+  </si>
+  <si>
+    <t>https://scholar.google.com/citations?user=nfeQtPQAAAAJ&amp;hl=pt-BR</t>
+  </si>
+  <si>
+    <t>Silvia D'Angelo</t>
+  </si>
+  <si>
+    <t>Trinity College Dublin</t>
+  </si>
+  <si>
+    <t>Clustering high-dimensional discrete data: a compressed approach</t>
+  </si>
+  <si>
+    <t>Custering high-dimensional data is a challenging task, typically addressed in the context of continuous numerical data. Recent literature is exploring strategies to cluster high-dimensional categorical and discrete data, which finds numerous applications, such as RNA sequencing and text data analysis. We propose a fast and easy-to-implement approach to cluster high-dimensional discrete data, scalable to datasets with thousands of dimensions where other strategies may be computationally unfeasible. Our approach relies on reducing the dimension of the data by performing a deterministic compression to a drastically lower dimension. The method employs a lossy compression that reduces the data to a collection of continuous features.
+We demonstrate that such compressed features can be treated as approximately normally distributed, allowing the application of standard finite Gaussian mixture models for model-based clustering. We discuss the approach and study its performance on a series of simulated scenarios with different dimensions and levels of complexity, involving both categorical and count data. Additionally, we illustrate the method on real-world data.</t>
+  </si>
+  <si>
+    <t>https://scholar.google.com/citations?user=d-Wde0EAAAAJ&amp;hl=en</t>
+  </si>
+  <si>
+    <t>https://www.tcd.ie/scss/people/academic-staff/dangelos/ ; https://sites.google.com/view/silviadangelo/home</t>
+  </si>
+  <si>
+    <t>Eoin O’Brien</t>
+  </si>
+  <si>
+    <t>Maynooth University</t>
+  </si>
+  <si>
+    <t>TBC</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>Philip Pearce</t>
+  </si>
+  <si>
+    <t>University College London</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>Email sent to Castltroy park hotel on 13 NOv 2025</t>
+  </si>
+  <si>
+    <t>Leah Keating</t>
+  </si>
+  <si>
+    <t>This is a just a place for those who are interested but that dont have a specific date in mind. (Ideally, a couple of these are people that we could invite with relatively short notice to fill missing slots.)</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Where are they from?</t>
+  </si>
+  <si>
+    <t>Adacemic Host</t>
+  </si>
+  <si>
+    <t>Colm</t>
+  </si>
+  <si>
+    <t>Niamh Cahill</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Niall Madden </t>
+  </si>
+  <si>
+    <t>Mehakpreet</t>
+  </si>
+  <si>
+    <t>Paul Weaver (invitation sent)</t>
+  </si>
+  <si>
+    <t>UL (Bernal)</t>
+  </si>
+  <si>
+    <t>Eleanor Doman</t>
+  </si>
+  <si>
+    <t>Manchester</t>
+  </si>
+  <si>
+    <t>Connor Hacket</t>
+  </si>
+  <si>
+    <t>MU</t>
+  </si>
+  <si>
+    <t>David Henry (?)</t>
+  </si>
+  <si>
+    <t>Jess Enright</t>
+  </si>
+  <si>
+    <t>Glasgow</t>
+  </si>
+  <si>
+    <t>JS/Networks</t>
+  </si>
+  <si>
+    <t>Ben Swallows</t>
+  </si>
+  <si>
+    <t>St Andrews</t>
+  </si>
+  <si>
+    <t>JS</t>
+  </si>
+  <si>
+    <t>Andrew Finlay</t>
+  </si>
+  <si>
+    <t>Uni Michigan</t>
+  </si>
+  <si>
+    <t>Denis Allard</t>
+  </si>
+  <si>
+    <t>INRAE</t>
+  </si>
+  <si>
+    <t>Nicholas J Clark</t>
+  </si>
+  <si>
+    <t>University of Queensland</t>
+  </si>
+  <si>
+    <t>Andrew Zammit Mangion</t>
+  </si>
+  <si>
+    <t>University of Wollongong</t>
+  </si>
+  <si>
+    <t>Trinity</t>
+  </si>
+  <si>
+    <t>DOS</t>
+  </si>
+  <si>
+    <t>Catherine Higgins</t>
+  </si>
+  <si>
+    <t>UCD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paul Weaver </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suzanne Fielding </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Doireann O'Kiely and Anthony </t>
+  </si>
+  <si>
+    <t>Possible speaker for next semester</t>
+  </si>
+  <si>
+    <t>Week</t>
+  </si>
+  <si>
+    <t>Speaker</t>
+  </si>
+  <si>
+    <t>Taken</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Taken </t>
+  </si>
+  <si>
+    <t>Seminar Series AY2024-25 Sem 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact david.osullivan@ul.ie &amp; mehakpreet.singh@ul.ie to book a speaker in. </t>
+  </si>
+  <si>
+    <t>Deptartmental contact</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>Robery Garvey</t>
+  </si>
+  <si>
+    <t>Tentative speaker</t>
+  </si>
+  <si>
+    <t>Leornard Henckel</t>
   </si>
 </sst>
 </file>
@@ -1267,7 +1267,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2108,9 +2108,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2148,7 +2148,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2254,7 +2254,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2396,7 +2396,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2410,7 +2410,7 @@
       <selection activeCell="K1" sqref="K1:L1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="11.140625" customWidth="1"/>
@@ -2435,7 +2435,7 @@
     <col min="25" max="25" width="37.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2446,7 +2446,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="30">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -2523,7 +2523,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" ht="13.5" customHeight="1">
       <c r="A3" s="2">
         <v>45317</v>
       </c>
@@ -2590,7 +2590,7 @@
       <c r="X3" s="13"/>
       <c r="Y3" s="13"/>
     </row>
-    <row r="4" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="13.5" customHeight="1">
       <c r="A4" s="2">
         <v>45323</v>
       </c>
@@ -2653,7 +2653,7 @@
       <c r="X4" s="13"/>
       <c r="Y4" s="13"/>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25">
       <c r="A5" s="2">
         <v>45324</v>
       </c>
@@ -2714,7 +2714,7 @@
       <c r="X5" s="13"/>
       <c r="Y5" s="13"/>
     </row>
-    <row r="6" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" ht="12.75" customHeight="1">
       <c r="A6" s="2">
         <v>45331</v>
       </c>
@@ -2781,7 +2781,7 @@
       <c r="X6" s="13"/>
       <c r="Y6" s="13"/>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25">
       <c r="A7" s="2">
         <v>45338</v>
       </c>
@@ -2850,7 +2850,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" ht="15" customHeight="1">
       <c r="A8" s="2">
         <v>45345</v>
       </c>
@@ -2917,7 +2917,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" ht="16.5" customHeight="1">
       <c r="A9" s="2">
         <v>45359</v>
       </c>
@@ -2970,7 +2970,7 @@
       <c r="X9" s="13"/>
       <c r="Y9" s="13"/>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25">
       <c r="A10" s="2">
         <v>45366</v>
       </c>
@@ -3039,7 +3039,7 @@
       <c r="X10" s="13"/>
       <c r="Y10" s="13"/>
     </row>
-    <row r="11" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" ht="15" customHeight="1">
       <c r="A11" s="2">
         <v>45379</v>
       </c>
@@ -3100,7 +3100,7 @@
       <c r="X11" s="13"/>
       <c r="Y11" s="13"/>
     </row>
-    <row r="12" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" ht="13.5" customHeight="1">
       <c r="A12" s="2">
         <v>45386</v>
       </c>
@@ -3163,7 +3163,7 @@
       <c r="X12" s="13"/>
       <c r="Y12" s="13"/>
     </row>
-    <row r="13" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" ht="16.5" customHeight="1">
       <c r="A13" s="2">
         <v>45387</v>
       </c>
@@ -3232,7 +3232,7 @@
       <c r="X13" s="13"/>
       <c r="Y13" s="13"/>
     </row>
-    <row r="14" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" ht="15.75" customHeight="1">
       <c r="A14" s="2">
         <v>45394</v>
       </c>
@@ -3293,7 +3293,7 @@
       <c r="X14" s="13"/>
       <c r="Y14" s="13"/>
     </row>
-    <row r="15" spans="1:25" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" ht="17.25" customHeight="1">
       <c r="A15" s="2">
         <v>45398</v>
       </c>
@@ -3362,7 +3362,7 @@
       <c r="X15" s="13"/>
       <c r="Y15" s="13"/>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25">
       <c r="A16" s="2">
         <v>45401</v>
       </c>
@@ -3425,7 +3425,7 @@
       <c r="X16" s="18"/>
       <c r="Y16" s="18"/>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25">
       <c r="A17" s="4">
         <v>45421</v>
       </c>
@@ -3496,7 +3496,7 @@
       <c r="X17" s="18"/>
       <c r="Y17" s="18"/>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25">
       <c r="A18" s="26">
         <v>45474</v>
       </c>
@@ -3547,7 +3547,7 @@
       <c r="X18" s="18"/>
       <c r="Y18" s="18"/>
     </row>
-    <row r="19" spans="1:25" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:25" ht="17.25" customHeight="1" thickBot="1">
       <c r="A19" s="26">
         <v>45505</v>
       </c>
@@ -3598,7 +3598,7 @@
       <c r="X19" s="18"/>
       <c r="Y19" s="18"/>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25">
       <c r="A20" s="26"/>
       <c r="B20" s="26"/>
       <c r="C20" s="26"/>
@@ -3645,7 +3645,7 @@
       <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="11.140625" customWidth="1"/>
@@ -3670,7 +3670,7 @@
     <col min="25" max="25" width="37.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3681,7 +3681,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" ht="30.75" thickBot="1">
       <c r="A2" s="145" t="s">
         <v>3</v>
       </c>
@@ -3758,7 +3758,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" ht="15" customHeight="1">
       <c r="A3" s="2">
         <v>45548</v>
       </c>
@@ -3823,7 +3823,7 @@
       <c r="X3" s="46"/>
       <c r="Y3" s="44"/>
     </row>
-    <row r="4" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="15" customHeight="1">
       <c r="A4" s="2">
         <v>45555</v>
       </c>
@@ -3872,7 +3872,7 @@
       <c r="X4" s="15"/>
       <c r="Y4" s="13"/>
     </row>
-    <row r="5" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" ht="15" customHeight="1">
       <c r="A5" s="2">
         <v>45562</v>
       </c>
@@ -3921,7 +3921,7 @@
       <c r="X5" s="15"/>
       <c r="Y5" s="13"/>
     </row>
-    <row r="6" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" ht="15" customHeight="1">
       <c r="A6" s="2">
         <v>45576</v>
       </c>
@@ -3970,7 +3970,7 @@
       <c r="X6" s="15"/>
       <c r="Y6" s="13"/>
     </row>
-    <row r="7" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" ht="15" customHeight="1">
       <c r="A7" s="2">
         <v>45583</v>
       </c>
@@ -4019,7 +4019,7 @@
       <c r="X7" s="15"/>
       <c r="Y7" s="13"/>
     </row>
-    <row r="8" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" ht="15" customHeight="1">
       <c r="A8" s="2">
         <v>45596</v>
       </c>
@@ -4068,7 +4068,7 @@
       <c r="X8" s="15"/>
       <c r="Y8" s="13"/>
     </row>
-    <row r="9" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" ht="15" customHeight="1">
       <c r="A9" s="2">
         <v>45604</v>
       </c>
@@ -4117,7 +4117,7 @@
       <c r="X9" s="15"/>
       <c r="Y9" s="13"/>
     </row>
-    <row r="10" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" ht="15" customHeight="1">
       <c r="A10" s="2">
         <v>45611</v>
       </c>
@@ -4166,7 +4166,7 @@
       <c r="X10" s="15"/>
       <c r="Y10" s="13"/>
     </row>
-    <row r="11" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" ht="15" customHeight="1">
       <c r="A11" s="2">
         <v>45625</v>
       </c>
@@ -4215,7 +4215,7 @@
       <c r="X11" s="15"/>
       <c r="Y11" s="13"/>
     </row>
-    <row r="12" spans="1:25" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:25" ht="15" customHeight="1" thickBot="1">
       <c r="A12" s="4">
         <v>45632</v>
       </c>
@@ -4272,20 +4272,20 @@
       <c r="X12" s="20"/>
       <c r="Y12" s="18"/>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25">
       <c r="A13" s="26"/>
       <c r="B13" s="26"/>
       <c r="C13" s="26"/>
       <c r="D13" s="26"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25">
       <c r="A14" s="26"/>
       <c r="B14" s="26"/>
       <c r="C14" s="26"/>
       <c r="D14" s="26"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10">
       <c r="A29" s="61"/>
       <c r="B29" s="61"/>
       <c r="C29" s="61"/>
@@ -4297,59 +4297,59 @@
       <c r="I29" s="61"/>
       <c r="J29" s="61"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10">
       <c r="A31" s="60"/>
       <c r="B31" s="60"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10">
       <c r="A32" s="60"/>
       <c r="B32" s="60"/>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2">
       <c r="A33" s="60"/>
       <c r="B33" s="60"/>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2">
       <c r="A34" s="60"/>
       <c r="B34" s="60"/>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2">
       <c r="A35" s="60"/>
       <c r="B35" s="60"/>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2">
       <c r="A36" s="60"/>
       <c r="B36" s="60"/>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2">
       <c r="A37" s="60"/>
       <c r="B37" s="60"/>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2">
       <c r="A38" s="60"/>
       <c r="B38" s="60"/>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2">
       <c r="A39" s="60"/>
       <c r="B39" s="60"/>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2">
       <c r="A40" s="60"/>
       <c r="B40" s="60"/>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2">
       <c r="A41" s="60"/>
       <c r="B41" s="60"/>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2">
       <c r="A42" s="60"/>
       <c r="B42" s="60"/>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2">
       <c r="A43" s="60"/>
       <c r="B43" s="60"/>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2">
       <c r="A44" s="60"/>
       <c r="B44" s="60"/>
     </row>
@@ -4383,7 +4383,7 @@
       <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.5703125" customWidth="1"/>
     <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1"/>
@@ -4411,7 +4411,7 @@
     <col min="25" max="25" width="37.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4422,7 +4422,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" ht="27.75" customHeight="1" thickBot="1">
       <c r="A2" s="64" t="s">
         <v>3</v>
       </c>
@@ -4499,7 +4499,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" ht="15" customHeight="1">
       <c r="A3" s="2">
         <v>45694</v>
       </c>
@@ -4551,7 +4551,7 @@
       <c r="X3" s="46"/>
       <c r="Y3" s="44"/>
     </row>
-    <row r="4" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="14.25" customHeight="1">
       <c r="A4" s="2">
         <v>45708</v>
       </c>
@@ -4609,7 +4609,7 @@
       <c r="X4" s="15"/>
       <c r="Y4" s="13"/>
     </row>
-    <row r="5" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" ht="14.25" customHeight="1">
       <c r="A5" s="2">
         <v>45722</v>
       </c>
@@ -4665,7 +4665,7 @@
       <c r="X5" s="15"/>
       <c r="Y5" s="13"/>
     </row>
-    <row r="6" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" ht="16.5" customHeight="1">
       <c r="A6" s="2">
         <v>45735</v>
       </c>
@@ -4721,7 +4721,7 @@
       <c r="X6" s="15"/>
       <c r="Y6" s="13"/>
     </row>
-    <row r="7" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" ht="18" customHeight="1">
       <c r="A7" s="2">
         <v>45750</v>
       </c>
@@ -4775,7 +4775,7 @@
       <c r="X7" s="15"/>
       <c r="Y7" s="13"/>
     </row>
-    <row r="8" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" ht="16.5" customHeight="1">
       <c r="A8" s="2">
         <v>45751</v>
       </c>
@@ -4834,7 +4834,7 @@
       <c r="X8" s="15"/>
       <c r="Y8" s="13"/>
     </row>
-    <row r="9" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" ht="15.75" customHeight="1">
       <c r="A9" s="2">
         <v>45757</v>
       </c>
@@ -4896,7 +4896,7 @@
       <c r="X9" s="15"/>
       <c r="Y9" s="13"/>
     </row>
-    <row r="10" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" ht="15.75" customHeight="1">
       <c r="A10" s="2">
         <v>45758</v>
       </c>
@@ -4950,7 +4950,7 @@
       <c r="X10" s="20"/>
       <c r="Y10" s="18"/>
     </row>
-    <row r="11" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" ht="15.75" customHeight="1">
       <c r="A11" s="4">
         <v>45764</v>
       </c>
@@ -5010,7 +5010,7 @@
       <c r="X11" s="35"/>
       <c r="Y11" s="35"/>
     </row>
-    <row r="12" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" ht="15.75" customHeight="1">
       <c r="A12" s="4">
         <v>45771</v>
       </c>
@@ -5071,7 +5071,7 @@
       <c r="X12" s="35"/>
       <c r="Y12" s="35"/>
     </row>
-    <row r="13" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" ht="15.75" customHeight="1">
       <c r="A13" s="2">
         <v>45785</v>
       </c>
@@ -5124,7 +5124,7 @@
       <c r="X13" s="35"/>
       <c r="Y13" s="35"/>
     </row>
-    <row r="14" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" ht="15.75" customHeight="1">
       <c r="A14" s="4">
         <v>45799</v>
       </c>
@@ -5170,7 +5170,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" ht="15.75" customHeight="1">
       <c r="A15" s="4">
         <v>45805</v>
       </c>
@@ -5204,101 +5204,101 @@
         <v>250</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" ht="15.75" customHeight="1">
       <c r="A16" s="75"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="A17" s="26"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2">
       <c r="A18" s="26"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2">
       <c r="A19" s="26"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2">
       <c r="A20" s="75"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2">
       <c r="A21" s="26"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2">
       <c r="A22" s="75"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2">
       <c r="A23" s="26"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2">
       <c r="A24" s="26"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2">
       <c r="A25" s="26"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2">
       <c r="A26" s="26"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2">
       <c r="A27" s="26"/>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2">
       <c r="A28" s="26"/>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2">
       <c r="B31" s="60"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2">
       <c r="A32" s="60"/>
       <c r="B32" s="60"/>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2">
       <c r="A33" s="60"/>
       <c r="B33" s="60"/>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2">
       <c r="A34" s="60"/>
       <c r="B34" s="60"/>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2">
       <c r="A35" s="60"/>
       <c r="B35" s="60"/>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2">
       <c r="A36" s="60"/>
       <c r="B36" s="60"/>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2">
       <c r="A37" s="60"/>
       <c r="B37" s="60"/>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2">
       <c r="A38" s="60"/>
       <c r="B38" s="60"/>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2">
       <c r="A39" s="60"/>
       <c r="B39" s="60"/>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2">
       <c r="A40" s="60"/>
       <c r="B40" s="60"/>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2">
       <c r="A41" s="60"/>
       <c r="B41" s="60"/>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2">
       <c r="A42" s="60"/>
       <c r="B42" s="60"/>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2">
       <c r="A43" s="60"/>
       <c r="B43" s="60"/>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2">
       <c r="A44" s="60"/>
       <c r="B44" s="60"/>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2">
       <c r="A45" s="60"/>
     </row>
   </sheetData>
@@ -5329,12 +5329,12 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="7" ySplit="19" topLeftCell="J20" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" customWidth="1"/>
@@ -5361,7 +5361,7 @@
     <col min="25" max="25" width="37.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5372,7 +5372,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="30">
       <c r="A2" s="78" t="s">
         <v>3</v>
       </c>
@@ -5449,7 +5449,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" ht="15" customHeight="1" thickBot="1">
       <c r="A3" s="159">
         <v>45911</v>
       </c>
@@ -5512,7 +5512,7 @@
       <c r="X3" s="46"/>
       <c r="Y3" s="44"/>
     </row>
-    <row r="4" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="15" customHeight="1">
       <c r="A4" s="160">
         <v>45917</v>
       </c>
@@ -5581,7 +5581,7 @@
       <c r="X4" s="15"/>
       <c r="Y4" s="13"/>
     </row>
-    <row r="5" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" ht="15" customHeight="1">
       <c r="A5" s="160">
         <v>45926</v>
       </c>
@@ -5639,7 +5639,7 @@
       <c r="X5" s="15"/>
       <c r="Y5" s="13"/>
     </row>
-    <row r="6" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" ht="15" customHeight="1">
       <c r="A6" s="160">
         <v>45939</v>
       </c>
@@ -5703,7 +5703,7 @@
       <c r="X6" s="15"/>
       <c r="Y6" s="13"/>
     </row>
-    <row r="7" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" ht="15" customHeight="1">
       <c r="A7" s="160">
         <v>45946</v>
       </c>
@@ -5760,7 +5760,7 @@
       <c r="X7" s="15"/>
       <c r="Y7" s="13"/>
     </row>
-    <row r="8" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" ht="15" customHeight="1">
       <c r="A8" s="160">
         <v>45953</v>
       </c>
@@ -5818,7 +5818,7 @@
       <c r="X8" s="15"/>
       <c r="Y8" s="13"/>
     </row>
-    <row r="9" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" ht="15" customHeight="1">
       <c r="A9" s="160">
         <v>45967</v>
       </c>
@@ -5880,7 +5880,7 @@
       <c r="X9" s="15"/>
       <c r="Y9" s="13"/>
     </row>
-    <row r="10" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" ht="15" customHeight="1">
       <c r="A10" s="160">
         <v>45974</v>
       </c>
@@ -5943,12 +5943,12 @@
       <c r="X10" s="15"/>
       <c r="Y10" s="13"/>
     </row>
-    <row r="11" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" ht="15" customHeight="1">
       <c r="A11" s="160">
         <v>45980</v>
       </c>
       <c r="B11" s="160" t="s">
-        <v>378</v>
+        <v>301</v>
       </c>
       <c r="C11" s="160" t="str">
         <f t="shared" si="2"/>
@@ -5962,7 +5962,7 @@
         <v>11</v>
       </c>
       <c r="F11" s="107" t="s">
-        <v>379</v>
+        <v>302</v>
       </c>
       <c r="G11" s="107" t="s">
         <v>269</v>
@@ -5971,15 +5971,15 @@
         <v>87</v>
       </c>
       <c r="I11" s="167" t="s">
-        <v>380</v>
+        <v>303</v>
       </c>
       <c r="J11" s="167" t="s">
-        <v>381</v>
+        <v>304</v>
       </c>
       <c r="K11" s="157"/>
       <c r="L11" s="156"/>
       <c r="M11" s="156" t="s">
-        <v>383</v>
+        <v>305</v>
       </c>
       <c r="N11" s="14"/>
       <c r="O11" s="35"/>
@@ -5994,7 +5994,7 @@
       <c r="X11" s="35"/>
       <c r="Y11" s="35"/>
     </row>
-    <row r="12" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" ht="16.5" customHeight="1">
       <c r="A12" s="160">
         <f>A10+7</f>
         <v>45981</v>
@@ -6015,7 +6015,7 @@
         <v>11</v>
       </c>
       <c r="F12" s="158" t="s">
-        <v>301</v>
+        <v>306</v>
       </c>
       <c r="G12" s="158" t="s">
         <v>68</v>
@@ -6024,13 +6024,13 @@
         <v>101</v>
       </c>
       <c r="I12" s="158" t="s">
-        <v>302</v>
+        <v>307</v>
       </c>
       <c r="J12" s="168" t="s">
-        <v>382</v>
+        <v>308</v>
       </c>
       <c r="K12" s="165" t="s">
-        <v>303</v>
+        <v>309</v>
       </c>
       <c r="L12" s="158"/>
       <c r="M12" s="158"/>
@@ -6047,7 +6047,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25">
       <c r="A13" s="160">
         <v>45986</v>
       </c>
@@ -6055,35 +6055,35 @@
         <v>28</v>
       </c>
       <c r="C13" s="103" t="s">
-        <v>304</v>
+        <v>310</v>
       </c>
       <c r="D13" s="103" t="s">
-        <v>305</v>
+        <v>311</v>
       </c>
       <c r="E13" s="103">
         <v>12</v>
       </c>
       <c r="F13" t="s">
-        <v>306</v>
+        <v>312</v>
       </c>
       <c r="G13" s="158" t="s">
-        <v>307</v>
+        <v>313</v>
       </c>
       <c r="H13" s="158" t="s">
         <v>40</v>
       </c>
       <c r="I13" s="158" t="s">
-        <v>308</v>
+        <v>314</v>
       </c>
       <c r="J13" s="158" t="s">
-        <v>309</v>
+        <v>315</v>
       </c>
       <c r="K13" s="165"/>
       <c r="L13" s="158"/>
       <c r="M13" s="158"/>
       <c r="N13" s="158"/>
     </row>
-    <row r="14" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" ht="15" customHeight="1">
       <c r="A14" s="160">
         <v>45988</v>
       </c>
@@ -6099,25 +6099,25 @@
         <v>Thursday</v>
       </c>
       <c r="E14" s="103">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F14" s="164" t="s">
-        <v>310</v>
+        <v>316</v>
       </c>
       <c r="G14" s="107" t="s">
-        <v>311</v>
+        <v>317</v>
       </c>
       <c r="H14" s="25" t="s">
         <v>211</v>
       </c>
       <c r="I14" s="97" t="s">
-        <v>312</v>
+        <v>318</v>
       </c>
       <c r="J14" s="97" t="s">
-        <v>313</v>
+        <v>319</v>
       </c>
       <c r="K14" s="157" t="s">
-        <v>314</v>
+        <v>320</v>
       </c>
       <c r="L14" s="25"/>
       <c r="M14" s="25"/>
@@ -6138,7 +6138,7 @@
       <c r="X14" s="15"/>
       <c r="Y14" s="13"/>
     </row>
-    <row r="15" spans="1:25" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:25" ht="15" customHeight="1" thickBot="1">
       <c r="A15" s="161">
         <v>45995</v>
       </c>
@@ -6154,30 +6154,29 @@
         <v>Thursday</v>
       </c>
       <c r="E15" s="106">
-        <f>E12+3</f>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F15" s="164" t="s">
-        <v>315</v>
+        <v>321</v>
       </c>
       <c r="G15" s="107" t="s">
-        <v>316</v>
+        <v>322</v>
       </c>
       <c r="H15" s="25" t="s">
         <v>101</v>
       </c>
       <c r="I15" s="97" t="s">
-        <v>317</v>
+        <v>323</v>
       </c>
       <c r="J15" s="132" t="s">
-        <v>318</v>
+        <v>324</v>
       </c>
       <c r="K15" s="157" t="s">
-        <v>319</v>
+        <v>325</v>
       </c>
       <c r="L15" s="25"/>
       <c r="M15" s="31" t="s">
-        <v>320</v>
+        <v>326</v>
       </c>
       <c r="N15" s="16" t="s">
         <v>44</v>
@@ -6202,35 +6201,35 @@
       <c r="X15" s="15"/>
       <c r="Y15" s="13"/>
     </row>
-    <row r="16" spans="1:25" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:25" ht="15" customHeight="1" thickBot="1">
       <c r="A16" s="26"/>
       <c r="B16" s="26"/>
       <c r="C16" s="26"/>
       <c r="X16" s="20"/>
       <c r="Y16" s="18"/>
     </row>
-    <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="15" customHeight="1">
       <c r="A17" s="26"/>
       <c r="B17" s="26"/>
       <c r="C17" s="26"/>
     </row>
-    <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="15" customHeight="1">
       <c r="A18" s="26"/>
       <c r="B18" s="26"/>
       <c r="C18" s="26"/>
     </row>
-    <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="15" customHeight="1">
       <c r="A19" s="26"/>
       <c r="B19" s="26"/>
       <c r="C19" s="26"/>
     </row>
-    <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:3" ht="15" customHeight="1"/>
+    <row r="21" spans="1:3" ht="15" customHeight="1"/>
+    <row r="22" spans="1:3" ht="15" customHeight="1"/>
+    <row r="23" spans="1:3" ht="15" customHeight="1"/>
+    <row r="24" spans="1:3" ht="15" customHeight="1"/>
+    <row r="25" spans="1:3" ht="15" customHeight="1"/>
+    <row r="26" spans="1:3" ht="15" customHeight="1"/>
   </sheetData>
   <protectedRanges>
     <protectedRange algorithmName="SHA-512" hashValue="pQyTzP/d7t5ThMimBt5mu8gGozgAm1OwF6BMILsn5/kmtZ5mZf81NMi09wwU8mvtItxf0EVNWa6V4MCa0DKeSQ==" saltValue="NzZBiAQ1yFjat+SeIqh2Uw==" spinCount="100000" sqref="A3:E19" name="Range3_1"/>
@@ -6266,7 +6265,7 @@
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.5703125" customWidth="1"/>
     <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1"/>
@@ -6293,7 +6292,7 @@
     <col min="25" max="25" width="37.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6304,7 +6303,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="30">
       <c r="A2" s="64" t="s">
         <v>3</v>
       </c>
@@ -6381,7 +6380,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" ht="15" customHeight="1">
       <c r="A3" s="75">
         <v>46051</v>
       </c>
@@ -6400,19 +6399,19 @@
         <v>1</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>321</v>
+        <v>327</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>322</v>
+        <v>328</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>87</v>
       </c>
       <c r="I3" s="98" t="s">
-        <v>323</v>
+        <v>329</v>
       </c>
       <c r="J3" s="98" t="s">
-        <v>323</v>
+        <v>329</v>
       </c>
       <c r="K3" s="73"/>
       <c r="L3" s="40"/>
@@ -6430,7 +6429,7 @@
       <c r="X3" s="46"/>
       <c r="Y3" s="44"/>
     </row>
-    <row r="4" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="15.75" customHeight="1">
       <c r="A4" s="75">
         <f>A3+14</f>
         <v>46065</v>
@@ -6451,19 +6450,19 @@
         <v>3</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>324</v>
+        <v>330</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>323</v>
+        <v>329</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>323</v>
+        <v>329</v>
       </c>
       <c r="I4" s="98" t="s">
-        <v>323</v>
+        <v>329</v>
       </c>
       <c r="J4" s="98" t="s">
-        <v>323</v>
+        <v>329</v>
       </c>
       <c r="K4" s="102"/>
       <c r="L4" s="5"/>
@@ -6481,7 +6480,7 @@
       <c r="X4" s="15"/>
       <c r="Y4" s="13"/>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25">
       <c r="A5" s="75">
         <f t="shared" ref="A5:A9" si="2">A4+14</f>
         <v>46079</v>
@@ -6502,29 +6501,29 @@
         <v>5</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>325</v>
+        <v>331</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>326</v>
+        <v>332</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>87</v>
       </c>
       <c r="I5" s="98" t="s">
-        <v>323</v>
+        <v>329</v>
       </c>
       <c r="J5" s="98" t="s">
-        <v>323</v>
+        <v>329</v>
       </c>
       <c r="K5" s="102"/>
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
       <c r="N5" s="16"/>
       <c r="O5" s="35" t="s">
-        <v>327</v>
+        <v>333</v>
       </c>
       <c r="P5" s="5" t="s">
-        <v>328</v>
+        <v>334</v>
       </c>
       <c r="Q5" s="5"/>
       <c r="R5" s="5"/>
@@ -6536,7 +6535,7 @@
       <c r="X5" s="15"/>
       <c r="Y5" s="13"/>
     </row>
-    <row r="6" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" ht="15.75" customHeight="1">
       <c r="A6" s="75">
         <f>A5+14</f>
         <v>46093</v>
@@ -6557,7 +6556,7 @@
         <v>7</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>329</v>
+        <v>335</v>
       </c>
       <c r="G6" s="14" t="s">
         <v>152</v>
@@ -6566,10 +6565,10 @@
         <v>95</v>
       </c>
       <c r="I6" s="98" t="s">
-        <v>323</v>
+        <v>329</v>
       </c>
       <c r="J6" s="98" t="s">
-        <v>323</v>
+        <v>329</v>
       </c>
       <c r="K6" s="102"/>
       <c r="L6" s="5"/>
@@ -6587,7 +6586,7 @@
       <c r="X6" s="15"/>
       <c r="Y6" s="13"/>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25">
       <c r="A7" s="75">
         <f t="shared" si="2"/>
         <v>46107</v>
@@ -6608,19 +6607,19 @@
         <v>9</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>324</v>
+        <v>330</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>323</v>
+        <v>329</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>323</v>
+        <v>329</v>
       </c>
       <c r="I7" s="98" t="s">
-        <v>323</v>
+        <v>329</v>
       </c>
       <c r="J7" s="98" t="s">
-        <v>323</v>
+        <v>329</v>
       </c>
       <c r="K7" s="102"/>
       <c r="L7" s="5"/>
@@ -6638,7 +6637,7 @@
       <c r="X7" s="15"/>
       <c r="Y7" s="13"/>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25">
       <c r="A8" s="75">
         <f t="shared" si="2"/>
         <v>46121</v>
@@ -6659,19 +6658,19 @@
         <v>11</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>324</v>
+        <v>330</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>323</v>
+        <v>329</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>323</v>
+        <v>329</v>
       </c>
       <c r="I8" s="98" t="s">
-        <v>323</v>
+        <v>329</v>
       </c>
       <c r="J8" s="98" t="s">
-        <v>323</v>
+        <v>329</v>
       </c>
       <c r="K8" s="102"/>
       <c r="L8" s="5"/>
@@ -6689,7 +6688,7 @@
       <c r="X8" s="15"/>
       <c r="Y8" s="13"/>
     </row>
-    <row r="9" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" ht="18.75" customHeight="1">
       <c r="A9" s="75">
         <f t="shared" si="2"/>
         <v>46135</v>
@@ -6710,19 +6709,19 @@
         <v>13</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>324</v>
+        <v>330</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>323</v>
+        <v>329</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>323</v>
+        <v>329</v>
       </c>
       <c r="I9" s="98" t="s">
-        <v>323</v>
+        <v>329</v>
       </c>
       <c r="J9" s="98" t="s">
-        <v>323</v>
+        <v>329</v>
       </c>
       <c r="K9" s="102"/>
       <c r="L9" s="5"/>
@@ -6740,24 +6739,24 @@
       <c r="X9" s="15"/>
       <c r="Y9" s="13"/>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25">
       <c r="A10" s="26"/>
       <c r="B10" s="26"/>
       <c r="C10" s="26"/>
       <c r="X10" s="20"/>
       <c r="Y10" s="18"/>
     </row>
-    <row r="11" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" ht="12.75" customHeight="1">
       <c r="A11" s="26"/>
       <c r="B11" s="26"/>
       <c r="C11" s="26"/>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25">
       <c r="A12" s="26"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25">
       <c r="A13" s="26"/>
       <c r="B13" s="26"/>
       <c r="C13" s="26"/>
@@ -6783,231 +6782,231 @@
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="31.28515625" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
     <col min="3" max="3" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="55" t="s">
-        <v>331</v>
+        <v>337</v>
       </c>
       <c r="B2" s="54" t="s">
-        <v>332</v>
+        <v>338</v>
       </c>
       <c r="C2" s="54" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="136" t="s">
-        <v>334</v>
+        <v>340</v>
       </c>
       <c r="B3" s="137"/>
       <c r="C3" s="138" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="5" t="s">
-        <v>335</v>
+        <v>341</v>
       </c>
       <c r="B4" s="52"/>
       <c r="C4" s="50" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" s="52" t="s">
-        <v>336</v>
+        <v>342</v>
       </c>
       <c r="B5" s="52"/>
       <c r="C5" s="50" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="52" t="s">
-        <v>338</v>
+        <v>344</v>
       </c>
       <c r="B6" s="52" t="s">
-        <v>339</v>
+        <v>345</v>
       </c>
       <c r="C6" s="50" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" s="52" t="s">
-        <v>340</v>
+        <v>346</v>
       </c>
       <c r="B7" s="52" t="s">
-        <v>341</v>
+        <v>347</v>
       </c>
       <c r="C7" s="50" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" s="52" t="s">
-        <v>342</v>
+        <v>348</v>
       </c>
       <c r="B8" s="52" t="s">
-        <v>343</v>
+        <v>349</v>
       </c>
       <c r="C8" s="50" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" s="52" t="s">
-        <v>344</v>
+        <v>350</v>
       </c>
       <c r="B9" s="52"/>
       <c r="C9" s="50"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" s="52" t="s">
+        <v>351</v>
+      </c>
+      <c r="B10" s="52" t="s">
+        <v>352</v>
+      </c>
+      <c r="C10" s="50" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="52" t="s">
+        <v>354</v>
+      </c>
+      <c r="B11" s="52" t="s">
+        <v>355</v>
+      </c>
+      <c r="C11" s="50" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="52" t="s">
+        <v>357</v>
+      </c>
+      <c r="B12" s="52" t="s">
+        <v>358</v>
+      </c>
+      <c r="C12" s="50" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="52" t="s">
+        <v>359</v>
+      </c>
+      <c r="B13" s="52" t="s">
+        <v>360</v>
+      </c>
+      <c r="C13" s="50" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="B14" s="52" t="s">
+        <v>362</v>
+      </c>
+      <c r="C14" s="50" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="52" t="s">
+        <v>363</v>
+      </c>
+      <c r="B15" s="52" t="s">
+        <v>364</v>
+      </c>
+      <c r="C15" s="50" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="137" t="s">
+        <v>321</v>
+      </c>
+      <c r="B16" s="137" t="s">
+        <v>365</v>
+      </c>
+      <c r="C16" s="139" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="52" t="s">
+        <v>367</v>
+      </c>
+      <c r="B17" s="52" t="s">
+        <v>368</v>
+      </c>
+      <c r="C17" s="50" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="52" t="s">
+        <v>369</v>
+      </c>
+      <c r="B18" s="52" t="s">
         <v>345</v>
-      </c>
-      <c r="B10" s="52" t="s">
-        <v>346</v>
-      </c>
-      <c r="C10" s="50" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="52" t="s">
-        <v>348</v>
-      </c>
-      <c r="B11" s="52" t="s">
-        <v>349</v>
-      </c>
-      <c r="C11" s="50" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="52" t="s">
-        <v>351</v>
-      </c>
-      <c r="B12" s="52" t="s">
-        <v>352</v>
-      </c>
-      <c r="C12" s="50" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="52" t="s">
-        <v>353</v>
-      </c>
-      <c r="B13" s="52" t="s">
-        <v>354</v>
-      </c>
-      <c r="C13" s="50" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="52" t="s">
-        <v>355</v>
-      </c>
-      <c r="B14" s="52" t="s">
-        <v>356</v>
-      </c>
-      <c r="C14" s="50" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="52" t="s">
-        <v>357</v>
-      </c>
-      <c r="B15" s="52" t="s">
-        <v>358</v>
-      </c>
-      <c r="C15" s="50" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="137" t="s">
-        <v>315</v>
-      </c>
-      <c r="B16" s="137" t="s">
-        <v>359</v>
-      </c>
-      <c r="C16" s="139" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="52" t="s">
-        <v>361</v>
-      </c>
-      <c r="B17" s="52" t="s">
-        <v>362</v>
-      </c>
-      <c r="C17" s="50" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="52" t="s">
-        <v>363</v>
-      </c>
-      <c r="B18" s="52" t="s">
-        <v>339</v>
       </c>
       <c r="C18" s="50" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="A19" s="53" t="s">
-        <v>364</v>
+        <v>370</v>
       </c>
       <c r="B19" s="53" t="s">
         <v>230</v>
       </c>
       <c r="C19" s="51" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>363</v>
+        <v>369</v>
       </c>
       <c r="B24" t="s">
-        <v>339</v>
+        <v>345</v>
       </c>
       <c r="C24" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>364</v>
+        <v>370</v>
       </c>
       <c r="B25" t="s">
         <v>230</v>
       </c>
       <c r="C25" t="s">
-        <v>365</v>
+        <v>371</v>
       </c>
     </row>
   </sheetData>
@@ -7028,24 +7027,24 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
     <col min="6" max="6" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1">
       <c r="A1" s="135" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="131" t="s">
-        <v>367</v>
+        <v>373</v>
       </c>
       <c r="C1" s="130" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" thickTop="1">
       <c r="A2" s="133">
         <v>45911</v>
       </c>
@@ -7053,7 +7052,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="134" t="s">
-        <v>369</v>
+        <v>375</v>
       </c>
       <c r="F2" s="75">
         <v>45911</v>
@@ -7073,7 +7072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="133">
         <f>A2+7</f>
         <v>45918</v>
@@ -7083,7 +7082,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="134" t="s">
-        <v>369</v>
+        <v>375</v>
       </c>
       <c r="F3" s="75">
         <v>45926</v>
@@ -7104,7 +7103,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="133">
         <f t="shared" ref="A4:A12" si="0">A3+7</f>
         <v>45925</v>
@@ -7114,7 +7113,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="134" t="s">
-        <v>369</v>
+        <v>375</v>
       </c>
       <c r="F4" s="75">
         <v>45939</v>
@@ -7135,7 +7134,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="133">
         <f t="shared" si="0"/>
         <v>45932</v>
@@ -7145,7 +7144,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="134" t="s">
-        <v>369</v>
+        <v>375</v>
       </c>
       <c r="F5" s="75">
         <v>45946</v>
@@ -7163,7 +7162,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="133">
         <f t="shared" si="0"/>
         <v>45939</v>
@@ -7173,7 +7172,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="134" t="s">
-        <v>369</v>
+        <v>375</v>
       </c>
       <c r="F6" s="75">
         <v>45953</v>
@@ -7194,7 +7193,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" s="133">
         <f t="shared" si="0"/>
         <v>45946</v>
@@ -7204,7 +7203,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="134" t="s">
-        <v>324</v>
+        <v>330</v>
       </c>
       <c r="F7" s="75">
         <v>45967</v>
@@ -7225,7 +7224,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" s="133">
         <f t="shared" si="0"/>
         <v>45953</v>
@@ -7235,7 +7234,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="134" t="s">
-        <v>370</v>
+        <v>376</v>
       </c>
       <c r="F8" s="75">
         <v>45974</v>
@@ -7255,7 +7254,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9" s="133">
         <f t="shared" si="0"/>
         <v>45960</v>
@@ -7265,7 +7264,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="134" t="s">
-        <v>369</v>
+        <v>375</v>
       </c>
       <c r="F9" s="75">
         <v>45981</v>
@@ -7286,7 +7285,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10" s="133">
         <f t="shared" si="0"/>
         <v>45967</v>
@@ -7296,7 +7295,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="134" t="s">
-        <v>370</v>
+        <v>376</v>
       </c>
       <c r="F10" s="75">
         <v>45995</v>
@@ -7317,7 +7316,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" s="133">
         <f t="shared" si="0"/>
         <v>45974</v>
@@ -7327,10 +7326,10 @@
         <v>10</v>
       </c>
       <c r="C11" s="134" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="133">
         <f t="shared" si="0"/>
         <v>45981</v>
@@ -7340,10 +7339,10 @@
         <v>11</v>
       </c>
       <c r="C12" s="134" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" s="133">
         <f t="shared" ref="A13:A14" si="6">A12+7</f>
         <v>45988</v>
@@ -7353,10 +7352,10 @@
         <v>12</v>
       </c>
       <c r="C13" s="134" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" s="133">
         <f t="shared" si="6"/>
         <v>45995</v>
@@ -7366,15 +7365,15 @@
         <v>13</v>
       </c>
       <c r="C14" s="134" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" s="133"/>
       <c r="B15" s="134"/>
       <c r="C15" s="134"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="G16" s="26"/>
     </row>
   </sheetData>
@@ -7405,7 +7404,7 @@
       <selection activeCell="F8" sqref="F8:H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.42578125" customWidth="1"/>
     <col min="2" max="2" width="9.140625" customWidth="1"/>
@@ -7417,17 +7416,17 @@
     <col min="9" max="9" width="64.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="23.25">
       <c r="A2" s="91" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="18.75">
       <c r="A3" s="79" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="37.5" x14ac:dyDescent="0.25">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="37.5">
       <c r="A5" s="80" t="s">
         <v>3</v>
       </c>
@@ -7450,13 +7449,13 @@
         <v>9</v>
       </c>
       <c r="H5" s="82" t="s">
-        <v>373</v>
+        <v>379</v>
       </c>
       <c r="I5" s="81" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="18.75">
       <c r="A6" s="92">
         <v>45694</v>
       </c>
@@ -7480,10 +7479,10 @@
       </c>
       <c r="H6" s="85"/>
       <c r="I6" s="84" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="18.75">
       <c r="A7" s="83">
         <v>45708</v>
       </c>
@@ -7512,7 +7511,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="18.75">
       <c r="A8" s="83">
         <v>45722</v>
       </c>
@@ -7539,7 +7538,7 @@
       </c>
       <c r="I8" s="86"/>
     </row>
-    <row r="9" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="18.75">
       <c r="A9" s="83">
         <v>45735</v>
       </c>
@@ -7550,7 +7549,7 @@
         <v>198</v>
       </c>
       <c r="D9" s="94" t="s">
-        <v>374</v>
+        <v>380</v>
       </c>
       <c r="E9" s="94">
         <v>8</v>
@@ -7565,10 +7564,10 @@
         <v>206</v>
       </c>
       <c r="I9" s="86" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="18.75">
       <c r="A10" s="83">
         <v>45744</v>
       </c>
@@ -7595,7 +7594,7 @@
       </c>
       <c r="I10" s="86"/>
     </row>
-    <row r="11" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="18.75">
       <c r="A11" s="83">
         <v>45750</v>
       </c>
@@ -7612,17 +7611,17 @@
         <v>10</v>
       </c>
       <c r="F11" s="87" t="s">
-        <v>375</v>
+        <v>381</v>
       </c>
       <c r="G11" s="87" t="s">
         <v>68</v>
       </c>
       <c r="H11" s="87"/>
       <c r="I11" s="86" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="18.75">
       <c r="A12" s="83">
         <v>45758</v>
       </c>
@@ -7648,10 +7647,10 @@
         <v>31</v>
       </c>
       <c r="I12" s="86" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="18.75">
       <c r="A13" s="83">
         <v>45764</v>
       </c>
@@ -7668,13 +7667,13 @@
         <v>12</v>
       </c>
       <c r="F13" s="87" t="s">
-        <v>376</v>
+        <v>382</v>
       </c>
       <c r="G13" s="87"/>
       <c r="H13" s="87"/>
       <c r="I13" s="86"/>
     </row>
-    <row r="14" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="18.75">
       <c r="A14" s="88">
         <v>45771</v>
       </c>
@@ -7691,7 +7690,7 @@
         <v>13</v>
       </c>
       <c r="F14" s="90" t="s">
-        <v>377</v>
+        <v>383</v>
       </c>
       <c r="G14" s="90" t="s">
         <v>77</v>
@@ -7703,7 +7702,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="20" spans="8:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="20" spans="8:8" ht="18.75">
       <c r="H20" s="79"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added next sem talks
</commit_message>
<xml_diff>
--- a/data/MACSI seminar series.xlsx
+++ b/data/MACSI seminar series.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ulcampus-my.sharepoint.com/personal/david_osullivan_ul_ie/Documents/Academic_work/_Misc/MACSI_Seminars/macsi-seminars.github.io/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="135" documentId="13_ncr:1_{12BE53B5-C8C7-44FE-8280-19C653D9122E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7D012B5B-DAEC-4BB1-A813-804AB271D699}"/>
+  <xr:revisionPtr revIDLastSave="138" documentId="13_ncr:1_{12BE53B5-C8C7-44FE-8280-19C653D9122E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{86A80FED-3B08-4A0A-80AB-9897C049654C}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AY2023-2024 Sem 2" sheetId="3" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="386">
   <si>
     <t>Fill in as much of the green boxes as possible. Ideally, this would be before you have finished your visitors travel dates (just to avoid double booking).</t>
   </si>
@@ -1114,6 +1114,9 @@
   </si>
   <si>
     <t>Leah Keating</t>
+  </si>
+  <si>
+    <t>Stuart Thomson</t>
   </si>
   <si>
     <t>Wednesday</t>
@@ -6265,7 +6268,7 @@
   <dimension ref="A1:Y14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6610,13 +6613,13 @@
         <v>9</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>330</v>
+        <v>336</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>329</v>
+        <v>52</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>329</v>
+        <v>87</v>
       </c>
       <c r="I7" s="98" t="s">
         <v>329</v>
@@ -6651,13 +6654,13 @@
         <v>209</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="E8">
         <v>11</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="G8" s="14" t="s">
         <v>77</v>
@@ -6841,23 +6844,23 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="55" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="B2" s="54" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="C2" s="54" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="136" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="B3" s="137"/>
       <c r="C3" s="138" t="s">
@@ -6866,7 +6869,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="5" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B4" s="52"/>
       <c r="C4" s="50" t="s">
@@ -6875,19 +6878,19 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="52" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B5" s="52"/>
       <c r="C5" s="50" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="52" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B6" s="52" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="C6" s="50" t="s">
         <v>87</v>
@@ -6895,10 +6898,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="52" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B7" s="52" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C7" s="50" t="s">
         <v>87</v>
@@ -6906,10 +6909,10 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="52" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B8" s="52" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="C8" s="50" t="s">
         <v>101</v>
@@ -6917,75 +6920,75 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="52" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B9" s="52"/>
       <c r="C9" s="50"/>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="52" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B10" s="52" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C10" s="50" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="52" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B11" s="52" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="C11" s="50" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="52" t="s">
+        <v>360</v>
+      </c>
+      <c r="B12" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="C12" s="50" t="s">
         <v>359</v>
-      </c>
-      <c r="B12" s="52" t="s">
-        <v>360</v>
-      </c>
-      <c r="C12" s="50" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="52" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B13" s="52" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="C13" s="50" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="52" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="B14" s="52" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="C14" s="50" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="52" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B15" s="52" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="C15" s="50" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -6993,29 +6996,29 @@
         <v>321</v>
       </c>
       <c r="B16" s="137" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C16" s="139" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="52" t="s">
+        <v>370</v>
+      </c>
+      <c r="B17" s="52" t="s">
+        <v>371</v>
+      </c>
+      <c r="C17" s="50" t="s">
         <v>369</v>
-      </c>
-      <c r="B17" s="52" t="s">
-        <v>370</v>
-      </c>
-      <c r="C17" s="50" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="52" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="B18" s="52" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="C18" s="50" t="s">
         <v>87</v>
@@ -7023,26 +7026,26 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="53" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B19" s="53" t="s">
         <v>230</v>
       </c>
       <c r="C19" s="51" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="B24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="C24" t="s">
         <v>87</v>
@@ -7050,13 +7053,13 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B25" t="s">
         <v>230</v>
       </c>
       <c r="C25" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
   </sheetData>
@@ -7088,10 +7091,10 @@
         <v>3</v>
       </c>
       <c r="B1" s="131" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C1" s="130" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickTop="1">
@@ -7102,7 +7105,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="134" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="F2" s="75">
         <v>45911</v>
@@ -7132,7 +7135,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="134" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="F3" s="75">
         <v>45926</v>
@@ -7163,7 +7166,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="134" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="F4" s="75">
         <v>45939</v>
@@ -7194,7 +7197,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="134" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="F5" s="75">
         <v>45946</v>
@@ -7222,7 +7225,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="134" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="F6" s="75">
         <v>45953</v>
@@ -7284,7 +7287,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="134" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="F8" s="75">
         <v>45974</v>
@@ -7314,7 +7317,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="134" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="F9" s="75">
         <v>45981</v>
@@ -7345,7 +7348,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="134" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="F10" s="75">
         <v>45995</v>
@@ -7376,7 +7379,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="134" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -7389,7 +7392,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="134" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -7415,7 +7418,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="134" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -7468,12 +7471,12 @@
   <sheetData>
     <row r="2" spans="1:9" ht="23.25">
       <c r="A2" s="91" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="18.75">
       <c r="A3" s="79" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="37.5">
@@ -7499,7 +7502,7 @@
         <v>9</v>
       </c>
       <c r="H5" s="82" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="I5" s="81" t="s">
         <v>11</v>
@@ -7599,7 +7602,7 @@
         <v>198</v>
       </c>
       <c r="D9" s="94" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="E9" s="94">
         <v>8</v>
@@ -7661,7 +7664,7 @@
         <v>10</v>
       </c>
       <c r="F11" s="87" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="G11" s="87" t="s">
         <v>68</v>
@@ -7717,7 +7720,7 @@
         <v>12</v>
       </c>
       <c r="F13" s="87" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="G13" s="87"/>
       <c r="H13" s="87"/>
@@ -7740,7 +7743,7 @@
         <v>13</v>
       </c>
       <c r="F14" s="90" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="G14" s="90" t="s">
         <v>77</v>

</xml_diff>

<commit_message>
added CF to schedule
</commit_message>
<xml_diff>
--- a/data/MACSI seminar series.xlsx
+++ b/data/MACSI seminar series.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29728"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29721"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ulcampus-my.sharepoint.com/personal/david_osullivan_ul_ie/Documents/Academic_work/_Misc/MACSI Seminars/macsi-seminars.github.io/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="227" documentId="13_ncr:1_{12BE53B5-C8C7-44FE-8280-19C653D9122E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C062F483-58F5-4F41-83B0-E516E91A3497}"/>
+  <xr:revisionPtr revIDLastSave="275" documentId="13_ncr:1_{12BE53B5-C8C7-44FE-8280-19C653D9122E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C542F36B-8CB7-4DDD-B53A-BB7BB2D15EE6}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="8" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AY2023-2024 Sem 2" sheetId="3" r:id="rId1"/>
@@ -21,7 +21,8 @@
     <sheet name="AY2026-2027 Sem 1" sheetId="10" r:id="rId6"/>
     <sheet name="Possbile speaker (reserve list)" sheetId="4" r:id="rId7"/>
     <sheet name="Open dates" sheetId="8" r:id="rId8"/>
-    <sheet name="Printed A2002" sheetId="5" state="hidden" r:id="rId9"/>
+    <sheet name="Sheet1" sheetId="11" r:id="rId9"/>
+    <sheet name="Printed A2002" sheetId="5" state="hidden" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="994" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="994" uniqueCount="403">
   <si>
     <t>Fill in as much of the green boxes as possible. Ideally, this would be before you have finished your visitors travel dates (just to avoid double booking).</t>
   </si>
@@ -1141,6 +1142,27 @@
     <t>Stuart Thomson</t>
   </si>
   <si>
+    <t>Cornelius Fritz</t>
+  </si>
+  <si>
+    <t>Trinity college Dublin</t>
+  </si>
+  <si>
+    <t>Scalable Durational Event Models: Application to Physical and Digital Interactions</t>
+  </si>
+  <si>
+    <t>Durable interactions are ubiquitous in social network analysis and are increasingly observed with precise time stamps. Phone and video calls, for example, are events to which a specific duration can be assigned. We term data encoding interactions with the start and end times “durational event data”. Recent advances in data collection have enabled the observation of such data over extended periods of time and between large populations of actors. Methodologically, we propose the Durational Event Model, an extension of Relational Event Models that decouples the modeling of event incidence from event duration. Computationally, we derive a fast, memory-efficient, and exact block-coordinate ascent algorithm to facilitate large-scale inference. Theoretical complexity analysis and numerical simulations demonstrate computational superiority of this approach over state-of-the-art methods. We apply the model to physical and digital interactions among college students in Copenhagen.  Our empirical findings reveal that past interactions drive physical interactions, whereas digital interactions are influenced predominantly by friendship ties and prior dyadic contact. </t>
+  </si>
+  <si>
+    <t>https://scholar.google.de/citations?user=0X7D4mwAAAAJ&amp;hl=en</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://arxiv.org/abs/2504.00049 </t>
+  </si>
+  <si>
+    <t>https://www.tcd.ie/scss/people/academic-staff/fritzc/ ; https://www.corneliusfritz.com/about/</t>
+  </si>
+  <si>
     <t xml:space="preserve">Chris Howland </t>
   </si>
   <si>
@@ -1304,7 +1326,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1386,6 +1408,14 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1834,7 +1864,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="170">
+  <cellXfs count="173">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -2119,6 +2149,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="12" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3688,6 +3721,326 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2BB5C5F-5790-4A91-A6E8-8841719DA1FC}">
+  <dimension ref="A2:I20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8:H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.7109375" customWidth="1"/>
+    <col min="7" max="7" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.42578125" customWidth="1"/>
+    <col min="9" max="9" width="64.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:9" ht="23.25">
+      <c r="A2" s="91" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="18.75">
+      <c r="A3" s="79" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="37.5">
+      <c r="A5" s="80" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="80" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="80" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="80" t="s">
+        <v>137</v>
+      </c>
+      <c r="E5" s="80" t="s">
+        <v>189</v>
+      </c>
+      <c r="F5" s="80" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="80" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="82" t="s">
+        <v>398</v>
+      </c>
+      <c r="I5" s="81" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="18.75">
+      <c r="A6" s="92">
+        <v>45694</v>
+      </c>
+      <c r="B6" s="92" t="s">
+        <v>190</v>
+      </c>
+      <c r="C6" s="92" t="s">
+        <v>191</v>
+      </c>
+      <c r="D6" s="93" t="s">
+        <v>278</v>
+      </c>
+      <c r="E6" s="93">
+        <v>2</v>
+      </c>
+      <c r="F6" s="85" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" s="85" t="s">
+        <v>68</v>
+      </c>
+      <c r="H6" s="85"/>
+      <c r="I6" s="84" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="18.75">
+      <c r="A7" s="83">
+        <v>45708</v>
+      </c>
+      <c r="B7" s="83" t="s">
+        <v>190</v>
+      </c>
+      <c r="C7" s="83" t="s">
+        <v>191</v>
+      </c>
+      <c r="D7" s="94" t="s">
+        <v>278</v>
+      </c>
+      <c r="E7" s="94">
+        <v>4</v>
+      </c>
+      <c r="F7" s="87" t="s">
+        <v>194</v>
+      </c>
+      <c r="G7" s="87" t="s">
+        <v>195</v>
+      </c>
+      <c r="H7" s="87" t="s">
+        <v>78</v>
+      </c>
+      <c r="I7" s="86" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="18.75">
+      <c r="A8" s="83">
+        <v>45722</v>
+      </c>
+      <c r="B8" s="83" t="s">
+        <v>190</v>
+      </c>
+      <c r="C8" s="83" t="s">
+        <v>198</v>
+      </c>
+      <c r="D8" s="94" t="s">
+        <v>278</v>
+      </c>
+      <c r="E8" s="94">
+        <v>6</v>
+      </c>
+      <c r="F8" s="87" t="s">
+        <v>199</v>
+      </c>
+      <c r="G8" s="87" t="s">
+        <v>68</v>
+      </c>
+      <c r="H8" s="87" t="s">
+        <v>200</v>
+      </c>
+      <c r="I8" s="86"/>
+    </row>
+    <row r="9" spans="1:9" ht="18.75">
+      <c r="A9" s="83">
+        <v>45735</v>
+      </c>
+      <c r="B9" s="83" t="s">
+        <v>139</v>
+      </c>
+      <c r="C9" s="83" t="s">
+        <v>198</v>
+      </c>
+      <c r="D9" s="94" t="s">
+        <v>399</v>
+      </c>
+      <c r="E9" s="94">
+        <v>8</v>
+      </c>
+      <c r="F9" s="87" t="s">
+        <v>204</v>
+      </c>
+      <c r="G9" s="87" t="s">
+        <v>205</v>
+      </c>
+      <c r="H9" s="87" t="s">
+        <v>206</v>
+      </c>
+      <c r="I9" s="86" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="18.75">
+      <c r="A10" s="83">
+        <v>45744</v>
+      </c>
+      <c r="B10" s="83" t="s">
+        <v>190</v>
+      </c>
+      <c r="C10" s="83" t="s">
+        <v>198</v>
+      </c>
+      <c r="D10" s="94" t="s">
+        <v>214</v>
+      </c>
+      <c r="E10" s="94">
+        <v>9</v>
+      </c>
+      <c r="F10" s="87" t="s">
+        <v>222</v>
+      </c>
+      <c r="G10" s="87" t="s">
+        <v>223</v>
+      </c>
+      <c r="H10" s="87" t="s">
+        <v>224</v>
+      </c>
+      <c r="I10" s="86"/>
+    </row>
+    <row r="11" spans="1:9" ht="18.75">
+      <c r="A11" s="83">
+        <v>45750</v>
+      </c>
+      <c r="B11" s="83" t="s">
+        <v>190</v>
+      </c>
+      <c r="C11" s="83" t="s">
+        <v>209</v>
+      </c>
+      <c r="D11" s="94" t="s">
+        <v>278</v>
+      </c>
+      <c r="E11" s="94">
+        <v>10</v>
+      </c>
+      <c r="F11" s="87" t="s">
+        <v>400</v>
+      </c>
+      <c r="G11" s="87" t="s">
+        <v>68</v>
+      </c>
+      <c r="H11" s="87"/>
+      <c r="I11" s="86" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="18.75">
+      <c r="A12" s="83">
+        <v>45758</v>
+      </c>
+      <c r="B12" s="83" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="83" t="s">
+        <v>209</v>
+      </c>
+      <c r="D12" s="94" t="s">
+        <v>214</v>
+      </c>
+      <c r="E12" s="94">
+        <v>11</v>
+      </c>
+      <c r="F12" s="87" t="s">
+        <v>229</v>
+      </c>
+      <c r="G12" s="87" t="s">
+        <v>172</v>
+      </c>
+      <c r="H12" s="87" t="s">
+        <v>31</v>
+      </c>
+      <c r="I12" s="86" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="18.75">
+      <c r="A13" s="83">
+        <v>45764</v>
+      </c>
+      <c r="B13" s="83" t="s">
+        <v>190</v>
+      </c>
+      <c r="C13" s="83" t="s">
+        <v>209</v>
+      </c>
+      <c r="D13" s="94" t="s">
+        <v>278</v>
+      </c>
+      <c r="E13" s="94">
+        <v>12</v>
+      </c>
+      <c r="F13" s="87" t="s">
+        <v>401</v>
+      </c>
+      <c r="G13" s="87"/>
+      <c r="H13" s="87"/>
+      <c r="I13" s="86"/>
+    </row>
+    <row r="14" spans="1:9" ht="18.75">
+      <c r="A14" s="88">
+        <v>45771</v>
+      </c>
+      <c r="B14" s="88" t="s">
+        <v>190</v>
+      </c>
+      <c r="C14" s="88" t="s">
+        <v>209</v>
+      </c>
+      <c r="D14" s="95" t="s">
+        <v>278</v>
+      </c>
+      <c r="E14" s="95">
+        <v>13</v>
+      </c>
+      <c r="F14" s="90" t="s">
+        <v>402</v>
+      </c>
+      <c r="G14" s="90" t="s">
+        <v>77</v>
+      </c>
+      <c r="H14" s="90" t="s">
+        <v>124</v>
+      </c>
+      <c r="I14" s="89" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="20" spans="8:8" ht="18.75">
+      <c r="H20" s="79"/>
+    </row>
+  </sheetData>
+  <protectedRanges>
+    <protectedRange algorithmName="SHA-512" hashValue="pQyTzP/d7t5ThMimBt5mu8gGozgAm1OwF6BMILsn5/kmtZ5mZf81NMi09wwU8mvtItxf0EVNWa6V4MCa0DKeSQ==" saltValue="NzZBiAQ1yFjat+SeIqh2Uw==" spinCount="100000" sqref="A6:E13" name="Range3_1"/>
+    <protectedRange algorithmName="SHA-512" hashValue="JNB4nrqrfZD45ijUCOmyuk44ibTGOz2xPKKqUb8Fu6IzynfOW0Plt2J4MjvTXFpCm0cEkYqWWfoKwgUFnGztPw==" saltValue="gktf/myRKhBCN9s2pCislA==" spinCount="100000" sqref="A5:I5" name="Range4_1"/>
+    <protectedRange sqref="F6:I13" name="Range8_1"/>
+    <protectedRange algorithmName="SHA-512" hashValue="pQyTzP/d7t5ThMimBt5mu8gGozgAm1OwF6BMILsn5/kmtZ5mZf81NMi09wwU8mvtItxf0EVNWa6V4MCa0DKeSQ==" saltValue="NzZBiAQ1yFjat+SeIqh2Uw==" spinCount="100000" sqref="A14" name="Range3_3"/>
+  </protectedRanges>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y44"/>
@@ -6310,10 +6663,10 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:Y13"/>
+  <dimension ref="A1:Y14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" topLeftCell="E2" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6489,11 +6842,11 @@
         <v>331</v>
       </c>
       <c r="C4" s="26" t="str">
-        <f t="shared" ref="C4:C8" si="0">TEXT(A4, "mmm")</f>
+        <f t="shared" ref="C4:C9" si="0">TEXT(A4, "mmm")</f>
         <v>Feb</v>
       </c>
       <c r="D4" s="27" t="str">
-        <f t="shared" ref="D4:D8" si="1">TEXT(A4, "dddd")</f>
+        <f t="shared" ref="D4:D9" si="1">TEXT(A4, "dddd")</f>
         <v>Tuesday</v>
       </c>
       <c r="E4">
@@ -6688,42 +7041,47 @@
       <c r="X7" s="15"/>
       <c r="Y7" s="13"/>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:25" ht="18" customHeight="1">
       <c r="A8" s="75">
-        <v>46120</v>
+        <f>A7+7</f>
+        <v>46114</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="C8" s="26" t="str">
-        <f t="shared" si="0"/>
-        <v>Apr</v>
-      </c>
-      <c r="D8" s="27" t="str">
-        <f t="shared" si="1"/>
-        <v>Wednesday</v>
+      <c r="C8" s="26" t="s">
+        <v>209</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>278</v>
       </c>
       <c r="E8">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F8" s="16" t="s">
         <v>344</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>77</v>
+        <v>345</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
       <c r="I8" s="98" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="J8" s="98" t="s">
-        <v>342</v>
-      </c>
-      <c r="K8" s="102"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
+        <v>347</v>
+      </c>
+      <c r="K8" s="102" t="s">
+        <v>348</v>
+      </c>
+      <c r="L8" s="24" t="s">
+        <v>349</v>
+      </c>
+      <c r="M8" s="24" t="s">
+        <v>350</v>
+      </c>
       <c r="N8" s="16"/>
       <c r="O8" s="35"/>
       <c r="P8" s="5"/>
@@ -6737,30 +7095,32 @@
       <c r="X8" s="15"/>
       <c r="Y8" s="13"/>
     </row>
-    <row r="9" spans="1:25" ht="18.75" customHeight="1">
+    <row r="9" spans="1:25">
       <c r="A9" s="75">
-        <v>46135</v>
+        <v>46120</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="C9" s="26" t="s">
-        <v>209</v>
-      </c>
-      <c r="D9" s="27" t="s">
-        <v>278</v>
+      <c r="C9" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>Apr</v>
+      </c>
+      <c r="D9" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v>Wednesday</v>
       </c>
       <c r="E9">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>345</v>
+        <v>351</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="I9" s="98" t="s">
         <v>342</v>
@@ -6784,19 +7144,61 @@
       <c r="X9" s="15"/>
       <c r="Y9" s="13"/>
     </row>
-    <row r="10" spans="1:25">
-      <c r="A10" s="26"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
-      <c r="X10" s="20"/>
-      <c r="Y10" s="18"/>
-    </row>
-    <row r="11" spans="1:25" ht="12.75" customHeight="1">
+    <row r="10" spans="1:25" ht="18.75" customHeight="1">
+      <c r="A10" s="75">
+        <v>46135</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>209</v>
+      </c>
+      <c r="D10" s="27" t="s">
+        <v>278</v>
+      </c>
+      <c r="E10">
+        <v>13</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>352</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="I10" s="98" t="s">
+        <v>342</v>
+      </c>
+      <c r="J10" s="98" t="s">
+        <v>342</v>
+      </c>
+      <c r="K10" s="102"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="35"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="5"/>
+      <c r="S10" s="16"/>
+      <c r="T10" s="35"/>
+      <c r="U10" s="5"/>
+      <c r="V10" s="5"/>
+      <c r="W10" s="5"/>
+      <c r="X10" s="15"/>
+      <c r="Y10" s="13"/>
+    </row>
+    <row r="11" spans="1:25">
       <c r="A11" s="26"/>
       <c r="B11" s="26"/>
       <c r="C11" s="26"/>
-    </row>
-    <row r="12" spans="1:25">
+      <c r="X11" s="20"/>
+      <c r="Y11" s="18"/>
+    </row>
+    <row r="12" spans="1:25" ht="12.75" customHeight="1">
       <c r="A12" s="26"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
@@ -6806,15 +7208,25 @@
       <c r="B13" s="26"/>
       <c r="C13" s="26"/>
     </row>
+    <row r="14" spans="1:25">
+      <c r="A14" s="26"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+    </row>
   </sheetData>
   <protectedRanges>
-    <protectedRange algorithmName="SHA-512" hashValue="pQyTzP/d7t5ThMimBt5mu8gGozgAm1OwF6BMILsn5/kmtZ5mZf81NMi09wwU8mvtItxf0EVNWa6V4MCa0DKeSQ==" saltValue="NzZBiAQ1yFjat+SeIqh2Uw==" spinCount="100000" sqref="A3:E13" name="Range3_1"/>
+    <protectedRange algorithmName="SHA-512" hashValue="pQyTzP/d7t5ThMimBt5mu8gGozgAm1OwF6BMILsn5/kmtZ5mZf81NMi09wwU8mvtItxf0EVNWa6V4MCa0DKeSQ==" saltValue="NzZBiAQ1yFjat+SeIqh2Uw==" spinCount="100000" sqref="A3:E14" name="Range3_1"/>
     <protectedRange algorithmName="SHA-512" hashValue="JNB4nrqrfZD45ijUCOmyuk44ibTGOz2xPKKqUb8Fu6IzynfOW0Plt2J4MjvTXFpCm0cEkYqWWfoKwgUFnGztPw==" saltValue="gktf/myRKhBCN9s2pCislA==" spinCount="100000" sqref="A2:L2 N2:Y2" name="Range4_1"/>
-    <protectedRange algorithmName="SHA-512" hashValue="B/N8xqtMc7pXr3rfrr4k91A6IFAPX6lxEHUr9qsJ3yHA+MBnFuw+x27DjsTYKp86iL5C7QQh1TPFTQHueWpZbw==" saltValue="c0IR/echnZmip5yS1t29Rw==" spinCount="100000" sqref="T3:T9" name="Range6_1"/>
-    <protectedRange algorithmName="SHA-512" hashValue="BKDH3ki5lE3XQdc5qZnIH6o8wW8E0PkHgMZFCkv/XYDEa+b/qenui0oReDIqPDXHceUVJ+rEgU3I9CDBHraDYg==" saltValue="ruXqG4NOhhm7cSLor8wHfw==" spinCount="100000" sqref="O2:O9" name="Range7_1"/>
-    <protectedRange sqref="X10:Y10 F3:Y9" name="Range8_1"/>
+    <protectedRange algorithmName="SHA-512" hashValue="B/N8xqtMc7pXr3rfrr4k91A6IFAPX6lxEHUr9qsJ3yHA+MBnFuw+x27DjsTYKp86iL5C7QQh1TPFTQHueWpZbw==" saltValue="c0IR/echnZmip5yS1t29Rw==" spinCount="100000" sqref="T3:T10" name="Range6_1"/>
+    <protectedRange algorithmName="SHA-512" hashValue="BKDH3ki5lE3XQdc5qZnIH6o8wW8E0PkHgMZFCkv/XYDEa+b/qenui0oReDIqPDXHceUVJ+rEgU3I9CDBHraDYg==" saltValue="ruXqG4NOhhm7cSLor8wHfw==" spinCount="100000" sqref="O2:O10" name="Range7_1"/>
+    <protectedRange sqref="X11:Y11 F3:Y10" name="Range8_1"/>
     <protectedRange algorithmName="SHA-512" hashValue="JNB4nrqrfZD45ijUCOmyuk44ibTGOz2xPKKqUb8Fu6IzynfOW0Plt2J4MjvTXFpCm0cEkYqWWfoKwgUFnGztPw==" saltValue="gktf/myRKhBCN9s2pCislA==" spinCount="100000" sqref="M2" name="Range4_1_1"/>
   </protectedRanges>
+  <hyperlinks>
+    <hyperlink ref="L8" r:id="rId1" xr:uid="{A4F5128F-E5C7-4066-B2E0-72C9A9E730AF}"/>
+    <hyperlink ref="M8" r:id="rId2" xr:uid="{58E46CD9-E829-4A89-8A0F-2BA3FCB0FBEC}"/>
+    <hyperlink ref="K8" r:id="rId3" xr:uid="{F42BC370-1CFD-46B8-99BD-1F21405A14EB}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -6961,7 +7373,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="G3" s="14" t="s">
         <v>342</v>
@@ -7012,7 +7424,7 @@
         <v>3</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="G4" s="14" t="s">
         <v>342</v>
@@ -7063,7 +7475,7 @@
         <v>5</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="G5" s="14" t="s">
         <v>342</v>
@@ -7118,7 +7530,7 @@
         <v>7</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="G6" s="14" t="s">
         <v>342</v>
@@ -7169,7 +7581,7 @@
         <v>9</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="G7" s="14" t="s">
         <v>342</v>
@@ -7218,7 +7630,7 @@
         <v>11</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="G8" s="14" t="s">
         <v>342</v>
@@ -7256,7 +7668,7 @@
         <v>190</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>347</v>
+        <v>354</v>
       </c>
       <c r="D9" s="27" t="s">
         <v>278</v>
@@ -7265,7 +7677,7 @@
         <v>13</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="G9" s="14" t="s">
         <v>342</v>
@@ -7348,23 +7760,23 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>348</v>
+        <v>355</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="55" t="s">
-        <v>349</v>
+        <v>356</v>
       </c>
       <c r="B2" s="54" t="s">
-        <v>350</v>
+        <v>357</v>
       </c>
       <c r="C2" s="54" t="s">
-        <v>351</v>
+        <v>358</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="136" t="s">
-        <v>352</v>
+        <v>359</v>
       </c>
       <c r="B3" s="137"/>
       <c r="C3" s="138" t="s">
@@ -7373,7 +7785,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="5" t="s">
-        <v>353</v>
+        <v>360</v>
       </c>
       <c r="B4" s="52"/>
       <c r="C4" s="50" t="s">
@@ -7382,19 +7794,19 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="52" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="B5" s="52"/>
       <c r="C5" s="50" t="s">
-        <v>355</v>
+        <v>362</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="52" t="s">
-        <v>356</v>
+        <v>363</v>
       </c>
       <c r="B6" s="52" t="s">
-        <v>357</v>
+        <v>364</v>
       </c>
       <c r="C6" s="50" t="s">
         <v>87</v>
@@ -7402,10 +7814,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="52" t="s">
-        <v>358</v>
+        <v>365</v>
       </c>
       <c r="B7" s="52" t="s">
-        <v>359</v>
+        <v>366</v>
       </c>
       <c r="C7" s="50" t="s">
         <v>87</v>
@@ -7413,10 +7825,10 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="52" t="s">
-        <v>360</v>
+        <v>367</v>
       </c>
       <c r="B8" s="52" t="s">
-        <v>361</v>
+        <v>368</v>
       </c>
       <c r="C8" s="50" t="s">
         <v>101</v>
@@ -7424,75 +7836,75 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="52" t="s">
-        <v>362</v>
+        <v>369</v>
       </c>
       <c r="B9" s="52"/>
       <c r="C9" s="50"/>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="52" t="s">
-        <v>363</v>
+        <v>370</v>
       </c>
       <c r="B10" s="52" t="s">
-        <v>364</v>
+        <v>371</v>
       </c>
       <c r="C10" s="50" t="s">
-        <v>365</v>
+        <v>372</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="52" t="s">
-        <v>366</v>
+        <v>373</v>
       </c>
       <c r="B11" s="52" t="s">
-        <v>367</v>
+        <v>374</v>
       </c>
       <c r="C11" s="50" t="s">
-        <v>368</v>
+        <v>375</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="52" t="s">
-        <v>369</v>
+        <v>376</v>
       </c>
       <c r="B12" s="52" t="s">
-        <v>370</v>
+        <v>377</v>
       </c>
       <c r="C12" s="50" t="s">
-        <v>368</v>
+        <v>375</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="52" t="s">
-        <v>371</v>
+        <v>378</v>
       </c>
       <c r="B13" s="52" t="s">
-        <v>372</v>
+        <v>379</v>
       </c>
       <c r="C13" s="50" t="s">
-        <v>368</v>
+        <v>375</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="52" t="s">
-        <v>373</v>
+        <v>380</v>
       </c>
       <c r="B14" s="52" t="s">
-        <v>374</v>
+        <v>381</v>
       </c>
       <c r="C14" s="50" t="s">
-        <v>368</v>
+        <v>375</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="52" t="s">
+        <v>382</v>
+      </c>
+      <c r="B15" s="52" t="s">
+        <v>383</v>
+      </c>
+      <c r="C15" s="50" t="s">
         <v>375</v>
-      </c>
-      <c r="B15" s="52" t="s">
-        <v>376</v>
-      </c>
-      <c r="C15" s="50" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -7500,29 +7912,29 @@
         <v>321</v>
       </c>
       <c r="B16" s="137" t="s">
-        <v>377</v>
+        <v>384</v>
       </c>
       <c r="C16" s="139" t="s">
-        <v>378</v>
+        <v>385</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="52" t="s">
-        <v>379</v>
+        <v>386</v>
       </c>
       <c r="B17" s="52" t="s">
-        <v>380</v>
+        <v>387</v>
       </c>
       <c r="C17" s="50" t="s">
-        <v>378</v>
+        <v>385</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="52" t="s">
-        <v>381</v>
+        <v>388</v>
       </c>
       <c r="B18" s="52" t="s">
-        <v>357</v>
+        <v>364</v>
       </c>
       <c r="C18" s="50" t="s">
         <v>87</v>
@@ -7530,26 +7942,26 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="53" t="s">
-        <v>382</v>
+        <v>389</v>
       </c>
       <c r="B19" s="53" t="s">
         <v>230</v>
       </c>
       <c r="C19" s="51" t="s">
-        <v>383</v>
+        <v>390</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>384</v>
+        <v>391</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>381</v>
+        <v>388</v>
       </c>
       <c r="B24" t="s">
-        <v>357</v>
+        <v>364</v>
       </c>
       <c r="C24" t="s">
         <v>87</v>
@@ -7557,13 +7969,13 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>382</v>
+        <v>389</v>
       </c>
       <c r="B25" t="s">
         <v>230</v>
       </c>
       <c r="C25" t="s">
-        <v>383</v>
+        <v>390</v>
       </c>
     </row>
   </sheetData>
@@ -7578,10 +7990,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AD19DE5-C22F-4D41-B540-76D70438E18B}">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A7" sqref="A7:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7590,356 +8002,236 @@
     <col min="6" max="6" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1">
+    <row r="1" spans="1:9" ht="15.75" thickBot="1">
       <c r="A1" s="135" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="131" t="s">
-        <v>385</v>
+        <v>392</v>
       </c>
       <c r="C1" s="130" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="15.75" thickTop="1">
-      <c r="A2" s="133">
-        <v>45911</v>
-      </c>
-      <c r="B2" s="134">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="170">
+        <v>46051</v>
+      </c>
+      <c r="B2" s="171">
         <v>1</v>
       </c>
-      <c r="C2" s="134" t="s">
-        <v>387</v>
-      </c>
-      <c r="F2" s="75">
-        <v>45911</v>
-      </c>
-      <c r="G2" s="77" t="s">
-        <v>190</v>
-      </c>
-      <c r="H2" s="29" t="str">
-        <f>TEXT(F2, "mmm")</f>
-        <v>Sep</v>
-      </c>
-      <c r="I2" s="55" t="str">
-        <f>TEXT(F2, "dddd")</f>
-        <v>Thursday</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="133">
+      <c r="C2" s="171" t="s">
+        <v>394</v>
+      </c>
+      <c r="F2" s="75"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="55"/>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="172">
         <f>A2+7</f>
-        <v>45918</v>
-      </c>
-      <c r="B3" s="134">
+        <v>46058</v>
+      </c>
+      <c r="B3" s="171">
         <f>B2+1</f>
         <v>2</v>
       </c>
-      <c r="C3" s="134" t="s">
-        <v>387</v>
-      </c>
-      <c r="F3" s="75">
-        <v>45926</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="H3" s="26" t="str">
-        <f>TEXT(F3, "mmm")</f>
-        <v>Sep</v>
-      </c>
-      <c r="I3" s="27" t="str">
-        <f>TEXT(F3, "dddd")</f>
-        <v>Friday</v>
-      </c>
-      <c r="J3">
-        <f>J2+2</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="133">
+      <c r="C3" s="171" t="s">
+        <v>353</v>
+      </c>
+      <c r="F3" s="75"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="27"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="172">
         <f t="shared" ref="A4:A12" si="0">A3+7</f>
-        <v>45925</v>
-      </c>
-      <c r="B4" s="134">
+        <v>46065</v>
+      </c>
+      <c r="B4" s="171">
         <f t="shared" ref="B4:B11" si="1">B3+1</f>
         <v>3</v>
       </c>
-      <c r="C4" s="134" t="s">
-        <v>387</v>
-      </c>
-      <c r="F4" s="75">
-        <v>45939</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="H4" s="26" t="str">
-        <f t="shared" ref="H4" si="2">TEXT(F4, "mmm")</f>
-        <v>Oct</v>
-      </c>
-      <c r="I4" s="27" t="str">
-        <f t="shared" ref="I4" si="3">TEXT(F4, "dddd")</f>
-        <v>Thursday</v>
-      </c>
-      <c r="J4">
-        <f>J3+2</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="133">
+      <c r="C4" s="171" t="s">
+        <v>394</v>
+      </c>
+      <c r="F4" s="75"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="27"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="172">
         <f t="shared" si="0"/>
-        <v>45932</v>
-      </c>
-      <c r="B5" s="134">
+        <v>46072</v>
+      </c>
+      <c r="B5" s="171">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="C5" s="134" t="s">
-        <v>387</v>
-      </c>
-      <c r="F5" s="75">
-        <v>45946</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="H5" s="26" t="s">
-        <v>277</v>
-      </c>
-      <c r="I5" s="27" t="s">
-        <v>278</v>
-      </c>
-      <c r="J5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="C5" s="171" t="s">
+        <v>353</v>
+      </c>
+      <c r="F5" s="75"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="27"/>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="133">
         <f t="shared" si="0"/>
-        <v>45939</v>
+        <v>46079</v>
       </c>
       <c r="B6" s="134">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="C6" s="134" t="s">
-        <v>387</v>
-      </c>
-      <c r="F6" s="75">
-        <v>45953</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="H6" s="26" t="str">
-        <f>TEXT(F6, "mmm")</f>
-        <v>Oct</v>
-      </c>
-      <c r="I6" s="27" t="str">
-        <f>TEXT(F6, "dddd")</f>
-        <v>Thursday</v>
-      </c>
-      <c r="J6">
-        <f>J4+2</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+        <v>394</v>
+      </c>
+      <c r="F6" s="75"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="27"/>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="133">
         <f t="shared" si="0"/>
-        <v>45946</v>
+        <v>46086</v>
       </c>
       <c r="B7" s="134">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="C7" s="134" t="s">
-        <v>346</v>
-      </c>
-      <c r="F7" s="75">
-        <v>45967</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="H7" s="26" t="str">
-        <f>TEXT(F7, "mmm")</f>
-        <v>Nov</v>
-      </c>
-      <c r="I7" s="27" t="str">
-        <f>TEXT(F7, "dddd")</f>
-        <v>Thursday</v>
-      </c>
-      <c r="J7">
-        <f>J6+2</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
+        <v>353</v>
+      </c>
+      <c r="F7" s="75"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="27"/>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="133">
         <f t="shared" si="0"/>
-        <v>45953</v>
+        <v>46093</v>
       </c>
       <c r="B8" s="134">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="C8" s="134" t="s">
-        <v>388</v>
-      </c>
-      <c r="F8" s="75">
-        <v>45974</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="H8" s="26" t="str">
-        <f>TEXT(F8, "mmm")</f>
-        <v>Nov</v>
-      </c>
-      <c r="I8" s="27" t="str">
-        <f>TEXT(F8, "dddd")</f>
-        <v>Thursday</v>
-      </c>
-      <c r="J8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
+        <v>395</v>
+      </c>
+      <c r="F8" s="75"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="27"/>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="133">
         <f t="shared" si="0"/>
-        <v>45960</v>
+        <v>46100</v>
       </c>
       <c r="B9" s="134">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="C9" s="134" t="s">
-        <v>387</v>
-      </c>
-      <c r="F9" s="75">
-        <v>45981</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="H9" s="26" t="str">
-        <f>TEXT(F9, "mmm")</f>
-        <v>Nov</v>
-      </c>
-      <c r="I9" s="27" t="str">
-        <f>TEXT(F9, "dddd")</f>
-        <v>Thursday</v>
-      </c>
-      <c r="J9">
-        <f>J7+2</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
+        <v>353</v>
+      </c>
+      <c r="F9" s="75"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="27"/>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="133">
         <f t="shared" si="0"/>
-        <v>45967</v>
+        <v>46107</v>
       </c>
       <c r="B10" s="134">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="C10" s="134" t="s">
-        <v>388</v>
-      </c>
-      <c r="F10" s="75">
-        <v>45995</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="H10" s="26" t="str">
-        <f>TEXT(F10, "mmm")</f>
-        <v>Dec</v>
-      </c>
-      <c r="I10" s="27" t="str">
-        <f>TEXT(F10, "dddd")</f>
-        <v>Thursday</v>
-      </c>
-      <c r="J10">
-        <f t="shared" ref="J10" si="4">J9+2</f>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
+        <v>395</v>
+      </c>
+      <c r="F10" s="75"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="27"/>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" s="133">
         <f t="shared" si="0"/>
-        <v>45974</v>
+        <v>46114</v>
       </c>
       <c r="B11" s="134">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="C11" s="134" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" s="133">
         <f t="shared" si="0"/>
-        <v>45981</v>
+        <v>46121</v>
       </c>
       <c r="B12" s="134">
-        <f t="shared" ref="B12:B14" si="5">B11+1</f>
+        <f t="shared" ref="B12:B14" si="2">B11+1</f>
         <v>11</v>
       </c>
       <c r="C12" s="134" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" s="133">
-        <f t="shared" ref="A13:A14" si="6">A12+7</f>
-        <v>45988</v>
+        <f t="shared" ref="A13:A14" si="3">A12+7</f>
+        <v>46128</v>
       </c>
       <c r="B13" s="134">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="C13" s="134" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" s="133">
-        <f t="shared" si="6"/>
-        <v>45995</v>
+        <f t="shared" si="3"/>
+        <v>46135</v>
       </c>
       <c r="B14" s="134">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="C14" s="134" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" s="133"/>
       <c r="B15" s="134"/>
       <c r="C15" s="134"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:9">
       <c r="G16" s="26"/>
     </row>
   </sheetData>
   <protectedRanges>
     <protectedRange algorithmName="SHA-512" hashValue="pQyTzP/d7t5ThMimBt5mu8gGozgAm1OwF6BMILsn5/kmtZ5mZf81NMi09wwU8mvtItxf0EVNWa6V4MCa0DKeSQ==" saltValue="NzZBiAQ1yFjat+SeIqh2Uw==" spinCount="100000" sqref="B2:B14" name="Range3"/>
     <protectedRange algorithmName="SHA-512" hashValue="JNB4nrqrfZD45ijUCOmyuk44ibTGOz2xPKKqUb8Fu6IzynfOW0Plt2J4MjvTXFpCm0cEkYqWWfoKwgUFnGztPw==" saltValue="gktf/myRKhBCN9s2pCislA==" spinCount="100000" sqref="B1" name="Range4"/>
-    <protectedRange algorithmName="SHA-512" hashValue="pQyTzP/d7t5ThMimBt5mu8gGozgAm1OwF6BMILsn5/kmtZ5mZf81NMi09wwU8mvtItxf0EVNWa6V4MCa0DKeSQ==" saltValue="NzZBiAQ1yFjat+SeIqh2Uw==" spinCount="100000" sqref="F2:J10" name="Range3_1"/>
+    <protectedRange algorithmName="SHA-512" hashValue="pQyTzP/d7t5ThMimBt5mu8gGozgAm1OwF6BMILsn5/kmtZ5mZf81NMi09wwU8mvtItxf0EVNWa6V4MCa0DKeSQ==" saltValue="NzZBiAQ1yFjat+SeIqh2Uw==" spinCount="100000" sqref="F9:J10" name="Range3_1"/>
+    <protectedRange algorithmName="SHA-512" hashValue="pQyTzP/d7t5ThMimBt5mu8gGozgAm1OwF6BMILsn5/kmtZ5mZf81NMi09wwU8mvtItxf0EVNWa6V4MCa0DKeSQ==" saltValue="NzZBiAQ1yFjat+SeIqh2Uw==" spinCount="100000" sqref="F2:J8 A2" name="Range3_1_1"/>
   </protectedRanges>
-  <conditionalFormatting sqref="A2:C14">
+  <conditionalFormatting sqref="A3:C14 B2:C2">
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Taken">
       <formula>NOT(ISERROR(SEARCH("Taken",A2)))</formula>
     </cfRule>
@@ -7954,321 +8246,15 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2BB5C5F-5790-4A91-A6E8-8841719DA1FC}">
-  <dimension ref="A2:I20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F91336BB-C868-4318-AE9D-93A4F8F322FF}">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8:H8"/>
+      <selection sqref="A1:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.7109375" customWidth="1"/>
-    <col min="7" max="7" width="38.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.42578125" customWidth="1"/>
-    <col min="9" max="9" width="64.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:9" ht="23.25">
-      <c r="A2" s="91" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="18.75">
-      <c r="A3" s="79" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="37.5">
-      <c r="A5" s="80" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="80" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="80" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="80" t="s">
-        <v>137</v>
-      </c>
-      <c r="E5" s="80" t="s">
-        <v>189</v>
-      </c>
-      <c r="F5" s="80" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" s="80" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" s="82" t="s">
-        <v>391</v>
-      </c>
-      <c r="I5" s="81" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="18.75">
-      <c r="A6" s="92">
-        <v>45694</v>
-      </c>
-      <c r="B6" s="92" t="s">
-        <v>190</v>
-      </c>
-      <c r="C6" s="92" t="s">
-        <v>191</v>
-      </c>
-      <c r="D6" s="93" t="s">
-        <v>278</v>
-      </c>
-      <c r="E6" s="93">
-        <v>2</v>
-      </c>
-      <c r="F6" s="85" t="s">
-        <v>40</v>
-      </c>
-      <c r="G6" s="85" t="s">
-        <v>68</v>
-      </c>
-      <c r="H6" s="85"/>
-      <c r="I6" s="84" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="18.75">
-      <c r="A7" s="83">
-        <v>45708</v>
-      </c>
-      <c r="B7" s="83" t="s">
-        <v>190</v>
-      </c>
-      <c r="C7" s="83" t="s">
-        <v>191</v>
-      </c>
-      <c r="D7" s="94" t="s">
-        <v>278</v>
-      </c>
-      <c r="E7" s="94">
-        <v>4</v>
-      </c>
-      <c r="F7" s="87" t="s">
-        <v>194</v>
-      </c>
-      <c r="G7" s="87" t="s">
-        <v>195</v>
-      </c>
-      <c r="H7" s="87" t="s">
-        <v>78</v>
-      </c>
-      <c r="I7" s="86" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="18.75">
-      <c r="A8" s="83">
-        <v>45722</v>
-      </c>
-      <c r="B8" s="83" t="s">
-        <v>190</v>
-      </c>
-      <c r="C8" s="83" t="s">
-        <v>198</v>
-      </c>
-      <c r="D8" s="94" t="s">
-        <v>278</v>
-      </c>
-      <c r="E8" s="94">
-        <v>6</v>
-      </c>
-      <c r="F8" s="87" t="s">
-        <v>199</v>
-      </c>
-      <c r="G8" s="87" t="s">
-        <v>68</v>
-      </c>
-      <c r="H8" s="87" t="s">
-        <v>200</v>
-      </c>
-      <c r="I8" s="86"/>
-    </row>
-    <row r="9" spans="1:9" ht="18.75">
-      <c r="A9" s="83">
-        <v>45735</v>
-      </c>
-      <c r="B9" s="83" t="s">
-        <v>139</v>
-      </c>
-      <c r="C9" s="83" t="s">
-        <v>198</v>
-      </c>
-      <c r="D9" s="94" t="s">
-        <v>392</v>
-      </c>
-      <c r="E9" s="94">
-        <v>8</v>
-      </c>
-      <c r="F9" s="87" t="s">
-        <v>204</v>
-      </c>
-      <c r="G9" s="87" t="s">
-        <v>205</v>
-      </c>
-      <c r="H9" s="87" t="s">
-        <v>206</v>
-      </c>
-      <c r="I9" s="86" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="18.75">
-      <c r="A10" s="83">
-        <v>45744</v>
-      </c>
-      <c r="B10" s="83" t="s">
-        <v>190</v>
-      </c>
-      <c r="C10" s="83" t="s">
-        <v>198</v>
-      </c>
-      <c r="D10" s="94" t="s">
-        <v>214</v>
-      </c>
-      <c r="E10" s="94">
-        <v>9</v>
-      </c>
-      <c r="F10" s="87" t="s">
-        <v>222</v>
-      </c>
-      <c r="G10" s="87" t="s">
-        <v>223</v>
-      </c>
-      <c r="H10" s="87" t="s">
-        <v>224</v>
-      </c>
-      <c r="I10" s="86"/>
-    </row>
-    <row r="11" spans="1:9" ht="18.75">
-      <c r="A11" s="83">
-        <v>45750</v>
-      </c>
-      <c r="B11" s="83" t="s">
-        <v>190</v>
-      </c>
-      <c r="C11" s="83" t="s">
-        <v>209</v>
-      </c>
-      <c r="D11" s="94" t="s">
-        <v>278</v>
-      </c>
-      <c r="E11" s="94">
-        <v>10</v>
-      </c>
-      <c r="F11" s="87" t="s">
-        <v>393</v>
-      </c>
-      <c r="G11" s="87" t="s">
-        <v>68</v>
-      </c>
-      <c r="H11" s="87"/>
-      <c r="I11" s="86" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="18.75">
-      <c r="A12" s="83">
-        <v>45758</v>
-      </c>
-      <c r="B12" s="83" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="83" t="s">
-        <v>209</v>
-      </c>
-      <c r="D12" s="94" t="s">
-        <v>214</v>
-      </c>
-      <c r="E12" s="94">
-        <v>11</v>
-      </c>
-      <c r="F12" s="87" t="s">
-        <v>229</v>
-      </c>
-      <c r="G12" s="87" t="s">
-        <v>172</v>
-      </c>
-      <c r="H12" s="87" t="s">
-        <v>31</v>
-      </c>
-      <c r="I12" s="86" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="18.75">
-      <c r="A13" s="83">
-        <v>45764</v>
-      </c>
-      <c r="B13" s="83" t="s">
-        <v>190</v>
-      </c>
-      <c r="C13" s="83" t="s">
-        <v>209</v>
-      </c>
-      <c r="D13" s="94" t="s">
-        <v>278</v>
-      </c>
-      <c r="E13" s="94">
-        <v>12</v>
-      </c>
-      <c r="F13" s="87" t="s">
-        <v>394</v>
-      </c>
-      <c r="G13" s="87"/>
-      <c r="H13" s="87"/>
-      <c r="I13" s="86"/>
-    </row>
-    <row r="14" spans="1:9" ht="18.75">
-      <c r="A14" s="88">
-        <v>45771</v>
-      </c>
-      <c r="B14" s="88" t="s">
-        <v>190</v>
-      </c>
-      <c r="C14" s="88" t="s">
-        <v>209</v>
-      </c>
-      <c r="D14" s="95" t="s">
-        <v>278</v>
-      </c>
-      <c r="E14" s="95">
-        <v>13</v>
-      </c>
-      <c r="F14" s="90" t="s">
-        <v>395</v>
-      </c>
-      <c r="G14" s="90" t="s">
-        <v>77</v>
-      </c>
-      <c r="H14" s="90" t="s">
-        <v>124</v>
-      </c>
-      <c r="I14" s="89" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="20" spans="8:8" ht="18.75">
-      <c r="H20" s="79"/>
-    </row>
-  </sheetData>
-  <protectedRanges>
-    <protectedRange algorithmName="SHA-512" hashValue="pQyTzP/d7t5ThMimBt5mu8gGozgAm1OwF6BMILsn5/kmtZ5mZf81NMi09wwU8mvtItxf0EVNWa6V4MCa0DKeSQ==" saltValue="NzZBiAQ1yFjat+SeIqh2Uw==" spinCount="100000" sqref="A6:E13" name="Range3_1"/>
-    <protectedRange algorithmName="SHA-512" hashValue="JNB4nrqrfZD45ijUCOmyuk44ibTGOz2xPKKqUb8Fu6IzynfOW0Plt2J4MjvTXFpCm0cEkYqWWfoKwgUFnGztPw==" saltValue="gktf/myRKhBCN9s2pCislA==" spinCount="100000" sqref="A5:I5" name="Range4_1"/>
-    <protectedRange sqref="F6:I13" name="Range8_1"/>
-    <protectedRange algorithmName="SHA-512" hashValue="pQyTzP/d7t5ThMimBt5mu8gGozgAm1OwF6BMILsn5/kmtZ5mZf81NMi09wwU8mvtItxf0EVNWa6V4MCa0DKeSQ==" saltValue="NzZBiAQ1yFjat+SeIqh2Uw==" spinCount="100000" sqref="A14" name="Range3_3"/>
-  </protectedRanges>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>